<commit_message>
read intro to rl till section 5.5
</commit_message>
<xml_diff>
--- a/thesis gantt chart.xlsx
+++ b/thesis gantt chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\OneDrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wings_stuff\srus\TUD\yr5\thesis\thesis_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E68A67B-2D89-402A-A265-77ADC60CFD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB7A9A6-9E09-4B81-AA1A-3EBDE04D4AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="3552" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -430,7 +430,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="159">
   <si>
     <t>WBS</t>
   </si>
@@ -1538,10 +1538,13 @@
     <t>read Barto &amp; Sutton</t>
   </si>
   <si>
-    <t>study flying V (literature TBD)</t>
+    <t>noting Willems' thesis, compiling list of RL MSc theses</t>
   </si>
   <si>
-    <t>noting Willems' thesis, compiling list of RL MSc theses</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>study flying V</t>
   </si>
 </sst>
 </file>
@@ -3245,15 +3248,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="70" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3266,7 +3260,28 @@
     <xf numFmtId="167" fontId="52" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="84" fillId="24" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -3303,18 +3318,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3509,13 +3512,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>192260</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>76041</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>186690</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3574,7 +3577,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
+          <xdr:colOff>110490</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -4159,7 +4162,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U12" sqref="U12"/>
+      <selection pane="bottomLeft" activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4236,21 +4239,21 @@
       <c r="K1" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="164"/>
-      <c r="AE1" s="164"/>
-      <c r="AF1" s="164"/>
-      <c r="AG1" s="164"/>
-      <c r="AH1" s="164"/>
-      <c r="AI1" s="164"/>
-      <c r="AJ1" s="164"/>
-      <c r="AK1" s="164"/>
-      <c r="AL1" s="164"/>
-      <c r="AM1" s="164"/>
-      <c r="AN1" s="164"/>
-      <c r="AO1" s="164"/>
-      <c r="AP1" s="164"/>
-      <c r="AQ1" s="164"/>
-      <c r="AR1" s="164"/>
+      <c r="AD1" s="168"/>
+      <c r="AE1" s="168"/>
+      <c r="AF1" s="168"/>
+      <c r="AG1" s="168"/>
+      <c r="AH1" s="168"/>
+      <c r="AI1" s="168"/>
+      <c r="AJ1" s="168"/>
+      <c r="AK1" s="168"/>
+      <c r="AL1" s="168"/>
+      <c r="AM1" s="168"/>
+      <c r="AN1" s="168"/>
+      <c r="AO1" s="168"/>
+      <c r="AP1" s="168"/>
+      <c r="AQ1" s="168"/>
+      <c r="AR1" s="168"/>
     </row>
     <row r="2" spans="1:255" s="59" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="112" t="s">
@@ -4330,729 +4333,729 @@
       <c r="B4" s="113" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="167">
+      <c r="C4" s="171">
         <v>45295</v>
       </c>
-      <c r="D4" s="168"/>
-      <c r="E4" s="169"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="173"/>
       <c r="H4" s="113" t="s">
         <v>72</v>
       </c>
       <c r="I4" s="114">
         <v>1</v>
       </c>
-      <c r="K4" s="159"/>
-      <c r="L4" s="160"/>
-      <c r="M4" s="160"/>
-      <c r="N4" s="160"/>
-      <c r="O4" s="160"/>
-      <c r="P4" s="160"/>
-      <c r="Q4" s="161"/>
-      <c r="R4" s="159" t="str">
+      <c r="K4" s="156"/>
+      <c r="L4" s="157"/>
+      <c r="M4" s="157"/>
+      <c r="N4" s="157"/>
+      <c r="O4" s="157"/>
+      <c r="P4" s="157"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="156" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="S4" s="160"/>
-      <c r="T4" s="160"/>
-      <c r="U4" s="160"/>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="159" t="str">
+      <c r="S4" s="157"/>
+      <c r="T4" s="157"/>
+      <c r="U4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="158"/>
+      <c r="Y4" s="156" t="str">
         <f t="shared" ref="Y4" si="0">"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="Z4" s="160"/>
-      <c r="AA4" s="160"/>
-      <c r="AB4" s="160"/>
-      <c r="AC4" s="160"/>
-      <c r="AD4" s="160"/>
-      <c r="AE4" s="161"/>
-      <c r="AF4" s="159" t="str">
+      <c r="Z4" s="157"/>
+      <c r="AA4" s="157"/>
+      <c r="AB4" s="157"/>
+      <c r="AC4" s="157"/>
+      <c r="AD4" s="157"/>
+      <c r="AE4" s="158"/>
+      <c r="AF4" s="156" t="str">
         <f t="shared" ref="AF4" si="1">"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="AG4" s="160"/>
-      <c r="AH4" s="160"/>
-      <c r="AI4" s="160"/>
-      <c r="AJ4" s="160"/>
-      <c r="AK4" s="160"/>
-      <c r="AL4" s="161"/>
-      <c r="AM4" s="159" t="str">
+      <c r="AG4" s="157"/>
+      <c r="AH4" s="157"/>
+      <c r="AI4" s="157"/>
+      <c r="AJ4" s="157"/>
+      <c r="AK4" s="157"/>
+      <c r="AL4" s="158"/>
+      <c r="AM4" s="156" t="str">
         <f t="shared" ref="AM4" si="2">"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AN4" s="160"/>
-      <c r="AO4" s="160"/>
-      <c r="AP4" s="160"/>
-      <c r="AQ4" s="160"/>
-      <c r="AR4" s="160"/>
-      <c r="AS4" s="161"/>
-      <c r="AT4" s="159" t="str">
+      <c r="AN4" s="157"/>
+      <c r="AO4" s="157"/>
+      <c r="AP4" s="157"/>
+      <c r="AQ4" s="157"/>
+      <c r="AR4" s="157"/>
+      <c r="AS4" s="158"/>
+      <c r="AT4" s="156" t="str">
         <f t="shared" ref="AT4" si="3">"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AU4" s="160"/>
-      <c r="AV4" s="160"/>
-      <c r="AW4" s="160"/>
-      <c r="AX4" s="160"/>
-      <c r="AY4" s="160"/>
-      <c r="AZ4" s="161"/>
-      <c r="BA4" s="159" t="str">
+      <c r="AU4" s="157"/>
+      <c r="AV4" s="157"/>
+      <c r="AW4" s="157"/>
+      <c r="AX4" s="157"/>
+      <c r="AY4" s="157"/>
+      <c r="AZ4" s="158"/>
+      <c r="BA4" s="156" t="str">
         <f t="shared" ref="BA4" si="4">"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="BB4" s="160"/>
-      <c r="BC4" s="160"/>
-      <c r="BD4" s="160"/>
-      <c r="BE4" s="160"/>
-      <c r="BF4" s="160"/>
-      <c r="BG4" s="161"/>
-      <c r="BH4" s="159" t="str">
+      <c r="BB4" s="157"/>
+      <c r="BC4" s="157"/>
+      <c r="BD4" s="157"/>
+      <c r="BE4" s="157"/>
+      <c r="BF4" s="157"/>
+      <c r="BG4" s="158"/>
+      <c r="BH4" s="156" t="str">
         <f t="shared" ref="BH4" si="5">"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BI4" s="160"/>
-      <c r="BJ4" s="160"/>
-      <c r="BK4" s="160"/>
-      <c r="BL4" s="160"/>
-      <c r="BM4" s="160"/>
-      <c r="BN4" s="161"/>
-      <c r="BO4" s="159" t="str">
+      <c r="BI4" s="157"/>
+      <c r="BJ4" s="157"/>
+      <c r="BK4" s="157"/>
+      <c r="BL4" s="157"/>
+      <c r="BM4" s="157"/>
+      <c r="BN4" s="158"/>
+      <c r="BO4" s="156" t="str">
         <f t="shared" ref="BO4" si="6">"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BP4" s="160"/>
-      <c r="BQ4" s="160"/>
-      <c r="BR4" s="160"/>
-      <c r="BS4" s="160"/>
-      <c r="BT4" s="160"/>
-      <c r="BU4" s="161"/>
-      <c r="BV4" s="159" t="str">
+      <c r="BP4" s="157"/>
+      <c r="BQ4" s="157"/>
+      <c r="BR4" s="157"/>
+      <c r="BS4" s="157"/>
+      <c r="BT4" s="157"/>
+      <c r="BU4" s="158"/>
+      <c r="BV4" s="156" t="str">
         <f t="shared" ref="BV4" si="7">"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BW4" s="160"/>
-      <c r="BX4" s="160"/>
-      <c r="BY4" s="160"/>
-      <c r="BZ4" s="160"/>
-      <c r="CA4" s="160"/>
-      <c r="CB4" s="161"/>
-      <c r="CC4" s="159" t="str">
+      <c r="BW4" s="157"/>
+      <c r="BX4" s="157"/>
+      <c r="BY4" s="157"/>
+      <c r="BZ4" s="157"/>
+      <c r="CA4" s="157"/>
+      <c r="CB4" s="158"/>
+      <c r="CC4" s="156" t="str">
         <f t="shared" ref="CC4" si="8">"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="CD4" s="160"/>
-      <c r="CE4" s="160"/>
-      <c r="CF4" s="160"/>
-      <c r="CG4" s="160"/>
-      <c r="CH4" s="160"/>
-      <c r="CI4" s="161"/>
-      <c r="CJ4" s="159" t="str">
+      <c r="CD4" s="157"/>
+      <c r="CE4" s="157"/>
+      <c r="CF4" s="157"/>
+      <c r="CG4" s="157"/>
+      <c r="CH4" s="157"/>
+      <c r="CI4" s="158"/>
+      <c r="CJ4" s="156" t="str">
         <f t="shared" ref="CJ4" si="9">"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CK4" s="160"/>
-      <c r="CL4" s="160"/>
-      <c r="CM4" s="160"/>
-      <c r="CN4" s="160"/>
-      <c r="CO4" s="160"/>
-      <c r="CP4" s="161"/>
-      <c r="CQ4" s="159" t="str">
+      <c r="CK4" s="157"/>
+      <c r="CL4" s="157"/>
+      <c r="CM4" s="157"/>
+      <c r="CN4" s="157"/>
+      <c r="CO4" s="157"/>
+      <c r="CP4" s="158"/>
+      <c r="CQ4" s="156" t="str">
         <f t="shared" ref="CQ4" si="10">"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CR4" s="160"/>
-      <c r="CS4" s="160"/>
-      <c r="CT4" s="160"/>
-      <c r="CU4" s="160"/>
-      <c r="CV4" s="160"/>
-      <c r="CW4" s="161"/>
-      <c r="CX4" s="159" t="str">
+      <c r="CR4" s="157"/>
+      <c r="CS4" s="157"/>
+      <c r="CT4" s="157"/>
+      <c r="CU4" s="157"/>
+      <c r="CV4" s="157"/>
+      <c r="CW4" s="158"/>
+      <c r="CX4" s="156" t="str">
         <f t="shared" ref="CX4" si="11">"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="CY4" s="160"/>
-      <c r="CZ4" s="160"/>
-      <c r="DA4" s="160"/>
-      <c r="DB4" s="160"/>
-      <c r="DC4" s="160"/>
-      <c r="DD4" s="161"/>
-      <c r="DE4" s="159" t="str">
+      <c r="CY4" s="157"/>
+      <c r="CZ4" s="157"/>
+      <c r="DA4" s="157"/>
+      <c r="DB4" s="157"/>
+      <c r="DC4" s="157"/>
+      <c r="DD4" s="158"/>
+      <c r="DE4" s="156" t="str">
         <f t="shared" ref="DE4" si="12">"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="DF4" s="160"/>
-      <c r="DG4" s="160"/>
-      <c r="DH4" s="160"/>
-      <c r="DI4" s="160"/>
-      <c r="DJ4" s="160"/>
-      <c r="DK4" s="161"/>
-      <c r="DL4" s="159" t="str">
+      <c r="DF4" s="157"/>
+      <c r="DG4" s="157"/>
+      <c r="DH4" s="157"/>
+      <c r="DI4" s="157"/>
+      <c r="DJ4" s="157"/>
+      <c r="DK4" s="158"/>
+      <c r="DL4" s="156" t="str">
         <f t="shared" ref="DL4" si="13">"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 15</v>
       </c>
-      <c r="DM4" s="160"/>
-      <c r="DN4" s="160"/>
-      <c r="DO4" s="160"/>
-      <c r="DP4" s="160"/>
-      <c r="DQ4" s="160"/>
-      <c r="DR4" s="161"/>
-      <c r="DS4" s="159" t="str">
+      <c r="DM4" s="157"/>
+      <c r="DN4" s="157"/>
+      <c r="DO4" s="157"/>
+      <c r="DP4" s="157"/>
+      <c r="DQ4" s="157"/>
+      <c r="DR4" s="158"/>
+      <c r="DS4" s="156" t="str">
         <f t="shared" ref="DS4" si="14">"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 16</v>
       </c>
-      <c r="DT4" s="160"/>
-      <c r="DU4" s="160"/>
-      <c r="DV4" s="160"/>
-      <c r="DW4" s="160"/>
-      <c r="DX4" s="160"/>
-      <c r="DY4" s="161"/>
-      <c r="DZ4" s="159" t="str">
+      <c r="DT4" s="157"/>
+      <c r="DU4" s="157"/>
+      <c r="DV4" s="157"/>
+      <c r="DW4" s="157"/>
+      <c r="DX4" s="157"/>
+      <c r="DY4" s="158"/>
+      <c r="DZ4" s="156" t="str">
         <f t="shared" ref="DZ4" si="15">"Week "&amp;(DS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 17</v>
       </c>
-      <c r="EA4" s="160"/>
-      <c r="EB4" s="160"/>
-      <c r="EC4" s="160"/>
-      <c r="ED4" s="160"/>
-      <c r="EE4" s="160"/>
-      <c r="EF4" s="161"/>
-      <c r="EG4" s="159" t="str">
+      <c r="EA4" s="157"/>
+      <c r="EB4" s="157"/>
+      <c r="EC4" s="157"/>
+      <c r="ED4" s="157"/>
+      <c r="EE4" s="157"/>
+      <c r="EF4" s="158"/>
+      <c r="EG4" s="156" t="str">
         <f t="shared" ref="EG4" si="16">"Week "&amp;(DZ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 18</v>
       </c>
-      <c r="EH4" s="160"/>
-      <c r="EI4" s="160"/>
-      <c r="EJ4" s="160"/>
-      <c r="EK4" s="160"/>
-      <c r="EL4" s="160"/>
-      <c r="EM4" s="161"/>
-      <c r="EN4" s="159" t="str">
+      <c r="EH4" s="157"/>
+      <c r="EI4" s="157"/>
+      <c r="EJ4" s="157"/>
+      <c r="EK4" s="157"/>
+      <c r="EL4" s="157"/>
+      <c r="EM4" s="158"/>
+      <c r="EN4" s="156" t="str">
         <f t="shared" ref="EN4" si="17">"Week "&amp;(EG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 19</v>
       </c>
-      <c r="EO4" s="160"/>
-      <c r="EP4" s="160"/>
-      <c r="EQ4" s="160"/>
-      <c r="ER4" s="160"/>
-      <c r="ES4" s="160"/>
-      <c r="ET4" s="161"/>
-      <c r="EU4" s="159" t="str">
+      <c r="EO4" s="157"/>
+      <c r="EP4" s="157"/>
+      <c r="EQ4" s="157"/>
+      <c r="ER4" s="157"/>
+      <c r="ES4" s="157"/>
+      <c r="ET4" s="158"/>
+      <c r="EU4" s="156" t="str">
         <f t="shared" ref="EU4" si="18">"Week "&amp;(EN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="EV4" s="160"/>
-      <c r="EW4" s="160"/>
-      <c r="EX4" s="160"/>
-      <c r="EY4" s="160"/>
-      <c r="EZ4" s="160"/>
-      <c r="FA4" s="161"/>
-      <c r="FB4" s="159" t="str">
+      <c r="EV4" s="157"/>
+      <c r="EW4" s="157"/>
+      <c r="EX4" s="157"/>
+      <c r="EY4" s="157"/>
+      <c r="EZ4" s="157"/>
+      <c r="FA4" s="158"/>
+      <c r="FB4" s="156" t="str">
         <f t="shared" ref="FB4" si="19">"Week "&amp;(EU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="FC4" s="160"/>
-      <c r="FD4" s="160"/>
-      <c r="FE4" s="160"/>
-      <c r="FF4" s="160"/>
-      <c r="FG4" s="160"/>
-      <c r="FH4" s="161"/>
-      <c r="FI4" s="159" t="str">
+      <c r="FC4" s="157"/>
+      <c r="FD4" s="157"/>
+      <c r="FE4" s="157"/>
+      <c r="FF4" s="157"/>
+      <c r="FG4" s="157"/>
+      <c r="FH4" s="158"/>
+      <c r="FI4" s="156" t="str">
         <f t="shared" ref="FI4" si="20">"Week "&amp;(FB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="FJ4" s="160"/>
-      <c r="FK4" s="160"/>
-      <c r="FL4" s="160"/>
-      <c r="FM4" s="160"/>
-      <c r="FN4" s="160"/>
-      <c r="FO4" s="161"/>
-      <c r="FP4" s="159" t="str">
+      <c r="FJ4" s="157"/>
+      <c r="FK4" s="157"/>
+      <c r="FL4" s="157"/>
+      <c r="FM4" s="157"/>
+      <c r="FN4" s="157"/>
+      <c r="FO4" s="158"/>
+      <c r="FP4" s="156" t="str">
         <f t="shared" ref="FP4" si="21">"Week "&amp;(FI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="FQ4" s="160"/>
-      <c r="FR4" s="160"/>
-      <c r="FS4" s="160"/>
-      <c r="FT4" s="160"/>
-      <c r="FU4" s="160"/>
-      <c r="FV4" s="161"/>
-      <c r="FW4" s="159" t="str">
+      <c r="FQ4" s="157"/>
+      <c r="FR4" s="157"/>
+      <c r="FS4" s="157"/>
+      <c r="FT4" s="157"/>
+      <c r="FU4" s="157"/>
+      <c r="FV4" s="158"/>
+      <c r="FW4" s="156" t="str">
         <f t="shared" ref="FW4" si="22">"Week "&amp;(FP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="FX4" s="160"/>
-      <c r="FY4" s="160"/>
-      <c r="FZ4" s="160"/>
-      <c r="GA4" s="160"/>
-      <c r="GB4" s="160"/>
-      <c r="GC4" s="161"/>
-      <c r="GD4" s="159" t="str">
+      <c r="FX4" s="157"/>
+      <c r="FY4" s="157"/>
+      <c r="FZ4" s="157"/>
+      <c r="GA4" s="157"/>
+      <c r="GB4" s="157"/>
+      <c r="GC4" s="158"/>
+      <c r="GD4" s="156" t="str">
         <f t="shared" ref="GD4" si="23">"Week "&amp;(FW6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="GE4" s="160"/>
-      <c r="GF4" s="160"/>
-      <c r="GG4" s="160"/>
-      <c r="GH4" s="160"/>
-      <c r="GI4" s="160"/>
-      <c r="GJ4" s="161"/>
-      <c r="GK4" s="159" t="str">
+      <c r="GE4" s="157"/>
+      <c r="GF4" s="157"/>
+      <c r="GG4" s="157"/>
+      <c r="GH4" s="157"/>
+      <c r="GI4" s="157"/>
+      <c r="GJ4" s="158"/>
+      <c r="GK4" s="156" t="str">
         <f t="shared" ref="GK4" si="24">"Week "&amp;(GD6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="GL4" s="160"/>
-      <c r="GM4" s="160"/>
-      <c r="GN4" s="160"/>
-      <c r="GO4" s="160"/>
-      <c r="GP4" s="160"/>
-      <c r="GQ4" s="161"/>
-      <c r="GR4" s="159" t="str">
+      <c r="GL4" s="157"/>
+      <c r="GM4" s="157"/>
+      <c r="GN4" s="157"/>
+      <c r="GO4" s="157"/>
+      <c r="GP4" s="157"/>
+      <c r="GQ4" s="158"/>
+      <c r="GR4" s="156" t="str">
         <f t="shared" ref="GR4" si="25">"Week "&amp;(GK6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="GS4" s="160"/>
-      <c r="GT4" s="160"/>
-      <c r="GU4" s="160"/>
-      <c r="GV4" s="160"/>
-      <c r="GW4" s="160"/>
-      <c r="GX4" s="161"/>
-      <c r="GY4" s="159" t="str">
+      <c r="GS4" s="157"/>
+      <c r="GT4" s="157"/>
+      <c r="GU4" s="157"/>
+      <c r="GV4" s="157"/>
+      <c r="GW4" s="157"/>
+      <c r="GX4" s="158"/>
+      <c r="GY4" s="156" t="str">
         <f t="shared" ref="GY4" si="26">"Week "&amp;(GR6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="GZ4" s="160"/>
-      <c r="HA4" s="160"/>
-      <c r="HB4" s="160"/>
-      <c r="HC4" s="160"/>
-      <c r="HD4" s="160"/>
-      <c r="HE4" s="161"/>
-      <c r="HF4" s="159" t="str">
+      <c r="GZ4" s="157"/>
+      <c r="HA4" s="157"/>
+      <c r="HB4" s="157"/>
+      <c r="HC4" s="157"/>
+      <c r="HD4" s="157"/>
+      <c r="HE4" s="158"/>
+      <c r="HF4" s="156" t="str">
         <f t="shared" ref="HF4" si="27">"Week "&amp;(GY6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="HG4" s="160"/>
-      <c r="HH4" s="160"/>
-      <c r="HI4" s="160"/>
-      <c r="HJ4" s="160"/>
-      <c r="HK4" s="160"/>
-      <c r="HL4" s="161"/>
-      <c r="HM4" s="159" t="str">
+      <c r="HG4" s="157"/>
+      <c r="HH4" s="157"/>
+      <c r="HI4" s="157"/>
+      <c r="HJ4" s="157"/>
+      <c r="HK4" s="157"/>
+      <c r="HL4" s="158"/>
+      <c r="HM4" s="156" t="str">
         <f t="shared" ref="HM4" si="28">"Week "&amp;(HF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="HN4" s="160"/>
-      <c r="HO4" s="160"/>
-      <c r="HP4" s="160"/>
-      <c r="HQ4" s="160"/>
-      <c r="HR4" s="160"/>
-      <c r="HS4" s="161"/>
-      <c r="HT4" s="159" t="str">
+      <c r="HN4" s="157"/>
+      <c r="HO4" s="157"/>
+      <c r="HP4" s="157"/>
+      <c r="HQ4" s="157"/>
+      <c r="HR4" s="157"/>
+      <c r="HS4" s="158"/>
+      <c r="HT4" s="156" t="str">
         <f t="shared" ref="HT4" si="29">"Week "&amp;(HM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="HU4" s="160"/>
-      <c r="HV4" s="160"/>
-      <c r="HW4" s="160"/>
-      <c r="HX4" s="160"/>
-      <c r="HY4" s="160"/>
-      <c r="HZ4" s="161"/>
-      <c r="IA4" s="159" t="str">
+      <c r="HU4" s="157"/>
+      <c r="HV4" s="157"/>
+      <c r="HW4" s="157"/>
+      <c r="HX4" s="157"/>
+      <c r="HY4" s="157"/>
+      <c r="HZ4" s="158"/>
+      <c r="IA4" s="156" t="str">
         <f t="shared" ref="IA4" si="30">"Week "&amp;(HT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="IB4" s="160"/>
-      <c r="IC4" s="160"/>
-      <c r="ID4" s="160"/>
-      <c r="IE4" s="160"/>
-      <c r="IF4" s="160"/>
-      <c r="IG4" s="161"/>
-      <c r="IH4" s="159" t="str">
+      <c r="IB4" s="157"/>
+      <c r="IC4" s="157"/>
+      <c r="ID4" s="157"/>
+      <c r="IE4" s="157"/>
+      <c r="IF4" s="157"/>
+      <c r="IG4" s="158"/>
+      <c r="IH4" s="156" t="str">
         <f t="shared" ref="IH4" si="31">"Week "&amp;(IA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 33</v>
       </c>
-      <c r="II4" s="160"/>
-      <c r="IJ4" s="160"/>
-      <c r="IK4" s="160"/>
-      <c r="IL4" s="160"/>
-      <c r="IM4" s="160"/>
-      <c r="IN4" s="161"/>
-      <c r="IO4" s="159" t="str">
+      <c r="II4" s="157"/>
+      <c r="IJ4" s="157"/>
+      <c r="IK4" s="157"/>
+      <c r="IL4" s="157"/>
+      <c r="IM4" s="157"/>
+      <c r="IN4" s="158"/>
+      <c r="IO4" s="156" t="str">
         <f t="shared" ref="IO4" si="32">"Week "&amp;(IH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 34</v>
       </c>
-      <c r="IP4" s="160"/>
-      <c r="IQ4" s="160"/>
-      <c r="IR4" s="160"/>
-      <c r="IS4" s="160"/>
-      <c r="IT4" s="160"/>
-      <c r="IU4" s="161"/>
+      <c r="IP4" s="157"/>
+      <c r="IQ4" s="157"/>
+      <c r="IR4" s="157"/>
+      <c r="IS4" s="157"/>
+      <c r="IT4" s="157"/>
+      <c r="IU4" s="158"/>
     </row>
     <row r="5" spans="1:255" s="55" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="111"/>
       <c r="B5" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="167" t="s">
+      <c r="C5" s="171" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="168"/>
-      <c r="E5" s="169"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="173"/>
       <c r="F5" s="111"/>
       <c r="G5" s="111"/>
       <c r="H5" s="111"/>
       <c r="I5" s="111"/>
-      <c r="K5" s="170">
+      <c r="K5" s="174">
         <f>K6</f>
         <v>45292</v>
       </c>
-      <c r="L5" s="157"/>
-      <c r="M5" s="157"/>
-      <c r="N5" s="157"/>
-      <c r="O5" s="157"/>
-      <c r="P5" s="157"/>
-      <c r="Q5" s="172"/>
-      <c r="R5" s="170">
+      <c r="L5" s="160"/>
+      <c r="M5" s="160"/>
+      <c r="N5" s="160"/>
+      <c r="O5" s="160"/>
+      <c r="P5" s="160"/>
+      <c r="Q5" s="176"/>
+      <c r="R5" s="174">
         <f>R6</f>
         <v>45299</v>
       </c>
-      <c r="S5" s="157"/>
-      <c r="T5" s="157"/>
-      <c r="U5" s="157"/>
-      <c r="V5" s="157"/>
-      <c r="W5" s="157"/>
-      <c r="X5" s="171"/>
-      <c r="Y5" s="173">
+      <c r="S5" s="160"/>
+      <c r="T5" s="160"/>
+      <c r="U5" s="160"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
+      <c r="X5" s="175"/>
+      <c r="Y5" s="177">
         <f>Y6</f>
         <v>45306</v>
       </c>
-      <c r="Z5" s="157"/>
-      <c r="AA5" s="157"/>
-      <c r="AB5" s="157"/>
-      <c r="AC5" s="157"/>
-      <c r="AD5" s="157"/>
-      <c r="AE5" s="174"/>
-      <c r="AF5" s="165">
+      <c r="Z5" s="160"/>
+      <c r="AA5" s="160"/>
+      <c r="AB5" s="160"/>
+      <c r="AC5" s="160"/>
+      <c r="AD5" s="160"/>
+      <c r="AE5" s="178"/>
+      <c r="AF5" s="169">
         <f>AF6</f>
         <v>45313</v>
       </c>
-      <c r="AG5" s="157"/>
-      <c r="AH5" s="157"/>
-      <c r="AI5" s="157"/>
-      <c r="AJ5" s="157"/>
-      <c r="AK5" s="157"/>
-      <c r="AL5" s="166"/>
-      <c r="AM5" s="175">
+      <c r="AG5" s="160"/>
+      <c r="AH5" s="160"/>
+      <c r="AI5" s="160"/>
+      <c r="AJ5" s="160"/>
+      <c r="AK5" s="160"/>
+      <c r="AL5" s="170"/>
+      <c r="AM5" s="162">
         <f>AM6</f>
         <v>45320</v>
       </c>
-      <c r="AN5" s="157"/>
-      <c r="AO5" s="157"/>
-      <c r="AP5" s="157"/>
-      <c r="AQ5" s="157"/>
-      <c r="AR5" s="157"/>
-      <c r="AS5" s="176"/>
-      <c r="AT5" s="177">
+      <c r="AN5" s="160"/>
+      <c r="AO5" s="160"/>
+      <c r="AP5" s="160"/>
+      <c r="AQ5" s="160"/>
+      <c r="AR5" s="160"/>
+      <c r="AS5" s="163"/>
+      <c r="AT5" s="164">
         <f>AT6</f>
         <v>45327</v>
       </c>
-      <c r="AU5" s="157"/>
-      <c r="AV5" s="157"/>
-      <c r="AW5" s="157"/>
-      <c r="AX5" s="157"/>
-      <c r="AY5" s="157"/>
-      <c r="AZ5" s="178"/>
-      <c r="BA5" s="156">
+      <c r="AU5" s="160"/>
+      <c r="AV5" s="160"/>
+      <c r="AW5" s="160"/>
+      <c r="AX5" s="160"/>
+      <c r="AY5" s="160"/>
+      <c r="AZ5" s="165"/>
+      <c r="BA5" s="166">
         <f>BA6</f>
         <v>45334</v>
       </c>
-      <c r="BB5" s="157"/>
-      <c r="BC5" s="157"/>
-      <c r="BD5" s="157"/>
-      <c r="BE5" s="157"/>
-      <c r="BF5" s="157"/>
-      <c r="BG5" s="158"/>
-      <c r="BH5" s="162">
+      <c r="BB5" s="160"/>
+      <c r="BC5" s="160"/>
+      <c r="BD5" s="160"/>
+      <c r="BE5" s="160"/>
+      <c r="BF5" s="160"/>
+      <c r="BG5" s="167"/>
+      <c r="BH5" s="159">
         <f>BH6</f>
         <v>45341</v>
       </c>
-      <c r="BI5" s="157"/>
-      <c r="BJ5" s="157"/>
-      <c r="BK5" s="157"/>
-      <c r="BL5" s="157"/>
-      <c r="BM5" s="157"/>
-      <c r="BN5" s="163"/>
-      <c r="BO5" s="156">
+      <c r="BI5" s="160"/>
+      <c r="BJ5" s="160"/>
+      <c r="BK5" s="160"/>
+      <c r="BL5" s="160"/>
+      <c r="BM5" s="160"/>
+      <c r="BN5" s="161"/>
+      <c r="BO5" s="166">
         <f>BO6</f>
         <v>45348</v>
       </c>
-      <c r="BP5" s="157"/>
-      <c r="BQ5" s="157"/>
-      <c r="BR5" s="157"/>
-      <c r="BS5" s="157"/>
-      <c r="BT5" s="157"/>
-      <c r="BU5" s="158"/>
-      <c r="BV5" s="162">
+      <c r="BP5" s="160"/>
+      <c r="BQ5" s="160"/>
+      <c r="BR5" s="160"/>
+      <c r="BS5" s="160"/>
+      <c r="BT5" s="160"/>
+      <c r="BU5" s="167"/>
+      <c r="BV5" s="159">
         <f>BV6</f>
         <v>45355</v>
       </c>
-      <c r="BW5" s="157"/>
-      <c r="BX5" s="157"/>
-      <c r="BY5" s="157"/>
-      <c r="BZ5" s="157"/>
-      <c r="CA5" s="157"/>
-      <c r="CB5" s="163"/>
-      <c r="CC5" s="162">
+      <c r="BW5" s="160"/>
+      <c r="BX5" s="160"/>
+      <c r="BY5" s="160"/>
+      <c r="BZ5" s="160"/>
+      <c r="CA5" s="160"/>
+      <c r="CB5" s="161"/>
+      <c r="CC5" s="159">
         <f>CC6</f>
         <v>45362</v>
       </c>
-      <c r="CD5" s="157"/>
-      <c r="CE5" s="157"/>
-      <c r="CF5" s="157"/>
-      <c r="CG5" s="157"/>
-      <c r="CH5" s="157"/>
-      <c r="CI5" s="163"/>
-      <c r="CJ5" s="156">
+      <c r="CD5" s="160"/>
+      <c r="CE5" s="160"/>
+      <c r="CF5" s="160"/>
+      <c r="CG5" s="160"/>
+      <c r="CH5" s="160"/>
+      <c r="CI5" s="161"/>
+      <c r="CJ5" s="166">
         <f>CJ6</f>
         <v>45369</v>
       </c>
-      <c r="CK5" s="157"/>
-      <c r="CL5" s="157"/>
-      <c r="CM5" s="157"/>
-      <c r="CN5" s="157"/>
-      <c r="CO5" s="157"/>
-      <c r="CP5" s="158"/>
-      <c r="CQ5" s="162">
+      <c r="CK5" s="160"/>
+      <c r="CL5" s="160"/>
+      <c r="CM5" s="160"/>
+      <c r="CN5" s="160"/>
+      <c r="CO5" s="160"/>
+      <c r="CP5" s="167"/>
+      <c r="CQ5" s="159">
         <f>CQ6</f>
         <v>45376</v>
       </c>
-      <c r="CR5" s="157"/>
-      <c r="CS5" s="157"/>
-      <c r="CT5" s="157"/>
-      <c r="CU5" s="157"/>
-      <c r="CV5" s="157"/>
-      <c r="CW5" s="163"/>
-      <c r="CX5" s="162">
+      <c r="CR5" s="160"/>
+      <c r="CS5" s="160"/>
+      <c r="CT5" s="160"/>
+      <c r="CU5" s="160"/>
+      <c r="CV5" s="160"/>
+      <c r="CW5" s="161"/>
+      <c r="CX5" s="159">
         <f t="shared" ref="CX5" si="33">CX6</f>
         <v>45383</v>
       </c>
-      <c r="CY5" s="157"/>
-      <c r="CZ5" s="157"/>
-      <c r="DA5" s="157"/>
-      <c r="DB5" s="157"/>
-      <c r="DC5" s="157"/>
-      <c r="DD5" s="163"/>
-      <c r="DE5" s="156">
+      <c r="CY5" s="160"/>
+      <c r="CZ5" s="160"/>
+      <c r="DA5" s="160"/>
+      <c r="DB5" s="160"/>
+      <c r="DC5" s="160"/>
+      <c r="DD5" s="161"/>
+      <c r="DE5" s="166">
         <f t="shared" ref="DE5" si="34">DE6</f>
         <v>45390</v>
       </c>
-      <c r="DF5" s="157"/>
-      <c r="DG5" s="157"/>
-      <c r="DH5" s="157"/>
-      <c r="DI5" s="157"/>
-      <c r="DJ5" s="157"/>
-      <c r="DK5" s="158"/>
-      <c r="DL5" s="162">
+      <c r="DF5" s="160"/>
+      <c r="DG5" s="160"/>
+      <c r="DH5" s="160"/>
+      <c r="DI5" s="160"/>
+      <c r="DJ5" s="160"/>
+      <c r="DK5" s="167"/>
+      <c r="DL5" s="159">
         <f t="shared" ref="DL5" si="35">DL6</f>
         <v>45397</v>
       </c>
-      <c r="DM5" s="157"/>
-      <c r="DN5" s="157"/>
-      <c r="DO5" s="157"/>
-      <c r="DP5" s="157"/>
-      <c r="DQ5" s="157"/>
-      <c r="DR5" s="163"/>
-      <c r="DS5" s="162">
+      <c r="DM5" s="160"/>
+      <c r="DN5" s="160"/>
+      <c r="DO5" s="160"/>
+      <c r="DP5" s="160"/>
+      <c r="DQ5" s="160"/>
+      <c r="DR5" s="161"/>
+      <c r="DS5" s="159">
         <f t="shared" ref="DS5" si="36">DS6</f>
         <v>45404</v>
       </c>
-      <c r="DT5" s="157"/>
-      <c r="DU5" s="157"/>
-      <c r="DV5" s="157"/>
-      <c r="DW5" s="157"/>
-      <c r="DX5" s="157"/>
-      <c r="DY5" s="163"/>
-      <c r="DZ5" s="156">
+      <c r="DT5" s="160"/>
+      <c r="DU5" s="160"/>
+      <c r="DV5" s="160"/>
+      <c r="DW5" s="160"/>
+      <c r="DX5" s="160"/>
+      <c r="DY5" s="161"/>
+      <c r="DZ5" s="166">
         <f t="shared" ref="DZ5" si="37">DZ6</f>
         <v>45411</v>
       </c>
-      <c r="EA5" s="157"/>
-      <c r="EB5" s="157"/>
-      <c r="EC5" s="157"/>
-      <c r="ED5" s="157"/>
-      <c r="EE5" s="157"/>
-      <c r="EF5" s="158"/>
-      <c r="EG5" s="162">
+      <c r="EA5" s="160"/>
+      <c r="EB5" s="160"/>
+      <c r="EC5" s="160"/>
+      <c r="ED5" s="160"/>
+      <c r="EE5" s="160"/>
+      <c r="EF5" s="167"/>
+      <c r="EG5" s="159">
         <f t="shared" ref="EG5" si="38">EG6</f>
         <v>45418</v>
       </c>
-      <c r="EH5" s="157"/>
-      <c r="EI5" s="157"/>
-      <c r="EJ5" s="157"/>
-      <c r="EK5" s="157"/>
-      <c r="EL5" s="157"/>
-      <c r="EM5" s="163"/>
-      <c r="EN5" s="162">
+      <c r="EH5" s="160"/>
+      <c r="EI5" s="160"/>
+      <c r="EJ5" s="160"/>
+      <c r="EK5" s="160"/>
+      <c r="EL5" s="160"/>
+      <c r="EM5" s="161"/>
+      <c r="EN5" s="159">
         <f>EN6</f>
         <v>45425</v>
       </c>
-      <c r="EO5" s="157"/>
-      <c r="EP5" s="157"/>
-      <c r="EQ5" s="157"/>
-      <c r="ER5" s="157"/>
-      <c r="ES5" s="157"/>
-      <c r="ET5" s="163"/>
-      <c r="EU5" s="156">
+      <c r="EO5" s="160"/>
+      <c r="EP5" s="160"/>
+      <c r="EQ5" s="160"/>
+      <c r="ER5" s="160"/>
+      <c r="ES5" s="160"/>
+      <c r="ET5" s="161"/>
+      <c r="EU5" s="166">
         <f>EU6</f>
         <v>45432</v>
       </c>
-      <c r="EV5" s="157"/>
-      <c r="EW5" s="157"/>
-      <c r="EX5" s="157"/>
-      <c r="EY5" s="157"/>
-      <c r="EZ5" s="157"/>
-      <c r="FA5" s="158"/>
-      <c r="FB5" s="162">
+      <c r="EV5" s="160"/>
+      <c r="EW5" s="160"/>
+      <c r="EX5" s="160"/>
+      <c r="EY5" s="160"/>
+      <c r="EZ5" s="160"/>
+      <c r="FA5" s="167"/>
+      <c r="FB5" s="159">
         <f>FB6</f>
         <v>45439</v>
       </c>
-      <c r="FC5" s="157"/>
-      <c r="FD5" s="157"/>
-      <c r="FE5" s="157"/>
-      <c r="FF5" s="157"/>
-      <c r="FG5" s="157"/>
-      <c r="FH5" s="163"/>
-      <c r="FI5" s="162">
+      <c r="FC5" s="160"/>
+      <c r="FD5" s="160"/>
+      <c r="FE5" s="160"/>
+      <c r="FF5" s="160"/>
+      <c r="FG5" s="160"/>
+      <c r="FH5" s="161"/>
+      <c r="FI5" s="159">
         <f t="shared" ref="FI5" si="39">FI6</f>
         <v>45446</v>
       </c>
-      <c r="FJ5" s="157"/>
-      <c r="FK5" s="157"/>
-      <c r="FL5" s="157"/>
-      <c r="FM5" s="157"/>
-      <c r="FN5" s="157"/>
-      <c r="FO5" s="163"/>
-      <c r="FP5" s="156">
+      <c r="FJ5" s="160"/>
+      <c r="FK5" s="160"/>
+      <c r="FL5" s="160"/>
+      <c r="FM5" s="160"/>
+      <c r="FN5" s="160"/>
+      <c r="FO5" s="161"/>
+      <c r="FP5" s="166">
         <f t="shared" ref="FP5" si="40">FP6</f>
         <v>45453</v>
       </c>
-      <c r="FQ5" s="157"/>
-      <c r="FR5" s="157"/>
-      <c r="FS5" s="157"/>
-      <c r="FT5" s="157"/>
-      <c r="FU5" s="157"/>
-      <c r="FV5" s="158"/>
-      <c r="FW5" s="162">
+      <c r="FQ5" s="160"/>
+      <c r="FR5" s="160"/>
+      <c r="FS5" s="160"/>
+      <c r="FT5" s="160"/>
+      <c r="FU5" s="160"/>
+      <c r="FV5" s="167"/>
+      <c r="FW5" s="159">
         <f t="shared" ref="FW5" si="41">FW6</f>
         <v>45460</v>
       </c>
-      <c r="FX5" s="157"/>
-      <c r="FY5" s="157"/>
-      <c r="FZ5" s="157"/>
-      <c r="GA5" s="157"/>
-      <c r="GB5" s="157"/>
-      <c r="GC5" s="163"/>
-      <c r="GD5" s="162">
+      <c r="FX5" s="160"/>
+      <c r="FY5" s="160"/>
+      <c r="FZ5" s="160"/>
+      <c r="GA5" s="160"/>
+      <c r="GB5" s="160"/>
+      <c r="GC5" s="161"/>
+      <c r="GD5" s="159">
         <f t="shared" ref="GD5" si="42">GD6</f>
         <v>45467</v>
       </c>
-      <c r="GE5" s="157"/>
-      <c r="GF5" s="157"/>
-      <c r="GG5" s="157"/>
-      <c r="GH5" s="157"/>
-      <c r="GI5" s="157"/>
-      <c r="GJ5" s="163"/>
-      <c r="GK5" s="156">
+      <c r="GE5" s="160"/>
+      <c r="GF5" s="160"/>
+      <c r="GG5" s="160"/>
+      <c r="GH5" s="160"/>
+      <c r="GI5" s="160"/>
+      <c r="GJ5" s="161"/>
+      <c r="GK5" s="166">
         <f t="shared" ref="GK5" si="43">GK6</f>
         <v>45474</v>
       </c>
-      <c r="GL5" s="157"/>
-      <c r="GM5" s="157"/>
-      <c r="GN5" s="157"/>
-      <c r="GO5" s="157"/>
-      <c r="GP5" s="157"/>
-      <c r="GQ5" s="158"/>
-      <c r="GR5" s="162">
+      <c r="GL5" s="160"/>
+      <c r="GM5" s="160"/>
+      <c r="GN5" s="160"/>
+      <c r="GO5" s="160"/>
+      <c r="GP5" s="160"/>
+      <c r="GQ5" s="167"/>
+      <c r="GR5" s="159">
         <f t="shared" ref="GR5" si="44">GR6</f>
         <v>45481</v>
       </c>
-      <c r="GS5" s="157"/>
-      <c r="GT5" s="157"/>
-      <c r="GU5" s="157"/>
-      <c r="GV5" s="157"/>
-      <c r="GW5" s="157"/>
-      <c r="GX5" s="163"/>
-      <c r="GY5" s="156">
+      <c r="GS5" s="160"/>
+      <c r="GT5" s="160"/>
+      <c r="GU5" s="160"/>
+      <c r="GV5" s="160"/>
+      <c r="GW5" s="160"/>
+      <c r="GX5" s="161"/>
+      <c r="GY5" s="166">
         <f t="shared" ref="GY5" si="45">GY6</f>
         <v>45488</v>
       </c>
-      <c r="GZ5" s="157"/>
-      <c r="HA5" s="157"/>
-      <c r="HB5" s="157"/>
-      <c r="HC5" s="157"/>
-      <c r="HD5" s="157"/>
-      <c r="HE5" s="158"/>
-      <c r="HF5" s="162">
+      <c r="GZ5" s="160"/>
+      <c r="HA5" s="160"/>
+      <c r="HB5" s="160"/>
+      <c r="HC5" s="160"/>
+      <c r="HD5" s="160"/>
+      <c r="HE5" s="167"/>
+      <c r="HF5" s="159">
         <f t="shared" ref="HF5" si="46">HF6</f>
         <v>45495</v>
       </c>
-      <c r="HG5" s="157"/>
-      <c r="HH5" s="157"/>
-      <c r="HI5" s="157"/>
-      <c r="HJ5" s="157"/>
-      <c r="HK5" s="157"/>
-      <c r="HL5" s="163"/>
-      <c r="HM5" s="156">
+      <c r="HG5" s="160"/>
+      <c r="HH5" s="160"/>
+      <c r="HI5" s="160"/>
+      <c r="HJ5" s="160"/>
+      <c r="HK5" s="160"/>
+      <c r="HL5" s="161"/>
+      <c r="HM5" s="166">
         <f t="shared" ref="HM5" si="47">HM6</f>
         <v>45502</v>
       </c>
-      <c r="HN5" s="157"/>
-      <c r="HO5" s="157"/>
-      <c r="HP5" s="157"/>
-      <c r="HQ5" s="157"/>
-      <c r="HR5" s="157"/>
-      <c r="HS5" s="158"/>
-      <c r="HT5" s="162">
+      <c r="HN5" s="160"/>
+      <c r="HO5" s="160"/>
+      <c r="HP5" s="160"/>
+      <c r="HQ5" s="160"/>
+      <c r="HR5" s="160"/>
+      <c r="HS5" s="167"/>
+      <c r="HT5" s="159">
         <f t="shared" ref="HT5" si="48">HT6</f>
         <v>45509</v>
       </c>
-      <c r="HU5" s="157"/>
-      <c r="HV5" s="157"/>
-      <c r="HW5" s="157"/>
-      <c r="HX5" s="157"/>
-      <c r="HY5" s="157"/>
-      <c r="HZ5" s="163"/>
-      <c r="IA5" s="156">
+      <c r="HU5" s="160"/>
+      <c r="HV5" s="160"/>
+      <c r="HW5" s="160"/>
+      <c r="HX5" s="160"/>
+      <c r="HY5" s="160"/>
+      <c r="HZ5" s="161"/>
+      <c r="IA5" s="166">
         <f t="shared" ref="IA5" si="49">IA6</f>
         <v>45516</v>
       </c>
-      <c r="IB5" s="157"/>
-      <c r="IC5" s="157"/>
-      <c r="ID5" s="157"/>
-      <c r="IE5" s="157"/>
-      <c r="IF5" s="157"/>
-      <c r="IG5" s="158"/>
-      <c r="IH5" s="162">
+      <c r="IB5" s="160"/>
+      <c r="IC5" s="160"/>
+      <c r="ID5" s="160"/>
+      <c r="IE5" s="160"/>
+      <c r="IF5" s="160"/>
+      <c r="IG5" s="167"/>
+      <c r="IH5" s="159">
         <f t="shared" ref="IH5" si="50">IH6</f>
         <v>45523</v>
       </c>
-      <c r="II5" s="157"/>
-      <c r="IJ5" s="157"/>
-      <c r="IK5" s="157"/>
-      <c r="IL5" s="157"/>
-      <c r="IM5" s="157"/>
-      <c r="IN5" s="163"/>
-      <c r="IO5" s="156">
+      <c r="II5" s="160"/>
+      <c r="IJ5" s="160"/>
+      <c r="IK5" s="160"/>
+      <c r="IL5" s="160"/>
+      <c r="IM5" s="160"/>
+      <c r="IN5" s="161"/>
+      <c r="IO5" s="166">
         <f t="shared" ref="IO5" si="51">IO6</f>
         <v>45530</v>
       </c>
-      <c r="IP5" s="157"/>
-      <c r="IQ5" s="157"/>
-      <c r="IR5" s="157"/>
-      <c r="IS5" s="157"/>
-      <c r="IT5" s="157"/>
-      <c r="IU5" s="158"/>
+      <c r="IP5" s="160"/>
+      <c r="IQ5" s="160"/>
+      <c r="IR5" s="160"/>
+      <c r="IS5" s="160"/>
+      <c r="IT5" s="160"/>
+      <c r="IU5" s="167"/>
     </row>
     <row r="6" spans="1:255" s="53" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="146"/>
@@ -7583,7 +7586,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" s="150"/>
       <c r="D10" s="33"/>
@@ -7866,17 +7869,17 @@
       </c>
       <c r="F11" s="84">
         <f t="shared" ref="F11:F12" si="258">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
-        <v>45301</v>
+        <v>45302</v>
       </c>
       <c r="G11" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H11" s="46">
         <v>0</v>
       </c>
       <c r="I11" s="102">
         <f t="shared" ref="I11:I12" si="259">IF(OR(F11=0,E11=0),0,NETWORKDAYS(E11,F11))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J11" s="94"/>
       <c r="K11" s="34"/>
@@ -8137,14 +8140,14 @@
       <c r="D12" s="33"/>
       <c r="E12" s="87">
         <f>F11+1</f>
-        <v>45302</v>
+        <v>45303</v>
       </c>
       <c r="F12" s="84">
         <f t="shared" si="258"/>
-        <v>45304</v>
+        <v>45306</v>
       </c>
       <c r="G12" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H12" s="46">
         <v>0</v>
@@ -8406,17 +8409,17 @@
         <v>1.1.4</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C13" s="150"/>
       <c r="D13" s="33"/>
       <c r="E13" s="87">
         <f>F12+1</f>
-        <v>45305</v>
+        <v>45307</v>
       </c>
       <c r="F13" s="84">
         <f t="shared" si="255"/>
-        <v>45307</v>
+        <v>45309</v>
       </c>
       <c r="G13" s="45">
         <v>3</v>
@@ -8426,7 +8429,7 @@
       </c>
       <c r="I13" s="102">
         <f t="shared" si="256"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13" s="94"/>
       <c r="K13" s="34"/>
@@ -8444,7 +8447,9 @@
       <c r="W13" s="34"/>
       <c r="X13" s="34"/>
       <c r="Y13" s="34"/>
-      <c r="Z13" s="34"/>
+      <c r="Z13" s="34" t="s">
+        <v>157</v>
+      </c>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
       <c r="AC13" s="34"/>
@@ -14925,49 +14930,20 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="73">
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="AD1:AR1"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AF5:AL5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="FI4:FO4"/>
-    <mergeCell ref="FP4:FV4"/>
-    <mergeCell ref="EG4:EM4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE5:DK5"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="DS5:DY5"/>
-    <mergeCell ref="DZ5:EF5"/>
-    <mergeCell ref="EG5:EM5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DS4:DY4"/>
-    <mergeCell ref="DZ4:EF4"/>
+    <mergeCell ref="IO5:IU5"/>
+    <mergeCell ref="IO4:IU4"/>
+    <mergeCell ref="HT4:HZ4"/>
+    <mergeCell ref="IA4:IG4"/>
+    <mergeCell ref="IH4:IN4"/>
+    <mergeCell ref="HM5:HS5"/>
+    <mergeCell ref="HT5:HZ5"/>
+    <mergeCell ref="IA5:IG5"/>
+    <mergeCell ref="IH5:IN5"/>
+    <mergeCell ref="GY4:HE4"/>
+    <mergeCell ref="HF4:HL4"/>
+    <mergeCell ref="GY5:HE5"/>
+    <mergeCell ref="HF5:HL5"/>
+    <mergeCell ref="HM4:HS4"/>
     <mergeCell ref="FW4:GC4"/>
     <mergeCell ref="GD4:GJ4"/>
     <mergeCell ref="GK4:GQ4"/>
@@ -14984,20 +14960,49 @@
     <mergeCell ref="EN4:ET4"/>
     <mergeCell ref="EU4:FA4"/>
     <mergeCell ref="FB4:FH4"/>
-    <mergeCell ref="HM5:HS5"/>
-    <mergeCell ref="HT5:HZ5"/>
-    <mergeCell ref="IA5:IG5"/>
-    <mergeCell ref="IH5:IN5"/>
-    <mergeCell ref="GY4:HE4"/>
-    <mergeCell ref="HF4:HL4"/>
-    <mergeCell ref="GY5:HE5"/>
-    <mergeCell ref="HF5:HL5"/>
-    <mergeCell ref="HM4:HS4"/>
-    <mergeCell ref="IO5:IU5"/>
-    <mergeCell ref="IO4:IU4"/>
-    <mergeCell ref="HT4:HZ4"/>
-    <mergeCell ref="IA4:IG4"/>
-    <mergeCell ref="IH4:IN4"/>
+    <mergeCell ref="FI4:FO4"/>
+    <mergeCell ref="FP4:FV4"/>
+    <mergeCell ref="EG4:EM4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="DS5:DY5"/>
+    <mergeCell ref="DZ5:EF5"/>
+    <mergeCell ref="EG5:EM5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DS4:DY4"/>
+    <mergeCell ref="DZ4:EF4"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="AD1:AR1"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="AF5:AL5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="BH4:BN4"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="AM5:AS5"/>
+    <mergeCell ref="AT4:AZ4"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="BA4:BG4"/>
+    <mergeCell ref="BA5:BG5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H33:H37 H8:H30">

</xml_diff>

<commit_message>
read intro to rl till ch 8
</commit_message>
<xml_diff>
--- a/thesis gantt chart.xlsx
+++ b/thesis gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wings_stuff\srus\TUD\yr5\thesis\thesis_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86314025-610F-4368-B531-57476F071499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4472DFA1-E061-4D7D-A2F7-530B9816384E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -430,7 +430,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="162">
   <si>
     <t>WBS</t>
   </si>
@@ -1548,6 +1548,12 @@
   </si>
   <si>
     <t>spring break</t>
+  </si>
+  <si>
+    <t>dirench atmaca - phd indi flying v</t>
+  </si>
+  <si>
+    <t>tim traas- who started september 2022, has the 9 month</t>
   </si>
 </sst>
 </file>
@@ -3251,6 +3257,15 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="70" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3263,28 +3278,7 @@
     <xf numFmtId="167" fontId="52" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="84" fillId="24" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -3321,6 +3315,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3574,13 +3580,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
+          <xdr:colOff>5443</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>99060</xdr:colOff>
+          <xdr:colOff>97971</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -4163,73 +4169,76 @@
   </sheetPr>
   <dimension ref="A1:IU41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10:AC10"/>
+      <selection pane="bottomLeft" activeCell="BZ19" sqref="BZ19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" style="25" customWidth="1"/>
-    <col min="2" max="2" width="45.88671875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" style="155" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" style="25" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.84375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="45.84375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="7.84375" style="155" customWidth="1"/>
+    <col min="4" max="4" width="6.84375" style="25" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="25" customWidth="1"/>
     <col min="7" max="7" width="6" style="25" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" style="25" customWidth="1"/>
-    <col min="10" max="10" width="0.5546875" style="25" customWidth="1"/>
-    <col min="11" max="66" width="2.44140625" style="25" customWidth="1"/>
-    <col min="67" max="68" width="2.44140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="2.109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="2.44140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="1.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="1.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="2.109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="78" max="99" width="2.44140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="100" max="101" width="1.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="1.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="2.109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="105" max="106" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="107" max="108" width="1.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="109" max="131" width="2.44140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="2.109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="134" max="136" width="1.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="1.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="139" max="162" width="2.44140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="163" max="164" width="1.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="1.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="2.109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="168" max="169" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="170" max="190" width="2.44140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="191" max="192" width="1.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="1.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="2.109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="196" max="197" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="198" max="199" width="1.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="200" max="221" width="2.44140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="2.109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="225" max="227" width="1.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.69140625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="5.53515625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="0.53515625" style="25" customWidth="1"/>
+    <col min="11" max="66" width="2.4609375" style="25" customWidth="1"/>
+    <col min="67" max="68" width="2.4609375" style="25" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="2.07421875" style="25" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="2.4609375" style="25" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="2.07421875" style="25" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="78" max="99" width="2.4609375" style="25" bestFit="1" customWidth="1"/>
+    <col min="100" max="101" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="2.07421875" style="25" bestFit="1" customWidth="1"/>
+    <col min="105" max="106" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="107" max="108" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="109" max="131" width="2.4609375" style="25" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="2.07421875" style="25" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="134" max="136" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="139" max="162" width="2.4609375" style="25" bestFit="1" customWidth="1"/>
+    <col min="163" max="164" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="2.07421875" style="25" bestFit="1" customWidth="1"/>
+    <col min="168" max="169" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="170" max="185" width="2.4609375" style="25" bestFit="1" customWidth="1"/>
+    <col min="186" max="192" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="1.61328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="2.15234375" style="25" bestFit="1" customWidth="1"/>
+    <col min="196" max="197" width="1.61328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="198" max="199" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="1.61328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="202" max="206" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="207" max="221" width="2.4609375" style="25" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="2.07421875" style="25" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="225" max="227" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="2" style="25" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="1.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="2.109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="231" max="252" width="2.44140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="253" max="254" width="2.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="1.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="256" max="16384" width="9.109375" style="25"/>
+    <col min="229" max="229" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="2.07421875" style="25" bestFit="1" customWidth="1"/>
+    <col min="231" max="252" width="2.4609375" style="25" bestFit="1" customWidth="1"/>
+    <col min="253" max="254" width="2.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="256" max="16384" width="9.07421875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:255" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="118" t="s">
         <v>139</v>
       </c>
@@ -4242,23 +4251,23 @@
       <c r="K1" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="168"/>
-      <c r="AE1" s="168"/>
-      <c r="AF1" s="168"/>
-      <c r="AG1" s="168"/>
-      <c r="AH1" s="168"/>
-      <c r="AI1" s="168"/>
-      <c r="AJ1" s="168"/>
-      <c r="AK1" s="168"/>
-      <c r="AL1" s="168"/>
-      <c r="AM1" s="168"/>
-      <c r="AN1" s="168"/>
-      <c r="AO1" s="168"/>
-      <c r="AP1" s="168"/>
-      <c r="AQ1" s="168"/>
-      <c r="AR1" s="168"/>
-    </row>
-    <row r="2" spans="1:255" s="59" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD1" s="164"/>
+      <c r="AE1" s="164"/>
+      <c r="AF1" s="164"/>
+      <c r="AG1" s="164"/>
+      <c r="AH1" s="164"/>
+      <c r="AI1" s="164"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="164"/>
+      <c r="AL1" s="164"/>
+      <c r="AM1" s="164"/>
+      <c r="AN1" s="164"/>
+      <c r="AO1" s="164"/>
+      <c r="AP1" s="164"/>
+      <c r="AQ1" s="164"/>
+      <c r="AR1" s="164"/>
+    </row>
+    <row r="2" spans="1:255" s="59" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="112" t="s">
         <v>140</v>
       </c>
@@ -4268,7 +4277,7 @@
       <c r="E2" s="56"/>
       <c r="F2" s="58"/>
     </row>
-    <row r="3" spans="1:255" s="100" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:255" s="100" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="96"/>
       <c r="B3" s="97"/>
       <c r="C3" s="145"/>
@@ -4332,735 +4341,735 @@
       <c r="BM3" s="116"/>
       <c r="BN3" s="117"/>
     </row>
-    <row r="4" spans="1:255" s="110" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:255" s="110" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="113" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="167">
         <v>45295</v>
       </c>
-      <c r="D4" s="172"/>
-      <c r="E4" s="173"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="169"/>
       <c r="H4" s="113" t="s">
         <v>72</v>
       </c>
       <c r="I4" s="114">
         <v>1</v>
       </c>
-      <c r="K4" s="156"/>
-      <c r="L4" s="157"/>
-      <c r="M4" s="157"/>
-      <c r="N4" s="157"/>
-      <c r="O4" s="157"/>
-      <c r="P4" s="157"/>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="156" t="str">
+      <c r="K4" s="159"/>
+      <c r="L4" s="160"/>
+      <c r="M4" s="160"/>
+      <c r="N4" s="160"/>
+      <c r="O4" s="160"/>
+      <c r="P4" s="160"/>
+      <c r="Q4" s="161"/>
+      <c r="R4" s="159" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="S4" s="157"/>
-      <c r="T4" s="157"/>
-      <c r="U4" s="157"/>
-      <c r="V4" s="157"/>
-      <c r="W4" s="157"/>
-      <c r="X4" s="158"/>
-      <c r="Y4" s="156" t="str">
+      <c r="S4" s="160"/>
+      <c r="T4" s="160"/>
+      <c r="U4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="159" t="str">
         <f t="shared" ref="Y4" si="0">"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="Z4" s="157"/>
-      <c r="AA4" s="157"/>
-      <c r="AB4" s="157"/>
-      <c r="AC4" s="157"/>
-      <c r="AD4" s="157"/>
-      <c r="AE4" s="158"/>
-      <c r="AF4" s="156" t="str">
+      <c r="Z4" s="160"/>
+      <c r="AA4" s="160"/>
+      <c r="AB4" s="160"/>
+      <c r="AC4" s="160"/>
+      <c r="AD4" s="160"/>
+      <c r="AE4" s="161"/>
+      <c r="AF4" s="159" t="str">
         <f t="shared" ref="AF4" si="1">"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="AG4" s="157"/>
-      <c r="AH4" s="157"/>
-      <c r="AI4" s="157"/>
-      <c r="AJ4" s="157"/>
-      <c r="AK4" s="157"/>
-      <c r="AL4" s="158"/>
-      <c r="AM4" s="156" t="str">
+      <c r="AG4" s="160"/>
+      <c r="AH4" s="160"/>
+      <c r="AI4" s="160"/>
+      <c r="AJ4" s="160"/>
+      <c r="AK4" s="160"/>
+      <c r="AL4" s="161"/>
+      <c r="AM4" s="159" t="str">
         <f t="shared" ref="AM4" si="2">"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AN4" s="157"/>
-      <c r="AO4" s="157"/>
-      <c r="AP4" s="157"/>
-      <c r="AQ4" s="157"/>
-      <c r="AR4" s="157"/>
-      <c r="AS4" s="158"/>
-      <c r="AT4" s="156" t="str">
+      <c r="AN4" s="160"/>
+      <c r="AO4" s="160"/>
+      <c r="AP4" s="160"/>
+      <c r="AQ4" s="160"/>
+      <c r="AR4" s="160"/>
+      <c r="AS4" s="161"/>
+      <c r="AT4" s="159" t="str">
         <f t="shared" ref="AT4" si="3">"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AU4" s="157"/>
-      <c r="AV4" s="157"/>
-      <c r="AW4" s="157"/>
-      <c r="AX4" s="157"/>
-      <c r="AY4" s="157"/>
-      <c r="AZ4" s="158"/>
-      <c r="BA4" s="156" t="str">
+      <c r="AU4" s="160"/>
+      <c r="AV4" s="160"/>
+      <c r="AW4" s="160"/>
+      <c r="AX4" s="160"/>
+      <c r="AY4" s="160"/>
+      <c r="AZ4" s="161"/>
+      <c r="BA4" s="159" t="str">
         <f t="shared" ref="BA4" si="4">"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="BB4" s="157"/>
-      <c r="BC4" s="157"/>
-      <c r="BD4" s="157"/>
-      <c r="BE4" s="157"/>
-      <c r="BF4" s="157"/>
-      <c r="BG4" s="158"/>
-      <c r="BH4" s="156" t="str">
+      <c r="BB4" s="160"/>
+      <c r="BC4" s="160"/>
+      <c r="BD4" s="160"/>
+      <c r="BE4" s="160"/>
+      <c r="BF4" s="160"/>
+      <c r="BG4" s="161"/>
+      <c r="BH4" s="159" t="str">
         <f t="shared" ref="BH4" si="5">"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BI4" s="157"/>
-      <c r="BJ4" s="157"/>
-      <c r="BK4" s="157"/>
-      <c r="BL4" s="157"/>
-      <c r="BM4" s="157"/>
-      <c r="BN4" s="158"/>
-      <c r="BO4" s="156" t="str">
+      <c r="BI4" s="160"/>
+      <c r="BJ4" s="160"/>
+      <c r="BK4" s="160"/>
+      <c r="BL4" s="160"/>
+      <c r="BM4" s="160"/>
+      <c r="BN4" s="161"/>
+      <c r="BO4" s="159" t="str">
         <f t="shared" ref="BO4" si="6">"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BP4" s="157"/>
-      <c r="BQ4" s="157"/>
-      <c r="BR4" s="157"/>
-      <c r="BS4" s="157"/>
-      <c r="BT4" s="157"/>
-      <c r="BU4" s="158"/>
-      <c r="BV4" s="156" t="str">
+      <c r="BP4" s="160"/>
+      <c r="BQ4" s="160"/>
+      <c r="BR4" s="160"/>
+      <c r="BS4" s="160"/>
+      <c r="BT4" s="160"/>
+      <c r="BU4" s="161"/>
+      <c r="BV4" s="159" t="str">
         <f t="shared" ref="BV4" si="7">"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BW4" s="157"/>
-      <c r="BX4" s="157"/>
-      <c r="BY4" s="157"/>
-      <c r="BZ4" s="157"/>
-      <c r="CA4" s="157"/>
-      <c r="CB4" s="158"/>
-      <c r="CC4" s="156" t="str">
+      <c r="BW4" s="160"/>
+      <c r="BX4" s="160"/>
+      <c r="BY4" s="160"/>
+      <c r="BZ4" s="160"/>
+      <c r="CA4" s="160"/>
+      <c r="CB4" s="161"/>
+      <c r="CC4" s="159" t="str">
         <f t="shared" ref="CC4" si="8">"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="CD4" s="157"/>
-      <c r="CE4" s="157"/>
-      <c r="CF4" s="157"/>
-      <c r="CG4" s="157"/>
-      <c r="CH4" s="157"/>
-      <c r="CI4" s="158"/>
-      <c r="CJ4" s="156" t="str">
+      <c r="CD4" s="160"/>
+      <c r="CE4" s="160"/>
+      <c r="CF4" s="160"/>
+      <c r="CG4" s="160"/>
+      <c r="CH4" s="160"/>
+      <c r="CI4" s="161"/>
+      <c r="CJ4" s="159" t="str">
         <f t="shared" ref="CJ4" si="9">"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CK4" s="157"/>
-      <c r="CL4" s="157"/>
-      <c r="CM4" s="157"/>
-      <c r="CN4" s="157"/>
-      <c r="CO4" s="157"/>
-      <c r="CP4" s="158"/>
-      <c r="CQ4" s="156" t="str">
+      <c r="CK4" s="160"/>
+      <c r="CL4" s="160"/>
+      <c r="CM4" s="160"/>
+      <c r="CN4" s="160"/>
+      <c r="CO4" s="160"/>
+      <c r="CP4" s="161"/>
+      <c r="CQ4" s="159" t="str">
         <f t="shared" ref="CQ4" si="10">"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CR4" s="157"/>
-      <c r="CS4" s="157"/>
-      <c r="CT4" s="157"/>
-      <c r="CU4" s="157"/>
-      <c r="CV4" s="157"/>
-      <c r="CW4" s="158"/>
-      <c r="CX4" s="156" t="str">
+      <c r="CR4" s="160"/>
+      <c r="CS4" s="160"/>
+      <c r="CT4" s="160"/>
+      <c r="CU4" s="160"/>
+      <c r="CV4" s="160"/>
+      <c r="CW4" s="161"/>
+      <c r="CX4" s="159" t="str">
         <f t="shared" ref="CX4" si="11">"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="CY4" s="157"/>
-      <c r="CZ4" s="157"/>
-      <c r="DA4" s="157"/>
-      <c r="DB4" s="157"/>
-      <c r="DC4" s="157"/>
-      <c r="DD4" s="158"/>
-      <c r="DE4" s="156" t="str">
+      <c r="CY4" s="160"/>
+      <c r="CZ4" s="160"/>
+      <c r="DA4" s="160"/>
+      <c r="DB4" s="160"/>
+      <c r="DC4" s="160"/>
+      <c r="DD4" s="161"/>
+      <c r="DE4" s="159" t="str">
         <f t="shared" ref="DE4" si="12">"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="DF4" s="157"/>
-      <c r="DG4" s="157"/>
-      <c r="DH4" s="157"/>
-      <c r="DI4" s="157"/>
-      <c r="DJ4" s="157"/>
-      <c r="DK4" s="158"/>
-      <c r="DL4" s="156" t="str">
+      <c r="DF4" s="160"/>
+      <c r="DG4" s="160"/>
+      <c r="DH4" s="160"/>
+      <c r="DI4" s="160"/>
+      <c r="DJ4" s="160"/>
+      <c r="DK4" s="161"/>
+      <c r="DL4" s="159" t="str">
         <f t="shared" ref="DL4" si="13">"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 15</v>
       </c>
-      <c r="DM4" s="157"/>
-      <c r="DN4" s="157"/>
-      <c r="DO4" s="157"/>
-      <c r="DP4" s="157"/>
-      <c r="DQ4" s="157"/>
-      <c r="DR4" s="158"/>
-      <c r="DS4" s="156" t="str">
+      <c r="DM4" s="160"/>
+      <c r="DN4" s="160"/>
+      <c r="DO4" s="160"/>
+      <c r="DP4" s="160"/>
+      <c r="DQ4" s="160"/>
+      <c r="DR4" s="161"/>
+      <c r="DS4" s="159" t="str">
         <f t="shared" ref="DS4" si="14">"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 16</v>
       </c>
-      <c r="DT4" s="157"/>
-      <c r="DU4" s="157"/>
-      <c r="DV4" s="157"/>
-      <c r="DW4" s="157"/>
-      <c r="DX4" s="157"/>
-      <c r="DY4" s="158"/>
-      <c r="DZ4" s="156" t="str">
+      <c r="DT4" s="160"/>
+      <c r="DU4" s="160"/>
+      <c r="DV4" s="160"/>
+      <c r="DW4" s="160"/>
+      <c r="DX4" s="160"/>
+      <c r="DY4" s="161"/>
+      <c r="DZ4" s="159" t="str">
         <f t="shared" ref="DZ4" si="15">"Week "&amp;(DS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 17</v>
       </c>
-      <c r="EA4" s="157"/>
-      <c r="EB4" s="157"/>
-      <c r="EC4" s="157"/>
-      <c r="ED4" s="157"/>
-      <c r="EE4" s="157"/>
-      <c r="EF4" s="158"/>
-      <c r="EG4" s="156" t="str">
+      <c r="EA4" s="160"/>
+      <c r="EB4" s="160"/>
+      <c r="EC4" s="160"/>
+      <c r="ED4" s="160"/>
+      <c r="EE4" s="160"/>
+      <c r="EF4" s="161"/>
+      <c r="EG4" s="159" t="str">
         <f t="shared" ref="EG4" si="16">"Week "&amp;(DZ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 18</v>
       </c>
-      <c r="EH4" s="157"/>
-      <c r="EI4" s="157"/>
-      <c r="EJ4" s="157"/>
-      <c r="EK4" s="157"/>
-      <c r="EL4" s="157"/>
-      <c r="EM4" s="158"/>
-      <c r="EN4" s="156" t="str">
+      <c r="EH4" s="160"/>
+      <c r="EI4" s="160"/>
+      <c r="EJ4" s="160"/>
+      <c r="EK4" s="160"/>
+      <c r="EL4" s="160"/>
+      <c r="EM4" s="161"/>
+      <c r="EN4" s="159" t="str">
         <f t="shared" ref="EN4" si="17">"Week "&amp;(EG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 19</v>
       </c>
-      <c r="EO4" s="157"/>
-      <c r="EP4" s="157"/>
-      <c r="EQ4" s="157"/>
-      <c r="ER4" s="157"/>
-      <c r="ES4" s="157"/>
-      <c r="ET4" s="158"/>
-      <c r="EU4" s="156" t="str">
+      <c r="EO4" s="160"/>
+      <c r="EP4" s="160"/>
+      <c r="EQ4" s="160"/>
+      <c r="ER4" s="160"/>
+      <c r="ES4" s="160"/>
+      <c r="ET4" s="161"/>
+      <c r="EU4" s="159" t="str">
         <f t="shared" ref="EU4" si="18">"Week "&amp;(EN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="EV4" s="157"/>
-      <c r="EW4" s="157"/>
-      <c r="EX4" s="157"/>
-      <c r="EY4" s="157"/>
-      <c r="EZ4" s="157"/>
-      <c r="FA4" s="158"/>
-      <c r="FB4" s="156" t="str">
+      <c r="EV4" s="160"/>
+      <c r="EW4" s="160"/>
+      <c r="EX4" s="160"/>
+      <c r="EY4" s="160"/>
+      <c r="EZ4" s="160"/>
+      <c r="FA4" s="161"/>
+      <c r="FB4" s="159" t="str">
         <f t="shared" ref="FB4" si="19">"Week "&amp;(EU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="FC4" s="157"/>
-      <c r="FD4" s="157"/>
-      <c r="FE4" s="157"/>
-      <c r="FF4" s="157"/>
-      <c r="FG4" s="157"/>
-      <c r="FH4" s="158"/>
-      <c r="FI4" s="156" t="str">
+      <c r="FC4" s="160"/>
+      <c r="FD4" s="160"/>
+      <c r="FE4" s="160"/>
+      <c r="FF4" s="160"/>
+      <c r="FG4" s="160"/>
+      <c r="FH4" s="161"/>
+      <c r="FI4" s="159" t="str">
         <f t="shared" ref="FI4" si="20">"Week "&amp;(FB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="FJ4" s="157"/>
-      <c r="FK4" s="157"/>
-      <c r="FL4" s="157"/>
-      <c r="FM4" s="157"/>
-      <c r="FN4" s="157"/>
-      <c r="FO4" s="158"/>
-      <c r="FP4" s="156" t="str">
+      <c r="FJ4" s="160"/>
+      <c r="FK4" s="160"/>
+      <c r="FL4" s="160"/>
+      <c r="FM4" s="160"/>
+      <c r="FN4" s="160"/>
+      <c r="FO4" s="161"/>
+      <c r="FP4" s="159" t="str">
         <f t="shared" ref="FP4" si="21">"Week "&amp;(FI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="FQ4" s="157"/>
-      <c r="FR4" s="157"/>
-      <c r="FS4" s="157"/>
-      <c r="FT4" s="157"/>
-      <c r="FU4" s="157"/>
-      <c r="FV4" s="158"/>
-      <c r="FW4" s="156" t="str">
+      <c r="FQ4" s="160"/>
+      <c r="FR4" s="160"/>
+      <c r="FS4" s="160"/>
+      <c r="FT4" s="160"/>
+      <c r="FU4" s="160"/>
+      <c r="FV4" s="161"/>
+      <c r="FW4" s="159" t="str">
         <f t="shared" ref="FW4" si="22">"Week "&amp;(FP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="FX4" s="157"/>
-      <c r="FY4" s="157"/>
-      <c r="FZ4" s="157"/>
-      <c r="GA4" s="157"/>
-      <c r="GB4" s="157"/>
-      <c r="GC4" s="158"/>
-      <c r="GD4" s="156" t="str">
+      <c r="FX4" s="160"/>
+      <c r="FY4" s="160"/>
+      <c r="FZ4" s="160"/>
+      <c r="GA4" s="160"/>
+      <c r="GB4" s="160"/>
+      <c r="GC4" s="161"/>
+      <c r="GD4" s="159" t="str">
         <f t="shared" ref="GD4" si="23">"Week "&amp;(FW6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="GE4" s="157"/>
-      <c r="GF4" s="157"/>
-      <c r="GG4" s="157"/>
-      <c r="GH4" s="157"/>
-      <c r="GI4" s="157"/>
-      <c r="GJ4" s="158"/>
-      <c r="GK4" s="156" t="str">
+      <c r="GE4" s="160"/>
+      <c r="GF4" s="160"/>
+      <c r="GG4" s="160"/>
+      <c r="GH4" s="160"/>
+      <c r="GI4" s="160"/>
+      <c r="GJ4" s="161"/>
+      <c r="GK4" s="159" t="str">
         <f t="shared" ref="GK4" si="24">"Week "&amp;(GD6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="GL4" s="157"/>
-      <c r="GM4" s="157"/>
-      <c r="GN4" s="157"/>
-      <c r="GO4" s="157"/>
-      <c r="GP4" s="157"/>
-      <c r="GQ4" s="158"/>
-      <c r="GR4" s="156" t="str">
+      <c r="GL4" s="160"/>
+      <c r="GM4" s="160"/>
+      <c r="GN4" s="160"/>
+      <c r="GO4" s="160"/>
+      <c r="GP4" s="160"/>
+      <c r="GQ4" s="161"/>
+      <c r="GR4" s="159" t="str">
         <f t="shared" ref="GR4" si="25">"Week "&amp;(GK6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="GS4" s="157"/>
-      <c r="GT4" s="157"/>
-      <c r="GU4" s="157"/>
-      <c r="GV4" s="157"/>
-      <c r="GW4" s="157"/>
-      <c r="GX4" s="158"/>
-      <c r="GY4" s="156" t="str">
+      <c r="GS4" s="160"/>
+      <c r="GT4" s="160"/>
+      <c r="GU4" s="160"/>
+      <c r="GV4" s="160"/>
+      <c r="GW4" s="160"/>
+      <c r="GX4" s="161"/>
+      <c r="GY4" s="159" t="str">
         <f t="shared" ref="GY4" si="26">"Week "&amp;(GR6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="GZ4" s="157"/>
-      <c r="HA4" s="157"/>
-      <c r="HB4" s="157"/>
-      <c r="HC4" s="157"/>
-      <c r="HD4" s="157"/>
-      <c r="HE4" s="158"/>
-      <c r="HF4" s="156" t="str">
+      <c r="GZ4" s="160"/>
+      <c r="HA4" s="160"/>
+      <c r="HB4" s="160"/>
+      <c r="HC4" s="160"/>
+      <c r="HD4" s="160"/>
+      <c r="HE4" s="161"/>
+      <c r="HF4" s="159" t="str">
         <f t="shared" ref="HF4" si="27">"Week "&amp;(GY6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="HG4" s="157"/>
-      <c r="HH4" s="157"/>
-      <c r="HI4" s="157"/>
-      <c r="HJ4" s="157"/>
-      <c r="HK4" s="157"/>
-      <c r="HL4" s="158"/>
-      <c r="HM4" s="156" t="str">
+      <c r="HG4" s="160"/>
+      <c r="HH4" s="160"/>
+      <c r="HI4" s="160"/>
+      <c r="HJ4" s="160"/>
+      <c r="HK4" s="160"/>
+      <c r="HL4" s="161"/>
+      <c r="HM4" s="159" t="str">
         <f t="shared" ref="HM4" si="28">"Week "&amp;(HF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="HN4" s="157"/>
-      <c r="HO4" s="157"/>
-      <c r="HP4" s="157"/>
-      <c r="HQ4" s="157"/>
-      <c r="HR4" s="157"/>
-      <c r="HS4" s="158"/>
-      <c r="HT4" s="156" t="str">
+      <c r="HN4" s="160"/>
+      <c r="HO4" s="160"/>
+      <c r="HP4" s="160"/>
+      <c r="HQ4" s="160"/>
+      <c r="HR4" s="160"/>
+      <c r="HS4" s="161"/>
+      <c r="HT4" s="159" t="str">
         <f t="shared" ref="HT4" si="29">"Week "&amp;(HM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="HU4" s="157"/>
-      <c r="HV4" s="157"/>
-      <c r="HW4" s="157"/>
-      <c r="HX4" s="157"/>
-      <c r="HY4" s="157"/>
-      <c r="HZ4" s="158"/>
-      <c r="IA4" s="156" t="str">
+      <c r="HU4" s="160"/>
+      <c r="HV4" s="160"/>
+      <c r="HW4" s="160"/>
+      <c r="HX4" s="160"/>
+      <c r="HY4" s="160"/>
+      <c r="HZ4" s="161"/>
+      <c r="IA4" s="159" t="str">
         <f t="shared" ref="IA4" si="30">"Week "&amp;(HT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="IB4" s="157"/>
-      <c r="IC4" s="157"/>
-      <c r="ID4" s="157"/>
-      <c r="IE4" s="157"/>
-      <c r="IF4" s="157"/>
-      <c r="IG4" s="158"/>
-      <c r="IH4" s="156" t="str">
+      <c r="IB4" s="160"/>
+      <c r="IC4" s="160"/>
+      <c r="ID4" s="160"/>
+      <c r="IE4" s="160"/>
+      <c r="IF4" s="160"/>
+      <c r="IG4" s="161"/>
+      <c r="IH4" s="159" t="str">
         <f t="shared" ref="IH4" si="31">"Week "&amp;(IA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 33</v>
       </c>
-      <c r="II4" s="157"/>
-      <c r="IJ4" s="157"/>
-      <c r="IK4" s="157"/>
-      <c r="IL4" s="157"/>
-      <c r="IM4" s="157"/>
-      <c r="IN4" s="158"/>
-      <c r="IO4" s="156" t="str">
+      <c r="II4" s="160"/>
+      <c r="IJ4" s="160"/>
+      <c r="IK4" s="160"/>
+      <c r="IL4" s="160"/>
+      <c r="IM4" s="160"/>
+      <c r="IN4" s="161"/>
+      <c r="IO4" s="159" t="str">
         <f t="shared" ref="IO4" si="32">"Week "&amp;(IH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 34</v>
       </c>
-      <c r="IP4" s="157"/>
-      <c r="IQ4" s="157"/>
-      <c r="IR4" s="157"/>
-      <c r="IS4" s="157"/>
-      <c r="IT4" s="157"/>
-      <c r="IU4" s="158"/>
-    </row>
-    <row r="5" spans="1:255" s="55" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="IP4" s="160"/>
+      <c r="IQ4" s="160"/>
+      <c r="IR4" s="160"/>
+      <c r="IS4" s="160"/>
+      <c r="IT4" s="160"/>
+      <c r="IU4" s="161"/>
+    </row>
+    <row r="5" spans="1:255" s="55" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="111"/>
       <c r="B5" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="171" t="s">
+      <c r="C5" s="167" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="172"/>
-      <c r="E5" s="173"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="169"/>
       <c r="F5" s="111"/>
       <c r="G5" s="111"/>
       <c r="H5" s="111"/>
       <c r="I5" s="111"/>
-      <c r="K5" s="174">
+      <c r="K5" s="170">
         <f>K6</f>
         <v>45292</v>
       </c>
-      <c r="L5" s="160"/>
-      <c r="M5" s="160"/>
-      <c r="N5" s="160"/>
-      <c r="O5" s="160"/>
-      <c r="P5" s="160"/>
-      <c r="Q5" s="176"/>
-      <c r="R5" s="174">
+      <c r="L5" s="157"/>
+      <c r="M5" s="157"/>
+      <c r="N5" s="157"/>
+      <c r="O5" s="157"/>
+      <c r="P5" s="157"/>
+      <c r="Q5" s="172"/>
+      <c r="R5" s="170">
         <f>R6</f>
         <v>45299</v>
       </c>
-      <c r="S5" s="160"/>
-      <c r="T5" s="160"/>
-      <c r="U5" s="160"/>
-      <c r="V5" s="160"/>
-      <c r="W5" s="160"/>
-      <c r="X5" s="175"/>
-      <c r="Y5" s="177">
+      <c r="S5" s="157"/>
+      <c r="T5" s="157"/>
+      <c r="U5" s="157"/>
+      <c r="V5" s="157"/>
+      <c r="W5" s="157"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="173">
         <f>Y6</f>
         <v>45306</v>
       </c>
-      <c r="Z5" s="160"/>
-      <c r="AA5" s="160"/>
-      <c r="AB5" s="160"/>
-      <c r="AC5" s="160"/>
-      <c r="AD5" s="160"/>
-      <c r="AE5" s="178"/>
-      <c r="AF5" s="169">
+      <c r="Z5" s="157"/>
+      <c r="AA5" s="157"/>
+      <c r="AB5" s="157"/>
+      <c r="AC5" s="157"/>
+      <c r="AD5" s="157"/>
+      <c r="AE5" s="174"/>
+      <c r="AF5" s="165">
         <f>AF6</f>
         <v>45313</v>
       </c>
-      <c r="AG5" s="160"/>
-      <c r="AH5" s="160"/>
-      <c r="AI5" s="160"/>
-      <c r="AJ5" s="160"/>
-      <c r="AK5" s="160"/>
-      <c r="AL5" s="170"/>
-      <c r="AM5" s="162">
+      <c r="AG5" s="157"/>
+      <c r="AH5" s="157"/>
+      <c r="AI5" s="157"/>
+      <c r="AJ5" s="157"/>
+      <c r="AK5" s="157"/>
+      <c r="AL5" s="166"/>
+      <c r="AM5" s="175">
         <f>AM6</f>
         <v>45320</v>
       </c>
-      <c r="AN5" s="160"/>
-      <c r="AO5" s="160"/>
-      <c r="AP5" s="160"/>
-      <c r="AQ5" s="160"/>
-      <c r="AR5" s="160"/>
-      <c r="AS5" s="163"/>
-      <c r="AT5" s="164">
+      <c r="AN5" s="157"/>
+      <c r="AO5" s="157"/>
+      <c r="AP5" s="157"/>
+      <c r="AQ5" s="157"/>
+      <c r="AR5" s="157"/>
+      <c r="AS5" s="176"/>
+      <c r="AT5" s="177">
         <f>AT6</f>
         <v>45327</v>
       </c>
-      <c r="AU5" s="160"/>
-      <c r="AV5" s="160"/>
-      <c r="AW5" s="160"/>
-      <c r="AX5" s="160"/>
-      <c r="AY5" s="160"/>
-      <c r="AZ5" s="165"/>
-      <c r="BA5" s="166">
+      <c r="AU5" s="157"/>
+      <c r="AV5" s="157"/>
+      <c r="AW5" s="157"/>
+      <c r="AX5" s="157"/>
+      <c r="AY5" s="157"/>
+      <c r="AZ5" s="178"/>
+      <c r="BA5" s="156">
         <f>BA6</f>
         <v>45334</v>
       </c>
-      <c r="BB5" s="160"/>
-      <c r="BC5" s="160"/>
-      <c r="BD5" s="160"/>
-      <c r="BE5" s="160"/>
-      <c r="BF5" s="160"/>
-      <c r="BG5" s="167"/>
-      <c r="BH5" s="159">
+      <c r="BB5" s="157"/>
+      <c r="BC5" s="157"/>
+      <c r="BD5" s="157"/>
+      <c r="BE5" s="157"/>
+      <c r="BF5" s="157"/>
+      <c r="BG5" s="158"/>
+      <c r="BH5" s="162">
         <f>BH6</f>
         <v>45341</v>
       </c>
-      <c r="BI5" s="160"/>
-      <c r="BJ5" s="160"/>
-      <c r="BK5" s="160"/>
-      <c r="BL5" s="160"/>
-      <c r="BM5" s="160"/>
-      <c r="BN5" s="161"/>
-      <c r="BO5" s="166">
+      <c r="BI5" s="157"/>
+      <c r="BJ5" s="157"/>
+      <c r="BK5" s="157"/>
+      <c r="BL5" s="157"/>
+      <c r="BM5" s="157"/>
+      <c r="BN5" s="163"/>
+      <c r="BO5" s="156">
         <f>BO6</f>
         <v>45348</v>
       </c>
-      <c r="BP5" s="160"/>
-      <c r="BQ5" s="160"/>
-      <c r="BR5" s="160"/>
-      <c r="BS5" s="160"/>
-      <c r="BT5" s="160"/>
-      <c r="BU5" s="167"/>
-      <c r="BV5" s="159">
+      <c r="BP5" s="157"/>
+      <c r="BQ5" s="157"/>
+      <c r="BR5" s="157"/>
+      <c r="BS5" s="157"/>
+      <c r="BT5" s="157"/>
+      <c r="BU5" s="158"/>
+      <c r="BV5" s="162">
         <f>BV6</f>
         <v>45355</v>
       </c>
-      <c r="BW5" s="160"/>
-      <c r="BX5" s="160"/>
-      <c r="BY5" s="160"/>
-      <c r="BZ5" s="160"/>
-      <c r="CA5" s="160"/>
-      <c r="CB5" s="161"/>
-      <c r="CC5" s="159">
+      <c r="BW5" s="157"/>
+      <c r="BX5" s="157"/>
+      <c r="BY5" s="157"/>
+      <c r="BZ5" s="157"/>
+      <c r="CA5" s="157"/>
+      <c r="CB5" s="163"/>
+      <c r="CC5" s="162">
         <f>CC6</f>
         <v>45362</v>
       </c>
-      <c r="CD5" s="160"/>
-      <c r="CE5" s="160"/>
-      <c r="CF5" s="160"/>
-      <c r="CG5" s="160"/>
-      <c r="CH5" s="160"/>
-      <c r="CI5" s="161"/>
-      <c r="CJ5" s="166">
+      <c r="CD5" s="157"/>
+      <c r="CE5" s="157"/>
+      <c r="CF5" s="157"/>
+      <c r="CG5" s="157"/>
+      <c r="CH5" s="157"/>
+      <c r="CI5" s="163"/>
+      <c r="CJ5" s="156">
         <f>CJ6</f>
         <v>45369</v>
       </c>
-      <c r="CK5" s="160"/>
-      <c r="CL5" s="160"/>
-      <c r="CM5" s="160"/>
-      <c r="CN5" s="160"/>
-      <c r="CO5" s="160"/>
-      <c r="CP5" s="167"/>
-      <c r="CQ5" s="159">
+      <c r="CK5" s="157"/>
+      <c r="CL5" s="157"/>
+      <c r="CM5" s="157"/>
+      <c r="CN5" s="157"/>
+      <c r="CO5" s="157"/>
+      <c r="CP5" s="158"/>
+      <c r="CQ5" s="162">
         <f>CQ6</f>
         <v>45376</v>
       </c>
-      <c r="CR5" s="160"/>
-      <c r="CS5" s="160"/>
-      <c r="CT5" s="160"/>
-      <c r="CU5" s="160"/>
-      <c r="CV5" s="160"/>
-      <c r="CW5" s="161"/>
-      <c r="CX5" s="159">
+      <c r="CR5" s="157"/>
+      <c r="CS5" s="157"/>
+      <c r="CT5" s="157"/>
+      <c r="CU5" s="157"/>
+      <c r="CV5" s="157"/>
+      <c r="CW5" s="163"/>
+      <c r="CX5" s="162">
         <f t="shared" ref="CX5" si="33">CX6</f>
         <v>45383</v>
       </c>
-      <c r="CY5" s="160"/>
-      <c r="CZ5" s="160"/>
-      <c r="DA5" s="160"/>
-      <c r="DB5" s="160"/>
-      <c r="DC5" s="160"/>
-      <c r="DD5" s="161"/>
-      <c r="DE5" s="166">
+      <c r="CY5" s="157"/>
+      <c r="CZ5" s="157"/>
+      <c r="DA5" s="157"/>
+      <c r="DB5" s="157"/>
+      <c r="DC5" s="157"/>
+      <c r="DD5" s="163"/>
+      <c r="DE5" s="156">
         <f t="shared" ref="DE5" si="34">DE6</f>
         <v>45390</v>
       </c>
-      <c r="DF5" s="160"/>
-      <c r="DG5" s="160"/>
-      <c r="DH5" s="160"/>
-      <c r="DI5" s="160"/>
-      <c r="DJ5" s="160"/>
-      <c r="DK5" s="167"/>
-      <c r="DL5" s="159">
+      <c r="DF5" s="157"/>
+      <c r="DG5" s="157"/>
+      <c r="DH5" s="157"/>
+      <c r="DI5" s="157"/>
+      <c r="DJ5" s="157"/>
+      <c r="DK5" s="158"/>
+      <c r="DL5" s="162">
         <f t="shared" ref="DL5" si="35">DL6</f>
         <v>45397</v>
       </c>
-      <c r="DM5" s="160"/>
-      <c r="DN5" s="160"/>
-      <c r="DO5" s="160"/>
-      <c r="DP5" s="160"/>
-      <c r="DQ5" s="160"/>
-      <c r="DR5" s="161"/>
-      <c r="DS5" s="159">
+      <c r="DM5" s="157"/>
+      <c r="DN5" s="157"/>
+      <c r="DO5" s="157"/>
+      <c r="DP5" s="157"/>
+      <c r="DQ5" s="157"/>
+      <c r="DR5" s="163"/>
+      <c r="DS5" s="162">
         <f t="shared" ref="DS5" si="36">DS6</f>
         <v>45404</v>
       </c>
-      <c r="DT5" s="160"/>
-      <c r="DU5" s="160"/>
-      <c r="DV5" s="160"/>
-      <c r="DW5" s="160"/>
-      <c r="DX5" s="160"/>
-      <c r="DY5" s="161"/>
-      <c r="DZ5" s="166">
+      <c r="DT5" s="157"/>
+      <c r="DU5" s="157"/>
+      <c r="DV5" s="157"/>
+      <c r="DW5" s="157"/>
+      <c r="DX5" s="157"/>
+      <c r="DY5" s="163"/>
+      <c r="DZ5" s="156">
         <f t="shared" ref="DZ5" si="37">DZ6</f>
         <v>45411</v>
       </c>
-      <c r="EA5" s="160"/>
-      <c r="EB5" s="160"/>
-      <c r="EC5" s="160"/>
-      <c r="ED5" s="160"/>
-      <c r="EE5" s="160"/>
-      <c r="EF5" s="167"/>
-      <c r="EG5" s="159">
+      <c r="EA5" s="157"/>
+      <c r="EB5" s="157"/>
+      <c r="EC5" s="157"/>
+      <c r="ED5" s="157"/>
+      <c r="EE5" s="157"/>
+      <c r="EF5" s="158"/>
+      <c r="EG5" s="162">
         <f t="shared" ref="EG5" si="38">EG6</f>
         <v>45418</v>
       </c>
-      <c r="EH5" s="160"/>
-      <c r="EI5" s="160"/>
-      <c r="EJ5" s="160"/>
-      <c r="EK5" s="160"/>
-      <c r="EL5" s="160"/>
-      <c r="EM5" s="161"/>
-      <c r="EN5" s="159">
+      <c r="EH5" s="157"/>
+      <c r="EI5" s="157"/>
+      <c r="EJ5" s="157"/>
+      <c r="EK5" s="157"/>
+      <c r="EL5" s="157"/>
+      <c r="EM5" s="163"/>
+      <c r="EN5" s="162">
         <f>EN6</f>
         <v>45425</v>
       </c>
-      <c r="EO5" s="160"/>
-      <c r="EP5" s="160"/>
-      <c r="EQ5" s="160"/>
-      <c r="ER5" s="160"/>
-      <c r="ES5" s="160"/>
-      <c r="ET5" s="161"/>
-      <c r="EU5" s="166">
+      <c r="EO5" s="157"/>
+      <c r="EP5" s="157"/>
+      <c r="EQ5" s="157"/>
+      <c r="ER5" s="157"/>
+      <c r="ES5" s="157"/>
+      <c r="ET5" s="163"/>
+      <c r="EU5" s="156">
         <f>EU6</f>
         <v>45432</v>
       </c>
-      <c r="EV5" s="160"/>
-      <c r="EW5" s="160"/>
-      <c r="EX5" s="160"/>
-      <c r="EY5" s="160"/>
-      <c r="EZ5" s="160"/>
-      <c r="FA5" s="167"/>
-      <c r="FB5" s="159">
+      <c r="EV5" s="157"/>
+      <c r="EW5" s="157"/>
+      <c r="EX5" s="157"/>
+      <c r="EY5" s="157"/>
+      <c r="EZ5" s="157"/>
+      <c r="FA5" s="158"/>
+      <c r="FB5" s="162">
         <f>FB6</f>
         <v>45439</v>
       </c>
-      <c r="FC5" s="160"/>
-      <c r="FD5" s="160"/>
-      <c r="FE5" s="160"/>
-      <c r="FF5" s="160"/>
-      <c r="FG5" s="160"/>
-      <c r="FH5" s="161"/>
-      <c r="FI5" s="159">
+      <c r="FC5" s="157"/>
+      <c r="FD5" s="157"/>
+      <c r="FE5" s="157"/>
+      <c r="FF5" s="157"/>
+      <c r="FG5" s="157"/>
+      <c r="FH5" s="163"/>
+      <c r="FI5" s="162">
         <f t="shared" ref="FI5" si="39">FI6</f>
         <v>45446</v>
       </c>
-      <c r="FJ5" s="160"/>
-      <c r="FK5" s="160"/>
-      <c r="FL5" s="160"/>
-      <c r="FM5" s="160"/>
-      <c r="FN5" s="160"/>
-      <c r="FO5" s="161"/>
-      <c r="FP5" s="166">
+      <c r="FJ5" s="157"/>
+      <c r="FK5" s="157"/>
+      <c r="FL5" s="157"/>
+      <c r="FM5" s="157"/>
+      <c r="FN5" s="157"/>
+      <c r="FO5" s="163"/>
+      <c r="FP5" s="156">
         <f t="shared" ref="FP5" si="40">FP6</f>
         <v>45453</v>
       </c>
-      <c r="FQ5" s="160"/>
-      <c r="FR5" s="160"/>
-      <c r="FS5" s="160"/>
-      <c r="FT5" s="160"/>
-      <c r="FU5" s="160"/>
-      <c r="FV5" s="167"/>
-      <c r="FW5" s="159">
+      <c r="FQ5" s="157"/>
+      <c r="FR5" s="157"/>
+      <c r="FS5" s="157"/>
+      <c r="FT5" s="157"/>
+      <c r="FU5" s="157"/>
+      <c r="FV5" s="158"/>
+      <c r="FW5" s="162">
         <f t="shared" ref="FW5" si="41">FW6</f>
         <v>45460</v>
       </c>
-      <c r="FX5" s="160"/>
-      <c r="FY5" s="160"/>
-      <c r="FZ5" s="160"/>
-      <c r="GA5" s="160"/>
-      <c r="GB5" s="160"/>
-      <c r="GC5" s="161"/>
-      <c r="GD5" s="159">
+      <c r="FX5" s="157"/>
+      <c r="FY5" s="157"/>
+      <c r="FZ5" s="157"/>
+      <c r="GA5" s="157"/>
+      <c r="GB5" s="157"/>
+      <c r="GC5" s="163"/>
+      <c r="GD5" s="162">
         <f t="shared" ref="GD5" si="42">GD6</f>
         <v>45467</v>
       </c>
-      <c r="GE5" s="160"/>
-      <c r="GF5" s="160"/>
-      <c r="GG5" s="160"/>
-      <c r="GH5" s="160"/>
-      <c r="GI5" s="160"/>
-      <c r="GJ5" s="161"/>
-      <c r="GK5" s="166">
+      <c r="GE5" s="157"/>
+      <c r="GF5" s="157"/>
+      <c r="GG5" s="157"/>
+      <c r="GH5" s="157"/>
+      <c r="GI5" s="157"/>
+      <c r="GJ5" s="163"/>
+      <c r="GK5" s="156">
         <f t="shared" ref="GK5" si="43">GK6</f>
         <v>45474</v>
       </c>
-      <c r="GL5" s="160"/>
-      <c r="GM5" s="160"/>
-      <c r="GN5" s="160"/>
-      <c r="GO5" s="160"/>
-      <c r="GP5" s="160"/>
-      <c r="GQ5" s="167"/>
-      <c r="GR5" s="159">
+      <c r="GL5" s="157"/>
+      <c r="GM5" s="157"/>
+      <c r="GN5" s="157"/>
+      <c r="GO5" s="157"/>
+      <c r="GP5" s="157"/>
+      <c r="GQ5" s="158"/>
+      <c r="GR5" s="162">
         <f t="shared" ref="GR5" si="44">GR6</f>
         <v>45481</v>
       </c>
-      <c r="GS5" s="160"/>
-      <c r="GT5" s="160"/>
-      <c r="GU5" s="160"/>
-      <c r="GV5" s="160"/>
-      <c r="GW5" s="160"/>
-      <c r="GX5" s="161"/>
-      <c r="GY5" s="166">
+      <c r="GS5" s="157"/>
+      <c r="GT5" s="157"/>
+      <c r="GU5" s="157"/>
+      <c r="GV5" s="157"/>
+      <c r="GW5" s="157"/>
+      <c r="GX5" s="163"/>
+      <c r="GY5" s="156">
         <f t="shared" ref="GY5" si="45">GY6</f>
         <v>45488</v>
       </c>
-      <c r="GZ5" s="160"/>
-      <c r="HA5" s="160"/>
-      <c r="HB5" s="160"/>
-      <c r="HC5" s="160"/>
-      <c r="HD5" s="160"/>
-      <c r="HE5" s="167"/>
-      <c r="HF5" s="159">
+      <c r="GZ5" s="157"/>
+      <c r="HA5" s="157"/>
+      <c r="HB5" s="157"/>
+      <c r="HC5" s="157"/>
+      <c r="HD5" s="157"/>
+      <c r="HE5" s="158"/>
+      <c r="HF5" s="162">
         <f t="shared" ref="HF5" si="46">HF6</f>
         <v>45495</v>
       </c>
-      <c r="HG5" s="160"/>
-      <c r="HH5" s="160"/>
-      <c r="HI5" s="160"/>
-      <c r="HJ5" s="160"/>
-      <c r="HK5" s="160"/>
-      <c r="HL5" s="161"/>
-      <c r="HM5" s="166">
+      <c r="HG5" s="157"/>
+      <c r="HH5" s="157"/>
+      <c r="HI5" s="157"/>
+      <c r="HJ5" s="157"/>
+      <c r="HK5" s="157"/>
+      <c r="HL5" s="163"/>
+      <c r="HM5" s="156">
         <f t="shared" ref="HM5" si="47">HM6</f>
         <v>45502</v>
       </c>
-      <c r="HN5" s="160"/>
-      <c r="HO5" s="160"/>
-      <c r="HP5" s="160"/>
-      <c r="HQ5" s="160"/>
-      <c r="HR5" s="160"/>
-      <c r="HS5" s="167"/>
-      <c r="HT5" s="159">
+      <c r="HN5" s="157"/>
+      <c r="HO5" s="157"/>
+      <c r="HP5" s="157"/>
+      <c r="HQ5" s="157"/>
+      <c r="HR5" s="157"/>
+      <c r="HS5" s="158"/>
+      <c r="HT5" s="162">
         <f t="shared" ref="HT5" si="48">HT6</f>
         <v>45509</v>
       </c>
-      <c r="HU5" s="160"/>
-      <c r="HV5" s="160"/>
-      <c r="HW5" s="160"/>
-      <c r="HX5" s="160"/>
-      <c r="HY5" s="160"/>
-      <c r="HZ5" s="161"/>
-      <c r="IA5" s="166">
+      <c r="HU5" s="157"/>
+      <c r="HV5" s="157"/>
+      <c r="HW5" s="157"/>
+      <c r="HX5" s="157"/>
+      <c r="HY5" s="157"/>
+      <c r="HZ5" s="163"/>
+      <c r="IA5" s="156">
         <f t="shared" ref="IA5" si="49">IA6</f>
         <v>45516</v>
       </c>
-      <c r="IB5" s="160"/>
-      <c r="IC5" s="160"/>
-      <c r="ID5" s="160"/>
-      <c r="IE5" s="160"/>
-      <c r="IF5" s="160"/>
-      <c r="IG5" s="167"/>
-      <c r="IH5" s="159">
+      <c r="IB5" s="157"/>
+      <c r="IC5" s="157"/>
+      <c r="ID5" s="157"/>
+      <c r="IE5" s="157"/>
+      <c r="IF5" s="157"/>
+      <c r="IG5" s="158"/>
+      <c r="IH5" s="162">
         <f t="shared" ref="IH5" si="50">IH6</f>
         <v>45523</v>
       </c>
-      <c r="II5" s="160"/>
-      <c r="IJ5" s="160"/>
-      <c r="IK5" s="160"/>
-      <c r="IL5" s="160"/>
-      <c r="IM5" s="160"/>
-      <c r="IN5" s="161"/>
-      <c r="IO5" s="166">
+      <c r="II5" s="157"/>
+      <c r="IJ5" s="157"/>
+      <c r="IK5" s="157"/>
+      <c r="IL5" s="157"/>
+      <c r="IM5" s="157"/>
+      <c r="IN5" s="163"/>
+      <c r="IO5" s="156">
         <f t="shared" ref="IO5" si="51">IO6</f>
         <v>45530</v>
       </c>
-      <c r="IP5" s="160"/>
-      <c r="IQ5" s="160"/>
-      <c r="IR5" s="160"/>
-      <c r="IS5" s="160"/>
-      <c r="IT5" s="160"/>
-      <c r="IU5" s="167"/>
-    </row>
-    <row r="6" spans="1:255" s="53" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="IP5" s="157"/>
+      <c r="IQ5" s="157"/>
+      <c r="IR5" s="157"/>
+      <c r="IS5" s="157"/>
+      <c r="IT5" s="157"/>
+      <c r="IU5" s="158"/>
+    </row>
+    <row r="6" spans="1:255" s="53" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="146"/>
       <c r="K6" s="64">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
@@ -6040,7 +6049,7 @@
       </c>
       <c r="IU6" s="76"/>
     </row>
-    <row r="7" spans="1:255" s="52" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:255" s="52" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
         <v>0</v>
       </c>
@@ -7047,7 +7056,7 @@
       </c>
       <c r="IU7" s="62"/>
     </row>
-    <row r="8" spans="1:255" s="26" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:255" s="26" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="90" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -7309,7 +7318,7 @@
       <c r="IT8" s="27"/>
       <c r="IU8" s="27"/>
     </row>
-    <row r="9" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A9" s="91" t="str">
         <f t="shared" ref="A9:A20" si="254">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -7583,7 +7592,7 @@
       <c r="IT9" s="34"/>
       <c r="IU9" s="34"/>
     </row>
-    <row r="10" spans="1:255" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:255" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="91" t="str">
         <f t="shared" ref="A10:A18" si="257">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -7857,7 +7866,7 @@
       <c r="IT10" s="34"/>
       <c r="IU10" s="34"/>
     </row>
-    <row r="11" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.2</v>
@@ -8131,7 +8140,7 @@
       <c r="IT11" s="34"/>
       <c r="IU11" s="34"/>
     </row>
-    <row r="12" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.3</v>
@@ -8153,7 +8162,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="46">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="I12" s="102">
         <f t="shared" si="259"/>
@@ -8406,7 +8415,7 @@
       <c r="IT12" s="34"/>
       <c r="IU12" s="34"/>
     </row>
-    <row r="13" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.4</v>
@@ -8427,7 +8436,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="46">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I13" s="102">
         <f t="shared" ref="I13" si="261">IF(OR(F13=0,E13=0),0,NETWORKDAYS(E13,F13))</f>
@@ -8680,7 +8689,7 @@
       <c r="IT13" s="34"/>
       <c r="IU13" s="34"/>
     </row>
-    <row r="14" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.5</v>
@@ -8957,7 +8966,7 @@
       <c r="IT14" s="34"/>
       <c r="IU14" s="34"/>
     </row>
-    <row r="15" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.6</v>
@@ -9233,7 +9242,7 @@
       <c r="IT15" s="34"/>
       <c r="IU15" s="34"/>
     </row>
-    <row r="16" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.7</v>
@@ -9509,7 +9518,7 @@
       <c r="IT16" s="34"/>
       <c r="IU16" s="34"/>
     </row>
-    <row r="17" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.8</v>
@@ -9785,7 +9794,7 @@
       <c r="IT17" s="34"/>
       <c r="IU17" s="34"/>
     </row>
-    <row r="18" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.9</v>
@@ -10062,7 +10071,7 @@
       <c r="IT18" s="34"/>
       <c r="IU18" s="34"/>
     </row>
-    <row r="19" spans="1:255" s="31" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:255" s="31" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="92" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -10324,7 +10333,7 @@
       <c r="IT19" s="36"/>
       <c r="IU19" s="36"/>
     </row>
-    <row r="20" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="91" t="str">
         <f t="shared" si="254"/>
         <v>2.1</v>
@@ -10599,7 +10608,7 @@
       <c r="IT20" s="34"/>
       <c r="IU20" s="34"/>
     </row>
-    <row r="21" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.1.1</v>
@@ -10876,7 +10885,7 @@
       <c r="IT21" s="34"/>
       <c r="IU21" s="34"/>
     </row>
-    <row r="22" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.1.2</v>
@@ -11152,7 +11161,7 @@
       <c r="IT22" s="34"/>
       <c r="IU22" s="34"/>
     </row>
-    <row r="23" spans="1:255" s="31" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:255" s="31" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A23" s="92" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
@@ -11414,7 +11423,7 @@
       <c r="IT23" s="36"/>
       <c r="IU23" s="36"/>
     </row>
-    <row r="24" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A24" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
@@ -11430,17 +11439,17 @@
       </c>
       <c r="F24" s="84">
         <f t="shared" ref="F24" si="271">IF(ISBLANK(E24)," - ",IF(G24=0,E24,E24+G24-1))</f>
-        <v>45499</v>
+        <v>45504</v>
       </c>
       <c r="G24" s="45">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H24" s="46">
         <v>0</v>
       </c>
       <c r="I24" s="102">
         <f>IF(OR(F24=0,E24=0),0,NETWORKDAYS(E24,F24))</f>
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J24" s="94"/>
       <c r="K24" s="34"/>
@@ -11689,7 +11698,7 @@
       <c r="IT24" s="34"/>
       <c r="IU24" s="34"/>
     </row>
-    <row r="25" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.1.1</v>
@@ -11703,11 +11712,11 @@
       <c r="D25" s="33"/>
       <c r="E25" s="87">
         <f>E26-14</f>
-        <v>45485</v>
+        <v>45489</v>
       </c>
       <c r="F25" s="84">
         <f t="shared" ref="F25" si="272">IF(ISBLANK(E25)," - ",IF(G25=0,E25,E25+G25-1))</f>
-        <v>45485</v>
+        <v>45489</v>
       </c>
       <c r="G25" s="45">
         <v>1</v>
@@ -11966,7 +11975,7 @@
       <c r="IT25" s="34"/>
       <c r="IU25" s="34"/>
     </row>
-    <row r="26" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A26" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.1.2</v>
@@ -11979,11 +11988,11 @@
       </c>
       <c r="D26" s="33"/>
       <c r="E26" s="87">
-        <v>45499</v>
+        <v>45503</v>
       </c>
       <c r="F26" s="84">
         <f t="shared" ref="F26" si="273">IF(ISBLANK(E26)," - ",IF(G26=0,E26,E26+G26-1))</f>
-        <v>45499</v>
+        <v>45503</v>
       </c>
       <c r="G26" s="45">
         <v>1</v>
@@ -12242,7 +12251,7 @@
       <c r="IT26" s="34"/>
       <c r="IU26" s="34"/>
     </row>
-    <row r="27" spans="1:255" s="31" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:255" s="31" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A27" s="92" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
@@ -12504,7 +12513,7 @@
       <c r="IT27" s="36"/>
       <c r="IU27" s="36"/>
     </row>
-    <row r="28" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A28" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
@@ -12516,21 +12525,21 @@
       <c r="D28" s="33"/>
       <c r="E28" s="87">
         <f>F24+1</f>
-        <v>45500</v>
+        <v>45505</v>
       </c>
       <c r="F28" s="84">
         <f t="shared" ref="F28" si="274">IF(ISBLANK(E28)," - ",IF(G28=0,E28,E28+G28-1))</f>
         <v>45534</v>
       </c>
       <c r="G28" s="45">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H28" s="46">
         <v>0</v>
       </c>
       <c r="I28" s="102">
         <f>IF(OR(F28=0,E28=0),0,NETWORKDAYS(E28,F28))</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J28" s="94"/>
       <c r="K28" s="34"/>
@@ -12779,7 +12788,7 @@
       <c r="IT28" s="34"/>
       <c r="IU28" s="34"/>
     </row>
-    <row r="29" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.1</v>
@@ -12792,12 +12801,12 @@
       </c>
       <c r="D29" s="33"/>
       <c r="E29" s="87">
-        <f>F31-32</f>
-        <v>45502</v>
+        <f>F31-29</f>
+        <v>45505</v>
       </c>
       <c r="F29" s="84">
         <f t="shared" ref="F29" si="275">IF(ISBLANK(E29)," - ",IF(G29=0,E29,E29+G29-1))</f>
-        <v>45502</v>
+        <v>45505</v>
       </c>
       <c r="G29" s="45">
         <v>1</v>
@@ -13056,7 +13065,7 @@
       <c r="IT29" s="34"/>
       <c r="IU29" s="34"/>
     </row>
-    <row r="30" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A30" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.2</v>
@@ -13332,7 +13341,7 @@
       <c r="IT30" s="34"/>
       <c r="IU30" s="34"/>
     </row>
-    <row r="31" spans="1:255" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.3</v>
@@ -13609,7 +13618,7 @@
       <c r="IT31" s="34"/>
       <c r="IU31" s="34"/>
     </row>
-    <row r="33" spans="1:255" s="40" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:255" s="40" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="105" t="s">
         <v>1</v>
       </c>
@@ -13868,7 +13877,7 @@
       <c r="IT33" s="34"/>
       <c r="IU33" s="34"/>
     </row>
-    <row r="34" spans="1:255" s="39" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:255" s="39" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A34" s="106" t="s">
         <v>75</v>
       </c>
@@ -14123,7 +14132,7 @@
       <c r="IT34" s="34"/>
       <c r="IU34" s="34"/>
     </row>
-    <row r="35" spans="1:255" s="39" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:255" s="39" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A35" s="92" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -14160,7 +14169,9 @@
       <c r="AC35" s="34"/>
       <c r="AD35" s="34"/>
       <c r="AE35" s="34"/>
-      <c r="AF35" s="34"/>
+      <c r="AF35" s="34" t="s">
+        <v>161</v>
+      </c>
       <c r="AG35" s="34"/>
       <c r="AH35" s="34"/>
       <c r="AI35" s="34"/>
@@ -14385,7 +14396,7 @@
       <c r="IT35" s="34"/>
       <c r="IU35" s="34"/>
     </row>
-    <row r="36" spans="1:255" s="39" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:255" s="39" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A36" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -14430,7 +14441,9 @@
       <c r="AC36" s="34"/>
       <c r="AD36" s="34"/>
       <c r="AE36" s="34"/>
-      <c r="AF36" s="34"/>
+      <c r="AF36" s="34" t="s">
+        <v>160</v>
+      </c>
       <c r="AG36" s="34"/>
       <c r="AH36" s="34"/>
       <c r="AI36" s="34"/>
@@ -14655,7 +14668,7 @@
       <c r="IT36" s="34"/>
       <c r="IU36" s="34"/>
     </row>
-    <row r="37" spans="1:255" s="39" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:255" s="39" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A37" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -14925,7 +14938,7 @@
       <c r="IT37" s="34"/>
       <c r="IU37" s="34"/>
     </row>
-    <row r="38" spans="1:255" s="39" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:255" s="39" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A38" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
@@ -15195,32 +15208,61 @@
       <c r="IT38" s="34"/>
       <c r="IU38" s="34"/>
     </row>
-    <row r="39" spans="1:255" s="41" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:255" s="41" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="142" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
       </c>
       <c r="C39" s="154"/>
     </row>
-    <row r="40" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="73">
-    <mergeCell ref="IO5:IU5"/>
-    <mergeCell ref="IO4:IU4"/>
-    <mergeCell ref="HT4:HZ4"/>
-    <mergeCell ref="IA4:IG4"/>
-    <mergeCell ref="IH4:IN4"/>
-    <mergeCell ref="HM5:HS5"/>
-    <mergeCell ref="HT5:HZ5"/>
-    <mergeCell ref="IA5:IG5"/>
-    <mergeCell ref="IH5:IN5"/>
-    <mergeCell ref="GY4:HE4"/>
-    <mergeCell ref="HF4:HL4"/>
-    <mergeCell ref="GY5:HE5"/>
-    <mergeCell ref="HF5:HL5"/>
-    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="BH4:BN4"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="AM5:AS5"/>
+    <mergeCell ref="AT4:AZ4"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="BA4:BG4"/>
+    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="AD1:AR1"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="AF5:AL5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="FI4:FO4"/>
+    <mergeCell ref="FP4:FV4"/>
+    <mergeCell ref="EG4:EM4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="DS5:DY5"/>
+    <mergeCell ref="DZ5:EF5"/>
+    <mergeCell ref="EG5:EM5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DS4:DY4"/>
+    <mergeCell ref="DZ4:EF4"/>
     <mergeCell ref="FW4:GC4"/>
     <mergeCell ref="GD4:GJ4"/>
     <mergeCell ref="GK4:GQ4"/>
@@ -15237,49 +15279,20 @@
     <mergeCell ref="EN4:ET4"/>
     <mergeCell ref="EU4:FA4"/>
     <mergeCell ref="FB4:FH4"/>
-    <mergeCell ref="FI4:FO4"/>
-    <mergeCell ref="FP4:FV4"/>
-    <mergeCell ref="EG4:EM4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE5:DK5"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="DS5:DY5"/>
-    <mergeCell ref="DZ5:EF5"/>
-    <mergeCell ref="EG5:EM5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DS4:DY4"/>
-    <mergeCell ref="DZ4:EF4"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="AD1:AR1"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AF5:AL5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="HM5:HS5"/>
+    <mergeCell ref="HT5:HZ5"/>
+    <mergeCell ref="IA5:IG5"/>
+    <mergeCell ref="IH5:IN5"/>
+    <mergeCell ref="GY4:HE4"/>
+    <mergeCell ref="HF4:HL4"/>
+    <mergeCell ref="GY5:HE5"/>
+    <mergeCell ref="HF5:HL5"/>
+    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="IO5:IU5"/>
+    <mergeCell ref="IO4:IU4"/>
+    <mergeCell ref="HT4:HZ4"/>
+    <mergeCell ref="IA4:IG4"/>
+    <mergeCell ref="IH4:IN4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H34:H38 H8:H31">
@@ -15317,7 +15330,7 @@
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Start Date." sqref="I4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.25"/>
@@ -15339,13 +15352,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:colOff>5443</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>28</xdr:col>
-                    <xdr:colOff>99060</xdr:colOff>
+                    <xdr:colOff>97971</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>
@@ -15390,62 +15403,62 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="90.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="5.53515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="90.4609375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>76</v>
       </c>
       <c r="B1" s="21"/>
     </row>
-    <row r="2" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A2" s="119" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A4" s="120" t="s">
         <v>77</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="56.6" x14ac:dyDescent="0.35">
       <c r="B5" s="121" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.3" x14ac:dyDescent="0.35">
       <c r="B7" s="121" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B9" s="119" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.3" x14ac:dyDescent="0.35">
       <c r="B11" s="122" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A13" s="179" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="179"/>
     </row>
-    <row r="15" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="123"/>
       <c r="B15" s="124" t="s">
         <v>79</v>
@@ -15453,7 +15466,7 @@
       <c r="C15" s="125"/>
       <c r="D15" s="125"/>
     </row>
-    <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="123"/>
       <c r="B16" s="124" t="s">
         <v>80</v>
@@ -15461,162 +15474,162 @@
       <c r="C16" s="125"/>
       <c r="D16" s="125"/>
     </row>
-    <row r="17" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A17" s="126"/>
       <c r="B17" s="124" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A18" s="126"/>
       <c r="B18" s="124" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A19" s="126"/>
       <c r="B19" s="124" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A20" s="126"/>
       <c r="B20" s="124" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A21" s="126"/>
       <c r="B21" s="127" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A22" s="126"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A23" s="179" t="s">
         <v>85</v>
       </c>
       <c r="B23" s="179"/>
     </row>
-    <row r="24" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="42.45" x14ac:dyDescent="0.4">
       <c r="A24" s="126"/>
       <c r="B24" s="124" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A25" s="126"/>
       <c r="B25" s="124"/>
     </row>
-    <row r="26" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A26" s="126"/>
       <c r="B26" s="128" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A27" s="126"/>
       <c r="B27" s="124" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A28" s="126"/>
       <c r="B28" s="124" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A29" s="126"/>
       <c r="B29" s="124"/>
     </row>
-    <row r="30" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A30" s="126"/>
       <c r="B30" s="128" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A31" s="126"/>
       <c r="B31" s="124" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A32" s="126"/>
       <c r="B32" s="124" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A33" s="126"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A34" s="126"/>
       <c r="B34" s="124" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A35" s="126"/>
       <c r="B35" s="129" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A36" s="126"/>
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A37" s="179" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="179"/>
     </row>
-    <row r="38" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B38" s="124" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="14.15" x14ac:dyDescent="0.3">
       <c r="B40" s="124" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B42" s="124" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B44" s="124" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B45" s="10"/>
     </row>
-    <row r="46" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B46" s="124" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A48" s="179" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="179"/>
     </row>
-    <row r="49" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B49" s="124" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A51" s="130" t="s">
         <v>8</v>
       </c>
@@ -15624,7 +15637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A52" s="130" t="s">
         <v>10</v>
       </c>
@@ -15632,7 +15645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A53" s="130" t="s">
         <v>12</v>
       </c>
@@ -15640,19 +15653,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A54" s="122"/>
       <c r="B54" s="124" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A55" s="122"/>
       <c r="B55" s="124" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A56" s="130" t="s">
         <v>14</v>
       </c>
@@ -15660,19 +15673,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A57" s="122"/>
       <c r="B57" s="124" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A58" s="122"/>
       <c r="B58" s="124" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A59" s="130" t="s">
         <v>16</v>
       </c>
@@ -15680,13 +15693,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A60" s="122"/>
       <c r="B60" s="124" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A61" s="130" t="s">
         <v>106</v>
       </c>
@@ -15694,33 +15707,33 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A62" s="131"/>
       <c r="B62" s="124" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A64" s="179" t="s">
         <v>6</v>
       </c>
       <c r="B64" s="179"/>
     </row>
-    <row r="65" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="42.45" x14ac:dyDescent="0.3">
       <c r="B65" s="124" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A67" s="179" t="s">
         <v>3</v>
       </c>
       <c r="B67" s="179"/>
     </row>
-    <row r="68" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A68" s="132" t="s">
         <v>4</v>
       </c>
@@ -15728,17 +15741,17 @@
         <v>110</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A69" s="131"/>
       <c r="B69" s="134" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A70" s="131"/>
       <c r="B70" s="135"/>
     </row>
-    <row r="71" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A71" s="132" t="s">
         <v>4</v>
       </c>
@@ -15746,17 +15759,17 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A72" s="131"/>
       <c r="B72" s="134" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A73" s="131"/>
       <c r="B73" s="135"/>
     </row>
-    <row r="74" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A74" s="132" t="s">
         <v>4</v>
       </c>
@@ -15764,17 +15777,17 @@
         <v>114</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A75" s="131"/>
       <c r="B75" s="121" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A76" s="131"/>
       <c r="B76" s="131"/>
     </row>
-    <row r="77" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A77" s="132" t="s">
         <v>4</v>
       </c>
@@ -15782,17 +15795,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A78" s="131"/>
       <c r="B78" s="121" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A79" s="131"/>
       <c r="B79" s="131"/>
     </row>
-    <row r="80" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A80" s="132" t="s">
         <v>4</v>
       </c>
@@ -15800,29 +15813,29 @@
         <v>118</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A81" s="131"/>
       <c r="B81" s="137" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A82" s="131"/>
       <c r="B82" s="137" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A83" s="131"/>
       <c r="B83" s="137" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A84" s="131"/>
       <c r="B84" s="138"/>
     </row>
-    <row r="85" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A85" s="132" t="s">
         <v>4</v>
       </c>
@@ -15830,29 +15843,29 @@
         <v>122</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A86" s="131"/>
       <c r="B86" s="121" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A87" s="131"/>
       <c r="B87" s="139" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A88" s="131"/>
       <c r="B88" s="140" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A89" s="131"/>
       <c r="B89" s="131"/>
     </row>
-    <row r="90" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A90" s="132" t="s">
         <v>4</v>
       </c>
@@ -15860,13 +15873,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A91" s="122"/>
       <c r="B91" s="137" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>51</v>
       </c>
@@ -15904,172 +15917,172 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="3" max="3" width="55.109375" customWidth="1"/>
+    <col min="1" max="1" width="5.53515625" customWidth="1"/>
+    <col min="2" max="2" width="37.69140625" customWidth="1"/>
+    <col min="3" max="3" width="55.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="C7" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="C13" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B18" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B22" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B26" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B34" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B42" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="B46" s="11" t="s">
         <v>21</v>
       </c>
@@ -16094,172 +16107,172 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.53515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="82.07421875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="20"/>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="B2" s="24"/>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="22"/>
       <c r="B3" s="17" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="23"/>
     </row>
-    <row r="4" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="7"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A6" s="5"/>
       <c r="B6" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="7"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="7"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" ht="46.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="45.9" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
       <c r="B10" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="7"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="7"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="30.45" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="7"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
       <c r="B18" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>

</xml_diff>

<commit_message>
added research objective, more notes to 2nd read
</commit_message>
<xml_diff>
--- a/thesis gantt chart.xlsx
+++ b/thesis gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wings_stuff\srus\TUD\yr5\thesis\thesis_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3DE479-D431-459E-8B98-65E61DAFEDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDF6B05-F0CB-473F-B44A-FD462D2819C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -3263,6 +3263,15 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="70" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3275,28 +3284,7 @@
     <xf numFmtId="167" fontId="52" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="84" fillId="24" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -3333,6 +3321,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3586,13 +3586,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>10886</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
+          <xdr:colOff>97971</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -4175,74 +4175,74 @@
   </sheetPr>
   <dimension ref="A1:IU43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
+      <selection pane="bottomLeft" activeCell="AN21" sqref="AN21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="25" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="155" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.84375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="45.84375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="7.84375" style="155" customWidth="1"/>
+    <col min="4" max="4" width="6.84375" style="25" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="25" customWidth="1"/>
     <col min="7" max="7" width="6" style="25" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="25" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="25" customWidth="1"/>
-    <col min="10" max="10" width="0.5703125" style="25" customWidth="1"/>
-    <col min="11" max="66" width="2.42578125" style="25" customWidth="1"/>
-    <col min="67" max="68" width="2.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="2.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="2.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="1.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="1.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="2.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="78" max="99" width="2.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="100" max="101" width="1.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="1.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="2.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="105" max="106" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="107" max="108" width="1.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="109" max="131" width="2.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="2.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="134" max="136" width="1.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="1.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="139" max="162" width="2.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="163" max="164" width="1.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="1.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="2.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="168" max="169" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="170" max="192" width="2.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="1.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="2.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="196" max="197" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="198" max="199" width="1.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="1.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="202" max="221" width="2.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="2.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="225" max="227" width="1.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.69140625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="5.53515625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="0.53515625" style="25" customWidth="1"/>
+    <col min="11" max="66" width="2.3828125" style="25" customWidth="1"/>
+    <col min="67" max="68" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="2.15234375" style="25" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="2.15234375" style="25" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="78" max="99" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="100" max="101" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="2.15234375" style="25" bestFit="1" customWidth="1"/>
+    <col min="105" max="106" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="107" max="108" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="109" max="131" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="2.15234375" style="25" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="134" max="136" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="139" max="162" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="163" max="164" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="2.15234375" style="25" bestFit="1" customWidth="1"/>
+    <col min="168" max="169" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="170" max="192" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="2.15234375" style="25" bestFit="1" customWidth="1"/>
+    <col min="196" max="197" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="198" max="199" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="1.84375" style="25" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="202" max="221" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="2.15234375" style="25" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="225" max="227" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="2" style="25" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="1.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="2.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="231" max="252" width="2.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="253" max="254" width="2.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="1.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="256" max="16384" width="9.140625" style="25"/>
+    <col min="229" max="229" width="1.53515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="2.15234375" style="25" bestFit="1" customWidth="1"/>
+    <col min="231" max="252" width="2.3828125" style="25" bestFit="1" customWidth="1"/>
+    <col min="253" max="254" width="2.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="1.69140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="256" max="16384" width="9.15234375" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:255" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="118" t="s">
         <v>138</v>
       </c>
@@ -4255,23 +4255,23 @@
       <c r="K1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="AD1" s="168"/>
-      <c r="AE1" s="168"/>
-      <c r="AF1" s="168"/>
-      <c r="AG1" s="168"/>
-      <c r="AH1" s="168"/>
-      <c r="AI1" s="168"/>
-      <c r="AJ1" s="168"/>
-      <c r="AK1" s="168"/>
-      <c r="AL1" s="168"/>
-      <c r="AM1" s="168"/>
-      <c r="AN1" s="168"/>
-      <c r="AO1" s="168"/>
-      <c r="AP1" s="168"/>
-      <c r="AQ1" s="168"/>
-      <c r="AR1" s="168"/>
-    </row>
-    <row r="2" spans="1:255" s="59" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD1" s="164"/>
+      <c r="AE1" s="164"/>
+      <c r="AF1" s="164"/>
+      <c r="AG1" s="164"/>
+      <c r="AH1" s="164"/>
+      <c r="AI1" s="164"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="164"/>
+      <c r="AL1" s="164"/>
+      <c r="AM1" s="164"/>
+      <c r="AN1" s="164"/>
+      <c r="AO1" s="164"/>
+      <c r="AP1" s="164"/>
+      <c r="AQ1" s="164"/>
+      <c r="AR1" s="164"/>
+    </row>
+    <row r="2" spans="1:255" s="59" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="112" t="s">
         <v>139</v>
       </c>
@@ -4281,7 +4281,7 @@
       <c r="E2" s="56"/>
       <c r="F2" s="58"/>
     </row>
-    <row r="3" spans="1:255" s="100" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:255" s="100" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="96"/>
       <c r="B3" s="97"/>
       <c r="C3" s="145"/>
@@ -4345,735 +4345,735 @@
       <c r="BM3" s="116"/>
       <c r="BN3" s="117"/>
     </row>
-    <row r="4" spans="1:255" s="110" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:255" s="110" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="113" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="167">
         <v>45295</v>
       </c>
-      <c r="D4" s="172"/>
-      <c r="E4" s="173"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="169"/>
       <c r="H4" s="113" t="s">
         <v>71</v>
       </c>
       <c r="I4" s="114">
         <v>1</v>
       </c>
-      <c r="K4" s="156"/>
-      <c r="L4" s="157"/>
-      <c r="M4" s="157"/>
-      <c r="N4" s="157"/>
-      <c r="O4" s="157"/>
-      <c r="P4" s="157"/>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="156" t="str">
+      <c r="K4" s="159"/>
+      <c r="L4" s="160"/>
+      <c r="M4" s="160"/>
+      <c r="N4" s="160"/>
+      <c r="O4" s="160"/>
+      <c r="P4" s="160"/>
+      <c r="Q4" s="161"/>
+      <c r="R4" s="159" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="S4" s="157"/>
-      <c r="T4" s="157"/>
-      <c r="U4" s="157"/>
-      <c r="V4" s="157"/>
-      <c r="W4" s="157"/>
-      <c r="X4" s="158"/>
-      <c r="Y4" s="156" t="str">
+      <c r="S4" s="160"/>
+      <c r="T4" s="160"/>
+      <c r="U4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="159" t="str">
         <f t="shared" ref="Y4" si="0">"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="Z4" s="157"/>
-      <c r="AA4" s="157"/>
-      <c r="AB4" s="157"/>
-      <c r="AC4" s="157"/>
-      <c r="AD4" s="157"/>
-      <c r="AE4" s="158"/>
-      <c r="AF4" s="156" t="str">
+      <c r="Z4" s="160"/>
+      <c r="AA4" s="160"/>
+      <c r="AB4" s="160"/>
+      <c r="AC4" s="160"/>
+      <c r="AD4" s="160"/>
+      <c r="AE4" s="161"/>
+      <c r="AF4" s="159" t="str">
         <f t="shared" ref="AF4" si="1">"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="AG4" s="157"/>
-      <c r="AH4" s="157"/>
-      <c r="AI4" s="157"/>
-      <c r="AJ4" s="157"/>
-      <c r="AK4" s="157"/>
-      <c r="AL4" s="158"/>
-      <c r="AM4" s="156" t="str">
+      <c r="AG4" s="160"/>
+      <c r="AH4" s="160"/>
+      <c r="AI4" s="160"/>
+      <c r="AJ4" s="160"/>
+      <c r="AK4" s="160"/>
+      <c r="AL4" s="161"/>
+      <c r="AM4" s="159" t="str">
         <f t="shared" ref="AM4" si="2">"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AN4" s="157"/>
-      <c r="AO4" s="157"/>
-      <c r="AP4" s="157"/>
-      <c r="AQ4" s="157"/>
-      <c r="AR4" s="157"/>
-      <c r="AS4" s="158"/>
-      <c r="AT4" s="156" t="str">
+      <c r="AN4" s="160"/>
+      <c r="AO4" s="160"/>
+      <c r="AP4" s="160"/>
+      <c r="AQ4" s="160"/>
+      <c r="AR4" s="160"/>
+      <c r="AS4" s="161"/>
+      <c r="AT4" s="159" t="str">
         <f t="shared" ref="AT4" si="3">"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AU4" s="157"/>
-      <c r="AV4" s="157"/>
-      <c r="AW4" s="157"/>
-      <c r="AX4" s="157"/>
-      <c r="AY4" s="157"/>
-      <c r="AZ4" s="158"/>
-      <c r="BA4" s="156" t="str">
+      <c r="AU4" s="160"/>
+      <c r="AV4" s="160"/>
+      <c r="AW4" s="160"/>
+      <c r="AX4" s="160"/>
+      <c r="AY4" s="160"/>
+      <c r="AZ4" s="161"/>
+      <c r="BA4" s="159" t="str">
         <f t="shared" ref="BA4" si="4">"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="BB4" s="157"/>
-      <c r="BC4" s="157"/>
-      <c r="BD4" s="157"/>
-      <c r="BE4" s="157"/>
-      <c r="BF4" s="157"/>
-      <c r="BG4" s="158"/>
-      <c r="BH4" s="156" t="str">
+      <c r="BB4" s="160"/>
+      <c r="BC4" s="160"/>
+      <c r="BD4" s="160"/>
+      <c r="BE4" s="160"/>
+      <c r="BF4" s="160"/>
+      <c r="BG4" s="161"/>
+      <c r="BH4" s="159" t="str">
         <f t="shared" ref="BH4" si="5">"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BI4" s="157"/>
-      <c r="BJ4" s="157"/>
-      <c r="BK4" s="157"/>
-      <c r="BL4" s="157"/>
-      <c r="BM4" s="157"/>
-      <c r="BN4" s="158"/>
-      <c r="BO4" s="156" t="str">
+      <c r="BI4" s="160"/>
+      <c r="BJ4" s="160"/>
+      <c r="BK4" s="160"/>
+      <c r="BL4" s="160"/>
+      <c r="BM4" s="160"/>
+      <c r="BN4" s="161"/>
+      <c r="BO4" s="159" t="str">
         <f t="shared" ref="BO4" si="6">"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BP4" s="157"/>
-      <c r="BQ4" s="157"/>
-      <c r="BR4" s="157"/>
-      <c r="BS4" s="157"/>
-      <c r="BT4" s="157"/>
-      <c r="BU4" s="158"/>
-      <c r="BV4" s="156" t="str">
+      <c r="BP4" s="160"/>
+      <c r="BQ4" s="160"/>
+      <c r="BR4" s="160"/>
+      <c r="BS4" s="160"/>
+      <c r="BT4" s="160"/>
+      <c r="BU4" s="161"/>
+      <c r="BV4" s="159" t="str">
         <f t="shared" ref="BV4" si="7">"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BW4" s="157"/>
-      <c r="BX4" s="157"/>
-      <c r="BY4" s="157"/>
-      <c r="BZ4" s="157"/>
-      <c r="CA4" s="157"/>
-      <c r="CB4" s="158"/>
-      <c r="CC4" s="156" t="str">
+      <c r="BW4" s="160"/>
+      <c r="BX4" s="160"/>
+      <c r="BY4" s="160"/>
+      <c r="BZ4" s="160"/>
+      <c r="CA4" s="160"/>
+      <c r="CB4" s="161"/>
+      <c r="CC4" s="159" t="str">
         <f t="shared" ref="CC4" si="8">"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="CD4" s="157"/>
-      <c r="CE4" s="157"/>
-      <c r="CF4" s="157"/>
-      <c r="CG4" s="157"/>
-      <c r="CH4" s="157"/>
-      <c r="CI4" s="158"/>
-      <c r="CJ4" s="156" t="str">
+      <c r="CD4" s="160"/>
+      <c r="CE4" s="160"/>
+      <c r="CF4" s="160"/>
+      <c r="CG4" s="160"/>
+      <c r="CH4" s="160"/>
+      <c r="CI4" s="161"/>
+      <c r="CJ4" s="159" t="str">
         <f t="shared" ref="CJ4" si="9">"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CK4" s="157"/>
-      <c r="CL4" s="157"/>
-      <c r="CM4" s="157"/>
-      <c r="CN4" s="157"/>
-      <c r="CO4" s="157"/>
-      <c r="CP4" s="158"/>
-      <c r="CQ4" s="156" t="str">
+      <c r="CK4" s="160"/>
+      <c r="CL4" s="160"/>
+      <c r="CM4" s="160"/>
+      <c r="CN4" s="160"/>
+      <c r="CO4" s="160"/>
+      <c r="CP4" s="161"/>
+      <c r="CQ4" s="159" t="str">
         <f t="shared" ref="CQ4" si="10">"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CR4" s="157"/>
-      <c r="CS4" s="157"/>
-      <c r="CT4" s="157"/>
-      <c r="CU4" s="157"/>
-      <c r="CV4" s="157"/>
-      <c r="CW4" s="158"/>
-      <c r="CX4" s="156" t="str">
+      <c r="CR4" s="160"/>
+      <c r="CS4" s="160"/>
+      <c r="CT4" s="160"/>
+      <c r="CU4" s="160"/>
+      <c r="CV4" s="160"/>
+      <c r="CW4" s="161"/>
+      <c r="CX4" s="159" t="str">
         <f t="shared" ref="CX4" si="11">"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="CY4" s="157"/>
-      <c r="CZ4" s="157"/>
-      <c r="DA4" s="157"/>
-      <c r="DB4" s="157"/>
-      <c r="DC4" s="157"/>
-      <c r="DD4" s="158"/>
-      <c r="DE4" s="156" t="str">
+      <c r="CY4" s="160"/>
+      <c r="CZ4" s="160"/>
+      <c r="DA4" s="160"/>
+      <c r="DB4" s="160"/>
+      <c r="DC4" s="160"/>
+      <c r="DD4" s="161"/>
+      <c r="DE4" s="159" t="str">
         <f t="shared" ref="DE4" si="12">"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="DF4" s="157"/>
-      <c r="DG4" s="157"/>
-      <c r="DH4" s="157"/>
-      <c r="DI4" s="157"/>
-      <c r="DJ4" s="157"/>
-      <c r="DK4" s="158"/>
-      <c r="DL4" s="156" t="str">
+      <c r="DF4" s="160"/>
+      <c r="DG4" s="160"/>
+      <c r="DH4" s="160"/>
+      <c r="DI4" s="160"/>
+      <c r="DJ4" s="160"/>
+      <c r="DK4" s="161"/>
+      <c r="DL4" s="159" t="str">
         <f t="shared" ref="DL4" si="13">"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 15</v>
       </c>
-      <c r="DM4" s="157"/>
-      <c r="DN4" s="157"/>
-      <c r="DO4" s="157"/>
-      <c r="DP4" s="157"/>
-      <c r="DQ4" s="157"/>
-      <c r="DR4" s="158"/>
-      <c r="DS4" s="156" t="str">
+      <c r="DM4" s="160"/>
+      <c r="DN4" s="160"/>
+      <c r="DO4" s="160"/>
+      <c r="DP4" s="160"/>
+      <c r="DQ4" s="160"/>
+      <c r="DR4" s="161"/>
+      <c r="DS4" s="159" t="str">
         <f t="shared" ref="DS4" si="14">"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 16</v>
       </c>
-      <c r="DT4" s="157"/>
-      <c r="DU4" s="157"/>
-      <c r="DV4" s="157"/>
-      <c r="DW4" s="157"/>
-      <c r="DX4" s="157"/>
-      <c r="DY4" s="158"/>
-      <c r="DZ4" s="156" t="str">
+      <c r="DT4" s="160"/>
+      <c r="DU4" s="160"/>
+      <c r="DV4" s="160"/>
+      <c r="DW4" s="160"/>
+      <c r="DX4" s="160"/>
+      <c r="DY4" s="161"/>
+      <c r="DZ4" s="159" t="str">
         <f t="shared" ref="DZ4" si="15">"Week "&amp;(DS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 17</v>
       </c>
-      <c r="EA4" s="157"/>
-      <c r="EB4" s="157"/>
-      <c r="EC4" s="157"/>
-      <c r="ED4" s="157"/>
-      <c r="EE4" s="157"/>
-      <c r="EF4" s="158"/>
-      <c r="EG4" s="156" t="str">
+      <c r="EA4" s="160"/>
+      <c r="EB4" s="160"/>
+      <c r="EC4" s="160"/>
+      <c r="ED4" s="160"/>
+      <c r="EE4" s="160"/>
+      <c r="EF4" s="161"/>
+      <c r="EG4" s="159" t="str">
         <f t="shared" ref="EG4" si="16">"Week "&amp;(DZ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 18</v>
       </c>
-      <c r="EH4" s="157"/>
-      <c r="EI4" s="157"/>
-      <c r="EJ4" s="157"/>
-      <c r="EK4" s="157"/>
-      <c r="EL4" s="157"/>
-      <c r="EM4" s="158"/>
-      <c r="EN4" s="156" t="str">
+      <c r="EH4" s="160"/>
+      <c r="EI4" s="160"/>
+      <c r="EJ4" s="160"/>
+      <c r="EK4" s="160"/>
+      <c r="EL4" s="160"/>
+      <c r="EM4" s="161"/>
+      <c r="EN4" s="159" t="str">
         <f t="shared" ref="EN4" si="17">"Week "&amp;(EG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 19</v>
       </c>
-      <c r="EO4" s="157"/>
-      <c r="EP4" s="157"/>
-      <c r="EQ4" s="157"/>
-      <c r="ER4" s="157"/>
-      <c r="ES4" s="157"/>
-      <c r="ET4" s="158"/>
-      <c r="EU4" s="156" t="str">
+      <c r="EO4" s="160"/>
+      <c r="EP4" s="160"/>
+      <c r="EQ4" s="160"/>
+      <c r="ER4" s="160"/>
+      <c r="ES4" s="160"/>
+      <c r="ET4" s="161"/>
+      <c r="EU4" s="159" t="str">
         <f t="shared" ref="EU4" si="18">"Week "&amp;(EN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="EV4" s="157"/>
-      <c r="EW4" s="157"/>
-      <c r="EX4" s="157"/>
-      <c r="EY4" s="157"/>
-      <c r="EZ4" s="157"/>
-      <c r="FA4" s="158"/>
-      <c r="FB4" s="156" t="str">
+      <c r="EV4" s="160"/>
+      <c r="EW4" s="160"/>
+      <c r="EX4" s="160"/>
+      <c r="EY4" s="160"/>
+      <c r="EZ4" s="160"/>
+      <c r="FA4" s="161"/>
+      <c r="FB4" s="159" t="str">
         <f t="shared" ref="FB4" si="19">"Week "&amp;(EU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="FC4" s="157"/>
-      <c r="FD4" s="157"/>
-      <c r="FE4" s="157"/>
-      <c r="FF4" s="157"/>
-      <c r="FG4" s="157"/>
-      <c r="FH4" s="158"/>
-      <c r="FI4" s="156" t="str">
+      <c r="FC4" s="160"/>
+      <c r="FD4" s="160"/>
+      <c r="FE4" s="160"/>
+      <c r="FF4" s="160"/>
+      <c r="FG4" s="160"/>
+      <c r="FH4" s="161"/>
+      <c r="FI4" s="159" t="str">
         <f t="shared" ref="FI4" si="20">"Week "&amp;(FB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="FJ4" s="157"/>
-      <c r="FK4" s="157"/>
-      <c r="FL4" s="157"/>
-      <c r="FM4" s="157"/>
-      <c r="FN4" s="157"/>
-      <c r="FO4" s="158"/>
-      <c r="FP4" s="156" t="str">
+      <c r="FJ4" s="160"/>
+      <c r="FK4" s="160"/>
+      <c r="FL4" s="160"/>
+      <c r="FM4" s="160"/>
+      <c r="FN4" s="160"/>
+      <c r="FO4" s="161"/>
+      <c r="FP4" s="159" t="str">
         <f t="shared" ref="FP4" si="21">"Week "&amp;(FI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="FQ4" s="157"/>
-      <c r="FR4" s="157"/>
-      <c r="FS4" s="157"/>
-      <c r="FT4" s="157"/>
-      <c r="FU4" s="157"/>
-      <c r="FV4" s="158"/>
-      <c r="FW4" s="156" t="str">
+      <c r="FQ4" s="160"/>
+      <c r="FR4" s="160"/>
+      <c r="FS4" s="160"/>
+      <c r="FT4" s="160"/>
+      <c r="FU4" s="160"/>
+      <c r="FV4" s="161"/>
+      <c r="FW4" s="159" t="str">
         <f t="shared" ref="FW4" si="22">"Week "&amp;(FP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="FX4" s="157"/>
-      <c r="FY4" s="157"/>
-      <c r="FZ4" s="157"/>
-      <c r="GA4" s="157"/>
-      <c r="GB4" s="157"/>
-      <c r="GC4" s="158"/>
-      <c r="GD4" s="156" t="str">
+      <c r="FX4" s="160"/>
+      <c r="FY4" s="160"/>
+      <c r="FZ4" s="160"/>
+      <c r="GA4" s="160"/>
+      <c r="GB4" s="160"/>
+      <c r="GC4" s="161"/>
+      <c r="GD4" s="159" t="str">
         <f t="shared" ref="GD4" si="23">"Week "&amp;(FW6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="GE4" s="157"/>
-      <c r="GF4" s="157"/>
-      <c r="GG4" s="157"/>
-      <c r="GH4" s="157"/>
-      <c r="GI4" s="157"/>
-      <c r="GJ4" s="158"/>
-      <c r="GK4" s="156" t="str">
+      <c r="GE4" s="160"/>
+      <c r="GF4" s="160"/>
+      <c r="GG4" s="160"/>
+      <c r="GH4" s="160"/>
+      <c r="GI4" s="160"/>
+      <c r="GJ4" s="161"/>
+      <c r="GK4" s="159" t="str">
         <f t="shared" ref="GK4" si="24">"Week "&amp;(GD6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="GL4" s="157"/>
-      <c r="GM4" s="157"/>
-      <c r="GN4" s="157"/>
-      <c r="GO4" s="157"/>
-      <c r="GP4" s="157"/>
-      <c r="GQ4" s="158"/>
-      <c r="GR4" s="156" t="str">
+      <c r="GL4" s="160"/>
+      <c r="GM4" s="160"/>
+      <c r="GN4" s="160"/>
+      <c r="GO4" s="160"/>
+      <c r="GP4" s="160"/>
+      <c r="GQ4" s="161"/>
+      <c r="GR4" s="159" t="str">
         <f t="shared" ref="GR4" si="25">"Week "&amp;(GK6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="GS4" s="157"/>
-      <c r="GT4" s="157"/>
-      <c r="GU4" s="157"/>
-      <c r="GV4" s="157"/>
-      <c r="GW4" s="157"/>
-      <c r="GX4" s="158"/>
-      <c r="GY4" s="156" t="str">
+      <c r="GS4" s="160"/>
+      <c r="GT4" s="160"/>
+      <c r="GU4" s="160"/>
+      <c r="GV4" s="160"/>
+      <c r="GW4" s="160"/>
+      <c r="GX4" s="161"/>
+      <c r="GY4" s="159" t="str">
         <f t="shared" ref="GY4" si="26">"Week "&amp;(GR6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="GZ4" s="157"/>
-      <c r="HA4" s="157"/>
-      <c r="HB4" s="157"/>
-      <c r="HC4" s="157"/>
-      <c r="HD4" s="157"/>
-      <c r="HE4" s="158"/>
-      <c r="HF4" s="156" t="str">
+      <c r="GZ4" s="160"/>
+      <c r="HA4" s="160"/>
+      <c r="HB4" s="160"/>
+      <c r="HC4" s="160"/>
+      <c r="HD4" s="160"/>
+      <c r="HE4" s="161"/>
+      <c r="HF4" s="159" t="str">
         <f t="shared" ref="HF4" si="27">"Week "&amp;(GY6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="HG4" s="157"/>
-      <c r="HH4" s="157"/>
-      <c r="HI4" s="157"/>
-      <c r="HJ4" s="157"/>
-      <c r="HK4" s="157"/>
-      <c r="HL4" s="158"/>
-      <c r="HM4" s="156" t="str">
+      <c r="HG4" s="160"/>
+      <c r="HH4" s="160"/>
+      <c r="HI4" s="160"/>
+      <c r="HJ4" s="160"/>
+      <c r="HK4" s="160"/>
+      <c r="HL4" s="161"/>
+      <c r="HM4" s="159" t="str">
         <f t="shared" ref="HM4" si="28">"Week "&amp;(HF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="HN4" s="157"/>
-      <c r="HO4" s="157"/>
-      <c r="HP4" s="157"/>
-      <c r="HQ4" s="157"/>
-      <c r="HR4" s="157"/>
-      <c r="HS4" s="158"/>
-      <c r="HT4" s="156" t="str">
+      <c r="HN4" s="160"/>
+      <c r="HO4" s="160"/>
+      <c r="HP4" s="160"/>
+      <c r="HQ4" s="160"/>
+      <c r="HR4" s="160"/>
+      <c r="HS4" s="161"/>
+      <c r="HT4" s="159" t="str">
         <f t="shared" ref="HT4" si="29">"Week "&amp;(HM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="HU4" s="157"/>
-      <c r="HV4" s="157"/>
-      <c r="HW4" s="157"/>
-      <c r="HX4" s="157"/>
-      <c r="HY4" s="157"/>
-      <c r="HZ4" s="158"/>
-      <c r="IA4" s="156" t="str">
+      <c r="HU4" s="160"/>
+      <c r="HV4" s="160"/>
+      <c r="HW4" s="160"/>
+      <c r="HX4" s="160"/>
+      <c r="HY4" s="160"/>
+      <c r="HZ4" s="161"/>
+      <c r="IA4" s="159" t="str">
         <f t="shared" ref="IA4" si="30">"Week "&amp;(HT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="IB4" s="157"/>
-      <c r="IC4" s="157"/>
-      <c r="ID4" s="157"/>
-      <c r="IE4" s="157"/>
-      <c r="IF4" s="157"/>
-      <c r="IG4" s="158"/>
-      <c r="IH4" s="156" t="str">
+      <c r="IB4" s="160"/>
+      <c r="IC4" s="160"/>
+      <c r="ID4" s="160"/>
+      <c r="IE4" s="160"/>
+      <c r="IF4" s="160"/>
+      <c r="IG4" s="161"/>
+      <c r="IH4" s="159" t="str">
         <f t="shared" ref="IH4" si="31">"Week "&amp;(IA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 33</v>
       </c>
-      <c r="II4" s="157"/>
-      <c r="IJ4" s="157"/>
-      <c r="IK4" s="157"/>
-      <c r="IL4" s="157"/>
-      <c r="IM4" s="157"/>
-      <c r="IN4" s="158"/>
-      <c r="IO4" s="156" t="str">
+      <c r="II4" s="160"/>
+      <c r="IJ4" s="160"/>
+      <c r="IK4" s="160"/>
+      <c r="IL4" s="160"/>
+      <c r="IM4" s="160"/>
+      <c r="IN4" s="161"/>
+      <c r="IO4" s="159" t="str">
         <f t="shared" ref="IO4" si="32">"Week "&amp;(IH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 34</v>
       </c>
-      <c r="IP4" s="157"/>
-      <c r="IQ4" s="157"/>
-      <c r="IR4" s="157"/>
-      <c r="IS4" s="157"/>
-      <c r="IT4" s="157"/>
-      <c r="IU4" s="158"/>
-    </row>
-    <row r="5" spans="1:255" s="55" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="IP4" s="160"/>
+      <c r="IQ4" s="160"/>
+      <c r="IR4" s="160"/>
+      <c r="IS4" s="160"/>
+      <c r="IT4" s="160"/>
+      <c r="IU4" s="161"/>
+    </row>
+    <row r="5" spans="1:255" s="55" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="111"/>
       <c r="B5" s="113" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="171" t="s">
+      <c r="C5" s="167" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="172"/>
-      <c r="E5" s="173"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="169"/>
       <c r="F5" s="111"/>
       <c r="G5" s="111"/>
       <c r="H5" s="111"/>
       <c r="I5" s="111"/>
-      <c r="K5" s="174">
+      <c r="K5" s="170">
         <f>K6</f>
         <v>45292</v>
       </c>
-      <c r="L5" s="160"/>
-      <c r="M5" s="160"/>
-      <c r="N5" s="160"/>
-      <c r="O5" s="160"/>
-      <c r="P5" s="160"/>
-      <c r="Q5" s="176"/>
-      <c r="R5" s="174">
+      <c r="L5" s="157"/>
+      <c r="M5" s="157"/>
+      <c r="N5" s="157"/>
+      <c r="O5" s="157"/>
+      <c r="P5" s="157"/>
+      <c r="Q5" s="172"/>
+      <c r="R5" s="170">
         <f>R6</f>
         <v>45299</v>
       </c>
-      <c r="S5" s="160"/>
-      <c r="T5" s="160"/>
-      <c r="U5" s="160"/>
-      <c r="V5" s="160"/>
-      <c r="W5" s="160"/>
-      <c r="X5" s="175"/>
-      <c r="Y5" s="177">
+      <c r="S5" s="157"/>
+      <c r="T5" s="157"/>
+      <c r="U5" s="157"/>
+      <c r="V5" s="157"/>
+      <c r="W5" s="157"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="173">
         <f>Y6</f>
         <v>45306</v>
       </c>
-      <c r="Z5" s="160"/>
-      <c r="AA5" s="160"/>
-      <c r="AB5" s="160"/>
-      <c r="AC5" s="160"/>
-      <c r="AD5" s="160"/>
-      <c r="AE5" s="178"/>
-      <c r="AF5" s="169">
+      <c r="Z5" s="157"/>
+      <c r="AA5" s="157"/>
+      <c r="AB5" s="157"/>
+      <c r="AC5" s="157"/>
+      <c r="AD5" s="157"/>
+      <c r="AE5" s="174"/>
+      <c r="AF5" s="165">
         <f>AF6</f>
         <v>45313</v>
       </c>
-      <c r="AG5" s="160"/>
-      <c r="AH5" s="160"/>
-      <c r="AI5" s="160"/>
-      <c r="AJ5" s="160"/>
-      <c r="AK5" s="160"/>
-      <c r="AL5" s="170"/>
-      <c r="AM5" s="162">
+      <c r="AG5" s="157"/>
+      <c r="AH5" s="157"/>
+      <c r="AI5" s="157"/>
+      <c r="AJ5" s="157"/>
+      <c r="AK5" s="157"/>
+      <c r="AL5" s="166"/>
+      <c r="AM5" s="175">
         <f>AM6</f>
         <v>45320</v>
       </c>
-      <c r="AN5" s="160"/>
-      <c r="AO5" s="160"/>
-      <c r="AP5" s="160"/>
-      <c r="AQ5" s="160"/>
-      <c r="AR5" s="160"/>
-      <c r="AS5" s="163"/>
-      <c r="AT5" s="164">
+      <c r="AN5" s="157"/>
+      <c r="AO5" s="157"/>
+      <c r="AP5" s="157"/>
+      <c r="AQ5" s="157"/>
+      <c r="AR5" s="157"/>
+      <c r="AS5" s="176"/>
+      <c r="AT5" s="177">
         <f>AT6</f>
         <v>45327</v>
       </c>
-      <c r="AU5" s="160"/>
-      <c r="AV5" s="160"/>
-      <c r="AW5" s="160"/>
-      <c r="AX5" s="160"/>
-      <c r="AY5" s="160"/>
-      <c r="AZ5" s="165"/>
-      <c r="BA5" s="166">
+      <c r="AU5" s="157"/>
+      <c r="AV5" s="157"/>
+      <c r="AW5" s="157"/>
+      <c r="AX5" s="157"/>
+      <c r="AY5" s="157"/>
+      <c r="AZ5" s="178"/>
+      <c r="BA5" s="156">
         <f>BA6</f>
         <v>45334</v>
       </c>
-      <c r="BB5" s="160"/>
-      <c r="BC5" s="160"/>
-      <c r="BD5" s="160"/>
-      <c r="BE5" s="160"/>
-      <c r="BF5" s="160"/>
-      <c r="BG5" s="167"/>
-      <c r="BH5" s="159">
+      <c r="BB5" s="157"/>
+      <c r="BC5" s="157"/>
+      <c r="BD5" s="157"/>
+      <c r="BE5" s="157"/>
+      <c r="BF5" s="157"/>
+      <c r="BG5" s="158"/>
+      <c r="BH5" s="162">
         <f>BH6</f>
         <v>45341</v>
       </c>
-      <c r="BI5" s="160"/>
-      <c r="BJ5" s="160"/>
-      <c r="BK5" s="160"/>
-      <c r="BL5" s="160"/>
-      <c r="BM5" s="160"/>
-      <c r="BN5" s="161"/>
-      <c r="BO5" s="166">
+      <c r="BI5" s="157"/>
+      <c r="BJ5" s="157"/>
+      <c r="BK5" s="157"/>
+      <c r="BL5" s="157"/>
+      <c r="BM5" s="157"/>
+      <c r="BN5" s="163"/>
+      <c r="BO5" s="156">
         <f>BO6</f>
         <v>45348</v>
       </c>
-      <c r="BP5" s="160"/>
-      <c r="BQ5" s="160"/>
-      <c r="BR5" s="160"/>
-      <c r="BS5" s="160"/>
-      <c r="BT5" s="160"/>
-      <c r="BU5" s="167"/>
-      <c r="BV5" s="159">
+      <c r="BP5" s="157"/>
+      <c r="BQ5" s="157"/>
+      <c r="BR5" s="157"/>
+      <c r="BS5" s="157"/>
+      <c r="BT5" s="157"/>
+      <c r="BU5" s="158"/>
+      <c r="BV5" s="162">
         <f>BV6</f>
         <v>45355</v>
       </c>
-      <c r="BW5" s="160"/>
-      <c r="BX5" s="160"/>
-      <c r="BY5" s="160"/>
-      <c r="BZ5" s="160"/>
-      <c r="CA5" s="160"/>
-      <c r="CB5" s="161"/>
-      <c r="CC5" s="159">
+      <c r="BW5" s="157"/>
+      <c r="BX5" s="157"/>
+      <c r="BY5" s="157"/>
+      <c r="BZ5" s="157"/>
+      <c r="CA5" s="157"/>
+      <c r="CB5" s="163"/>
+      <c r="CC5" s="162">
         <f>CC6</f>
         <v>45362</v>
       </c>
-      <c r="CD5" s="160"/>
-      <c r="CE5" s="160"/>
-      <c r="CF5" s="160"/>
-      <c r="CG5" s="160"/>
-      <c r="CH5" s="160"/>
-      <c r="CI5" s="161"/>
-      <c r="CJ5" s="166">
+      <c r="CD5" s="157"/>
+      <c r="CE5" s="157"/>
+      <c r="CF5" s="157"/>
+      <c r="CG5" s="157"/>
+      <c r="CH5" s="157"/>
+      <c r="CI5" s="163"/>
+      <c r="CJ5" s="156">
         <f>CJ6</f>
         <v>45369</v>
       </c>
-      <c r="CK5" s="160"/>
-      <c r="CL5" s="160"/>
-      <c r="CM5" s="160"/>
-      <c r="CN5" s="160"/>
-      <c r="CO5" s="160"/>
-      <c r="CP5" s="167"/>
-      <c r="CQ5" s="159">
+      <c r="CK5" s="157"/>
+      <c r="CL5" s="157"/>
+      <c r="CM5" s="157"/>
+      <c r="CN5" s="157"/>
+      <c r="CO5" s="157"/>
+      <c r="CP5" s="158"/>
+      <c r="CQ5" s="162">
         <f>CQ6</f>
         <v>45376</v>
       </c>
-      <c r="CR5" s="160"/>
-      <c r="CS5" s="160"/>
-      <c r="CT5" s="160"/>
-      <c r="CU5" s="160"/>
-      <c r="CV5" s="160"/>
-      <c r="CW5" s="161"/>
-      <c r="CX5" s="159">
+      <c r="CR5" s="157"/>
+      <c r="CS5" s="157"/>
+      <c r="CT5" s="157"/>
+      <c r="CU5" s="157"/>
+      <c r="CV5" s="157"/>
+      <c r="CW5" s="163"/>
+      <c r="CX5" s="162">
         <f t="shared" ref="CX5" si="33">CX6</f>
         <v>45383</v>
       </c>
-      <c r="CY5" s="160"/>
-      <c r="CZ5" s="160"/>
-      <c r="DA5" s="160"/>
-      <c r="DB5" s="160"/>
-      <c r="DC5" s="160"/>
-      <c r="DD5" s="161"/>
-      <c r="DE5" s="166">
+      <c r="CY5" s="157"/>
+      <c r="CZ5" s="157"/>
+      <c r="DA5" s="157"/>
+      <c r="DB5" s="157"/>
+      <c r="DC5" s="157"/>
+      <c r="DD5" s="163"/>
+      <c r="DE5" s="156">
         <f t="shared" ref="DE5" si="34">DE6</f>
         <v>45390</v>
       </c>
-      <c r="DF5" s="160"/>
-      <c r="DG5" s="160"/>
-      <c r="DH5" s="160"/>
-      <c r="DI5" s="160"/>
-      <c r="DJ5" s="160"/>
-      <c r="DK5" s="167"/>
-      <c r="DL5" s="159">
+      <c r="DF5" s="157"/>
+      <c r="DG5" s="157"/>
+      <c r="DH5" s="157"/>
+      <c r="DI5" s="157"/>
+      <c r="DJ5" s="157"/>
+      <c r="DK5" s="158"/>
+      <c r="DL5" s="162">
         <f t="shared" ref="DL5" si="35">DL6</f>
         <v>45397</v>
       </c>
-      <c r="DM5" s="160"/>
-      <c r="DN5" s="160"/>
-      <c r="DO5" s="160"/>
-      <c r="DP5" s="160"/>
-      <c r="DQ5" s="160"/>
-      <c r="DR5" s="161"/>
-      <c r="DS5" s="159">
+      <c r="DM5" s="157"/>
+      <c r="DN5" s="157"/>
+      <c r="DO5" s="157"/>
+      <c r="DP5" s="157"/>
+      <c r="DQ5" s="157"/>
+      <c r="DR5" s="163"/>
+      <c r="DS5" s="162">
         <f t="shared" ref="DS5" si="36">DS6</f>
         <v>45404</v>
       </c>
-      <c r="DT5" s="160"/>
-      <c r="DU5" s="160"/>
-      <c r="DV5" s="160"/>
-      <c r="DW5" s="160"/>
-      <c r="DX5" s="160"/>
-      <c r="DY5" s="161"/>
-      <c r="DZ5" s="166">
+      <c r="DT5" s="157"/>
+      <c r="DU5" s="157"/>
+      <c r="DV5" s="157"/>
+      <c r="DW5" s="157"/>
+      <c r="DX5" s="157"/>
+      <c r="DY5" s="163"/>
+      <c r="DZ5" s="156">
         <f t="shared" ref="DZ5" si="37">DZ6</f>
         <v>45411</v>
       </c>
-      <c r="EA5" s="160"/>
-      <c r="EB5" s="160"/>
-      <c r="EC5" s="160"/>
-      <c r="ED5" s="160"/>
-      <c r="EE5" s="160"/>
-      <c r="EF5" s="167"/>
-      <c r="EG5" s="159">
+      <c r="EA5" s="157"/>
+      <c r="EB5" s="157"/>
+      <c r="EC5" s="157"/>
+      <c r="ED5" s="157"/>
+      <c r="EE5" s="157"/>
+      <c r="EF5" s="158"/>
+      <c r="EG5" s="162">
         <f t="shared" ref="EG5" si="38">EG6</f>
         <v>45418</v>
       </c>
-      <c r="EH5" s="160"/>
-      <c r="EI5" s="160"/>
-      <c r="EJ5" s="160"/>
-      <c r="EK5" s="160"/>
-      <c r="EL5" s="160"/>
-      <c r="EM5" s="161"/>
-      <c r="EN5" s="159">
+      <c r="EH5" s="157"/>
+      <c r="EI5" s="157"/>
+      <c r="EJ5" s="157"/>
+      <c r="EK5" s="157"/>
+      <c r="EL5" s="157"/>
+      <c r="EM5" s="163"/>
+      <c r="EN5" s="162">
         <f>EN6</f>
         <v>45425</v>
       </c>
-      <c r="EO5" s="160"/>
-      <c r="EP5" s="160"/>
-      <c r="EQ5" s="160"/>
-      <c r="ER5" s="160"/>
-      <c r="ES5" s="160"/>
-      <c r="ET5" s="161"/>
-      <c r="EU5" s="166">
+      <c r="EO5" s="157"/>
+      <c r="EP5" s="157"/>
+      <c r="EQ5" s="157"/>
+      <c r="ER5" s="157"/>
+      <c r="ES5" s="157"/>
+      <c r="ET5" s="163"/>
+      <c r="EU5" s="156">
         <f>EU6</f>
         <v>45432</v>
       </c>
-      <c r="EV5" s="160"/>
-      <c r="EW5" s="160"/>
-      <c r="EX5" s="160"/>
-      <c r="EY5" s="160"/>
-      <c r="EZ5" s="160"/>
-      <c r="FA5" s="167"/>
-      <c r="FB5" s="159">
+      <c r="EV5" s="157"/>
+      <c r="EW5" s="157"/>
+      <c r="EX5" s="157"/>
+      <c r="EY5" s="157"/>
+      <c r="EZ5" s="157"/>
+      <c r="FA5" s="158"/>
+      <c r="FB5" s="162">
         <f>FB6</f>
         <v>45439</v>
       </c>
-      <c r="FC5" s="160"/>
-      <c r="FD5" s="160"/>
-      <c r="FE5" s="160"/>
-      <c r="FF5" s="160"/>
-      <c r="FG5" s="160"/>
-      <c r="FH5" s="161"/>
-      <c r="FI5" s="159">
+      <c r="FC5" s="157"/>
+      <c r="FD5" s="157"/>
+      <c r="FE5" s="157"/>
+      <c r="FF5" s="157"/>
+      <c r="FG5" s="157"/>
+      <c r="FH5" s="163"/>
+      <c r="FI5" s="162">
         <f t="shared" ref="FI5" si="39">FI6</f>
         <v>45446</v>
       </c>
-      <c r="FJ5" s="160"/>
-      <c r="FK5" s="160"/>
-      <c r="FL5" s="160"/>
-      <c r="FM5" s="160"/>
-      <c r="FN5" s="160"/>
-      <c r="FO5" s="161"/>
-      <c r="FP5" s="166">
+      <c r="FJ5" s="157"/>
+      <c r="FK5" s="157"/>
+      <c r="FL5" s="157"/>
+      <c r="FM5" s="157"/>
+      <c r="FN5" s="157"/>
+      <c r="FO5" s="163"/>
+      <c r="FP5" s="156">
         <f t="shared" ref="FP5" si="40">FP6</f>
         <v>45453</v>
       </c>
-      <c r="FQ5" s="160"/>
-      <c r="FR5" s="160"/>
-      <c r="FS5" s="160"/>
-      <c r="FT5" s="160"/>
-      <c r="FU5" s="160"/>
-      <c r="FV5" s="167"/>
-      <c r="FW5" s="159">
+      <c r="FQ5" s="157"/>
+      <c r="FR5" s="157"/>
+      <c r="FS5" s="157"/>
+      <c r="FT5" s="157"/>
+      <c r="FU5" s="157"/>
+      <c r="FV5" s="158"/>
+      <c r="FW5" s="162">
         <f t="shared" ref="FW5" si="41">FW6</f>
         <v>45460</v>
       </c>
-      <c r="FX5" s="160"/>
-      <c r="FY5" s="160"/>
-      <c r="FZ5" s="160"/>
-      <c r="GA5" s="160"/>
-      <c r="GB5" s="160"/>
-      <c r="GC5" s="161"/>
-      <c r="GD5" s="159">
+      <c r="FX5" s="157"/>
+      <c r="FY5" s="157"/>
+      <c r="FZ5" s="157"/>
+      <c r="GA5" s="157"/>
+      <c r="GB5" s="157"/>
+      <c r="GC5" s="163"/>
+      <c r="GD5" s="162">
         <f t="shared" ref="GD5" si="42">GD6</f>
         <v>45467</v>
       </c>
-      <c r="GE5" s="160"/>
-      <c r="GF5" s="160"/>
-      <c r="GG5" s="160"/>
-      <c r="GH5" s="160"/>
-      <c r="GI5" s="160"/>
-      <c r="GJ5" s="161"/>
-      <c r="GK5" s="166">
+      <c r="GE5" s="157"/>
+      <c r="GF5" s="157"/>
+      <c r="GG5" s="157"/>
+      <c r="GH5" s="157"/>
+      <c r="GI5" s="157"/>
+      <c r="GJ5" s="163"/>
+      <c r="GK5" s="156">
         <f t="shared" ref="GK5" si="43">GK6</f>
         <v>45474</v>
       </c>
-      <c r="GL5" s="160"/>
-      <c r="GM5" s="160"/>
-      <c r="GN5" s="160"/>
-      <c r="GO5" s="160"/>
-      <c r="GP5" s="160"/>
-      <c r="GQ5" s="167"/>
-      <c r="GR5" s="159">
+      <c r="GL5" s="157"/>
+      <c r="GM5" s="157"/>
+      <c r="GN5" s="157"/>
+      <c r="GO5" s="157"/>
+      <c r="GP5" s="157"/>
+      <c r="GQ5" s="158"/>
+      <c r="GR5" s="162">
         <f t="shared" ref="GR5" si="44">GR6</f>
         <v>45481</v>
       </c>
-      <c r="GS5" s="160"/>
-      <c r="GT5" s="160"/>
-      <c r="GU5" s="160"/>
-      <c r="GV5" s="160"/>
-      <c r="GW5" s="160"/>
-      <c r="GX5" s="161"/>
-      <c r="GY5" s="166">
+      <c r="GS5" s="157"/>
+      <c r="GT5" s="157"/>
+      <c r="GU5" s="157"/>
+      <c r="GV5" s="157"/>
+      <c r="GW5" s="157"/>
+      <c r="GX5" s="163"/>
+      <c r="GY5" s="156">
         <f t="shared" ref="GY5" si="45">GY6</f>
         <v>45488</v>
       </c>
-      <c r="GZ5" s="160"/>
-      <c r="HA5" s="160"/>
-      <c r="HB5" s="160"/>
-      <c r="HC5" s="160"/>
-      <c r="HD5" s="160"/>
-      <c r="HE5" s="167"/>
-      <c r="HF5" s="159">
+      <c r="GZ5" s="157"/>
+      <c r="HA5" s="157"/>
+      <c r="HB5" s="157"/>
+      <c r="HC5" s="157"/>
+      <c r="HD5" s="157"/>
+      <c r="HE5" s="158"/>
+      <c r="HF5" s="162">
         <f t="shared" ref="HF5" si="46">HF6</f>
         <v>45495</v>
       </c>
-      <c r="HG5" s="160"/>
-      <c r="HH5" s="160"/>
-      <c r="HI5" s="160"/>
-      <c r="HJ5" s="160"/>
-      <c r="HK5" s="160"/>
-      <c r="HL5" s="161"/>
-      <c r="HM5" s="166">
+      <c r="HG5" s="157"/>
+      <c r="HH5" s="157"/>
+      <c r="HI5" s="157"/>
+      <c r="HJ5" s="157"/>
+      <c r="HK5" s="157"/>
+      <c r="HL5" s="163"/>
+      <c r="HM5" s="156">
         <f t="shared" ref="HM5" si="47">HM6</f>
         <v>45502</v>
       </c>
-      <c r="HN5" s="160"/>
-      <c r="HO5" s="160"/>
-      <c r="HP5" s="160"/>
-      <c r="HQ5" s="160"/>
-      <c r="HR5" s="160"/>
-      <c r="HS5" s="167"/>
-      <c r="HT5" s="159">
+      <c r="HN5" s="157"/>
+      <c r="HO5" s="157"/>
+      <c r="HP5" s="157"/>
+      <c r="HQ5" s="157"/>
+      <c r="HR5" s="157"/>
+      <c r="HS5" s="158"/>
+      <c r="HT5" s="162">
         <f t="shared" ref="HT5" si="48">HT6</f>
         <v>45509</v>
       </c>
-      <c r="HU5" s="160"/>
-      <c r="HV5" s="160"/>
-      <c r="HW5" s="160"/>
-      <c r="HX5" s="160"/>
-      <c r="HY5" s="160"/>
-      <c r="HZ5" s="161"/>
-      <c r="IA5" s="166">
+      <c r="HU5" s="157"/>
+      <c r="HV5" s="157"/>
+      <c r="HW5" s="157"/>
+      <c r="HX5" s="157"/>
+      <c r="HY5" s="157"/>
+      <c r="HZ5" s="163"/>
+      <c r="IA5" s="156">
         <f t="shared" ref="IA5" si="49">IA6</f>
         <v>45516</v>
       </c>
-      <c r="IB5" s="160"/>
-      <c r="IC5" s="160"/>
-      <c r="ID5" s="160"/>
-      <c r="IE5" s="160"/>
-      <c r="IF5" s="160"/>
-      <c r="IG5" s="167"/>
-      <c r="IH5" s="159">
+      <c r="IB5" s="157"/>
+      <c r="IC5" s="157"/>
+      <c r="ID5" s="157"/>
+      <c r="IE5" s="157"/>
+      <c r="IF5" s="157"/>
+      <c r="IG5" s="158"/>
+      <c r="IH5" s="162">
         <f t="shared" ref="IH5" si="50">IH6</f>
         <v>45523</v>
       </c>
-      <c r="II5" s="160"/>
-      <c r="IJ5" s="160"/>
-      <c r="IK5" s="160"/>
-      <c r="IL5" s="160"/>
-      <c r="IM5" s="160"/>
-      <c r="IN5" s="161"/>
-      <c r="IO5" s="166">
+      <c r="II5" s="157"/>
+      <c r="IJ5" s="157"/>
+      <c r="IK5" s="157"/>
+      <c r="IL5" s="157"/>
+      <c r="IM5" s="157"/>
+      <c r="IN5" s="163"/>
+      <c r="IO5" s="156">
         <f t="shared" ref="IO5" si="51">IO6</f>
         <v>45530</v>
       </c>
-      <c r="IP5" s="160"/>
-      <c r="IQ5" s="160"/>
-      <c r="IR5" s="160"/>
-      <c r="IS5" s="160"/>
-      <c r="IT5" s="160"/>
-      <c r="IU5" s="167"/>
-    </row>
-    <row r="6" spans="1:255" s="53" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="IP5" s="157"/>
+      <c r="IQ5" s="157"/>
+      <c r="IR5" s="157"/>
+      <c r="IS5" s="157"/>
+      <c r="IT5" s="157"/>
+      <c r="IU5" s="158"/>
+    </row>
+    <row r="6" spans="1:255" s="53" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="146"/>
       <c r="K6" s="64">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="IU6" s="76"/>
     </row>
-    <row r="7" spans="1:255" s="52" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:255" s="52" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
         <v>0</v>
       </c>
@@ -7060,7 +7060,7 @@
       </c>
       <c r="IU7" s="62"/>
     </row>
-    <row r="8" spans="1:255" s="26" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:255" s="26" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="90" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -7322,7 +7322,7 @@
       <c r="IT8" s="27"/>
       <c r="IU8" s="27"/>
     </row>
-    <row r="9" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A9" s="91" t="str">
         <f t="shared" ref="A9:A22" si="254">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -7596,7 +7596,7 @@
       <c r="IT9" s="34"/>
       <c r="IU9" s="34"/>
     </row>
-    <row r="10" spans="1:255" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:255" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="91" t="str">
         <f t="shared" ref="A10:A20" si="257">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -7870,7 +7870,7 @@
       <c r="IT10" s="34"/>
       <c r="IU10" s="34"/>
     </row>
-    <row r="11" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.2</v>
@@ -8144,7 +8144,7 @@
       <c r="IT11" s="34"/>
       <c r="IU11" s="34"/>
     </row>
-    <row r="12" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.3</v>
@@ -8419,7 +8419,7 @@
       <c r="IT12" s="34"/>
       <c r="IU12" s="34"/>
     </row>
-    <row r="13" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.4</v>
@@ -8693,7 +8693,7 @@
       <c r="IT13" s="34"/>
       <c r="IU13" s="34"/>
     </row>
-    <row r="14" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.5</v>
@@ -8709,13 +8709,13 @@
       </c>
       <c r="F14" s="84">
         <f t="shared" si="255"/>
-        <v>45312</v>
+        <v>45311</v>
       </c>
       <c r="G14" s="45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H14" s="46">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I14" s="102">
         <f t="shared" si="256"/>
@@ -8970,7 +8970,7 @@
       <c r="IT14" s="34"/>
       <c r="IU14" s="34"/>
     </row>
-    <row r="15" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.6</v>
@@ -8982,11 +8982,11 @@
       <c r="D15" s="33"/>
       <c r="E15" s="87">
         <f>F14</f>
-        <v>45312</v>
+        <v>45311</v>
       </c>
       <c r="F15" s="84">
         <f t="shared" ref="F15" si="262">IF(ISBLANK(E15)," - ",IF(G15=0,E15,E15+G15-1))</f>
-        <v>45317</v>
+        <v>45316</v>
       </c>
       <c r="G15" s="45">
         <v>6</v>
@@ -8996,7 +8996,7 @@
       </c>
       <c r="I15" s="102">
         <f t="shared" ref="I15" si="263">IF(OR(F15=0,E15=0),0,NETWORKDAYS(E15,F15))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J15" s="94"/>
       <c r="K15" s="34"/>
@@ -9247,7 +9247,7 @@
       <c r="IT15" s="34"/>
       <c r="IU15" s="34"/>
     </row>
-    <row r="16" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.7</v>
@@ -9523,7 +9523,7 @@
       <c r="IT16" s="34"/>
       <c r="IU16" s="34"/>
     </row>
-    <row r="17" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:255" s="32" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.8</v>
@@ -9799,7 +9799,7 @@
       <c r="IT17" s="34"/>
       <c r="IU17" s="34"/>
     </row>
-    <row r="18" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.9</v>
@@ -10075,7 +10075,7 @@
       <c r="IT18" s="34"/>
       <c r="IU18" s="34"/>
     </row>
-    <row r="19" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.10</v>
@@ -10351,7 +10351,7 @@
       <c r="IT19" s="34"/>
       <c r="IU19" s="34"/>
     </row>
-    <row r="20" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="91" t="str">
         <f t="shared" si="257"/>
         <v>1.1.11</v>
@@ -10628,7 +10628,7 @@
       <c r="IT20" s="34"/>
       <c r="IU20" s="34"/>
     </row>
-    <row r="21" spans="1:255" s="31" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:255" s="31" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="92" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -10890,7 +10890,7 @@
       <c r="IT21" s="36"/>
       <c r="IU21" s="36"/>
     </row>
-    <row r="22" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="91" t="str">
         <f t="shared" si="254"/>
         <v>2.1</v>
@@ -11165,7 +11165,7 @@
       <c r="IT22" s="34"/>
       <c r="IU22" s="34"/>
     </row>
-    <row r="23" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A23" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.1.1</v>
@@ -11442,7 +11442,7 @@
       <c r="IT23" s="34"/>
       <c r="IU23" s="34"/>
     </row>
-    <row r="24" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A24" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.1.2</v>
@@ -11718,7 +11718,7 @@
       <c r="IT24" s="34"/>
       <c r="IU24" s="34"/>
     </row>
-    <row r="25" spans="1:255" s="31" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:255" s="31" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
@@ -11980,7 +11980,7 @@
       <c r="IT25" s="36"/>
       <c r="IU25" s="36"/>
     </row>
-    <row r="26" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A26" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
@@ -12255,7 +12255,7 @@
       <c r="IT26" s="34"/>
       <c r="IU26" s="34"/>
     </row>
-    <row r="27" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A27" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.1.1</v>
@@ -12532,7 +12532,7 @@
       <c r="IT27" s="34"/>
       <c r="IU27" s="34"/>
     </row>
-    <row r="28" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A28" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.1.2</v>
@@ -12808,7 +12808,7 @@
       <c r="IT28" s="34"/>
       <c r="IU28" s="34"/>
     </row>
-    <row r="29" spans="1:255" s="31" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:255" s="31" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="92" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
@@ -13070,7 +13070,7 @@
       <c r="IT29" s="36"/>
       <c r="IU29" s="36"/>
     </row>
-    <row r="30" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A30" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
@@ -13345,7 +13345,7 @@
       <c r="IT30" s="34"/>
       <c r="IU30" s="34"/>
     </row>
-    <row r="31" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.1</v>
@@ -13622,7 +13622,7 @@
       <c r="IT31" s="34"/>
       <c r="IU31" s="34"/>
     </row>
-    <row r="32" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.2</v>
@@ -13898,7 +13898,7 @@
       <c r="IT32" s="34"/>
       <c r="IU32" s="34"/>
     </row>
-    <row r="33" spans="1:255" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:255" s="32" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A33" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.3</v>
@@ -14175,7 +14175,7 @@
       <c r="IT33" s="34"/>
       <c r="IU33" s="34"/>
     </row>
-    <row r="35" spans="1:255" s="40" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:255" s="40" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="105" t="s">
         <v>1</v>
       </c>
@@ -14434,7 +14434,7 @@
       <c r="IT35" s="34"/>
       <c r="IU35" s="34"/>
     </row>
-    <row r="36" spans="1:255" s="39" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:255" s="39" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A36" s="106" t="s">
         <v>74</v>
       </c>
@@ -14689,7 +14689,7 @@
       <c r="IT36" s="34"/>
       <c r="IU36" s="34"/>
     </row>
-    <row r="37" spans="1:255" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:255" s="39" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A37" s="92" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -14953,7 +14953,7 @@
       <c r="IT37" s="34"/>
       <c r="IU37" s="34"/>
     </row>
-    <row r="38" spans="1:255" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:255" s="39" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A38" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -15225,7 +15225,7 @@
       <c r="IT38" s="34"/>
       <c r="IU38" s="34"/>
     </row>
-    <row r="39" spans="1:255" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:255" s="39" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A39" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -15495,7 +15495,7 @@
       <c r="IT39" s="34"/>
       <c r="IU39" s="34"/>
     </row>
-    <row r="40" spans="1:255" s="39" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:255" s="39" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A40" s="91" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
@@ -15765,32 +15765,61 @@
       <c r="IT40" s="34"/>
       <c r="IU40" s="34"/>
     </row>
-    <row r="41" spans="1:255" s="41" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:255" s="41" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="142" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
       </c>
       <c r="C41" s="154"/>
     </row>
-    <row r="42" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="73">
-    <mergeCell ref="IO5:IU5"/>
-    <mergeCell ref="IO4:IU4"/>
-    <mergeCell ref="HT4:HZ4"/>
-    <mergeCell ref="IA4:IG4"/>
-    <mergeCell ref="IH4:IN4"/>
-    <mergeCell ref="HM5:HS5"/>
-    <mergeCell ref="HT5:HZ5"/>
-    <mergeCell ref="IA5:IG5"/>
-    <mergeCell ref="IH5:IN5"/>
-    <mergeCell ref="GY4:HE4"/>
-    <mergeCell ref="HF4:HL4"/>
-    <mergeCell ref="GY5:HE5"/>
-    <mergeCell ref="HF5:HL5"/>
-    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="BH4:BN4"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="AM5:AS5"/>
+    <mergeCell ref="AT4:AZ4"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="BA4:BG4"/>
+    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="AD1:AR1"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="AF5:AL5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="FI4:FO4"/>
+    <mergeCell ref="FP4:FV4"/>
+    <mergeCell ref="EG4:EM4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="DS5:DY5"/>
+    <mergeCell ref="DZ5:EF5"/>
+    <mergeCell ref="EG5:EM5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DS4:DY4"/>
+    <mergeCell ref="DZ4:EF4"/>
     <mergeCell ref="FW4:GC4"/>
     <mergeCell ref="GD4:GJ4"/>
     <mergeCell ref="GK4:GQ4"/>
@@ -15807,49 +15836,20 @@
     <mergeCell ref="EN4:ET4"/>
     <mergeCell ref="EU4:FA4"/>
     <mergeCell ref="FB4:FH4"/>
-    <mergeCell ref="FI4:FO4"/>
-    <mergeCell ref="FP4:FV4"/>
-    <mergeCell ref="EG4:EM4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE5:DK5"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="DS5:DY5"/>
-    <mergeCell ref="DZ5:EF5"/>
-    <mergeCell ref="EG5:EM5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DS4:DY4"/>
-    <mergeCell ref="DZ4:EF4"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="AD1:AR1"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AF5:AL5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="HM5:HS5"/>
+    <mergeCell ref="HT5:HZ5"/>
+    <mergeCell ref="IA5:IG5"/>
+    <mergeCell ref="IH5:IN5"/>
+    <mergeCell ref="GY4:HE4"/>
+    <mergeCell ref="HF4:HL4"/>
+    <mergeCell ref="GY5:HE5"/>
+    <mergeCell ref="HF5:HL5"/>
+    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="IO5:IU5"/>
+    <mergeCell ref="IO4:IU4"/>
+    <mergeCell ref="HT4:HZ4"/>
+    <mergeCell ref="IA4:IG4"/>
+    <mergeCell ref="IH4:IN4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H36:H40 H8:H33">
@@ -15909,13 +15909,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>10886</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>28</xdr:col>
-                    <xdr:colOff>95250</xdr:colOff>
+                    <xdr:colOff>97971</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>
@@ -15960,62 +15960,62 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="90.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="5.53515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="90.3828125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B1" s="21"/>
     </row>
-    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A2" s="119" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A4" s="120" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="56.6" x14ac:dyDescent="0.35">
       <c r="B5" s="121" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="28.3" x14ac:dyDescent="0.35">
       <c r="B7" s="121" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B9" s="119" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="28.3" x14ac:dyDescent="0.35">
       <c r="B11" s="122" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A13" s="179" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="179"/>
     </row>
-    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="123"/>
       <c r="B15" s="124" t="s">
         <v>78</v>
@@ -16023,7 +16023,7 @@
       <c r="C15" s="125"/>
       <c r="D15" s="125"/>
     </row>
-    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="123"/>
       <c r="B16" s="124" t="s">
         <v>79</v>
@@ -16031,162 +16031,162 @@
       <c r="C16" s="125"/>
       <c r="D16" s="125"/>
     </row>
-    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A17" s="126"/>
       <c r="B17" s="124" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A18" s="126"/>
       <c r="B18" s="124" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A19" s="126"/>
       <c r="B19" s="124" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A20" s="126"/>
       <c r="B20" s="124" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A21" s="126"/>
       <c r="B21" s="127" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A22" s="126"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A23" s="179" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="179"/>
     </row>
-    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="42.45" x14ac:dyDescent="0.4">
       <c r="A24" s="126"/>
       <c r="B24" s="124" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A25" s="126"/>
       <c r="B25" s="124"/>
     </row>
-    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A26" s="126"/>
       <c r="B26" s="128" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A27" s="126"/>
       <c r="B27" s="124" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A28" s="126"/>
       <c r="B28" s="124" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A29" s="126"/>
       <c r="B29" s="124"/>
     </row>
-    <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A30" s="126"/>
       <c r="B30" s="128" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A31" s="126"/>
       <c r="B31" s="124" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A32" s="126"/>
       <c r="B32" s="124" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A33" s="126"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A34" s="126"/>
       <c r="B34" s="124" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A35" s="126"/>
       <c r="B35" s="129" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A36" s="126"/>
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A37" s="179" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="179"/>
     </row>
-    <row r="38" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B38" s="124" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="14.15" x14ac:dyDescent="0.3">
       <c r="B40" s="124" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B42" s="124" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B44" s="124" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B45" s="10"/>
     </row>
-    <row r="46" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B46" s="124" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A48" s="179" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="179"/>
     </row>
-    <row r="49" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="B49" s="124" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A51" s="130" t="s">
         <v>8</v>
       </c>
@@ -16194,7 +16194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A52" s="130" t="s">
         <v>10</v>
       </c>
@@ -16202,7 +16202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A53" s="130" t="s">
         <v>12</v>
       </c>
@@ -16210,19 +16210,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A54" s="122"/>
       <c r="B54" s="124" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A55" s="122"/>
       <c r="B55" s="124" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A56" s="130" t="s">
         <v>14</v>
       </c>
@@ -16230,19 +16230,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A57" s="122"/>
       <c r="B57" s="124" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A58" s="122"/>
       <c r="B58" s="124" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A59" s="130" t="s">
         <v>16</v>
       </c>
@@ -16250,13 +16250,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A60" s="122"/>
       <c r="B60" s="124" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A61" s="130" t="s">
         <v>105</v>
       </c>
@@ -16264,33 +16264,33 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A62" s="131"/>
       <c r="B62" s="124" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A64" s="179" t="s">
         <v>6</v>
       </c>
       <c r="B64" s="179"/>
     </row>
-    <row r="65" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="42.45" x14ac:dyDescent="0.3">
       <c r="B65" s="124" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A67" s="179" t="s">
         <v>3</v>
       </c>
       <c r="B67" s="179"/>
     </row>
-    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A68" s="132" t="s">
         <v>4</v>
       </c>
@@ -16298,17 +16298,17 @@
         <v>109</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A69" s="131"/>
       <c r="B69" s="134" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A70" s="131"/>
       <c r="B70" s="135"/>
     </row>
-    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A71" s="132" t="s">
         <v>4</v>
       </c>
@@ -16316,17 +16316,17 @@
         <v>111</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A72" s="131"/>
       <c r="B72" s="134" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A73" s="131"/>
       <c r="B73" s="135"/>
     </row>
-    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A74" s="132" t="s">
         <v>4</v>
       </c>
@@ -16334,17 +16334,17 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A75" s="131"/>
       <c r="B75" s="121" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A76" s="131"/>
       <c r="B76" s="131"/>
     </row>
-    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A77" s="132" t="s">
         <v>4</v>
       </c>
@@ -16352,17 +16352,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A78" s="131"/>
       <c r="B78" s="121" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A79" s="131"/>
       <c r="B79" s="131"/>
     </row>
-    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A80" s="132" t="s">
         <v>4</v>
       </c>
@@ -16370,29 +16370,29 @@
         <v>117</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A81" s="131"/>
       <c r="B81" s="137" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A82" s="131"/>
       <c r="B82" s="137" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A83" s="131"/>
       <c r="B83" s="137" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A84" s="131"/>
       <c r="B84" s="138"/>
     </row>
-    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A85" s="132" t="s">
         <v>4</v>
       </c>
@@ -16400,29 +16400,29 @@
         <v>121</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A86" s="131"/>
       <c r="B86" s="121" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A87" s="131"/>
       <c r="B87" s="139" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A88" s="131"/>
       <c r="B88" s="140" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A89" s="131"/>
       <c r="B89" s="131"/>
     </row>
-    <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A90" s="132" t="s">
         <v>4</v>
       </c>
@@ -16430,13 +16430,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A91" s="122"/>
       <c r="B91" s="137" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>51</v>
       </c>
@@ -16474,172 +16474,172 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.53515625" customWidth="1"/>
+    <col min="2" max="2" width="37.69140625" customWidth="1"/>
+    <col min="3" max="3" width="55.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="C7" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="C13" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B18" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B22" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B26" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B34" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" ht="14.15" x14ac:dyDescent="0.35">
       <c r="B42" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="B46" s="11" t="s">
         <v>21</v>
       </c>
@@ -16664,172 +16664,172 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.53515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="82.15234375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="20"/>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="B2" s="24"/>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="22"/>
       <c r="B3" s="17" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="23"/>
     </row>
-    <row r="4" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="7"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A6" s="5"/>
       <c r="B6" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="7"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="7"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="45.9" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
       <c r="B10" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="7"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="7"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" ht="30.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="30.45" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="7"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
       <c r="B18" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>

</xml_diff>

<commit_message>
found some interesting papers that may propose novel RL algorithms based on adaptive critic designs
</commit_message>
<xml_diff>
--- a/thesis gantt chart.xlsx
+++ b/thesis gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wings_stuff\srus\TUD\yr5\thesis\thesis_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913FBFBD-5CCA-49FA-B834-364F76DC0F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD24E9CA-444A-43B2-8D11-584EC6EB0A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3263,15 +3263,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="70" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3284,7 +3275,28 @@
     <xf numFmtId="167" fontId="52" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="84" fillId="24" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -3321,18 +3333,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4177,7 +4177,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC16" sqref="AC16"/>
+      <selection pane="bottomLeft" activeCell="AJ18" sqref="AJ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -4255,21 +4255,21 @@
       <c r="K1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="AD1" s="164"/>
-      <c r="AE1" s="164"/>
-      <c r="AF1" s="164"/>
-      <c r="AG1" s="164"/>
-      <c r="AH1" s="164"/>
-      <c r="AI1" s="164"/>
-      <c r="AJ1" s="164"/>
-      <c r="AK1" s="164"/>
-      <c r="AL1" s="164"/>
-      <c r="AM1" s="164"/>
-      <c r="AN1" s="164"/>
-      <c r="AO1" s="164"/>
-      <c r="AP1" s="164"/>
-      <c r="AQ1" s="164"/>
-      <c r="AR1" s="164"/>
+      <c r="AD1" s="168"/>
+      <c r="AE1" s="168"/>
+      <c r="AF1" s="168"/>
+      <c r="AG1" s="168"/>
+      <c r="AH1" s="168"/>
+      <c r="AI1" s="168"/>
+      <c r="AJ1" s="168"/>
+      <c r="AK1" s="168"/>
+      <c r="AL1" s="168"/>
+      <c r="AM1" s="168"/>
+      <c r="AN1" s="168"/>
+      <c r="AO1" s="168"/>
+      <c r="AP1" s="168"/>
+      <c r="AQ1" s="168"/>
+      <c r="AR1" s="168"/>
     </row>
     <row r="2" spans="1:255" s="59" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="112" t="s">
@@ -4349,729 +4349,729 @@
       <c r="B4" s="113" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="167">
+      <c r="C4" s="171">
         <v>45295</v>
       </c>
-      <c r="D4" s="168"/>
-      <c r="E4" s="169"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="173"/>
       <c r="H4" s="113" t="s">
         <v>71</v>
       </c>
       <c r="I4" s="114">
         <v>1</v>
       </c>
-      <c r="K4" s="159"/>
-      <c r="L4" s="160"/>
-      <c r="M4" s="160"/>
-      <c r="N4" s="160"/>
-      <c r="O4" s="160"/>
-      <c r="P4" s="160"/>
-      <c r="Q4" s="161"/>
-      <c r="R4" s="159" t="str">
+      <c r="K4" s="156"/>
+      <c r="L4" s="157"/>
+      <c r="M4" s="157"/>
+      <c r="N4" s="157"/>
+      <c r="O4" s="157"/>
+      <c r="P4" s="157"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="156" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="S4" s="160"/>
-      <c r="T4" s="160"/>
-      <c r="U4" s="160"/>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="159" t="str">
+      <c r="S4" s="157"/>
+      <c r="T4" s="157"/>
+      <c r="U4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="158"/>
+      <c r="Y4" s="156" t="str">
         <f t="shared" ref="Y4" si="0">"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="Z4" s="160"/>
-      <c r="AA4" s="160"/>
-      <c r="AB4" s="160"/>
-      <c r="AC4" s="160"/>
-      <c r="AD4" s="160"/>
-      <c r="AE4" s="161"/>
-      <c r="AF4" s="159" t="str">
+      <c r="Z4" s="157"/>
+      <c r="AA4" s="157"/>
+      <c r="AB4" s="157"/>
+      <c r="AC4" s="157"/>
+      <c r="AD4" s="157"/>
+      <c r="AE4" s="158"/>
+      <c r="AF4" s="156" t="str">
         <f t="shared" ref="AF4" si="1">"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="AG4" s="160"/>
-      <c r="AH4" s="160"/>
-      <c r="AI4" s="160"/>
-      <c r="AJ4" s="160"/>
-      <c r="AK4" s="160"/>
-      <c r="AL4" s="161"/>
-      <c r="AM4" s="159" t="str">
+      <c r="AG4" s="157"/>
+      <c r="AH4" s="157"/>
+      <c r="AI4" s="157"/>
+      <c r="AJ4" s="157"/>
+      <c r="AK4" s="157"/>
+      <c r="AL4" s="158"/>
+      <c r="AM4" s="156" t="str">
         <f t="shared" ref="AM4" si="2">"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AN4" s="160"/>
-      <c r="AO4" s="160"/>
-      <c r="AP4" s="160"/>
-      <c r="AQ4" s="160"/>
-      <c r="AR4" s="160"/>
-      <c r="AS4" s="161"/>
-      <c r="AT4" s="159" t="str">
+      <c r="AN4" s="157"/>
+      <c r="AO4" s="157"/>
+      <c r="AP4" s="157"/>
+      <c r="AQ4" s="157"/>
+      <c r="AR4" s="157"/>
+      <c r="AS4" s="158"/>
+      <c r="AT4" s="156" t="str">
         <f t="shared" ref="AT4" si="3">"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AU4" s="160"/>
-      <c r="AV4" s="160"/>
-      <c r="AW4" s="160"/>
-      <c r="AX4" s="160"/>
-      <c r="AY4" s="160"/>
-      <c r="AZ4" s="161"/>
-      <c r="BA4" s="159" t="str">
+      <c r="AU4" s="157"/>
+      <c r="AV4" s="157"/>
+      <c r="AW4" s="157"/>
+      <c r="AX4" s="157"/>
+      <c r="AY4" s="157"/>
+      <c r="AZ4" s="158"/>
+      <c r="BA4" s="156" t="str">
         <f t="shared" ref="BA4" si="4">"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="BB4" s="160"/>
-      <c r="BC4" s="160"/>
-      <c r="BD4" s="160"/>
-      <c r="BE4" s="160"/>
-      <c r="BF4" s="160"/>
-      <c r="BG4" s="161"/>
-      <c r="BH4" s="159" t="str">
+      <c r="BB4" s="157"/>
+      <c r="BC4" s="157"/>
+      <c r="BD4" s="157"/>
+      <c r="BE4" s="157"/>
+      <c r="BF4" s="157"/>
+      <c r="BG4" s="158"/>
+      <c r="BH4" s="156" t="str">
         <f t="shared" ref="BH4" si="5">"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BI4" s="160"/>
-      <c r="BJ4" s="160"/>
-      <c r="BK4" s="160"/>
-      <c r="BL4" s="160"/>
-      <c r="BM4" s="160"/>
-      <c r="BN4" s="161"/>
-      <c r="BO4" s="159" t="str">
+      <c r="BI4" s="157"/>
+      <c r="BJ4" s="157"/>
+      <c r="BK4" s="157"/>
+      <c r="BL4" s="157"/>
+      <c r="BM4" s="157"/>
+      <c r="BN4" s="158"/>
+      <c r="BO4" s="156" t="str">
         <f t="shared" ref="BO4" si="6">"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BP4" s="160"/>
-      <c r="BQ4" s="160"/>
-      <c r="BR4" s="160"/>
-      <c r="BS4" s="160"/>
-      <c r="BT4" s="160"/>
-      <c r="BU4" s="161"/>
-      <c r="BV4" s="159" t="str">
+      <c r="BP4" s="157"/>
+      <c r="BQ4" s="157"/>
+      <c r="BR4" s="157"/>
+      <c r="BS4" s="157"/>
+      <c r="BT4" s="157"/>
+      <c r="BU4" s="158"/>
+      <c r="BV4" s="156" t="str">
         <f t="shared" ref="BV4" si="7">"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BW4" s="160"/>
-      <c r="BX4" s="160"/>
-      <c r="BY4" s="160"/>
-      <c r="BZ4" s="160"/>
-      <c r="CA4" s="160"/>
-      <c r="CB4" s="161"/>
-      <c r="CC4" s="159" t="str">
+      <c r="BW4" s="157"/>
+      <c r="BX4" s="157"/>
+      <c r="BY4" s="157"/>
+      <c r="BZ4" s="157"/>
+      <c r="CA4" s="157"/>
+      <c r="CB4" s="158"/>
+      <c r="CC4" s="156" t="str">
         <f t="shared" ref="CC4" si="8">"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="CD4" s="160"/>
-      <c r="CE4" s="160"/>
-      <c r="CF4" s="160"/>
-      <c r="CG4" s="160"/>
-      <c r="CH4" s="160"/>
-      <c r="CI4" s="161"/>
-      <c r="CJ4" s="159" t="str">
+      <c r="CD4" s="157"/>
+      <c r="CE4" s="157"/>
+      <c r="CF4" s="157"/>
+      <c r="CG4" s="157"/>
+      <c r="CH4" s="157"/>
+      <c r="CI4" s="158"/>
+      <c r="CJ4" s="156" t="str">
         <f t="shared" ref="CJ4" si="9">"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CK4" s="160"/>
-      <c r="CL4" s="160"/>
-      <c r="CM4" s="160"/>
-      <c r="CN4" s="160"/>
-      <c r="CO4" s="160"/>
-      <c r="CP4" s="161"/>
-      <c r="CQ4" s="159" t="str">
+      <c r="CK4" s="157"/>
+      <c r="CL4" s="157"/>
+      <c r="CM4" s="157"/>
+      <c r="CN4" s="157"/>
+      <c r="CO4" s="157"/>
+      <c r="CP4" s="158"/>
+      <c r="CQ4" s="156" t="str">
         <f t="shared" ref="CQ4" si="10">"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CR4" s="160"/>
-      <c r="CS4" s="160"/>
-      <c r="CT4" s="160"/>
-      <c r="CU4" s="160"/>
-      <c r="CV4" s="160"/>
-      <c r="CW4" s="161"/>
-      <c r="CX4" s="159" t="str">
+      <c r="CR4" s="157"/>
+      <c r="CS4" s="157"/>
+      <c r="CT4" s="157"/>
+      <c r="CU4" s="157"/>
+      <c r="CV4" s="157"/>
+      <c r="CW4" s="158"/>
+      <c r="CX4" s="156" t="str">
         <f t="shared" ref="CX4" si="11">"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="CY4" s="160"/>
-      <c r="CZ4" s="160"/>
-      <c r="DA4" s="160"/>
-      <c r="DB4" s="160"/>
-      <c r="DC4" s="160"/>
-      <c r="DD4" s="161"/>
-      <c r="DE4" s="159" t="str">
+      <c r="CY4" s="157"/>
+      <c r="CZ4" s="157"/>
+      <c r="DA4" s="157"/>
+      <c r="DB4" s="157"/>
+      <c r="DC4" s="157"/>
+      <c r="DD4" s="158"/>
+      <c r="DE4" s="156" t="str">
         <f t="shared" ref="DE4" si="12">"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="DF4" s="160"/>
-      <c r="DG4" s="160"/>
-      <c r="DH4" s="160"/>
-      <c r="DI4" s="160"/>
-      <c r="DJ4" s="160"/>
-      <c r="DK4" s="161"/>
-      <c r="DL4" s="159" t="str">
+      <c r="DF4" s="157"/>
+      <c r="DG4" s="157"/>
+      <c r="DH4" s="157"/>
+      <c r="DI4" s="157"/>
+      <c r="DJ4" s="157"/>
+      <c r="DK4" s="158"/>
+      <c r="DL4" s="156" t="str">
         <f t="shared" ref="DL4" si="13">"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 15</v>
       </c>
-      <c r="DM4" s="160"/>
-      <c r="DN4" s="160"/>
-      <c r="DO4" s="160"/>
-      <c r="DP4" s="160"/>
-      <c r="DQ4" s="160"/>
-      <c r="DR4" s="161"/>
-      <c r="DS4" s="159" t="str">
+      <c r="DM4" s="157"/>
+      <c r="DN4" s="157"/>
+      <c r="DO4" s="157"/>
+      <c r="DP4" s="157"/>
+      <c r="DQ4" s="157"/>
+      <c r="DR4" s="158"/>
+      <c r="DS4" s="156" t="str">
         <f t="shared" ref="DS4" si="14">"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 16</v>
       </c>
-      <c r="DT4" s="160"/>
-      <c r="DU4" s="160"/>
-      <c r="DV4" s="160"/>
-      <c r="DW4" s="160"/>
-      <c r="DX4" s="160"/>
-      <c r="DY4" s="161"/>
-      <c r="DZ4" s="159" t="str">
+      <c r="DT4" s="157"/>
+      <c r="DU4" s="157"/>
+      <c r="DV4" s="157"/>
+      <c r="DW4" s="157"/>
+      <c r="DX4" s="157"/>
+      <c r="DY4" s="158"/>
+      <c r="DZ4" s="156" t="str">
         <f t="shared" ref="DZ4" si="15">"Week "&amp;(DS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 17</v>
       </c>
-      <c r="EA4" s="160"/>
-      <c r="EB4" s="160"/>
-      <c r="EC4" s="160"/>
-      <c r="ED4" s="160"/>
-      <c r="EE4" s="160"/>
-      <c r="EF4" s="161"/>
-      <c r="EG4" s="159" t="str">
+      <c r="EA4" s="157"/>
+      <c r="EB4" s="157"/>
+      <c r="EC4" s="157"/>
+      <c r="ED4" s="157"/>
+      <c r="EE4" s="157"/>
+      <c r="EF4" s="158"/>
+      <c r="EG4" s="156" t="str">
         <f t="shared" ref="EG4" si="16">"Week "&amp;(DZ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 18</v>
       </c>
-      <c r="EH4" s="160"/>
-      <c r="EI4" s="160"/>
-      <c r="EJ4" s="160"/>
-      <c r="EK4" s="160"/>
-      <c r="EL4" s="160"/>
-      <c r="EM4" s="161"/>
-      <c r="EN4" s="159" t="str">
+      <c r="EH4" s="157"/>
+      <c r="EI4" s="157"/>
+      <c r="EJ4" s="157"/>
+      <c r="EK4" s="157"/>
+      <c r="EL4" s="157"/>
+      <c r="EM4" s="158"/>
+      <c r="EN4" s="156" t="str">
         <f t="shared" ref="EN4" si="17">"Week "&amp;(EG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 19</v>
       </c>
-      <c r="EO4" s="160"/>
-      <c r="EP4" s="160"/>
-      <c r="EQ4" s="160"/>
-      <c r="ER4" s="160"/>
-      <c r="ES4" s="160"/>
-      <c r="ET4" s="161"/>
-      <c r="EU4" s="159" t="str">
+      <c r="EO4" s="157"/>
+      <c r="EP4" s="157"/>
+      <c r="EQ4" s="157"/>
+      <c r="ER4" s="157"/>
+      <c r="ES4" s="157"/>
+      <c r="ET4" s="158"/>
+      <c r="EU4" s="156" t="str">
         <f t="shared" ref="EU4" si="18">"Week "&amp;(EN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="EV4" s="160"/>
-      <c r="EW4" s="160"/>
-      <c r="EX4" s="160"/>
-      <c r="EY4" s="160"/>
-      <c r="EZ4" s="160"/>
-      <c r="FA4" s="161"/>
-      <c r="FB4" s="159" t="str">
+      <c r="EV4" s="157"/>
+      <c r="EW4" s="157"/>
+      <c r="EX4" s="157"/>
+      <c r="EY4" s="157"/>
+      <c r="EZ4" s="157"/>
+      <c r="FA4" s="158"/>
+      <c r="FB4" s="156" t="str">
         <f t="shared" ref="FB4" si="19">"Week "&amp;(EU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="FC4" s="160"/>
-      <c r="FD4" s="160"/>
-      <c r="FE4" s="160"/>
-      <c r="FF4" s="160"/>
-      <c r="FG4" s="160"/>
-      <c r="FH4" s="161"/>
-      <c r="FI4" s="159" t="str">
+      <c r="FC4" s="157"/>
+      <c r="FD4" s="157"/>
+      <c r="FE4" s="157"/>
+      <c r="FF4" s="157"/>
+      <c r="FG4" s="157"/>
+      <c r="FH4" s="158"/>
+      <c r="FI4" s="156" t="str">
         <f t="shared" ref="FI4" si="20">"Week "&amp;(FB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="FJ4" s="160"/>
-      <c r="FK4" s="160"/>
-      <c r="FL4" s="160"/>
-      <c r="FM4" s="160"/>
-      <c r="FN4" s="160"/>
-      <c r="FO4" s="161"/>
-      <c r="FP4" s="159" t="str">
+      <c r="FJ4" s="157"/>
+      <c r="FK4" s="157"/>
+      <c r="FL4" s="157"/>
+      <c r="FM4" s="157"/>
+      <c r="FN4" s="157"/>
+      <c r="FO4" s="158"/>
+      <c r="FP4" s="156" t="str">
         <f t="shared" ref="FP4" si="21">"Week "&amp;(FI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="FQ4" s="160"/>
-      <c r="FR4" s="160"/>
-      <c r="FS4" s="160"/>
-      <c r="FT4" s="160"/>
-      <c r="FU4" s="160"/>
-      <c r="FV4" s="161"/>
-      <c r="FW4" s="159" t="str">
+      <c r="FQ4" s="157"/>
+      <c r="FR4" s="157"/>
+      <c r="FS4" s="157"/>
+      <c r="FT4" s="157"/>
+      <c r="FU4" s="157"/>
+      <c r="FV4" s="158"/>
+      <c r="FW4" s="156" t="str">
         <f t="shared" ref="FW4" si="22">"Week "&amp;(FP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="FX4" s="160"/>
-      <c r="FY4" s="160"/>
-      <c r="FZ4" s="160"/>
-      <c r="GA4" s="160"/>
-      <c r="GB4" s="160"/>
-      <c r="GC4" s="161"/>
-      <c r="GD4" s="159" t="str">
+      <c r="FX4" s="157"/>
+      <c r="FY4" s="157"/>
+      <c r="FZ4" s="157"/>
+      <c r="GA4" s="157"/>
+      <c r="GB4" s="157"/>
+      <c r="GC4" s="158"/>
+      <c r="GD4" s="156" t="str">
         <f t="shared" ref="GD4" si="23">"Week "&amp;(FW6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="GE4" s="160"/>
-      <c r="GF4" s="160"/>
-      <c r="GG4" s="160"/>
-      <c r="GH4" s="160"/>
-      <c r="GI4" s="160"/>
-      <c r="GJ4" s="161"/>
-      <c r="GK4" s="159" t="str">
+      <c r="GE4" s="157"/>
+      <c r="GF4" s="157"/>
+      <c r="GG4" s="157"/>
+      <c r="GH4" s="157"/>
+      <c r="GI4" s="157"/>
+      <c r="GJ4" s="158"/>
+      <c r="GK4" s="156" t="str">
         <f t="shared" ref="GK4" si="24">"Week "&amp;(GD6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="GL4" s="160"/>
-      <c r="GM4" s="160"/>
-      <c r="GN4" s="160"/>
-      <c r="GO4" s="160"/>
-      <c r="GP4" s="160"/>
-      <c r="GQ4" s="161"/>
-      <c r="GR4" s="159" t="str">
+      <c r="GL4" s="157"/>
+      <c r="GM4" s="157"/>
+      <c r="GN4" s="157"/>
+      <c r="GO4" s="157"/>
+      <c r="GP4" s="157"/>
+      <c r="GQ4" s="158"/>
+      <c r="GR4" s="156" t="str">
         <f t="shared" ref="GR4" si="25">"Week "&amp;(GK6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="GS4" s="160"/>
-      <c r="GT4" s="160"/>
-      <c r="GU4" s="160"/>
-      <c r="GV4" s="160"/>
-      <c r="GW4" s="160"/>
-      <c r="GX4" s="161"/>
-      <c r="GY4" s="159" t="str">
+      <c r="GS4" s="157"/>
+      <c r="GT4" s="157"/>
+      <c r="GU4" s="157"/>
+      <c r="GV4" s="157"/>
+      <c r="GW4" s="157"/>
+      <c r="GX4" s="158"/>
+      <c r="GY4" s="156" t="str">
         <f t="shared" ref="GY4" si="26">"Week "&amp;(GR6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="GZ4" s="160"/>
-      <c r="HA4" s="160"/>
-      <c r="HB4" s="160"/>
-      <c r="HC4" s="160"/>
-      <c r="HD4" s="160"/>
-      <c r="HE4" s="161"/>
-      <c r="HF4" s="159" t="str">
+      <c r="GZ4" s="157"/>
+      <c r="HA4" s="157"/>
+      <c r="HB4" s="157"/>
+      <c r="HC4" s="157"/>
+      <c r="HD4" s="157"/>
+      <c r="HE4" s="158"/>
+      <c r="HF4" s="156" t="str">
         <f t="shared" ref="HF4" si="27">"Week "&amp;(GY6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="HG4" s="160"/>
-      <c r="HH4" s="160"/>
-      <c r="HI4" s="160"/>
-      <c r="HJ4" s="160"/>
-      <c r="HK4" s="160"/>
-      <c r="HL4" s="161"/>
-      <c r="HM4" s="159" t="str">
+      <c r="HG4" s="157"/>
+      <c r="HH4" s="157"/>
+      <c r="HI4" s="157"/>
+      <c r="HJ4" s="157"/>
+      <c r="HK4" s="157"/>
+      <c r="HL4" s="158"/>
+      <c r="HM4" s="156" t="str">
         <f t="shared" ref="HM4" si="28">"Week "&amp;(HF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="HN4" s="160"/>
-      <c r="HO4" s="160"/>
-      <c r="HP4" s="160"/>
-      <c r="HQ4" s="160"/>
-      <c r="HR4" s="160"/>
-      <c r="HS4" s="161"/>
-      <c r="HT4" s="159" t="str">
+      <c r="HN4" s="157"/>
+      <c r="HO4" s="157"/>
+      <c r="HP4" s="157"/>
+      <c r="HQ4" s="157"/>
+      <c r="HR4" s="157"/>
+      <c r="HS4" s="158"/>
+      <c r="HT4" s="156" t="str">
         <f t="shared" ref="HT4" si="29">"Week "&amp;(HM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="HU4" s="160"/>
-      <c r="HV4" s="160"/>
-      <c r="HW4" s="160"/>
-      <c r="HX4" s="160"/>
-      <c r="HY4" s="160"/>
-      <c r="HZ4" s="161"/>
-      <c r="IA4" s="159" t="str">
+      <c r="HU4" s="157"/>
+      <c r="HV4" s="157"/>
+      <c r="HW4" s="157"/>
+      <c r="HX4" s="157"/>
+      <c r="HY4" s="157"/>
+      <c r="HZ4" s="158"/>
+      <c r="IA4" s="156" t="str">
         <f t="shared" ref="IA4" si="30">"Week "&amp;(HT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="IB4" s="160"/>
-      <c r="IC4" s="160"/>
-      <c r="ID4" s="160"/>
-      <c r="IE4" s="160"/>
-      <c r="IF4" s="160"/>
-      <c r="IG4" s="161"/>
-      <c r="IH4" s="159" t="str">
+      <c r="IB4" s="157"/>
+      <c r="IC4" s="157"/>
+      <c r="ID4" s="157"/>
+      <c r="IE4" s="157"/>
+      <c r="IF4" s="157"/>
+      <c r="IG4" s="158"/>
+      <c r="IH4" s="156" t="str">
         <f t="shared" ref="IH4" si="31">"Week "&amp;(IA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 33</v>
       </c>
-      <c r="II4" s="160"/>
-      <c r="IJ4" s="160"/>
-      <c r="IK4" s="160"/>
-      <c r="IL4" s="160"/>
-      <c r="IM4" s="160"/>
-      <c r="IN4" s="161"/>
-      <c r="IO4" s="159" t="str">
+      <c r="II4" s="157"/>
+      <c r="IJ4" s="157"/>
+      <c r="IK4" s="157"/>
+      <c r="IL4" s="157"/>
+      <c r="IM4" s="157"/>
+      <c r="IN4" s="158"/>
+      <c r="IO4" s="156" t="str">
         <f t="shared" ref="IO4" si="32">"Week "&amp;(IH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 34</v>
       </c>
-      <c r="IP4" s="160"/>
-      <c r="IQ4" s="160"/>
-      <c r="IR4" s="160"/>
-      <c r="IS4" s="160"/>
-      <c r="IT4" s="160"/>
-      <c r="IU4" s="161"/>
+      <c r="IP4" s="157"/>
+      <c r="IQ4" s="157"/>
+      <c r="IR4" s="157"/>
+      <c r="IS4" s="157"/>
+      <c r="IT4" s="157"/>
+      <c r="IU4" s="158"/>
     </row>
     <row r="5" spans="1:255" s="55" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="111"/>
       <c r="B5" s="113" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="167" t="s">
+      <c r="C5" s="171" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="168"/>
-      <c r="E5" s="169"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="173"/>
       <c r="F5" s="111"/>
       <c r="G5" s="111"/>
       <c r="H5" s="111"/>
       <c r="I5" s="111"/>
-      <c r="K5" s="170">
+      <c r="K5" s="174">
         <f>K6</f>
         <v>45292</v>
       </c>
-      <c r="L5" s="157"/>
-      <c r="M5" s="157"/>
-      <c r="N5" s="157"/>
-      <c r="O5" s="157"/>
-      <c r="P5" s="157"/>
-      <c r="Q5" s="172"/>
-      <c r="R5" s="170">
+      <c r="L5" s="160"/>
+      <c r="M5" s="160"/>
+      <c r="N5" s="160"/>
+      <c r="O5" s="160"/>
+      <c r="P5" s="160"/>
+      <c r="Q5" s="176"/>
+      <c r="R5" s="174">
         <f>R6</f>
         <v>45299</v>
       </c>
-      <c r="S5" s="157"/>
-      <c r="T5" s="157"/>
-      <c r="U5" s="157"/>
-      <c r="V5" s="157"/>
-      <c r="W5" s="157"/>
-      <c r="X5" s="171"/>
-      <c r="Y5" s="173">
+      <c r="S5" s="160"/>
+      <c r="T5" s="160"/>
+      <c r="U5" s="160"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
+      <c r="X5" s="175"/>
+      <c r="Y5" s="177">
         <f>Y6</f>
         <v>45306</v>
       </c>
-      <c r="Z5" s="157"/>
-      <c r="AA5" s="157"/>
-      <c r="AB5" s="157"/>
-      <c r="AC5" s="157"/>
-      <c r="AD5" s="157"/>
-      <c r="AE5" s="174"/>
-      <c r="AF5" s="165">
+      <c r="Z5" s="160"/>
+      <c r="AA5" s="160"/>
+      <c r="AB5" s="160"/>
+      <c r="AC5" s="160"/>
+      <c r="AD5" s="160"/>
+      <c r="AE5" s="178"/>
+      <c r="AF5" s="169">
         <f>AF6</f>
         <v>45313</v>
       </c>
-      <c r="AG5" s="157"/>
-      <c r="AH5" s="157"/>
-      <c r="AI5" s="157"/>
-      <c r="AJ5" s="157"/>
-      <c r="AK5" s="157"/>
-      <c r="AL5" s="166"/>
-      <c r="AM5" s="175">
+      <c r="AG5" s="160"/>
+      <c r="AH5" s="160"/>
+      <c r="AI5" s="160"/>
+      <c r="AJ5" s="160"/>
+      <c r="AK5" s="160"/>
+      <c r="AL5" s="170"/>
+      <c r="AM5" s="162">
         <f>AM6</f>
         <v>45320</v>
       </c>
-      <c r="AN5" s="157"/>
-      <c r="AO5" s="157"/>
-      <c r="AP5" s="157"/>
-      <c r="AQ5" s="157"/>
-      <c r="AR5" s="157"/>
-      <c r="AS5" s="176"/>
-      <c r="AT5" s="177">
+      <c r="AN5" s="160"/>
+      <c r="AO5" s="160"/>
+      <c r="AP5" s="160"/>
+      <c r="AQ5" s="160"/>
+      <c r="AR5" s="160"/>
+      <c r="AS5" s="163"/>
+      <c r="AT5" s="164">
         <f>AT6</f>
         <v>45327</v>
       </c>
-      <c r="AU5" s="157"/>
-      <c r="AV5" s="157"/>
-      <c r="AW5" s="157"/>
-      <c r="AX5" s="157"/>
-      <c r="AY5" s="157"/>
-      <c r="AZ5" s="178"/>
-      <c r="BA5" s="156">
+      <c r="AU5" s="160"/>
+      <c r="AV5" s="160"/>
+      <c r="AW5" s="160"/>
+      <c r="AX5" s="160"/>
+      <c r="AY5" s="160"/>
+      <c r="AZ5" s="165"/>
+      <c r="BA5" s="166">
         <f>BA6</f>
         <v>45334</v>
       </c>
-      <c r="BB5" s="157"/>
-      <c r="BC5" s="157"/>
-      <c r="BD5" s="157"/>
-      <c r="BE5" s="157"/>
-      <c r="BF5" s="157"/>
-      <c r="BG5" s="158"/>
-      <c r="BH5" s="162">
+      <c r="BB5" s="160"/>
+      <c r="BC5" s="160"/>
+      <c r="BD5" s="160"/>
+      <c r="BE5" s="160"/>
+      <c r="BF5" s="160"/>
+      <c r="BG5" s="167"/>
+      <c r="BH5" s="159">
         <f>BH6</f>
         <v>45341</v>
       </c>
-      <c r="BI5" s="157"/>
-      <c r="BJ5" s="157"/>
-      <c r="BK5" s="157"/>
-      <c r="BL5" s="157"/>
-      <c r="BM5" s="157"/>
-      <c r="BN5" s="163"/>
-      <c r="BO5" s="156">
+      <c r="BI5" s="160"/>
+      <c r="BJ5" s="160"/>
+      <c r="BK5" s="160"/>
+      <c r="BL5" s="160"/>
+      <c r="BM5" s="160"/>
+      <c r="BN5" s="161"/>
+      <c r="BO5" s="166">
         <f>BO6</f>
         <v>45348</v>
       </c>
-      <c r="BP5" s="157"/>
-      <c r="BQ5" s="157"/>
-      <c r="BR5" s="157"/>
-      <c r="BS5" s="157"/>
-      <c r="BT5" s="157"/>
-      <c r="BU5" s="158"/>
-      <c r="BV5" s="162">
+      <c r="BP5" s="160"/>
+      <c r="BQ5" s="160"/>
+      <c r="BR5" s="160"/>
+      <c r="BS5" s="160"/>
+      <c r="BT5" s="160"/>
+      <c r="BU5" s="167"/>
+      <c r="BV5" s="159">
         <f>BV6</f>
         <v>45355</v>
       </c>
-      <c r="BW5" s="157"/>
-      <c r="BX5" s="157"/>
-      <c r="BY5" s="157"/>
-      <c r="BZ5" s="157"/>
-      <c r="CA5" s="157"/>
-      <c r="CB5" s="163"/>
-      <c r="CC5" s="162">
+      <c r="BW5" s="160"/>
+      <c r="BX5" s="160"/>
+      <c r="BY5" s="160"/>
+      <c r="BZ5" s="160"/>
+      <c r="CA5" s="160"/>
+      <c r="CB5" s="161"/>
+      <c r="CC5" s="159">
         <f>CC6</f>
         <v>45362</v>
       </c>
-      <c r="CD5" s="157"/>
-      <c r="CE5" s="157"/>
-      <c r="CF5" s="157"/>
-      <c r="CG5" s="157"/>
-      <c r="CH5" s="157"/>
-      <c r="CI5" s="163"/>
-      <c r="CJ5" s="156">
+      <c r="CD5" s="160"/>
+      <c r="CE5" s="160"/>
+      <c r="CF5" s="160"/>
+      <c r="CG5" s="160"/>
+      <c r="CH5" s="160"/>
+      <c r="CI5" s="161"/>
+      <c r="CJ5" s="166">
         <f>CJ6</f>
         <v>45369</v>
       </c>
-      <c r="CK5" s="157"/>
-      <c r="CL5" s="157"/>
-      <c r="CM5" s="157"/>
-      <c r="CN5" s="157"/>
-      <c r="CO5" s="157"/>
-      <c r="CP5" s="158"/>
-      <c r="CQ5" s="162">
+      <c r="CK5" s="160"/>
+      <c r="CL5" s="160"/>
+      <c r="CM5" s="160"/>
+      <c r="CN5" s="160"/>
+      <c r="CO5" s="160"/>
+      <c r="CP5" s="167"/>
+      <c r="CQ5" s="159">
         <f>CQ6</f>
         <v>45376</v>
       </c>
-      <c r="CR5" s="157"/>
-      <c r="CS5" s="157"/>
-      <c r="CT5" s="157"/>
-      <c r="CU5" s="157"/>
-      <c r="CV5" s="157"/>
-      <c r="CW5" s="163"/>
-      <c r="CX5" s="162">
+      <c r="CR5" s="160"/>
+      <c r="CS5" s="160"/>
+      <c r="CT5" s="160"/>
+      <c r="CU5" s="160"/>
+      <c r="CV5" s="160"/>
+      <c r="CW5" s="161"/>
+      <c r="CX5" s="159">
         <f t="shared" ref="CX5" si="33">CX6</f>
         <v>45383</v>
       </c>
-      <c r="CY5" s="157"/>
-      <c r="CZ5" s="157"/>
-      <c r="DA5" s="157"/>
-      <c r="DB5" s="157"/>
-      <c r="DC5" s="157"/>
-      <c r="DD5" s="163"/>
-      <c r="DE5" s="156">
+      <c r="CY5" s="160"/>
+      <c r="CZ5" s="160"/>
+      <c r="DA5" s="160"/>
+      <c r="DB5" s="160"/>
+      <c r="DC5" s="160"/>
+      <c r="DD5" s="161"/>
+      <c r="DE5" s="166">
         <f t="shared" ref="DE5" si="34">DE6</f>
         <v>45390</v>
       </c>
-      <c r="DF5" s="157"/>
-      <c r="DG5" s="157"/>
-      <c r="DH5" s="157"/>
-      <c r="DI5" s="157"/>
-      <c r="DJ5" s="157"/>
-      <c r="DK5" s="158"/>
-      <c r="DL5" s="162">
+      <c r="DF5" s="160"/>
+      <c r="DG5" s="160"/>
+      <c r="DH5" s="160"/>
+      <c r="DI5" s="160"/>
+      <c r="DJ5" s="160"/>
+      <c r="DK5" s="167"/>
+      <c r="DL5" s="159">
         <f t="shared" ref="DL5" si="35">DL6</f>
         <v>45397</v>
       </c>
-      <c r="DM5" s="157"/>
-      <c r="DN5" s="157"/>
-      <c r="DO5" s="157"/>
-      <c r="DP5" s="157"/>
-      <c r="DQ5" s="157"/>
-      <c r="DR5" s="163"/>
-      <c r="DS5" s="162">
+      <c r="DM5" s="160"/>
+      <c r="DN5" s="160"/>
+      <c r="DO5" s="160"/>
+      <c r="DP5" s="160"/>
+      <c r="DQ5" s="160"/>
+      <c r="DR5" s="161"/>
+      <c r="DS5" s="159">
         <f t="shared" ref="DS5" si="36">DS6</f>
         <v>45404</v>
       </c>
-      <c r="DT5" s="157"/>
-      <c r="DU5" s="157"/>
-      <c r="DV5" s="157"/>
-      <c r="DW5" s="157"/>
-      <c r="DX5" s="157"/>
-      <c r="DY5" s="163"/>
-      <c r="DZ5" s="156">
+      <c r="DT5" s="160"/>
+      <c r="DU5" s="160"/>
+      <c r="DV5" s="160"/>
+      <c r="DW5" s="160"/>
+      <c r="DX5" s="160"/>
+      <c r="DY5" s="161"/>
+      <c r="DZ5" s="166">
         <f t="shared" ref="DZ5" si="37">DZ6</f>
         <v>45411</v>
       </c>
-      <c r="EA5" s="157"/>
-      <c r="EB5" s="157"/>
-      <c r="EC5" s="157"/>
-      <c r="ED5" s="157"/>
-      <c r="EE5" s="157"/>
-      <c r="EF5" s="158"/>
-      <c r="EG5" s="162">
+      <c r="EA5" s="160"/>
+      <c r="EB5" s="160"/>
+      <c r="EC5" s="160"/>
+      <c r="ED5" s="160"/>
+      <c r="EE5" s="160"/>
+      <c r="EF5" s="167"/>
+      <c r="EG5" s="159">
         <f t="shared" ref="EG5" si="38">EG6</f>
         <v>45418</v>
       </c>
-      <c r="EH5" s="157"/>
-      <c r="EI5" s="157"/>
-      <c r="EJ5" s="157"/>
-      <c r="EK5" s="157"/>
-      <c r="EL5" s="157"/>
-      <c r="EM5" s="163"/>
-      <c r="EN5" s="162">
+      <c r="EH5" s="160"/>
+      <c r="EI5" s="160"/>
+      <c r="EJ5" s="160"/>
+      <c r="EK5" s="160"/>
+      <c r="EL5" s="160"/>
+      <c r="EM5" s="161"/>
+      <c r="EN5" s="159">
         <f>EN6</f>
         <v>45425</v>
       </c>
-      <c r="EO5" s="157"/>
-      <c r="EP5" s="157"/>
-      <c r="EQ5" s="157"/>
-      <c r="ER5" s="157"/>
-      <c r="ES5" s="157"/>
-      <c r="ET5" s="163"/>
-      <c r="EU5" s="156">
+      <c r="EO5" s="160"/>
+      <c r="EP5" s="160"/>
+      <c r="EQ5" s="160"/>
+      <c r="ER5" s="160"/>
+      <c r="ES5" s="160"/>
+      <c r="ET5" s="161"/>
+      <c r="EU5" s="166">
         <f>EU6</f>
         <v>45432</v>
       </c>
-      <c r="EV5" s="157"/>
-      <c r="EW5" s="157"/>
-      <c r="EX5" s="157"/>
-      <c r="EY5" s="157"/>
-      <c r="EZ5" s="157"/>
-      <c r="FA5" s="158"/>
-      <c r="FB5" s="162">
+      <c r="EV5" s="160"/>
+      <c r="EW5" s="160"/>
+      <c r="EX5" s="160"/>
+      <c r="EY5" s="160"/>
+      <c r="EZ5" s="160"/>
+      <c r="FA5" s="167"/>
+      <c r="FB5" s="159">
         <f>FB6</f>
         <v>45439</v>
       </c>
-      <c r="FC5" s="157"/>
-      <c r="FD5" s="157"/>
-      <c r="FE5" s="157"/>
-      <c r="FF5" s="157"/>
-      <c r="FG5" s="157"/>
-      <c r="FH5" s="163"/>
-      <c r="FI5" s="162">
+      <c r="FC5" s="160"/>
+      <c r="FD5" s="160"/>
+      <c r="FE5" s="160"/>
+      <c r="FF5" s="160"/>
+      <c r="FG5" s="160"/>
+      <c r="FH5" s="161"/>
+      <c r="FI5" s="159">
         <f t="shared" ref="FI5" si="39">FI6</f>
         <v>45446</v>
       </c>
-      <c r="FJ5" s="157"/>
-      <c r="FK5" s="157"/>
-      <c r="FL5" s="157"/>
-      <c r="FM5" s="157"/>
-      <c r="FN5" s="157"/>
-      <c r="FO5" s="163"/>
-      <c r="FP5" s="156">
+      <c r="FJ5" s="160"/>
+      <c r="FK5" s="160"/>
+      <c r="FL5" s="160"/>
+      <c r="FM5" s="160"/>
+      <c r="FN5" s="160"/>
+      <c r="FO5" s="161"/>
+      <c r="FP5" s="166">
         <f t="shared" ref="FP5" si="40">FP6</f>
         <v>45453</v>
       </c>
-      <c r="FQ5" s="157"/>
-      <c r="FR5" s="157"/>
-      <c r="FS5" s="157"/>
-      <c r="FT5" s="157"/>
-      <c r="FU5" s="157"/>
-      <c r="FV5" s="158"/>
-      <c r="FW5" s="162">
+      <c r="FQ5" s="160"/>
+      <c r="FR5" s="160"/>
+      <c r="FS5" s="160"/>
+      <c r="FT5" s="160"/>
+      <c r="FU5" s="160"/>
+      <c r="FV5" s="167"/>
+      <c r="FW5" s="159">
         <f t="shared" ref="FW5" si="41">FW6</f>
         <v>45460</v>
       </c>
-      <c r="FX5" s="157"/>
-      <c r="FY5" s="157"/>
-      <c r="FZ5" s="157"/>
-      <c r="GA5" s="157"/>
-      <c r="GB5" s="157"/>
-      <c r="GC5" s="163"/>
-      <c r="GD5" s="162">
+      <c r="FX5" s="160"/>
+      <c r="FY5" s="160"/>
+      <c r="FZ5" s="160"/>
+      <c r="GA5" s="160"/>
+      <c r="GB5" s="160"/>
+      <c r="GC5" s="161"/>
+      <c r="GD5" s="159">
         <f t="shared" ref="GD5" si="42">GD6</f>
         <v>45467</v>
       </c>
-      <c r="GE5" s="157"/>
-      <c r="GF5" s="157"/>
-      <c r="GG5" s="157"/>
-      <c r="GH5" s="157"/>
-      <c r="GI5" s="157"/>
-      <c r="GJ5" s="163"/>
-      <c r="GK5" s="156">
+      <c r="GE5" s="160"/>
+      <c r="GF5" s="160"/>
+      <c r="GG5" s="160"/>
+      <c r="GH5" s="160"/>
+      <c r="GI5" s="160"/>
+      <c r="GJ5" s="161"/>
+      <c r="GK5" s="166">
         <f t="shared" ref="GK5" si="43">GK6</f>
         <v>45474</v>
       </c>
-      <c r="GL5" s="157"/>
-      <c r="GM5" s="157"/>
-      <c r="GN5" s="157"/>
-      <c r="GO5" s="157"/>
-      <c r="GP5" s="157"/>
-      <c r="GQ5" s="158"/>
-      <c r="GR5" s="162">
+      <c r="GL5" s="160"/>
+      <c r="GM5" s="160"/>
+      <c r="GN5" s="160"/>
+      <c r="GO5" s="160"/>
+      <c r="GP5" s="160"/>
+      <c r="GQ5" s="167"/>
+      <c r="GR5" s="159">
         <f t="shared" ref="GR5" si="44">GR6</f>
         <v>45481</v>
       </c>
-      <c r="GS5" s="157"/>
-      <c r="GT5" s="157"/>
-      <c r="GU5" s="157"/>
-      <c r="GV5" s="157"/>
-      <c r="GW5" s="157"/>
-      <c r="GX5" s="163"/>
-      <c r="GY5" s="156">
+      <c r="GS5" s="160"/>
+      <c r="GT5" s="160"/>
+      <c r="GU5" s="160"/>
+      <c r="GV5" s="160"/>
+      <c r="GW5" s="160"/>
+      <c r="GX5" s="161"/>
+      <c r="GY5" s="166">
         <f t="shared" ref="GY5" si="45">GY6</f>
         <v>45488</v>
       </c>
-      <c r="GZ5" s="157"/>
-      <c r="HA5" s="157"/>
-      <c r="HB5" s="157"/>
-      <c r="HC5" s="157"/>
-      <c r="HD5" s="157"/>
-      <c r="HE5" s="158"/>
-      <c r="HF5" s="162">
+      <c r="GZ5" s="160"/>
+      <c r="HA5" s="160"/>
+      <c r="HB5" s="160"/>
+      <c r="HC5" s="160"/>
+      <c r="HD5" s="160"/>
+      <c r="HE5" s="167"/>
+      <c r="HF5" s="159">
         <f t="shared" ref="HF5" si="46">HF6</f>
         <v>45495</v>
       </c>
-      <c r="HG5" s="157"/>
-      <c r="HH5" s="157"/>
-      <c r="HI5" s="157"/>
-      <c r="HJ5" s="157"/>
-      <c r="HK5" s="157"/>
-      <c r="HL5" s="163"/>
-      <c r="HM5" s="156">
+      <c r="HG5" s="160"/>
+      <c r="HH5" s="160"/>
+      <c r="HI5" s="160"/>
+      <c r="HJ5" s="160"/>
+      <c r="HK5" s="160"/>
+      <c r="HL5" s="161"/>
+      <c r="HM5" s="166">
         <f t="shared" ref="HM5" si="47">HM6</f>
         <v>45502</v>
       </c>
-      <c r="HN5" s="157"/>
-      <c r="HO5" s="157"/>
-      <c r="HP5" s="157"/>
-      <c r="HQ5" s="157"/>
-      <c r="HR5" s="157"/>
-      <c r="HS5" s="158"/>
-      <c r="HT5" s="162">
+      <c r="HN5" s="160"/>
+      <c r="HO5" s="160"/>
+      <c r="HP5" s="160"/>
+      <c r="HQ5" s="160"/>
+      <c r="HR5" s="160"/>
+      <c r="HS5" s="167"/>
+      <c r="HT5" s="159">
         <f t="shared" ref="HT5" si="48">HT6</f>
         <v>45509</v>
       </c>
-      <c r="HU5" s="157"/>
-      <c r="HV5" s="157"/>
-      <c r="HW5" s="157"/>
-      <c r="HX5" s="157"/>
-      <c r="HY5" s="157"/>
-      <c r="HZ5" s="163"/>
-      <c r="IA5" s="156">
+      <c r="HU5" s="160"/>
+      <c r="HV5" s="160"/>
+      <c r="HW5" s="160"/>
+      <c r="HX5" s="160"/>
+      <c r="HY5" s="160"/>
+      <c r="HZ5" s="161"/>
+      <c r="IA5" s="166">
         <f t="shared" ref="IA5" si="49">IA6</f>
         <v>45516</v>
       </c>
-      <c r="IB5" s="157"/>
-      <c r="IC5" s="157"/>
-      <c r="ID5" s="157"/>
-      <c r="IE5" s="157"/>
-      <c r="IF5" s="157"/>
-      <c r="IG5" s="158"/>
-      <c r="IH5" s="162">
+      <c r="IB5" s="160"/>
+      <c r="IC5" s="160"/>
+      <c r="ID5" s="160"/>
+      <c r="IE5" s="160"/>
+      <c r="IF5" s="160"/>
+      <c r="IG5" s="167"/>
+      <c r="IH5" s="159">
         <f t="shared" ref="IH5" si="50">IH6</f>
         <v>45523</v>
       </c>
-      <c r="II5" s="157"/>
-      <c r="IJ5" s="157"/>
-      <c r="IK5" s="157"/>
-      <c r="IL5" s="157"/>
-      <c r="IM5" s="157"/>
-      <c r="IN5" s="163"/>
-      <c r="IO5" s="156">
+      <c r="II5" s="160"/>
+      <c r="IJ5" s="160"/>
+      <c r="IK5" s="160"/>
+      <c r="IL5" s="160"/>
+      <c r="IM5" s="160"/>
+      <c r="IN5" s="161"/>
+      <c r="IO5" s="166">
         <f t="shared" ref="IO5" si="51">IO6</f>
         <v>45530</v>
       </c>
-      <c r="IP5" s="157"/>
-      <c r="IQ5" s="157"/>
-      <c r="IR5" s="157"/>
-      <c r="IS5" s="157"/>
-      <c r="IT5" s="157"/>
-      <c r="IU5" s="158"/>
+      <c r="IP5" s="160"/>
+      <c r="IQ5" s="160"/>
+      <c r="IR5" s="160"/>
+      <c r="IS5" s="160"/>
+      <c r="IT5" s="160"/>
+      <c r="IU5" s="167"/>
     </row>
     <row r="6" spans="1:255" s="53" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="146"/>
@@ -8715,7 +8715,7 @@
         <v>4</v>
       </c>
       <c r="H14" s="46">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I14" s="102">
         <f t="shared" si="256"/>
@@ -15777,49 +15777,20 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="73">
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="AD1:AR1"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AF5:AL5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="FI4:FO4"/>
-    <mergeCell ref="FP4:FV4"/>
-    <mergeCell ref="EG4:EM4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE5:DK5"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="DS5:DY5"/>
-    <mergeCell ref="DZ5:EF5"/>
-    <mergeCell ref="EG5:EM5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DS4:DY4"/>
-    <mergeCell ref="DZ4:EF4"/>
+    <mergeCell ref="IO5:IU5"/>
+    <mergeCell ref="IO4:IU4"/>
+    <mergeCell ref="HT4:HZ4"/>
+    <mergeCell ref="IA4:IG4"/>
+    <mergeCell ref="IH4:IN4"/>
+    <mergeCell ref="HM5:HS5"/>
+    <mergeCell ref="HT5:HZ5"/>
+    <mergeCell ref="IA5:IG5"/>
+    <mergeCell ref="IH5:IN5"/>
+    <mergeCell ref="GY4:HE4"/>
+    <mergeCell ref="HF4:HL4"/>
+    <mergeCell ref="GY5:HE5"/>
+    <mergeCell ref="HF5:HL5"/>
+    <mergeCell ref="HM4:HS4"/>
     <mergeCell ref="FW4:GC4"/>
     <mergeCell ref="GD4:GJ4"/>
     <mergeCell ref="GK4:GQ4"/>
@@ -15836,20 +15807,49 @@
     <mergeCell ref="EN4:ET4"/>
     <mergeCell ref="EU4:FA4"/>
     <mergeCell ref="FB4:FH4"/>
-    <mergeCell ref="HM5:HS5"/>
-    <mergeCell ref="HT5:HZ5"/>
-    <mergeCell ref="IA5:IG5"/>
-    <mergeCell ref="IH5:IN5"/>
-    <mergeCell ref="GY4:HE4"/>
-    <mergeCell ref="HF4:HL4"/>
-    <mergeCell ref="GY5:HE5"/>
-    <mergeCell ref="HF5:HL5"/>
-    <mergeCell ref="HM4:HS4"/>
-    <mergeCell ref="IO5:IU5"/>
-    <mergeCell ref="IO4:IU4"/>
-    <mergeCell ref="HT4:HZ4"/>
-    <mergeCell ref="IA4:IG4"/>
-    <mergeCell ref="IH4:IN4"/>
+    <mergeCell ref="FI4:FO4"/>
+    <mergeCell ref="FP4:FV4"/>
+    <mergeCell ref="EG4:EM4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="DS5:DY5"/>
+    <mergeCell ref="DZ5:EF5"/>
+    <mergeCell ref="EG5:EM5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DS4:DY4"/>
+    <mergeCell ref="DZ4:EF4"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="AD1:AR1"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="AF5:AL5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="BH4:BN4"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="AM5:AS5"/>
+    <mergeCell ref="AT4:AZ4"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="BA4:BG4"/>
+    <mergeCell ref="BA5:BG5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H36:H40 H8:H33">
@@ -15887,7 +15887,7 @@
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Start Date." sqref="I4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.25"/>

</xml_diff>

<commit_message>
read IADP, IDHP, IGDHPa papers
</commit_message>
<xml_diff>
--- a/thesis gantt chart.xlsx
+++ b/thesis gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wings_stuff\srus\TUD\yr5\thesis\thesis_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD24E9CA-444A-43B2-8D11-584EC6EB0A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7226C94-D8D1-4779-AA92-E33AD96A26E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3263,6 +3263,15 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="70" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3275,28 +3284,7 @@
     <xf numFmtId="167" fontId="52" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="84" fillId="24" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -3333,6 +3321,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="52" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4177,7 +4177,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ18" sqref="AJ18"/>
+      <selection pane="bottomLeft" activeCell="AK16" sqref="AK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -4255,21 +4255,21 @@
       <c r="K1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="AD1" s="168"/>
-      <c r="AE1" s="168"/>
-      <c r="AF1" s="168"/>
-      <c r="AG1" s="168"/>
-      <c r="AH1" s="168"/>
-      <c r="AI1" s="168"/>
-      <c r="AJ1" s="168"/>
-      <c r="AK1" s="168"/>
-      <c r="AL1" s="168"/>
-      <c r="AM1" s="168"/>
-      <c r="AN1" s="168"/>
-      <c r="AO1" s="168"/>
-      <c r="AP1" s="168"/>
-      <c r="AQ1" s="168"/>
-      <c r="AR1" s="168"/>
+      <c r="AD1" s="164"/>
+      <c r="AE1" s="164"/>
+      <c r="AF1" s="164"/>
+      <c r="AG1" s="164"/>
+      <c r="AH1" s="164"/>
+      <c r="AI1" s="164"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="164"/>
+      <c r="AL1" s="164"/>
+      <c r="AM1" s="164"/>
+      <c r="AN1" s="164"/>
+      <c r="AO1" s="164"/>
+      <c r="AP1" s="164"/>
+      <c r="AQ1" s="164"/>
+      <c r="AR1" s="164"/>
     </row>
     <row r="2" spans="1:255" s="59" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="112" t="s">
@@ -4349,729 +4349,729 @@
       <c r="B4" s="113" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="167">
         <v>45295</v>
       </c>
-      <c r="D4" s="172"/>
-      <c r="E4" s="173"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="169"/>
       <c r="H4" s="113" t="s">
         <v>71</v>
       </c>
       <c r="I4" s="114">
         <v>1</v>
       </c>
-      <c r="K4" s="156"/>
-      <c r="L4" s="157"/>
-      <c r="M4" s="157"/>
-      <c r="N4" s="157"/>
-      <c r="O4" s="157"/>
-      <c r="P4" s="157"/>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="156" t="str">
+      <c r="K4" s="159"/>
+      <c r="L4" s="160"/>
+      <c r="M4" s="160"/>
+      <c r="N4" s="160"/>
+      <c r="O4" s="160"/>
+      <c r="P4" s="160"/>
+      <c r="Q4" s="161"/>
+      <c r="R4" s="159" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="S4" s="157"/>
-      <c r="T4" s="157"/>
-      <c r="U4" s="157"/>
-      <c r="V4" s="157"/>
-      <c r="W4" s="157"/>
-      <c r="X4" s="158"/>
-      <c r="Y4" s="156" t="str">
+      <c r="S4" s="160"/>
+      <c r="T4" s="160"/>
+      <c r="U4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="159" t="str">
         <f t="shared" ref="Y4" si="0">"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="Z4" s="157"/>
-      <c r="AA4" s="157"/>
-      <c r="AB4" s="157"/>
-      <c r="AC4" s="157"/>
-      <c r="AD4" s="157"/>
-      <c r="AE4" s="158"/>
-      <c r="AF4" s="156" t="str">
+      <c r="Z4" s="160"/>
+      <c r="AA4" s="160"/>
+      <c r="AB4" s="160"/>
+      <c r="AC4" s="160"/>
+      <c r="AD4" s="160"/>
+      <c r="AE4" s="161"/>
+      <c r="AF4" s="159" t="str">
         <f t="shared" ref="AF4" si="1">"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="AG4" s="157"/>
-      <c r="AH4" s="157"/>
-      <c r="AI4" s="157"/>
-      <c r="AJ4" s="157"/>
-      <c r="AK4" s="157"/>
-      <c r="AL4" s="158"/>
-      <c r="AM4" s="156" t="str">
+      <c r="AG4" s="160"/>
+      <c r="AH4" s="160"/>
+      <c r="AI4" s="160"/>
+      <c r="AJ4" s="160"/>
+      <c r="AK4" s="160"/>
+      <c r="AL4" s="161"/>
+      <c r="AM4" s="159" t="str">
         <f t="shared" ref="AM4" si="2">"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AN4" s="157"/>
-      <c r="AO4" s="157"/>
-      <c r="AP4" s="157"/>
-      <c r="AQ4" s="157"/>
-      <c r="AR4" s="157"/>
-      <c r="AS4" s="158"/>
-      <c r="AT4" s="156" t="str">
+      <c r="AN4" s="160"/>
+      <c r="AO4" s="160"/>
+      <c r="AP4" s="160"/>
+      <c r="AQ4" s="160"/>
+      <c r="AR4" s="160"/>
+      <c r="AS4" s="161"/>
+      <c r="AT4" s="159" t="str">
         <f t="shared" ref="AT4" si="3">"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AU4" s="157"/>
-      <c r="AV4" s="157"/>
-      <c r="AW4" s="157"/>
-      <c r="AX4" s="157"/>
-      <c r="AY4" s="157"/>
-      <c r="AZ4" s="158"/>
-      <c r="BA4" s="156" t="str">
+      <c r="AU4" s="160"/>
+      <c r="AV4" s="160"/>
+      <c r="AW4" s="160"/>
+      <c r="AX4" s="160"/>
+      <c r="AY4" s="160"/>
+      <c r="AZ4" s="161"/>
+      <c r="BA4" s="159" t="str">
         <f t="shared" ref="BA4" si="4">"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="BB4" s="157"/>
-      <c r="BC4" s="157"/>
-      <c r="BD4" s="157"/>
-      <c r="BE4" s="157"/>
-      <c r="BF4" s="157"/>
-      <c r="BG4" s="158"/>
-      <c r="BH4" s="156" t="str">
+      <c r="BB4" s="160"/>
+      <c r="BC4" s="160"/>
+      <c r="BD4" s="160"/>
+      <c r="BE4" s="160"/>
+      <c r="BF4" s="160"/>
+      <c r="BG4" s="161"/>
+      <c r="BH4" s="159" t="str">
         <f t="shared" ref="BH4" si="5">"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BI4" s="157"/>
-      <c r="BJ4" s="157"/>
-      <c r="BK4" s="157"/>
-      <c r="BL4" s="157"/>
-      <c r="BM4" s="157"/>
-      <c r="BN4" s="158"/>
-      <c r="BO4" s="156" t="str">
+      <c r="BI4" s="160"/>
+      <c r="BJ4" s="160"/>
+      <c r="BK4" s="160"/>
+      <c r="BL4" s="160"/>
+      <c r="BM4" s="160"/>
+      <c r="BN4" s="161"/>
+      <c r="BO4" s="159" t="str">
         <f t="shared" ref="BO4" si="6">"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BP4" s="157"/>
-      <c r="BQ4" s="157"/>
-      <c r="BR4" s="157"/>
-      <c r="BS4" s="157"/>
-      <c r="BT4" s="157"/>
-      <c r="BU4" s="158"/>
-      <c r="BV4" s="156" t="str">
+      <c r="BP4" s="160"/>
+      <c r="BQ4" s="160"/>
+      <c r="BR4" s="160"/>
+      <c r="BS4" s="160"/>
+      <c r="BT4" s="160"/>
+      <c r="BU4" s="161"/>
+      <c r="BV4" s="159" t="str">
         <f t="shared" ref="BV4" si="7">"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BW4" s="157"/>
-      <c r="BX4" s="157"/>
-      <c r="BY4" s="157"/>
-      <c r="BZ4" s="157"/>
-      <c r="CA4" s="157"/>
-      <c r="CB4" s="158"/>
-      <c r="CC4" s="156" t="str">
+      <c r="BW4" s="160"/>
+      <c r="BX4" s="160"/>
+      <c r="BY4" s="160"/>
+      <c r="BZ4" s="160"/>
+      <c r="CA4" s="160"/>
+      <c r="CB4" s="161"/>
+      <c r="CC4" s="159" t="str">
         <f t="shared" ref="CC4" si="8">"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="CD4" s="157"/>
-      <c r="CE4" s="157"/>
-      <c r="CF4" s="157"/>
-      <c r="CG4" s="157"/>
-      <c r="CH4" s="157"/>
-      <c r="CI4" s="158"/>
-      <c r="CJ4" s="156" t="str">
+      <c r="CD4" s="160"/>
+      <c r="CE4" s="160"/>
+      <c r="CF4" s="160"/>
+      <c r="CG4" s="160"/>
+      <c r="CH4" s="160"/>
+      <c r="CI4" s="161"/>
+      <c r="CJ4" s="159" t="str">
         <f t="shared" ref="CJ4" si="9">"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CK4" s="157"/>
-      <c r="CL4" s="157"/>
-      <c r="CM4" s="157"/>
-      <c r="CN4" s="157"/>
-      <c r="CO4" s="157"/>
-      <c r="CP4" s="158"/>
-      <c r="CQ4" s="156" t="str">
+      <c r="CK4" s="160"/>
+      <c r="CL4" s="160"/>
+      <c r="CM4" s="160"/>
+      <c r="CN4" s="160"/>
+      <c r="CO4" s="160"/>
+      <c r="CP4" s="161"/>
+      <c r="CQ4" s="159" t="str">
         <f t="shared" ref="CQ4" si="10">"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CR4" s="157"/>
-      <c r="CS4" s="157"/>
-      <c r="CT4" s="157"/>
-      <c r="CU4" s="157"/>
-      <c r="CV4" s="157"/>
-      <c r="CW4" s="158"/>
-      <c r="CX4" s="156" t="str">
+      <c r="CR4" s="160"/>
+      <c r="CS4" s="160"/>
+      <c r="CT4" s="160"/>
+      <c r="CU4" s="160"/>
+      <c r="CV4" s="160"/>
+      <c r="CW4" s="161"/>
+      <c r="CX4" s="159" t="str">
         <f t="shared" ref="CX4" si="11">"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="CY4" s="157"/>
-      <c r="CZ4" s="157"/>
-      <c r="DA4" s="157"/>
-      <c r="DB4" s="157"/>
-      <c r="DC4" s="157"/>
-      <c r="DD4" s="158"/>
-      <c r="DE4" s="156" t="str">
+      <c r="CY4" s="160"/>
+      <c r="CZ4" s="160"/>
+      <c r="DA4" s="160"/>
+      <c r="DB4" s="160"/>
+      <c r="DC4" s="160"/>
+      <c r="DD4" s="161"/>
+      <c r="DE4" s="159" t="str">
         <f t="shared" ref="DE4" si="12">"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="DF4" s="157"/>
-      <c r="DG4" s="157"/>
-      <c r="DH4" s="157"/>
-      <c r="DI4" s="157"/>
-      <c r="DJ4" s="157"/>
-      <c r="DK4" s="158"/>
-      <c r="DL4" s="156" t="str">
+      <c r="DF4" s="160"/>
+      <c r="DG4" s="160"/>
+      <c r="DH4" s="160"/>
+      <c r="DI4" s="160"/>
+      <c r="DJ4" s="160"/>
+      <c r="DK4" s="161"/>
+      <c r="DL4" s="159" t="str">
         <f t="shared" ref="DL4" si="13">"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 15</v>
       </c>
-      <c r="DM4" s="157"/>
-      <c r="DN4" s="157"/>
-      <c r="DO4" s="157"/>
-      <c r="DP4" s="157"/>
-      <c r="DQ4" s="157"/>
-      <c r="DR4" s="158"/>
-      <c r="DS4" s="156" t="str">
+      <c r="DM4" s="160"/>
+      <c r="DN4" s="160"/>
+      <c r="DO4" s="160"/>
+      <c r="DP4" s="160"/>
+      <c r="DQ4" s="160"/>
+      <c r="DR4" s="161"/>
+      <c r="DS4" s="159" t="str">
         <f t="shared" ref="DS4" si="14">"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 16</v>
       </c>
-      <c r="DT4" s="157"/>
-      <c r="DU4" s="157"/>
-      <c r="DV4" s="157"/>
-      <c r="DW4" s="157"/>
-      <c r="DX4" s="157"/>
-      <c r="DY4" s="158"/>
-      <c r="DZ4" s="156" t="str">
+      <c r="DT4" s="160"/>
+      <c r="DU4" s="160"/>
+      <c r="DV4" s="160"/>
+      <c r="DW4" s="160"/>
+      <c r="DX4" s="160"/>
+      <c r="DY4" s="161"/>
+      <c r="DZ4" s="159" t="str">
         <f t="shared" ref="DZ4" si="15">"Week "&amp;(DS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 17</v>
       </c>
-      <c r="EA4" s="157"/>
-      <c r="EB4" s="157"/>
-      <c r="EC4" s="157"/>
-      <c r="ED4" s="157"/>
-      <c r="EE4" s="157"/>
-      <c r="EF4" s="158"/>
-      <c r="EG4" s="156" t="str">
+      <c r="EA4" s="160"/>
+      <c r="EB4" s="160"/>
+      <c r="EC4" s="160"/>
+      <c r="ED4" s="160"/>
+      <c r="EE4" s="160"/>
+      <c r="EF4" s="161"/>
+      <c r="EG4" s="159" t="str">
         <f t="shared" ref="EG4" si="16">"Week "&amp;(DZ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 18</v>
       </c>
-      <c r="EH4" s="157"/>
-      <c r="EI4" s="157"/>
-      <c r="EJ4" s="157"/>
-      <c r="EK4" s="157"/>
-      <c r="EL4" s="157"/>
-      <c r="EM4" s="158"/>
-      <c r="EN4" s="156" t="str">
+      <c r="EH4" s="160"/>
+      <c r="EI4" s="160"/>
+      <c r="EJ4" s="160"/>
+      <c r="EK4" s="160"/>
+      <c r="EL4" s="160"/>
+      <c r="EM4" s="161"/>
+      <c r="EN4" s="159" t="str">
         <f t="shared" ref="EN4" si="17">"Week "&amp;(EG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 19</v>
       </c>
-      <c r="EO4" s="157"/>
-      <c r="EP4" s="157"/>
-      <c r="EQ4" s="157"/>
-      <c r="ER4" s="157"/>
-      <c r="ES4" s="157"/>
-      <c r="ET4" s="158"/>
-      <c r="EU4" s="156" t="str">
+      <c r="EO4" s="160"/>
+      <c r="EP4" s="160"/>
+      <c r="EQ4" s="160"/>
+      <c r="ER4" s="160"/>
+      <c r="ES4" s="160"/>
+      <c r="ET4" s="161"/>
+      <c r="EU4" s="159" t="str">
         <f t="shared" ref="EU4" si="18">"Week "&amp;(EN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="EV4" s="157"/>
-      <c r="EW4" s="157"/>
-      <c r="EX4" s="157"/>
-      <c r="EY4" s="157"/>
-      <c r="EZ4" s="157"/>
-      <c r="FA4" s="158"/>
-      <c r="FB4" s="156" t="str">
+      <c r="EV4" s="160"/>
+      <c r="EW4" s="160"/>
+      <c r="EX4" s="160"/>
+      <c r="EY4" s="160"/>
+      <c r="EZ4" s="160"/>
+      <c r="FA4" s="161"/>
+      <c r="FB4" s="159" t="str">
         <f t="shared" ref="FB4" si="19">"Week "&amp;(EU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="FC4" s="157"/>
-      <c r="FD4" s="157"/>
-      <c r="FE4" s="157"/>
-      <c r="FF4" s="157"/>
-      <c r="FG4" s="157"/>
-      <c r="FH4" s="158"/>
-      <c r="FI4" s="156" t="str">
+      <c r="FC4" s="160"/>
+      <c r="FD4" s="160"/>
+      <c r="FE4" s="160"/>
+      <c r="FF4" s="160"/>
+      <c r="FG4" s="160"/>
+      <c r="FH4" s="161"/>
+      <c r="FI4" s="159" t="str">
         <f t="shared" ref="FI4" si="20">"Week "&amp;(FB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="FJ4" s="157"/>
-      <c r="FK4" s="157"/>
-      <c r="FL4" s="157"/>
-      <c r="FM4" s="157"/>
-      <c r="FN4" s="157"/>
-      <c r="FO4" s="158"/>
-      <c r="FP4" s="156" t="str">
+      <c r="FJ4" s="160"/>
+      <c r="FK4" s="160"/>
+      <c r="FL4" s="160"/>
+      <c r="FM4" s="160"/>
+      <c r="FN4" s="160"/>
+      <c r="FO4" s="161"/>
+      <c r="FP4" s="159" t="str">
         <f t="shared" ref="FP4" si="21">"Week "&amp;(FI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="FQ4" s="157"/>
-      <c r="FR4" s="157"/>
-      <c r="FS4" s="157"/>
-      <c r="FT4" s="157"/>
-      <c r="FU4" s="157"/>
-      <c r="FV4" s="158"/>
-      <c r="FW4" s="156" t="str">
+      <c r="FQ4" s="160"/>
+      <c r="FR4" s="160"/>
+      <c r="FS4" s="160"/>
+      <c r="FT4" s="160"/>
+      <c r="FU4" s="160"/>
+      <c r="FV4" s="161"/>
+      <c r="FW4" s="159" t="str">
         <f t="shared" ref="FW4" si="22">"Week "&amp;(FP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="FX4" s="157"/>
-      <c r="FY4" s="157"/>
-      <c r="FZ4" s="157"/>
-      <c r="GA4" s="157"/>
-      <c r="GB4" s="157"/>
-      <c r="GC4" s="158"/>
-      <c r="GD4" s="156" t="str">
+      <c r="FX4" s="160"/>
+      <c r="FY4" s="160"/>
+      <c r="FZ4" s="160"/>
+      <c r="GA4" s="160"/>
+      <c r="GB4" s="160"/>
+      <c r="GC4" s="161"/>
+      <c r="GD4" s="159" t="str">
         <f t="shared" ref="GD4" si="23">"Week "&amp;(FW6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="GE4" s="157"/>
-      <c r="GF4" s="157"/>
-      <c r="GG4" s="157"/>
-      <c r="GH4" s="157"/>
-      <c r="GI4" s="157"/>
-      <c r="GJ4" s="158"/>
-      <c r="GK4" s="156" t="str">
+      <c r="GE4" s="160"/>
+      <c r="GF4" s="160"/>
+      <c r="GG4" s="160"/>
+      <c r="GH4" s="160"/>
+      <c r="GI4" s="160"/>
+      <c r="GJ4" s="161"/>
+      <c r="GK4" s="159" t="str">
         <f t="shared" ref="GK4" si="24">"Week "&amp;(GD6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="GL4" s="157"/>
-      <c r="GM4" s="157"/>
-      <c r="GN4" s="157"/>
-      <c r="GO4" s="157"/>
-      <c r="GP4" s="157"/>
-      <c r="GQ4" s="158"/>
-      <c r="GR4" s="156" t="str">
+      <c r="GL4" s="160"/>
+      <c r="GM4" s="160"/>
+      <c r="GN4" s="160"/>
+      <c r="GO4" s="160"/>
+      <c r="GP4" s="160"/>
+      <c r="GQ4" s="161"/>
+      <c r="GR4" s="159" t="str">
         <f t="shared" ref="GR4" si="25">"Week "&amp;(GK6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="GS4" s="157"/>
-      <c r="GT4" s="157"/>
-      <c r="GU4" s="157"/>
-      <c r="GV4" s="157"/>
-      <c r="GW4" s="157"/>
-      <c r="GX4" s="158"/>
-      <c r="GY4" s="156" t="str">
+      <c r="GS4" s="160"/>
+      <c r="GT4" s="160"/>
+      <c r="GU4" s="160"/>
+      <c r="GV4" s="160"/>
+      <c r="GW4" s="160"/>
+      <c r="GX4" s="161"/>
+      <c r="GY4" s="159" t="str">
         <f t="shared" ref="GY4" si="26">"Week "&amp;(GR6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="GZ4" s="157"/>
-      <c r="HA4" s="157"/>
-      <c r="HB4" s="157"/>
-      <c r="HC4" s="157"/>
-      <c r="HD4" s="157"/>
-      <c r="HE4" s="158"/>
-      <c r="HF4" s="156" t="str">
+      <c r="GZ4" s="160"/>
+      <c r="HA4" s="160"/>
+      <c r="HB4" s="160"/>
+      <c r="HC4" s="160"/>
+      <c r="HD4" s="160"/>
+      <c r="HE4" s="161"/>
+      <c r="HF4" s="159" t="str">
         <f t="shared" ref="HF4" si="27">"Week "&amp;(GY6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="HG4" s="157"/>
-      <c r="HH4" s="157"/>
-      <c r="HI4" s="157"/>
-      <c r="HJ4" s="157"/>
-      <c r="HK4" s="157"/>
-      <c r="HL4" s="158"/>
-      <c r="HM4" s="156" t="str">
+      <c r="HG4" s="160"/>
+      <c r="HH4" s="160"/>
+      <c r="HI4" s="160"/>
+      <c r="HJ4" s="160"/>
+      <c r="HK4" s="160"/>
+      <c r="HL4" s="161"/>
+      <c r="HM4" s="159" t="str">
         <f t="shared" ref="HM4" si="28">"Week "&amp;(HF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="HN4" s="157"/>
-      <c r="HO4" s="157"/>
-      <c r="HP4" s="157"/>
-      <c r="HQ4" s="157"/>
-      <c r="HR4" s="157"/>
-      <c r="HS4" s="158"/>
-      <c r="HT4" s="156" t="str">
+      <c r="HN4" s="160"/>
+      <c r="HO4" s="160"/>
+      <c r="HP4" s="160"/>
+      <c r="HQ4" s="160"/>
+      <c r="HR4" s="160"/>
+      <c r="HS4" s="161"/>
+      <c r="HT4" s="159" t="str">
         <f t="shared" ref="HT4" si="29">"Week "&amp;(HM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="HU4" s="157"/>
-      <c r="HV4" s="157"/>
-      <c r="HW4" s="157"/>
-      <c r="HX4" s="157"/>
-      <c r="HY4" s="157"/>
-      <c r="HZ4" s="158"/>
-      <c r="IA4" s="156" t="str">
+      <c r="HU4" s="160"/>
+      <c r="HV4" s="160"/>
+      <c r="HW4" s="160"/>
+      <c r="HX4" s="160"/>
+      <c r="HY4" s="160"/>
+      <c r="HZ4" s="161"/>
+      <c r="IA4" s="159" t="str">
         <f t="shared" ref="IA4" si="30">"Week "&amp;(HT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="IB4" s="157"/>
-      <c r="IC4" s="157"/>
-      <c r="ID4" s="157"/>
-      <c r="IE4" s="157"/>
-      <c r="IF4" s="157"/>
-      <c r="IG4" s="158"/>
-      <c r="IH4" s="156" t="str">
+      <c r="IB4" s="160"/>
+      <c r="IC4" s="160"/>
+      <c r="ID4" s="160"/>
+      <c r="IE4" s="160"/>
+      <c r="IF4" s="160"/>
+      <c r="IG4" s="161"/>
+      <c r="IH4" s="159" t="str">
         <f t="shared" ref="IH4" si="31">"Week "&amp;(IA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 33</v>
       </c>
-      <c r="II4" s="157"/>
-      <c r="IJ4" s="157"/>
-      <c r="IK4" s="157"/>
-      <c r="IL4" s="157"/>
-      <c r="IM4" s="157"/>
-      <c r="IN4" s="158"/>
-      <c r="IO4" s="156" t="str">
+      <c r="II4" s="160"/>
+      <c r="IJ4" s="160"/>
+      <c r="IK4" s="160"/>
+      <c r="IL4" s="160"/>
+      <c r="IM4" s="160"/>
+      <c r="IN4" s="161"/>
+      <c r="IO4" s="159" t="str">
         <f t="shared" ref="IO4" si="32">"Week "&amp;(IH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 34</v>
       </c>
-      <c r="IP4" s="157"/>
-      <c r="IQ4" s="157"/>
-      <c r="IR4" s="157"/>
-      <c r="IS4" s="157"/>
-      <c r="IT4" s="157"/>
-      <c r="IU4" s="158"/>
+      <c r="IP4" s="160"/>
+      <c r="IQ4" s="160"/>
+      <c r="IR4" s="160"/>
+      <c r="IS4" s="160"/>
+      <c r="IT4" s="160"/>
+      <c r="IU4" s="161"/>
     </row>
     <row r="5" spans="1:255" s="55" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="111"/>
       <c r="B5" s="113" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="171" t="s">
+      <c r="C5" s="167" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="172"/>
-      <c r="E5" s="173"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="169"/>
       <c r="F5" s="111"/>
       <c r="G5" s="111"/>
       <c r="H5" s="111"/>
       <c r="I5" s="111"/>
-      <c r="K5" s="174">
+      <c r="K5" s="170">
         <f>K6</f>
         <v>45292</v>
       </c>
-      <c r="L5" s="160"/>
-      <c r="M5" s="160"/>
-      <c r="N5" s="160"/>
-      <c r="O5" s="160"/>
-      <c r="P5" s="160"/>
-      <c r="Q5" s="176"/>
-      <c r="R5" s="174">
+      <c r="L5" s="157"/>
+      <c r="M5" s="157"/>
+      <c r="N5" s="157"/>
+      <c r="O5" s="157"/>
+      <c r="P5" s="157"/>
+      <c r="Q5" s="172"/>
+      <c r="R5" s="170">
         <f>R6</f>
         <v>45299</v>
       </c>
-      <c r="S5" s="160"/>
-      <c r="T5" s="160"/>
-      <c r="U5" s="160"/>
-      <c r="V5" s="160"/>
-      <c r="W5" s="160"/>
-      <c r="X5" s="175"/>
-      <c r="Y5" s="177">
+      <c r="S5" s="157"/>
+      <c r="T5" s="157"/>
+      <c r="U5" s="157"/>
+      <c r="V5" s="157"/>
+      <c r="W5" s="157"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="173">
         <f>Y6</f>
         <v>45306</v>
       </c>
-      <c r="Z5" s="160"/>
-      <c r="AA5" s="160"/>
-      <c r="AB5" s="160"/>
-      <c r="AC5" s="160"/>
-      <c r="AD5" s="160"/>
-      <c r="AE5" s="178"/>
-      <c r="AF5" s="169">
+      <c r="Z5" s="157"/>
+      <c r="AA5" s="157"/>
+      <c r="AB5" s="157"/>
+      <c r="AC5" s="157"/>
+      <c r="AD5" s="157"/>
+      <c r="AE5" s="174"/>
+      <c r="AF5" s="165">
         <f>AF6</f>
         <v>45313</v>
       </c>
-      <c r="AG5" s="160"/>
-      <c r="AH5" s="160"/>
-      <c r="AI5" s="160"/>
-      <c r="AJ5" s="160"/>
-      <c r="AK5" s="160"/>
-      <c r="AL5" s="170"/>
-      <c r="AM5" s="162">
+      <c r="AG5" s="157"/>
+      <c r="AH5" s="157"/>
+      <c r="AI5" s="157"/>
+      <c r="AJ5" s="157"/>
+      <c r="AK5" s="157"/>
+      <c r="AL5" s="166"/>
+      <c r="AM5" s="175">
         <f>AM6</f>
         <v>45320</v>
       </c>
-      <c r="AN5" s="160"/>
-      <c r="AO5" s="160"/>
-      <c r="AP5" s="160"/>
-      <c r="AQ5" s="160"/>
-      <c r="AR5" s="160"/>
-      <c r="AS5" s="163"/>
-      <c r="AT5" s="164">
+      <c r="AN5" s="157"/>
+      <c r="AO5" s="157"/>
+      <c r="AP5" s="157"/>
+      <c r="AQ5" s="157"/>
+      <c r="AR5" s="157"/>
+      <c r="AS5" s="176"/>
+      <c r="AT5" s="177">
         <f>AT6</f>
         <v>45327</v>
       </c>
-      <c r="AU5" s="160"/>
-      <c r="AV5" s="160"/>
-      <c r="AW5" s="160"/>
-      <c r="AX5" s="160"/>
-      <c r="AY5" s="160"/>
-      <c r="AZ5" s="165"/>
-      <c r="BA5" s="166">
+      <c r="AU5" s="157"/>
+      <c r="AV5" s="157"/>
+      <c r="AW5" s="157"/>
+      <c r="AX5" s="157"/>
+      <c r="AY5" s="157"/>
+      <c r="AZ5" s="178"/>
+      <c r="BA5" s="156">
         <f>BA6</f>
         <v>45334</v>
       </c>
-      <c r="BB5" s="160"/>
-      <c r="BC5" s="160"/>
-      <c r="BD5" s="160"/>
-      <c r="BE5" s="160"/>
-      <c r="BF5" s="160"/>
-      <c r="BG5" s="167"/>
-      <c r="BH5" s="159">
+      <c r="BB5" s="157"/>
+      <c r="BC5" s="157"/>
+      <c r="BD5" s="157"/>
+      <c r="BE5" s="157"/>
+      <c r="BF5" s="157"/>
+      <c r="BG5" s="158"/>
+      <c r="BH5" s="162">
         <f>BH6</f>
         <v>45341</v>
       </c>
-      <c r="BI5" s="160"/>
-      <c r="BJ5" s="160"/>
-      <c r="BK5" s="160"/>
-      <c r="BL5" s="160"/>
-      <c r="BM5" s="160"/>
-      <c r="BN5" s="161"/>
-      <c r="BO5" s="166">
+      <c r="BI5" s="157"/>
+      <c r="BJ5" s="157"/>
+      <c r="BK5" s="157"/>
+      <c r="BL5" s="157"/>
+      <c r="BM5" s="157"/>
+      <c r="BN5" s="163"/>
+      <c r="BO5" s="156">
         <f>BO6</f>
         <v>45348</v>
       </c>
-      <c r="BP5" s="160"/>
-      <c r="BQ5" s="160"/>
-      <c r="BR5" s="160"/>
-      <c r="BS5" s="160"/>
-      <c r="BT5" s="160"/>
-      <c r="BU5" s="167"/>
-      <c r="BV5" s="159">
+      <c r="BP5" s="157"/>
+      <c r="BQ5" s="157"/>
+      <c r="BR5" s="157"/>
+      <c r="BS5" s="157"/>
+      <c r="BT5" s="157"/>
+      <c r="BU5" s="158"/>
+      <c r="BV5" s="162">
         <f>BV6</f>
         <v>45355</v>
       </c>
-      <c r="BW5" s="160"/>
-      <c r="BX5" s="160"/>
-      <c r="BY5" s="160"/>
-      <c r="BZ5" s="160"/>
-      <c r="CA5" s="160"/>
-      <c r="CB5" s="161"/>
-      <c r="CC5" s="159">
+      <c r="BW5" s="157"/>
+      <c r="BX5" s="157"/>
+      <c r="BY5" s="157"/>
+      <c r="BZ5" s="157"/>
+      <c r="CA5" s="157"/>
+      <c r="CB5" s="163"/>
+      <c r="CC5" s="162">
         <f>CC6</f>
         <v>45362</v>
       </c>
-      <c r="CD5" s="160"/>
-      <c r="CE5" s="160"/>
-      <c r="CF5" s="160"/>
-      <c r="CG5" s="160"/>
-      <c r="CH5" s="160"/>
-      <c r="CI5" s="161"/>
-      <c r="CJ5" s="166">
+      <c r="CD5" s="157"/>
+      <c r="CE5" s="157"/>
+      <c r="CF5" s="157"/>
+      <c r="CG5" s="157"/>
+      <c r="CH5" s="157"/>
+      <c r="CI5" s="163"/>
+      <c r="CJ5" s="156">
         <f>CJ6</f>
         <v>45369</v>
       </c>
-      <c r="CK5" s="160"/>
-      <c r="CL5" s="160"/>
-      <c r="CM5" s="160"/>
-      <c r="CN5" s="160"/>
-      <c r="CO5" s="160"/>
-      <c r="CP5" s="167"/>
-      <c r="CQ5" s="159">
+      <c r="CK5" s="157"/>
+      <c r="CL5" s="157"/>
+      <c r="CM5" s="157"/>
+      <c r="CN5" s="157"/>
+      <c r="CO5" s="157"/>
+      <c r="CP5" s="158"/>
+      <c r="CQ5" s="162">
         <f>CQ6</f>
         <v>45376</v>
       </c>
-      <c r="CR5" s="160"/>
-      <c r="CS5" s="160"/>
-      <c r="CT5" s="160"/>
-      <c r="CU5" s="160"/>
-      <c r="CV5" s="160"/>
-      <c r="CW5" s="161"/>
-      <c r="CX5" s="159">
+      <c r="CR5" s="157"/>
+      <c r="CS5" s="157"/>
+      <c r="CT5" s="157"/>
+      <c r="CU5" s="157"/>
+      <c r="CV5" s="157"/>
+      <c r="CW5" s="163"/>
+      <c r="CX5" s="162">
         <f t="shared" ref="CX5" si="33">CX6</f>
         <v>45383</v>
       </c>
-      <c r="CY5" s="160"/>
-      <c r="CZ5" s="160"/>
-      <c r="DA5" s="160"/>
-      <c r="DB5" s="160"/>
-      <c r="DC5" s="160"/>
-      <c r="DD5" s="161"/>
-      <c r="DE5" s="166">
+      <c r="CY5" s="157"/>
+      <c r="CZ5" s="157"/>
+      <c r="DA5" s="157"/>
+      <c r="DB5" s="157"/>
+      <c r="DC5" s="157"/>
+      <c r="DD5" s="163"/>
+      <c r="DE5" s="156">
         <f t="shared" ref="DE5" si="34">DE6</f>
         <v>45390</v>
       </c>
-      <c r="DF5" s="160"/>
-      <c r="DG5" s="160"/>
-      <c r="DH5" s="160"/>
-      <c r="DI5" s="160"/>
-      <c r="DJ5" s="160"/>
-      <c r="DK5" s="167"/>
-      <c r="DL5" s="159">
+      <c r="DF5" s="157"/>
+      <c r="DG5" s="157"/>
+      <c r="DH5" s="157"/>
+      <c r="DI5" s="157"/>
+      <c r="DJ5" s="157"/>
+      <c r="DK5" s="158"/>
+      <c r="DL5" s="162">
         <f t="shared" ref="DL5" si="35">DL6</f>
         <v>45397</v>
       </c>
-      <c r="DM5" s="160"/>
-      <c r="DN5" s="160"/>
-      <c r="DO5" s="160"/>
-      <c r="DP5" s="160"/>
-      <c r="DQ5" s="160"/>
-      <c r="DR5" s="161"/>
-      <c r="DS5" s="159">
+      <c r="DM5" s="157"/>
+      <c r="DN5" s="157"/>
+      <c r="DO5" s="157"/>
+      <c r="DP5" s="157"/>
+      <c r="DQ5" s="157"/>
+      <c r="DR5" s="163"/>
+      <c r="DS5" s="162">
         <f t="shared" ref="DS5" si="36">DS6</f>
         <v>45404</v>
       </c>
-      <c r="DT5" s="160"/>
-      <c r="DU5" s="160"/>
-      <c r="DV5" s="160"/>
-      <c r="DW5" s="160"/>
-      <c r="DX5" s="160"/>
-      <c r="DY5" s="161"/>
-      <c r="DZ5" s="166">
+      <c r="DT5" s="157"/>
+      <c r="DU5" s="157"/>
+      <c r="DV5" s="157"/>
+      <c r="DW5" s="157"/>
+      <c r="DX5" s="157"/>
+      <c r="DY5" s="163"/>
+      <c r="DZ5" s="156">
         <f t="shared" ref="DZ5" si="37">DZ6</f>
         <v>45411</v>
       </c>
-      <c r="EA5" s="160"/>
-      <c r="EB5" s="160"/>
-      <c r="EC5" s="160"/>
-      <c r="ED5" s="160"/>
-      <c r="EE5" s="160"/>
-      <c r="EF5" s="167"/>
-      <c r="EG5" s="159">
+      <c r="EA5" s="157"/>
+      <c r="EB5" s="157"/>
+      <c r="EC5" s="157"/>
+      <c r="ED5" s="157"/>
+      <c r="EE5" s="157"/>
+      <c r="EF5" s="158"/>
+      <c r="EG5" s="162">
         <f t="shared" ref="EG5" si="38">EG6</f>
         <v>45418</v>
       </c>
-      <c r="EH5" s="160"/>
-      <c r="EI5" s="160"/>
-      <c r="EJ5" s="160"/>
-      <c r="EK5" s="160"/>
-      <c r="EL5" s="160"/>
-      <c r="EM5" s="161"/>
-      <c r="EN5" s="159">
+      <c r="EH5" s="157"/>
+      <c r="EI5" s="157"/>
+      <c r="EJ5" s="157"/>
+      <c r="EK5" s="157"/>
+      <c r="EL5" s="157"/>
+      <c r="EM5" s="163"/>
+      <c r="EN5" s="162">
         <f>EN6</f>
         <v>45425</v>
       </c>
-      <c r="EO5" s="160"/>
-      <c r="EP5" s="160"/>
-      <c r="EQ5" s="160"/>
-      <c r="ER5" s="160"/>
-      <c r="ES5" s="160"/>
-      <c r="ET5" s="161"/>
-      <c r="EU5" s="166">
+      <c r="EO5" s="157"/>
+      <c r="EP5" s="157"/>
+      <c r="EQ5" s="157"/>
+      <c r="ER5" s="157"/>
+      <c r="ES5" s="157"/>
+      <c r="ET5" s="163"/>
+      <c r="EU5" s="156">
         <f>EU6</f>
         <v>45432</v>
       </c>
-      <c r="EV5" s="160"/>
-      <c r="EW5" s="160"/>
-      <c r="EX5" s="160"/>
-      <c r="EY5" s="160"/>
-      <c r="EZ5" s="160"/>
-      <c r="FA5" s="167"/>
-      <c r="FB5" s="159">
+      <c r="EV5" s="157"/>
+      <c r="EW5" s="157"/>
+      <c r="EX5" s="157"/>
+      <c r="EY5" s="157"/>
+      <c r="EZ5" s="157"/>
+      <c r="FA5" s="158"/>
+      <c r="FB5" s="162">
         <f>FB6</f>
         <v>45439</v>
       </c>
-      <c r="FC5" s="160"/>
-      <c r="FD5" s="160"/>
-      <c r="FE5" s="160"/>
-      <c r="FF5" s="160"/>
-      <c r="FG5" s="160"/>
-      <c r="FH5" s="161"/>
-      <c r="FI5" s="159">
+      <c r="FC5" s="157"/>
+      <c r="FD5" s="157"/>
+      <c r="FE5" s="157"/>
+      <c r="FF5" s="157"/>
+      <c r="FG5" s="157"/>
+      <c r="FH5" s="163"/>
+      <c r="FI5" s="162">
         <f t="shared" ref="FI5" si="39">FI6</f>
         <v>45446</v>
       </c>
-      <c r="FJ5" s="160"/>
-      <c r="FK5" s="160"/>
-      <c r="FL5" s="160"/>
-      <c r="FM5" s="160"/>
-      <c r="FN5" s="160"/>
-      <c r="FO5" s="161"/>
-      <c r="FP5" s="166">
+      <c r="FJ5" s="157"/>
+      <c r="FK5" s="157"/>
+      <c r="FL5" s="157"/>
+      <c r="FM5" s="157"/>
+      <c r="FN5" s="157"/>
+      <c r="FO5" s="163"/>
+      <c r="FP5" s="156">
         <f t="shared" ref="FP5" si="40">FP6</f>
         <v>45453</v>
       </c>
-      <c r="FQ5" s="160"/>
-      <c r="FR5" s="160"/>
-      <c r="FS5" s="160"/>
-      <c r="FT5" s="160"/>
-      <c r="FU5" s="160"/>
-      <c r="FV5" s="167"/>
-      <c r="FW5" s="159">
+      <c r="FQ5" s="157"/>
+      <c r="FR5" s="157"/>
+      <c r="FS5" s="157"/>
+      <c r="FT5" s="157"/>
+      <c r="FU5" s="157"/>
+      <c r="FV5" s="158"/>
+      <c r="FW5" s="162">
         <f t="shared" ref="FW5" si="41">FW6</f>
         <v>45460</v>
       </c>
-      <c r="FX5" s="160"/>
-      <c r="FY5" s="160"/>
-      <c r="FZ5" s="160"/>
-      <c r="GA5" s="160"/>
-      <c r="GB5" s="160"/>
-      <c r="GC5" s="161"/>
-      <c r="GD5" s="159">
+      <c r="FX5" s="157"/>
+      <c r="FY5" s="157"/>
+      <c r="FZ5" s="157"/>
+      <c r="GA5" s="157"/>
+      <c r="GB5" s="157"/>
+      <c r="GC5" s="163"/>
+      <c r="GD5" s="162">
         <f t="shared" ref="GD5" si="42">GD6</f>
         <v>45467</v>
       </c>
-      <c r="GE5" s="160"/>
-      <c r="GF5" s="160"/>
-      <c r="GG5" s="160"/>
-      <c r="GH5" s="160"/>
-      <c r="GI5" s="160"/>
-      <c r="GJ5" s="161"/>
-      <c r="GK5" s="166">
+      <c r="GE5" s="157"/>
+      <c r="GF5" s="157"/>
+      <c r="GG5" s="157"/>
+      <c r="GH5" s="157"/>
+      <c r="GI5" s="157"/>
+      <c r="GJ5" s="163"/>
+      <c r="GK5" s="156">
         <f t="shared" ref="GK5" si="43">GK6</f>
         <v>45474</v>
       </c>
-      <c r="GL5" s="160"/>
-      <c r="GM5" s="160"/>
-      <c r="GN5" s="160"/>
-      <c r="GO5" s="160"/>
-      <c r="GP5" s="160"/>
-      <c r="GQ5" s="167"/>
-      <c r="GR5" s="159">
+      <c r="GL5" s="157"/>
+      <c r="GM5" s="157"/>
+      <c r="GN5" s="157"/>
+      <c r="GO5" s="157"/>
+      <c r="GP5" s="157"/>
+      <c r="GQ5" s="158"/>
+      <c r="GR5" s="162">
         <f t="shared" ref="GR5" si="44">GR6</f>
         <v>45481</v>
       </c>
-      <c r="GS5" s="160"/>
-      <c r="GT5" s="160"/>
-      <c r="GU5" s="160"/>
-      <c r="GV5" s="160"/>
-      <c r="GW5" s="160"/>
-      <c r="GX5" s="161"/>
-      <c r="GY5" s="166">
+      <c r="GS5" s="157"/>
+      <c r="GT5" s="157"/>
+      <c r="GU5" s="157"/>
+      <c r="GV5" s="157"/>
+      <c r="GW5" s="157"/>
+      <c r="GX5" s="163"/>
+      <c r="GY5" s="156">
         <f t="shared" ref="GY5" si="45">GY6</f>
         <v>45488</v>
       </c>
-      <c r="GZ5" s="160"/>
-      <c r="HA5" s="160"/>
-      <c r="HB5" s="160"/>
-      <c r="HC5" s="160"/>
-      <c r="HD5" s="160"/>
-      <c r="HE5" s="167"/>
-      <c r="HF5" s="159">
+      <c r="GZ5" s="157"/>
+      <c r="HA5" s="157"/>
+      <c r="HB5" s="157"/>
+      <c r="HC5" s="157"/>
+      <c r="HD5" s="157"/>
+      <c r="HE5" s="158"/>
+      <c r="HF5" s="162">
         <f t="shared" ref="HF5" si="46">HF6</f>
         <v>45495</v>
       </c>
-      <c r="HG5" s="160"/>
-      <c r="HH5" s="160"/>
-      <c r="HI5" s="160"/>
-      <c r="HJ5" s="160"/>
-      <c r="HK5" s="160"/>
-      <c r="HL5" s="161"/>
-      <c r="HM5" s="166">
+      <c r="HG5" s="157"/>
+      <c r="HH5" s="157"/>
+      <c r="HI5" s="157"/>
+      <c r="HJ5" s="157"/>
+      <c r="HK5" s="157"/>
+      <c r="HL5" s="163"/>
+      <c r="HM5" s="156">
         <f t="shared" ref="HM5" si="47">HM6</f>
         <v>45502</v>
       </c>
-      <c r="HN5" s="160"/>
-      <c r="HO5" s="160"/>
-      <c r="HP5" s="160"/>
-      <c r="HQ5" s="160"/>
-      <c r="HR5" s="160"/>
-      <c r="HS5" s="167"/>
-      <c r="HT5" s="159">
+      <c r="HN5" s="157"/>
+      <c r="HO5" s="157"/>
+      <c r="HP5" s="157"/>
+      <c r="HQ5" s="157"/>
+      <c r="HR5" s="157"/>
+      <c r="HS5" s="158"/>
+      <c r="HT5" s="162">
         <f t="shared" ref="HT5" si="48">HT6</f>
         <v>45509</v>
       </c>
-      <c r="HU5" s="160"/>
-      <c r="HV5" s="160"/>
-      <c r="HW5" s="160"/>
-      <c r="HX5" s="160"/>
-      <c r="HY5" s="160"/>
-      <c r="HZ5" s="161"/>
-      <c r="IA5" s="166">
+      <c r="HU5" s="157"/>
+      <c r="HV5" s="157"/>
+      <c r="HW5" s="157"/>
+      <c r="HX5" s="157"/>
+      <c r="HY5" s="157"/>
+      <c r="HZ5" s="163"/>
+      <c r="IA5" s="156">
         <f t="shared" ref="IA5" si="49">IA6</f>
         <v>45516</v>
       </c>
-      <c r="IB5" s="160"/>
-      <c r="IC5" s="160"/>
-      <c r="ID5" s="160"/>
-      <c r="IE5" s="160"/>
-      <c r="IF5" s="160"/>
-      <c r="IG5" s="167"/>
-      <c r="IH5" s="159">
+      <c r="IB5" s="157"/>
+      <c r="IC5" s="157"/>
+      <c r="ID5" s="157"/>
+      <c r="IE5" s="157"/>
+      <c r="IF5" s="157"/>
+      <c r="IG5" s="158"/>
+      <c r="IH5" s="162">
         <f t="shared" ref="IH5" si="50">IH6</f>
         <v>45523</v>
       </c>
-      <c r="II5" s="160"/>
-      <c r="IJ5" s="160"/>
-      <c r="IK5" s="160"/>
-      <c r="IL5" s="160"/>
-      <c r="IM5" s="160"/>
-      <c r="IN5" s="161"/>
-      <c r="IO5" s="166">
+      <c r="II5" s="157"/>
+      <c r="IJ5" s="157"/>
+      <c r="IK5" s="157"/>
+      <c r="IL5" s="157"/>
+      <c r="IM5" s="157"/>
+      <c r="IN5" s="163"/>
+      <c r="IO5" s="156">
         <f t="shared" ref="IO5" si="51">IO6</f>
         <v>45530</v>
       </c>
-      <c r="IP5" s="160"/>
-      <c r="IQ5" s="160"/>
-      <c r="IR5" s="160"/>
-      <c r="IS5" s="160"/>
-      <c r="IT5" s="160"/>
-      <c r="IU5" s="167"/>
+      <c r="IP5" s="157"/>
+      <c r="IQ5" s="157"/>
+      <c r="IR5" s="157"/>
+      <c r="IS5" s="157"/>
+      <c r="IT5" s="157"/>
+      <c r="IU5" s="158"/>
     </row>
     <row r="6" spans="1:255" s="53" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="146"/>
@@ -8715,7 +8715,7 @@
         <v>4</v>
       </c>
       <c r="H14" s="46">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="I14" s="102">
         <f t="shared" si="256"/>
@@ -8986,17 +8986,17 @@
       </c>
       <c r="F15" s="84">
         <f t="shared" ref="F15" si="262">IF(ISBLANK(E15)," - ",IF(G15=0,E15,E15+G15-1))</f>
-        <v>45316</v>
+        <v>45317</v>
       </c>
       <c r="G15" s="45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H15" s="46">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I15" s="102">
         <f t="shared" ref="I15" si="263">IF(OR(F15=0,E15=0),0,NETWORKDAYS(E15,F15))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J15" s="94"/>
       <c r="K15" s="34"/>
@@ -15777,20 +15777,49 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="73">
-    <mergeCell ref="IO5:IU5"/>
-    <mergeCell ref="IO4:IU4"/>
-    <mergeCell ref="HT4:HZ4"/>
-    <mergeCell ref="IA4:IG4"/>
-    <mergeCell ref="IH4:IN4"/>
-    <mergeCell ref="HM5:HS5"/>
-    <mergeCell ref="HT5:HZ5"/>
-    <mergeCell ref="IA5:IG5"/>
-    <mergeCell ref="IH5:IN5"/>
-    <mergeCell ref="GY4:HE4"/>
-    <mergeCell ref="HF4:HL4"/>
-    <mergeCell ref="GY5:HE5"/>
-    <mergeCell ref="HF5:HL5"/>
-    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="BH4:BN4"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="AM5:AS5"/>
+    <mergeCell ref="AT4:AZ4"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="BA4:BG4"/>
+    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="AD1:AR1"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="AF5:AL5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="FI4:FO4"/>
+    <mergeCell ref="FP4:FV4"/>
+    <mergeCell ref="EG4:EM4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="DS5:DY5"/>
+    <mergeCell ref="DZ5:EF5"/>
+    <mergeCell ref="EG5:EM5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DS4:DY4"/>
+    <mergeCell ref="DZ4:EF4"/>
     <mergeCell ref="FW4:GC4"/>
     <mergeCell ref="GD4:GJ4"/>
     <mergeCell ref="GK4:GQ4"/>
@@ -15807,49 +15836,20 @@
     <mergeCell ref="EN4:ET4"/>
     <mergeCell ref="EU4:FA4"/>
     <mergeCell ref="FB4:FH4"/>
-    <mergeCell ref="FI4:FO4"/>
-    <mergeCell ref="FP4:FV4"/>
-    <mergeCell ref="EG4:EM4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE5:DK5"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="DS5:DY5"/>
-    <mergeCell ref="DZ5:EF5"/>
-    <mergeCell ref="EG5:EM5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DS4:DY4"/>
-    <mergeCell ref="DZ4:EF4"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="AD1:AR1"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AF5:AL5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="HM5:HS5"/>
+    <mergeCell ref="HT5:HZ5"/>
+    <mergeCell ref="IA5:IG5"/>
+    <mergeCell ref="IH5:IN5"/>
+    <mergeCell ref="GY4:HE4"/>
+    <mergeCell ref="HF4:HL4"/>
+    <mergeCell ref="GY5:HE5"/>
+    <mergeCell ref="HF5:HL5"/>
+    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="IO5:IU5"/>
+    <mergeCell ref="IO4:IU4"/>
+    <mergeCell ref="HT4:HZ4"/>
+    <mergeCell ref="IA4:IG4"/>
+    <mergeCell ref="IH4:IN4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H36:H40 H8:H33">

</xml_diff>

<commit_message>
refactored for zettel besten
</commit_message>
<xml_diff>
--- a/thesis gantt chart.xlsx
+++ b/thesis gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wings_stuff\srus\TUD\yr5\thesis\thesis_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF7F3FA-AF89-45F9-8B2E-8C92B583D73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6EAB2A-60D2-40D4-8909-DAF9BB45D606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="3210" windowWidth="23235" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -2627,6 +2627,15 @@
     <xf numFmtId="0" fontId="28" fillId="35" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="59" fillId="23" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2639,28 +2648,7 @@
     <xf numFmtId="167" fontId="41" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="41" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="63" fillId="24" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -2697,6 +2685,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="41" fillId="23" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3295,8 +3295,8 @@
   <dimension ref="A1:IU62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <pane ySplit="7" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3375,21 +3375,21 @@
       <c r="K1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="208"/>
-      <c r="AE1" s="208"/>
-      <c r="AF1" s="208"/>
-      <c r="AG1" s="208"/>
-      <c r="AH1" s="208"/>
-      <c r="AI1" s="208"/>
-      <c r="AJ1" s="208"/>
-      <c r="AK1" s="208"/>
-      <c r="AL1" s="208"/>
-      <c r="AM1" s="208"/>
-      <c r="AN1" s="208"/>
-      <c r="AO1" s="208"/>
-      <c r="AP1" s="208"/>
-      <c r="AQ1" s="208"/>
-      <c r="AR1" s="208"/>
+      <c r="AD1" s="204"/>
+      <c r="AE1" s="204"/>
+      <c r="AF1" s="204"/>
+      <c r="AG1" s="204"/>
+      <c r="AH1" s="204"/>
+      <c r="AI1" s="204"/>
+      <c r="AJ1" s="204"/>
+      <c r="AK1" s="204"/>
+      <c r="AL1" s="204"/>
+      <c r="AM1" s="204"/>
+      <c r="AN1" s="204"/>
+      <c r="AO1" s="204"/>
+      <c r="AP1" s="204"/>
+      <c r="AQ1" s="204"/>
+      <c r="AR1" s="204"/>
     </row>
     <row r="2" spans="1:255" s="28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="72" t="s">
@@ -3469,729 +3469,729 @@
       <c r="B4" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="211">
+      <c r="C4" s="207">
         <v>45295</v>
       </c>
-      <c r="D4" s="212"/>
-      <c r="E4" s="213"/>
+      <c r="D4" s="208"/>
+      <c r="E4" s="209"/>
       <c r="H4" s="73" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="74">
         <v>9</v>
       </c>
-      <c r="K4" s="196"/>
-      <c r="L4" s="197"/>
-      <c r="M4" s="197"/>
-      <c r="N4" s="197"/>
-      <c r="O4" s="197"/>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="198"/>
-      <c r="R4" s="196" t="str">
+      <c r="K4" s="199"/>
+      <c r="L4" s="200"/>
+      <c r="M4" s="200"/>
+      <c r="N4" s="200"/>
+      <c r="O4" s="200"/>
+      <c r="P4" s="200"/>
+      <c r="Q4" s="201"/>
+      <c r="R4" s="199" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="S4" s="197"/>
-      <c r="T4" s="197"/>
-      <c r="U4" s="197"/>
-      <c r="V4" s="197"/>
-      <c r="W4" s="197"/>
-      <c r="X4" s="198"/>
-      <c r="Y4" s="196" t="str">
+      <c r="S4" s="200"/>
+      <c r="T4" s="200"/>
+      <c r="U4" s="200"/>
+      <c r="V4" s="200"/>
+      <c r="W4" s="200"/>
+      <c r="X4" s="201"/>
+      <c r="Y4" s="199" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="Z4" s="197"/>
-      <c r="AA4" s="197"/>
-      <c r="AB4" s="197"/>
-      <c r="AC4" s="197"/>
-      <c r="AD4" s="197"/>
-      <c r="AE4" s="198"/>
-      <c r="AF4" s="196" t="str">
+      <c r="Z4" s="200"/>
+      <c r="AA4" s="200"/>
+      <c r="AB4" s="200"/>
+      <c r="AC4" s="200"/>
+      <c r="AD4" s="200"/>
+      <c r="AE4" s="201"/>
+      <c r="AF4" s="199" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="AG4" s="197"/>
-      <c r="AH4" s="197"/>
-      <c r="AI4" s="197"/>
-      <c r="AJ4" s="197"/>
-      <c r="AK4" s="197"/>
-      <c r="AL4" s="198"/>
-      <c r="AM4" s="196" t="str">
+      <c r="AG4" s="200"/>
+      <c r="AH4" s="200"/>
+      <c r="AI4" s="200"/>
+      <c r="AJ4" s="200"/>
+      <c r="AK4" s="200"/>
+      <c r="AL4" s="201"/>
+      <c r="AM4" s="199" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="AN4" s="197"/>
-      <c r="AO4" s="197"/>
-      <c r="AP4" s="197"/>
-      <c r="AQ4" s="197"/>
-      <c r="AR4" s="197"/>
-      <c r="AS4" s="198"/>
-      <c r="AT4" s="196" t="str">
+      <c r="AN4" s="200"/>
+      <c r="AO4" s="200"/>
+      <c r="AP4" s="200"/>
+      <c r="AQ4" s="200"/>
+      <c r="AR4" s="200"/>
+      <c r="AS4" s="201"/>
+      <c r="AT4" s="199" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="AU4" s="197"/>
-      <c r="AV4" s="197"/>
-      <c r="AW4" s="197"/>
-      <c r="AX4" s="197"/>
-      <c r="AY4" s="197"/>
-      <c r="AZ4" s="198"/>
-      <c r="BA4" s="196" t="str">
+      <c r="AU4" s="200"/>
+      <c r="AV4" s="200"/>
+      <c r="AW4" s="200"/>
+      <c r="AX4" s="200"/>
+      <c r="AY4" s="200"/>
+      <c r="AZ4" s="201"/>
+      <c r="BA4" s="199" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="BB4" s="197"/>
-      <c r="BC4" s="197"/>
-      <c r="BD4" s="197"/>
-      <c r="BE4" s="197"/>
-      <c r="BF4" s="197"/>
-      <c r="BG4" s="198"/>
-      <c r="BH4" s="196" t="str">
+      <c r="BB4" s="200"/>
+      <c r="BC4" s="200"/>
+      <c r="BD4" s="200"/>
+      <c r="BE4" s="200"/>
+      <c r="BF4" s="200"/>
+      <c r="BG4" s="201"/>
+      <c r="BH4" s="199" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 15</v>
       </c>
-      <c r="BI4" s="197"/>
-      <c r="BJ4" s="197"/>
-      <c r="BK4" s="197"/>
-      <c r="BL4" s="197"/>
-      <c r="BM4" s="197"/>
-      <c r="BN4" s="198"/>
-      <c r="BO4" s="196" t="str">
+      <c r="BI4" s="200"/>
+      <c r="BJ4" s="200"/>
+      <c r="BK4" s="200"/>
+      <c r="BL4" s="200"/>
+      <c r="BM4" s="200"/>
+      <c r="BN4" s="201"/>
+      <c r="BO4" s="199" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 16</v>
       </c>
-      <c r="BP4" s="197"/>
-      <c r="BQ4" s="197"/>
-      <c r="BR4" s="197"/>
-      <c r="BS4" s="197"/>
-      <c r="BT4" s="197"/>
-      <c r="BU4" s="198"/>
-      <c r="BV4" s="196" t="str">
+      <c r="BP4" s="200"/>
+      <c r="BQ4" s="200"/>
+      <c r="BR4" s="200"/>
+      <c r="BS4" s="200"/>
+      <c r="BT4" s="200"/>
+      <c r="BU4" s="201"/>
+      <c r="BV4" s="199" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 17</v>
       </c>
-      <c r="BW4" s="197"/>
-      <c r="BX4" s="197"/>
-      <c r="BY4" s="197"/>
-      <c r="BZ4" s="197"/>
-      <c r="CA4" s="197"/>
-      <c r="CB4" s="198"/>
-      <c r="CC4" s="196" t="str">
+      <c r="BW4" s="200"/>
+      <c r="BX4" s="200"/>
+      <c r="BY4" s="200"/>
+      <c r="BZ4" s="200"/>
+      <c r="CA4" s="200"/>
+      <c r="CB4" s="201"/>
+      <c r="CC4" s="199" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 18</v>
       </c>
-      <c r="CD4" s="197"/>
-      <c r="CE4" s="197"/>
-      <c r="CF4" s="197"/>
-      <c r="CG4" s="197"/>
-      <c r="CH4" s="197"/>
-      <c r="CI4" s="198"/>
-      <c r="CJ4" s="196" t="str">
+      <c r="CD4" s="200"/>
+      <c r="CE4" s="200"/>
+      <c r="CF4" s="200"/>
+      <c r="CG4" s="200"/>
+      <c r="CH4" s="200"/>
+      <c r="CI4" s="201"/>
+      <c r="CJ4" s="199" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 19</v>
       </c>
-      <c r="CK4" s="197"/>
-      <c r="CL4" s="197"/>
-      <c r="CM4" s="197"/>
-      <c r="CN4" s="197"/>
-      <c r="CO4" s="197"/>
-      <c r="CP4" s="198"/>
-      <c r="CQ4" s="196" t="str">
+      <c r="CK4" s="200"/>
+      <c r="CL4" s="200"/>
+      <c r="CM4" s="200"/>
+      <c r="CN4" s="200"/>
+      <c r="CO4" s="200"/>
+      <c r="CP4" s="201"/>
+      <c r="CQ4" s="199" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="CR4" s="197"/>
-      <c r="CS4" s="197"/>
-      <c r="CT4" s="197"/>
-      <c r="CU4" s="197"/>
-      <c r="CV4" s="197"/>
-      <c r="CW4" s="198"/>
-      <c r="CX4" s="196" t="str">
+      <c r="CR4" s="200"/>
+      <c r="CS4" s="200"/>
+      <c r="CT4" s="200"/>
+      <c r="CU4" s="200"/>
+      <c r="CV4" s="200"/>
+      <c r="CW4" s="201"/>
+      <c r="CX4" s="199" t="str">
         <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="CY4" s="197"/>
-      <c r="CZ4" s="197"/>
-      <c r="DA4" s="197"/>
-      <c r="DB4" s="197"/>
-      <c r="DC4" s="197"/>
-      <c r="DD4" s="198"/>
-      <c r="DE4" s="196" t="str">
+      <c r="CY4" s="200"/>
+      <c r="CZ4" s="200"/>
+      <c r="DA4" s="200"/>
+      <c r="DB4" s="200"/>
+      <c r="DC4" s="200"/>
+      <c r="DD4" s="201"/>
+      <c r="DE4" s="199" t="str">
         <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="DF4" s="197"/>
-      <c r="DG4" s="197"/>
-      <c r="DH4" s="197"/>
-      <c r="DI4" s="197"/>
-      <c r="DJ4" s="197"/>
-      <c r="DK4" s="198"/>
-      <c r="DL4" s="196" t="str">
+      <c r="DF4" s="200"/>
+      <c r="DG4" s="200"/>
+      <c r="DH4" s="200"/>
+      <c r="DI4" s="200"/>
+      <c r="DJ4" s="200"/>
+      <c r="DK4" s="201"/>
+      <c r="DL4" s="199" t="str">
         <f>"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="DM4" s="197"/>
-      <c r="DN4" s="197"/>
-      <c r="DO4" s="197"/>
-      <c r="DP4" s="197"/>
-      <c r="DQ4" s="197"/>
-      <c r="DR4" s="198"/>
-      <c r="DS4" s="196" t="str">
+      <c r="DM4" s="200"/>
+      <c r="DN4" s="200"/>
+      <c r="DO4" s="200"/>
+      <c r="DP4" s="200"/>
+      <c r="DQ4" s="200"/>
+      <c r="DR4" s="201"/>
+      <c r="DS4" s="199" t="str">
         <f>"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="DT4" s="197"/>
-      <c r="DU4" s="197"/>
-      <c r="DV4" s="197"/>
-      <c r="DW4" s="197"/>
-      <c r="DX4" s="197"/>
-      <c r="DY4" s="198"/>
-      <c r="DZ4" s="196" t="str">
+      <c r="DT4" s="200"/>
+      <c r="DU4" s="200"/>
+      <c r="DV4" s="200"/>
+      <c r="DW4" s="200"/>
+      <c r="DX4" s="200"/>
+      <c r="DY4" s="201"/>
+      <c r="DZ4" s="199" t="str">
         <f>"Week "&amp;(DS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="EA4" s="197"/>
-      <c r="EB4" s="197"/>
-      <c r="EC4" s="197"/>
-      <c r="ED4" s="197"/>
-      <c r="EE4" s="197"/>
-      <c r="EF4" s="198"/>
-      <c r="EG4" s="196" t="str">
+      <c r="EA4" s="200"/>
+      <c r="EB4" s="200"/>
+      <c r="EC4" s="200"/>
+      <c r="ED4" s="200"/>
+      <c r="EE4" s="200"/>
+      <c r="EF4" s="201"/>
+      <c r="EG4" s="199" t="str">
         <f>"Week "&amp;(DZ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="EH4" s="197"/>
-      <c r="EI4" s="197"/>
-      <c r="EJ4" s="197"/>
-      <c r="EK4" s="197"/>
-      <c r="EL4" s="197"/>
-      <c r="EM4" s="198"/>
-      <c r="EN4" s="196" t="str">
+      <c r="EH4" s="200"/>
+      <c r="EI4" s="200"/>
+      <c r="EJ4" s="200"/>
+      <c r="EK4" s="200"/>
+      <c r="EL4" s="200"/>
+      <c r="EM4" s="201"/>
+      <c r="EN4" s="199" t="str">
         <f>"Week "&amp;(EG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="EO4" s="197"/>
-      <c r="EP4" s="197"/>
-      <c r="EQ4" s="197"/>
-      <c r="ER4" s="197"/>
-      <c r="ES4" s="197"/>
-      <c r="ET4" s="198"/>
-      <c r="EU4" s="196" t="str">
+      <c r="EO4" s="200"/>
+      <c r="EP4" s="200"/>
+      <c r="EQ4" s="200"/>
+      <c r="ER4" s="200"/>
+      <c r="ES4" s="200"/>
+      <c r="ET4" s="201"/>
+      <c r="EU4" s="199" t="str">
         <f>"Week "&amp;(EN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="EV4" s="197"/>
-      <c r="EW4" s="197"/>
-      <c r="EX4" s="197"/>
-      <c r="EY4" s="197"/>
-      <c r="EZ4" s="197"/>
-      <c r="FA4" s="198"/>
-      <c r="FB4" s="196" t="str">
+      <c r="EV4" s="200"/>
+      <c r="EW4" s="200"/>
+      <c r="EX4" s="200"/>
+      <c r="EY4" s="200"/>
+      <c r="EZ4" s="200"/>
+      <c r="FA4" s="201"/>
+      <c r="FB4" s="199" t="str">
         <f>"Week "&amp;(EU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="FC4" s="197"/>
-      <c r="FD4" s="197"/>
-      <c r="FE4" s="197"/>
-      <c r="FF4" s="197"/>
-      <c r="FG4" s="197"/>
-      <c r="FH4" s="198"/>
-      <c r="FI4" s="196" t="str">
+      <c r="FC4" s="200"/>
+      <c r="FD4" s="200"/>
+      <c r="FE4" s="200"/>
+      <c r="FF4" s="200"/>
+      <c r="FG4" s="200"/>
+      <c r="FH4" s="201"/>
+      <c r="FI4" s="199" t="str">
         <f>"Week "&amp;(FB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="FJ4" s="197"/>
-      <c r="FK4" s="197"/>
-      <c r="FL4" s="197"/>
-      <c r="FM4" s="197"/>
-      <c r="FN4" s="197"/>
-      <c r="FO4" s="198"/>
-      <c r="FP4" s="196" t="str">
+      <c r="FJ4" s="200"/>
+      <c r="FK4" s="200"/>
+      <c r="FL4" s="200"/>
+      <c r="FM4" s="200"/>
+      <c r="FN4" s="200"/>
+      <c r="FO4" s="201"/>
+      <c r="FP4" s="199" t="str">
         <f>"Week "&amp;(FI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="FQ4" s="197"/>
-      <c r="FR4" s="197"/>
-      <c r="FS4" s="197"/>
-      <c r="FT4" s="197"/>
-      <c r="FU4" s="197"/>
-      <c r="FV4" s="198"/>
-      <c r="FW4" s="196" t="str">
+      <c r="FQ4" s="200"/>
+      <c r="FR4" s="200"/>
+      <c r="FS4" s="200"/>
+      <c r="FT4" s="200"/>
+      <c r="FU4" s="200"/>
+      <c r="FV4" s="201"/>
+      <c r="FW4" s="199" t="str">
         <f>"Week "&amp;(FP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="FX4" s="197"/>
-      <c r="FY4" s="197"/>
-      <c r="FZ4" s="197"/>
-      <c r="GA4" s="197"/>
-      <c r="GB4" s="197"/>
-      <c r="GC4" s="198"/>
-      <c r="GD4" s="196" t="str">
+      <c r="FX4" s="200"/>
+      <c r="FY4" s="200"/>
+      <c r="FZ4" s="200"/>
+      <c r="GA4" s="200"/>
+      <c r="GB4" s="200"/>
+      <c r="GC4" s="201"/>
+      <c r="GD4" s="199" t="str">
         <f>"Week "&amp;(FW6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 33</v>
       </c>
-      <c r="GE4" s="197"/>
-      <c r="GF4" s="197"/>
-      <c r="GG4" s="197"/>
-      <c r="GH4" s="197"/>
-      <c r="GI4" s="197"/>
-      <c r="GJ4" s="198"/>
-      <c r="GK4" s="196" t="str">
+      <c r="GE4" s="200"/>
+      <c r="GF4" s="200"/>
+      <c r="GG4" s="200"/>
+      <c r="GH4" s="200"/>
+      <c r="GI4" s="200"/>
+      <c r="GJ4" s="201"/>
+      <c r="GK4" s="199" t="str">
         <f>"Week "&amp;(GD6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 34</v>
       </c>
-      <c r="GL4" s="197"/>
-      <c r="GM4" s="197"/>
-      <c r="GN4" s="197"/>
-      <c r="GO4" s="197"/>
-      <c r="GP4" s="197"/>
-      <c r="GQ4" s="198"/>
-      <c r="GR4" s="196" t="str">
+      <c r="GL4" s="200"/>
+      <c r="GM4" s="200"/>
+      <c r="GN4" s="200"/>
+      <c r="GO4" s="200"/>
+      <c r="GP4" s="200"/>
+      <c r="GQ4" s="201"/>
+      <c r="GR4" s="199" t="str">
         <f>"Week "&amp;(GK6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 35</v>
       </c>
-      <c r="GS4" s="197"/>
-      <c r="GT4" s="197"/>
-      <c r="GU4" s="197"/>
-      <c r="GV4" s="197"/>
-      <c r="GW4" s="197"/>
-      <c r="GX4" s="198"/>
-      <c r="GY4" s="196" t="str">
+      <c r="GS4" s="200"/>
+      <c r="GT4" s="200"/>
+      <c r="GU4" s="200"/>
+      <c r="GV4" s="200"/>
+      <c r="GW4" s="200"/>
+      <c r="GX4" s="201"/>
+      <c r="GY4" s="199" t="str">
         <f>"Week "&amp;(GR6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 36</v>
       </c>
-      <c r="GZ4" s="197"/>
-      <c r="HA4" s="197"/>
-      <c r="HB4" s="197"/>
-      <c r="HC4" s="197"/>
-      <c r="HD4" s="197"/>
-      <c r="HE4" s="198"/>
-      <c r="HF4" s="196" t="str">
+      <c r="GZ4" s="200"/>
+      <c r="HA4" s="200"/>
+      <c r="HB4" s="200"/>
+      <c r="HC4" s="200"/>
+      <c r="HD4" s="200"/>
+      <c r="HE4" s="201"/>
+      <c r="HF4" s="199" t="str">
         <f>"Week "&amp;(GY6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 37</v>
       </c>
-      <c r="HG4" s="197"/>
-      <c r="HH4" s="197"/>
-      <c r="HI4" s="197"/>
-      <c r="HJ4" s="197"/>
-      <c r="HK4" s="197"/>
-      <c r="HL4" s="198"/>
-      <c r="HM4" s="196" t="str">
+      <c r="HG4" s="200"/>
+      <c r="HH4" s="200"/>
+      <c r="HI4" s="200"/>
+      <c r="HJ4" s="200"/>
+      <c r="HK4" s="200"/>
+      <c r="HL4" s="201"/>
+      <c r="HM4" s="199" t="str">
         <f>"Week "&amp;(HF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 38</v>
       </c>
-      <c r="HN4" s="197"/>
-      <c r="HO4" s="197"/>
-      <c r="HP4" s="197"/>
-      <c r="HQ4" s="197"/>
-      <c r="HR4" s="197"/>
-      <c r="HS4" s="198"/>
-      <c r="HT4" s="196" t="str">
+      <c r="HN4" s="200"/>
+      <c r="HO4" s="200"/>
+      <c r="HP4" s="200"/>
+      <c r="HQ4" s="200"/>
+      <c r="HR4" s="200"/>
+      <c r="HS4" s="201"/>
+      <c r="HT4" s="199" t="str">
         <f>"Week "&amp;(HM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 39</v>
       </c>
-      <c r="HU4" s="197"/>
-      <c r="HV4" s="197"/>
-      <c r="HW4" s="197"/>
-      <c r="HX4" s="197"/>
-      <c r="HY4" s="197"/>
-      <c r="HZ4" s="198"/>
-      <c r="IA4" s="196" t="str">
+      <c r="HU4" s="200"/>
+      <c r="HV4" s="200"/>
+      <c r="HW4" s="200"/>
+      <c r="HX4" s="200"/>
+      <c r="HY4" s="200"/>
+      <c r="HZ4" s="201"/>
+      <c r="IA4" s="199" t="str">
         <f>"Week "&amp;(HT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 40</v>
       </c>
-      <c r="IB4" s="197"/>
-      <c r="IC4" s="197"/>
-      <c r="ID4" s="197"/>
-      <c r="IE4" s="197"/>
-      <c r="IF4" s="197"/>
-      <c r="IG4" s="198"/>
-      <c r="IH4" s="196" t="str">
+      <c r="IB4" s="200"/>
+      <c r="IC4" s="200"/>
+      <c r="ID4" s="200"/>
+      <c r="IE4" s="200"/>
+      <c r="IF4" s="200"/>
+      <c r="IG4" s="201"/>
+      <c r="IH4" s="199" t="str">
         <f>"Week "&amp;(IA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 41</v>
       </c>
-      <c r="II4" s="197"/>
-      <c r="IJ4" s="197"/>
-      <c r="IK4" s="197"/>
-      <c r="IL4" s="197"/>
-      <c r="IM4" s="197"/>
-      <c r="IN4" s="198"/>
-      <c r="IO4" s="196" t="str">
+      <c r="II4" s="200"/>
+      <c r="IJ4" s="200"/>
+      <c r="IK4" s="200"/>
+      <c r="IL4" s="200"/>
+      <c r="IM4" s="200"/>
+      <c r="IN4" s="201"/>
+      <c r="IO4" s="199" t="str">
         <f>"Week "&amp;(IH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 42</v>
       </c>
-      <c r="IP4" s="197"/>
-      <c r="IQ4" s="197"/>
-      <c r="IR4" s="197"/>
-      <c r="IS4" s="197"/>
-      <c r="IT4" s="197"/>
-      <c r="IU4" s="198"/>
+      <c r="IP4" s="200"/>
+      <c r="IQ4" s="200"/>
+      <c r="IR4" s="200"/>
+      <c r="IS4" s="200"/>
+      <c r="IT4" s="200"/>
+      <c r="IU4" s="201"/>
     </row>
     <row r="5" spans="1:255" s="24" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
       <c r="B5" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="211" t="s">
+      <c r="C5" s="207" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="212"/>
-      <c r="E5" s="213"/>
+      <c r="D5" s="208"/>
+      <c r="E5" s="209"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
       <c r="H5" s="71"/>
       <c r="I5" s="71"/>
-      <c r="K5" s="214">
+      <c r="K5" s="210">
         <f>K6</f>
         <v>45348</v>
       </c>
-      <c r="L5" s="200"/>
-      <c r="M5" s="200"/>
-      <c r="N5" s="200"/>
-      <c r="O5" s="200"/>
-      <c r="P5" s="200"/>
-      <c r="Q5" s="216"/>
-      <c r="R5" s="214">
+      <c r="L5" s="197"/>
+      <c r="M5" s="197"/>
+      <c r="N5" s="197"/>
+      <c r="O5" s="197"/>
+      <c r="P5" s="197"/>
+      <c r="Q5" s="212"/>
+      <c r="R5" s="210">
         <f>R6</f>
         <v>45355</v>
       </c>
-      <c r="S5" s="200"/>
-      <c r="T5" s="200"/>
-      <c r="U5" s="200"/>
-      <c r="V5" s="200"/>
-      <c r="W5" s="200"/>
-      <c r="X5" s="215"/>
-      <c r="Y5" s="217">
+      <c r="S5" s="197"/>
+      <c r="T5" s="197"/>
+      <c r="U5" s="197"/>
+      <c r="V5" s="197"/>
+      <c r="W5" s="197"/>
+      <c r="X5" s="211"/>
+      <c r="Y5" s="213">
         <f>Y6</f>
         <v>45362</v>
       </c>
-      <c r="Z5" s="200"/>
-      <c r="AA5" s="200"/>
-      <c r="AB5" s="200"/>
-      <c r="AC5" s="200"/>
-      <c r="AD5" s="200"/>
-      <c r="AE5" s="218"/>
-      <c r="AF5" s="209">
+      <c r="Z5" s="197"/>
+      <c r="AA5" s="197"/>
+      <c r="AB5" s="197"/>
+      <c r="AC5" s="197"/>
+      <c r="AD5" s="197"/>
+      <c r="AE5" s="214"/>
+      <c r="AF5" s="205">
         <f>AF6</f>
         <v>45369</v>
       </c>
-      <c r="AG5" s="200"/>
-      <c r="AH5" s="200"/>
-      <c r="AI5" s="200"/>
-      <c r="AJ5" s="200"/>
-      <c r="AK5" s="200"/>
-      <c r="AL5" s="210"/>
-      <c r="AM5" s="202">
+      <c r="AG5" s="197"/>
+      <c r="AH5" s="197"/>
+      <c r="AI5" s="197"/>
+      <c r="AJ5" s="197"/>
+      <c r="AK5" s="197"/>
+      <c r="AL5" s="206"/>
+      <c r="AM5" s="215">
         <f>AM6</f>
         <v>45376</v>
       </c>
-      <c r="AN5" s="200"/>
-      <c r="AO5" s="200"/>
-      <c r="AP5" s="200"/>
-      <c r="AQ5" s="200"/>
-      <c r="AR5" s="200"/>
-      <c r="AS5" s="203"/>
-      <c r="AT5" s="204">
+      <c r="AN5" s="197"/>
+      <c r="AO5" s="197"/>
+      <c r="AP5" s="197"/>
+      <c r="AQ5" s="197"/>
+      <c r="AR5" s="197"/>
+      <c r="AS5" s="216"/>
+      <c r="AT5" s="217">
         <f>AT6</f>
         <v>45383</v>
       </c>
-      <c r="AU5" s="200"/>
-      <c r="AV5" s="200"/>
-      <c r="AW5" s="200"/>
-      <c r="AX5" s="200"/>
-      <c r="AY5" s="200"/>
-      <c r="AZ5" s="205"/>
-      <c r="BA5" s="206">
+      <c r="AU5" s="197"/>
+      <c r="AV5" s="197"/>
+      <c r="AW5" s="197"/>
+      <c r="AX5" s="197"/>
+      <c r="AY5" s="197"/>
+      <c r="AZ5" s="218"/>
+      <c r="BA5" s="196">
         <f>BA6</f>
         <v>45390</v>
       </c>
-      <c r="BB5" s="200"/>
-      <c r="BC5" s="200"/>
-      <c r="BD5" s="200"/>
-      <c r="BE5" s="200"/>
-      <c r="BF5" s="200"/>
-      <c r="BG5" s="207"/>
-      <c r="BH5" s="199">
+      <c r="BB5" s="197"/>
+      <c r="BC5" s="197"/>
+      <c r="BD5" s="197"/>
+      <c r="BE5" s="197"/>
+      <c r="BF5" s="197"/>
+      <c r="BG5" s="198"/>
+      <c r="BH5" s="202">
         <f>BH6</f>
         <v>45397</v>
       </c>
-      <c r="BI5" s="200"/>
-      <c r="BJ5" s="200"/>
-      <c r="BK5" s="200"/>
-      <c r="BL5" s="200"/>
-      <c r="BM5" s="200"/>
-      <c r="BN5" s="201"/>
-      <c r="BO5" s="206">
+      <c r="BI5" s="197"/>
+      <c r="BJ5" s="197"/>
+      <c r="BK5" s="197"/>
+      <c r="BL5" s="197"/>
+      <c r="BM5" s="197"/>
+      <c r="BN5" s="203"/>
+      <c r="BO5" s="196">
         <f>BO6</f>
         <v>45404</v>
       </c>
-      <c r="BP5" s="200"/>
-      <c r="BQ5" s="200"/>
-      <c r="BR5" s="200"/>
-      <c r="BS5" s="200"/>
-      <c r="BT5" s="200"/>
-      <c r="BU5" s="207"/>
-      <c r="BV5" s="199">
+      <c r="BP5" s="197"/>
+      <c r="BQ5" s="197"/>
+      <c r="BR5" s="197"/>
+      <c r="BS5" s="197"/>
+      <c r="BT5" s="197"/>
+      <c r="BU5" s="198"/>
+      <c r="BV5" s="202">
         <f>BV6</f>
         <v>45411</v>
       </c>
-      <c r="BW5" s="200"/>
-      <c r="BX5" s="200"/>
-      <c r="BY5" s="200"/>
-      <c r="BZ5" s="200"/>
-      <c r="CA5" s="200"/>
-      <c r="CB5" s="201"/>
-      <c r="CC5" s="199">
+      <c r="BW5" s="197"/>
+      <c r="BX5" s="197"/>
+      <c r="BY5" s="197"/>
+      <c r="BZ5" s="197"/>
+      <c r="CA5" s="197"/>
+      <c r="CB5" s="203"/>
+      <c r="CC5" s="202">
         <f>CC6</f>
         <v>45418</v>
       </c>
-      <c r="CD5" s="200"/>
-      <c r="CE5" s="200"/>
-      <c r="CF5" s="200"/>
-      <c r="CG5" s="200"/>
-      <c r="CH5" s="200"/>
-      <c r="CI5" s="201"/>
-      <c r="CJ5" s="206">
+      <c r="CD5" s="197"/>
+      <c r="CE5" s="197"/>
+      <c r="CF5" s="197"/>
+      <c r="CG5" s="197"/>
+      <c r="CH5" s="197"/>
+      <c r="CI5" s="203"/>
+      <c r="CJ5" s="196">
         <f>CJ6</f>
         <v>45425</v>
       </c>
-      <c r="CK5" s="200"/>
-      <c r="CL5" s="200"/>
-      <c r="CM5" s="200"/>
-      <c r="CN5" s="200"/>
-      <c r="CO5" s="200"/>
-      <c r="CP5" s="207"/>
-      <c r="CQ5" s="199">
+      <c r="CK5" s="197"/>
+      <c r="CL5" s="197"/>
+      <c r="CM5" s="197"/>
+      <c r="CN5" s="197"/>
+      <c r="CO5" s="197"/>
+      <c r="CP5" s="198"/>
+      <c r="CQ5" s="202">
         <f>CQ6</f>
         <v>45432</v>
       </c>
-      <c r="CR5" s="200"/>
-      <c r="CS5" s="200"/>
-      <c r="CT5" s="200"/>
-      <c r="CU5" s="200"/>
-      <c r="CV5" s="200"/>
-      <c r="CW5" s="201"/>
-      <c r="CX5" s="199">
+      <c r="CR5" s="197"/>
+      <c r="CS5" s="197"/>
+      <c r="CT5" s="197"/>
+      <c r="CU5" s="197"/>
+      <c r="CV5" s="197"/>
+      <c r="CW5" s="203"/>
+      <c r="CX5" s="202">
         <f>CX6</f>
         <v>45439</v>
       </c>
-      <c r="CY5" s="200"/>
-      <c r="CZ5" s="200"/>
-      <c r="DA5" s="200"/>
-      <c r="DB5" s="200"/>
-      <c r="DC5" s="200"/>
-      <c r="DD5" s="201"/>
-      <c r="DE5" s="206">
+      <c r="CY5" s="197"/>
+      <c r="CZ5" s="197"/>
+      <c r="DA5" s="197"/>
+      <c r="DB5" s="197"/>
+      <c r="DC5" s="197"/>
+      <c r="DD5" s="203"/>
+      <c r="DE5" s="196">
         <f>DE6</f>
         <v>45446</v>
       </c>
-      <c r="DF5" s="200"/>
-      <c r="DG5" s="200"/>
-      <c r="DH5" s="200"/>
-      <c r="DI5" s="200"/>
-      <c r="DJ5" s="200"/>
-      <c r="DK5" s="207"/>
-      <c r="DL5" s="199">
+      <c r="DF5" s="197"/>
+      <c r="DG5" s="197"/>
+      <c r="DH5" s="197"/>
+      <c r="DI5" s="197"/>
+      <c r="DJ5" s="197"/>
+      <c r="DK5" s="198"/>
+      <c r="DL5" s="202">
         <f>DL6</f>
         <v>45453</v>
       </c>
-      <c r="DM5" s="200"/>
-      <c r="DN5" s="200"/>
-      <c r="DO5" s="200"/>
-      <c r="DP5" s="200"/>
-      <c r="DQ5" s="200"/>
-      <c r="DR5" s="201"/>
-      <c r="DS5" s="199">
+      <c r="DM5" s="197"/>
+      <c r="DN5" s="197"/>
+      <c r="DO5" s="197"/>
+      <c r="DP5" s="197"/>
+      <c r="DQ5" s="197"/>
+      <c r="DR5" s="203"/>
+      <c r="DS5" s="202">
         <f>DS6</f>
         <v>45460</v>
       </c>
-      <c r="DT5" s="200"/>
-      <c r="DU5" s="200"/>
-      <c r="DV5" s="200"/>
-      <c r="DW5" s="200"/>
-      <c r="DX5" s="200"/>
-      <c r="DY5" s="201"/>
-      <c r="DZ5" s="206">
+      <c r="DT5" s="197"/>
+      <c r="DU5" s="197"/>
+      <c r="DV5" s="197"/>
+      <c r="DW5" s="197"/>
+      <c r="DX5" s="197"/>
+      <c r="DY5" s="203"/>
+      <c r="DZ5" s="196">
         <f>DZ6</f>
         <v>45467</v>
       </c>
-      <c r="EA5" s="200"/>
-      <c r="EB5" s="200"/>
-      <c r="EC5" s="200"/>
-      <c r="ED5" s="200"/>
-      <c r="EE5" s="200"/>
-      <c r="EF5" s="207"/>
-      <c r="EG5" s="199">
+      <c r="EA5" s="197"/>
+      <c r="EB5" s="197"/>
+      <c r="EC5" s="197"/>
+      <c r="ED5" s="197"/>
+      <c r="EE5" s="197"/>
+      <c r="EF5" s="198"/>
+      <c r="EG5" s="202">
         <f>EG6</f>
         <v>45474</v>
       </c>
-      <c r="EH5" s="200"/>
-      <c r="EI5" s="200"/>
-      <c r="EJ5" s="200"/>
-      <c r="EK5" s="200"/>
-      <c r="EL5" s="200"/>
-      <c r="EM5" s="201"/>
-      <c r="EN5" s="199">
+      <c r="EH5" s="197"/>
+      <c r="EI5" s="197"/>
+      <c r="EJ5" s="197"/>
+      <c r="EK5" s="197"/>
+      <c r="EL5" s="197"/>
+      <c r="EM5" s="203"/>
+      <c r="EN5" s="202">
         <f>EN6</f>
         <v>45481</v>
       </c>
-      <c r="EO5" s="200"/>
-      <c r="EP5" s="200"/>
-      <c r="EQ5" s="200"/>
-      <c r="ER5" s="200"/>
-      <c r="ES5" s="200"/>
-      <c r="ET5" s="201"/>
-      <c r="EU5" s="206">
+      <c r="EO5" s="197"/>
+      <c r="EP5" s="197"/>
+      <c r="EQ5" s="197"/>
+      <c r="ER5" s="197"/>
+      <c r="ES5" s="197"/>
+      <c r="ET5" s="203"/>
+      <c r="EU5" s="196">
         <f>EU6</f>
         <v>45488</v>
       </c>
-      <c r="EV5" s="200"/>
-      <c r="EW5" s="200"/>
-      <c r="EX5" s="200"/>
-      <c r="EY5" s="200"/>
-      <c r="EZ5" s="200"/>
-      <c r="FA5" s="207"/>
-      <c r="FB5" s="199">
+      <c r="EV5" s="197"/>
+      <c r="EW5" s="197"/>
+      <c r="EX5" s="197"/>
+      <c r="EY5" s="197"/>
+      <c r="EZ5" s="197"/>
+      <c r="FA5" s="198"/>
+      <c r="FB5" s="202">
         <f>FB6</f>
         <v>45495</v>
       </c>
-      <c r="FC5" s="200"/>
-      <c r="FD5" s="200"/>
-      <c r="FE5" s="200"/>
-      <c r="FF5" s="200"/>
-      <c r="FG5" s="200"/>
-      <c r="FH5" s="201"/>
-      <c r="FI5" s="199">
+      <c r="FC5" s="197"/>
+      <c r="FD5" s="197"/>
+      <c r="FE5" s="197"/>
+      <c r="FF5" s="197"/>
+      <c r="FG5" s="197"/>
+      <c r="FH5" s="203"/>
+      <c r="FI5" s="202">
         <f>FI6</f>
         <v>45502</v>
       </c>
-      <c r="FJ5" s="200"/>
-      <c r="FK5" s="200"/>
-      <c r="FL5" s="200"/>
-      <c r="FM5" s="200"/>
-      <c r="FN5" s="200"/>
-      <c r="FO5" s="201"/>
-      <c r="FP5" s="206">
+      <c r="FJ5" s="197"/>
+      <c r="FK5" s="197"/>
+      <c r="FL5" s="197"/>
+      <c r="FM5" s="197"/>
+      <c r="FN5" s="197"/>
+      <c r="FO5" s="203"/>
+      <c r="FP5" s="196">
         <f>FP6</f>
         <v>45509</v>
       </c>
-      <c r="FQ5" s="200"/>
-      <c r="FR5" s="200"/>
-      <c r="FS5" s="200"/>
-      <c r="FT5" s="200"/>
-      <c r="FU5" s="200"/>
-      <c r="FV5" s="207"/>
-      <c r="FW5" s="199">
+      <c r="FQ5" s="197"/>
+      <c r="FR5" s="197"/>
+      <c r="FS5" s="197"/>
+      <c r="FT5" s="197"/>
+      <c r="FU5" s="197"/>
+      <c r="FV5" s="198"/>
+      <c r="FW5" s="202">
         <f>FW6</f>
         <v>45516</v>
       </c>
-      <c r="FX5" s="200"/>
-      <c r="FY5" s="200"/>
-      <c r="FZ5" s="200"/>
-      <c r="GA5" s="200"/>
-      <c r="GB5" s="200"/>
-      <c r="GC5" s="201"/>
-      <c r="GD5" s="199">
+      <c r="FX5" s="197"/>
+      <c r="FY5" s="197"/>
+      <c r="FZ5" s="197"/>
+      <c r="GA5" s="197"/>
+      <c r="GB5" s="197"/>
+      <c r="GC5" s="203"/>
+      <c r="GD5" s="202">
         <f>GD6</f>
         <v>45523</v>
       </c>
-      <c r="GE5" s="200"/>
-      <c r="GF5" s="200"/>
-      <c r="GG5" s="200"/>
-      <c r="GH5" s="200"/>
-      <c r="GI5" s="200"/>
-      <c r="GJ5" s="201"/>
-      <c r="GK5" s="206">
+      <c r="GE5" s="197"/>
+      <c r="GF5" s="197"/>
+      <c r="GG5" s="197"/>
+      <c r="GH5" s="197"/>
+      <c r="GI5" s="197"/>
+      <c r="GJ5" s="203"/>
+      <c r="GK5" s="196">
         <f>GK6</f>
         <v>45530</v>
       </c>
-      <c r="GL5" s="200"/>
-      <c r="GM5" s="200"/>
-      <c r="GN5" s="200"/>
-      <c r="GO5" s="200"/>
-      <c r="GP5" s="200"/>
-      <c r="GQ5" s="207"/>
-      <c r="GR5" s="199">
+      <c r="GL5" s="197"/>
+      <c r="GM5" s="197"/>
+      <c r="GN5" s="197"/>
+      <c r="GO5" s="197"/>
+      <c r="GP5" s="197"/>
+      <c r="GQ5" s="198"/>
+      <c r="GR5" s="202">
         <f>GR6</f>
         <v>45537</v>
       </c>
-      <c r="GS5" s="200"/>
-      <c r="GT5" s="200"/>
-      <c r="GU5" s="200"/>
-      <c r="GV5" s="200"/>
-      <c r="GW5" s="200"/>
-      <c r="GX5" s="201"/>
-      <c r="GY5" s="206">
+      <c r="GS5" s="197"/>
+      <c r="GT5" s="197"/>
+      <c r="GU5" s="197"/>
+      <c r="GV5" s="197"/>
+      <c r="GW5" s="197"/>
+      <c r="GX5" s="203"/>
+      <c r="GY5" s="196">
         <f>GY6</f>
         <v>45544</v>
       </c>
-      <c r="GZ5" s="200"/>
-      <c r="HA5" s="200"/>
-      <c r="HB5" s="200"/>
-      <c r="HC5" s="200"/>
-      <c r="HD5" s="200"/>
-      <c r="HE5" s="207"/>
-      <c r="HF5" s="199">
+      <c r="GZ5" s="197"/>
+      <c r="HA5" s="197"/>
+      <c r="HB5" s="197"/>
+      <c r="HC5" s="197"/>
+      <c r="HD5" s="197"/>
+      <c r="HE5" s="198"/>
+      <c r="HF5" s="202">
         <f>HF6</f>
         <v>45551</v>
       </c>
-      <c r="HG5" s="200"/>
-      <c r="HH5" s="200"/>
-      <c r="HI5" s="200"/>
-      <c r="HJ5" s="200"/>
-      <c r="HK5" s="200"/>
-      <c r="HL5" s="201"/>
-      <c r="HM5" s="206">
+      <c r="HG5" s="197"/>
+      <c r="HH5" s="197"/>
+      <c r="HI5" s="197"/>
+      <c r="HJ5" s="197"/>
+      <c r="HK5" s="197"/>
+      <c r="HL5" s="203"/>
+      <c r="HM5" s="196">
         <f>HM6</f>
         <v>45558</v>
       </c>
-      <c r="HN5" s="200"/>
-      <c r="HO5" s="200"/>
-      <c r="HP5" s="200"/>
-      <c r="HQ5" s="200"/>
-      <c r="HR5" s="200"/>
-      <c r="HS5" s="207"/>
-      <c r="HT5" s="199">
+      <c r="HN5" s="197"/>
+      <c r="HO5" s="197"/>
+      <c r="HP5" s="197"/>
+      <c r="HQ5" s="197"/>
+      <c r="HR5" s="197"/>
+      <c r="HS5" s="198"/>
+      <c r="HT5" s="202">
         <f>HT6</f>
         <v>45565</v>
       </c>
-      <c r="HU5" s="200"/>
-      <c r="HV5" s="200"/>
-      <c r="HW5" s="200"/>
-      <c r="HX5" s="200"/>
-      <c r="HY5" s="200"/>
-      <c r="HZ5" s="201"/>
-      <c r="IA5" s="206">
+      <c r="HU5" s="197"/>
+      <c r="HV5" s="197"/>
+      <c r="HW5" s="197"/>
+      <c r="HX5" s="197"/>
+      <c r="HY5" s="197"/>
+      <c r="HZ5" s="203"/>
+      <c r="IA5" s="196">
         <f>IA6</f>
         <v>45572</v>
       </c>
-      <c r="IB5" s="200"/>
-      <c r="IC5" s="200"/>
-      <c r="ID5" s="200"/>
-      <c r="IE5" s="200"/>
-      <c r="IF5" s="200"/>
-      <c r="IG5" s="207"/>
-      <c r="IH5" s="199">
+      <c r="IB5" s="197"/>
+      <c r="IC5" s="197"/>
+      <c r="ID5" s="197"/>
+      <c r="IE5" s="197"/>
+      <c r="IF5" s="197"/>
+      <c r="IG5" s="198"/>
+      <c r="IH5" s="202">
         <f>IH6</f>
         <v>45579</v>
       </c>
-      <c r="II5" s="200"/>
-      <c r="IJ5" s="200"/>
-      <c r="IK5" s="200"/>
-      <c r="IL5" s="200"/>
-      <c r="IM5" s="200"/>
-      <c r="IN5" s="201"/>
-      <c r="IO5" s="206">
+      <c r="II5" s="197"/>
+      <c r="IJ5" s="197"/>
+      <c r="IK5" s="197"/>
+      <c r="IL5" s="197"/>
+      <c r="IM5" s="197"/>
+      <c r="IN5" s="203"/>
+      <c r="IO5" s="196">
         <f>IO6</f>
         <v>45586</v>
       </c>
-      <c r="IP5" s="200"/>
-      <c r="IQ5" s="200"/>
-      <c r="IR5" s="200"/>
-      <c r="IS5" s="200"/>
-      <c r="IT5" s="200"/>
-      <c r="IU5" s="207"/>
+      <c r="IP5" s="197"/>
+      <c r="IQ5" s="197"/>
+      <c r="IR5" s="197"/>
+      <c r="IS5" s="197"/>
+      <c r="IT5" s="197"/>
+      <c r="IU5" s="198"/>
     </row>
     <row r="6" spans="1:255" s="22" customFormat="1" ht="7.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="84"/>
@@ -8366,7 +8366,7 @@
       <c r="IT15" s="152"/>
       <c r="IU15" s="152"/>
     </row>
-    <row r="16" spans="1:255" s="153" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.6</v>
@@ -11647,7 +11647,7 @@
       <c r="IT27" s="104"/>
       <c r="IU27" s="104"/>
     </row>
-    <row r="28" spans="1:255" s="105" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="95">
         <v>2.5</v>
       </c>
@@ -12475,7 +12475,7 @@
       <c r="IT30" s="104"/>
       <c r="IU30" s="104"/>
     </row>
-    <row r="31" spans="1:255" s="105" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="95">
         <v>2.8</v>
       </c>
@@ -20093,20 +20093,49 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="73">
-    <mergeCell ref="IO5:IU5"/>
-    <mergeCell ref="IO4:IU4"/>
-    <mergeCell ref="HT4:HZ4"/>
-    <mergeCell ref="IA4:IG4"/>
-    <mergeCell ref="IH4:IN4"/>
-    <mergeCell ref="HM5:HS5"/>
-    <mergeCell ref="HT5:HZ5"/>
-    <mergeCell ref="IA5:IG5"/>
-    <mergeCell ref="IH5:IN5"/>
-    <mergeCell ref="GY4:HE4"/>
-    <mergeCell ref="HF4:HL4"/>
-    <mergeCell ref="GY5:HE5"/>
-    <mergeCell ref="HF5:HL5"/>
-    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="BH4:BN4"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="AM5:AS5"/>
+    <mergeCell ref="AT4:AZ4"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="BA4:BG4"/>
+    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="AD1:AR1"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="AF5:AL5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="FI4:FO4"/>
+    <mergeCell ref="FP4:FV4"/>
+    <mergeCell ref="EG4:EM4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="DS5:DY5"/>
+    <mergeCell ref="DZ5:EF5"/>
+    <mergeCell ref="EG5:EM5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DS4:DY4"/>
+    <mergeCell ref="DZ4:EF4"/>
     <mergeCell ref="FW4:GC4"/>
     <mergeCell ref="GD4:GJ4"/>
     <mergeCell ref="GK4:GQ4"/>
@@ -20123,49 +20152,20 @@
     <mergeCell ref="EN4:ET4"/>
     <mergeCell ref="EU4:FA4"/>
     <mergeCell ref="FB4:FH4"/>
-    <mergeCell ref="FI4:FO4"/>
-    <mergeCell ref="FP4:FV4"/>
-    <mergeCell ref="EG4:EM4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE5:DK5"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="DS5:DY5"/>
-    <mergeCell ref="DZ5:EF5"/>
-    <mergeCell ref="EG5:EM5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DS4:DY4"/>
-    <mergeCell ref="DZ4:EF4"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="AD1:AR1"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AF5:AL5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="HM5:HS5"/>
+    <mergeCell ref="HT5:HZ5"/>
+    <mergeCell ref="IA5:IG5"/>
+    <mergeCell ref="IH5:IN5"/>
+    <mergeCell ref="GY4:HE4"/>
+    <mergeCell ref="HF4:HL4"/>
+    <mergeCell ref="GY5:HE5"/>
+    <mergeCell ref="HF5:HL5"/>
+    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="IO5:IU5"/>
+    <mergeCell ref="IO4:IU4"/>
+    <mergeCell ref="HT4:HZ4"/>
+    <mergeCell ref="IA4:IG4"/>
+    <mergeCell ref="IH4:IN4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H55:H59 H8:H52">

</xml_diff>

<commit_message>
updated objectives, gantt chart, pics
</commit_message>
<xml_diff>
--- a/thesis gantt chart.xlsx
+++ b/thesis gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wings_stuff\srus\TUD\yr5\thesis\thesis_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6537BD04-C794-4A65-AEB0-ABEAD1A2E452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391B2875-5A2A-4B1B-8608-C7DA8288FA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="3210" windowWidth="23235" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -2885,7 +2885,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="9"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="15"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2954,13 +2954,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>99060</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -3294,75 +3294,70 @@
   </sheetPr>
   <dimension ref="A1:IU62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG32" sqref="AG32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AW25" sqref="AW25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="4" style="91" customWidth="1"/>
-    <col min="4" max="4" width="0.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="0.5546875" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.44140625" style="1" customWidth="1"/>
-    <col min="67" max="68" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="2.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="1.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="1.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="2.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="99" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="100" max="101" width="1.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="1.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="2.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="105" max="106" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="107" max="108" width="1.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="109" max="131" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="2.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="134" max="136" width="1.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="1.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="139" max="162" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="163" max="164" width="1.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="1.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="2.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="168" max="169" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="170" max="192" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="1.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="2.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="196" max="197" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="198" max="199" width="1.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="1.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="202" max="221" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="2.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="225" max="227" width="1.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="0.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="0.5703125" style="1" customWidth="1"/>
+    <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
+    <col min="67" max="68" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="74" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="99" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="100" max="102" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="105" max="106" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="107" max="108" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="109" max="131" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="134" max="137" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="139" max="162" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="163" max="165" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="168" max="169" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="170" max="192" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="196" max="197" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="198" max="200" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="202" max="221" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="225" max="227" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="2.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="231" max="252" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="253" max="254" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="1.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="256" max="16384" width="9.109375" style="1"/>
+    <col min="229" max="229" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="231" max="252" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="253" max="254" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="256" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="12" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:255" s="12" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="78" t="s">
         <v>24</v>
       </c>
@@ -3391,7 +3386,7 @@
       <c r="AQ1" s="204"/>
       <c r="AR1" s="204"/>
     </row>
-    <row r="2" spans="1:255" s="28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:255" s="28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="72" t="s">
         <v>25</v>
       </c>
@@ -3465,7 +3460,7 @@
       <c r="BM3" s="76"/>
       <c r="BN3" s="77"/>
     </row>
-    <row r="4" spans="1:255" s="70" customFormat="1" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:255" s="70" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="73" t="s">
         <v>17</v>
       </c>
@@ -3478,7 +3473,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="74">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="K4" s="199"/>
       <c r="L4" s="200"/>
@@ -3489,7 +3484,7 @@
       <c r="Q4" s="201"/>
       <c r="R4" s="199" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 9</v>
+        <v>Week 15</v>
       </c>
       <c r="S4" s="200"/>
       <c r="T4" s="200"/>
@@ -3499,7 +3494,7 @@
       <c r="X4" s="201"/>
       <c r="Y4" s="199" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 10</v>
+        <v>Week 16</v>
       </c>
       <c r="Z4" s="200"/>
       <c r="AA4" s="200"/>
@@ -3509,7 +3504,7 @@
       <c r="AE4" s="201"/>
       <c r="AF4" s="199" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 11</v>
+        <v>Week 17</v>
       </c>
       <c r="AG4" s="200"/>
       <c r="AH4" s="200"/>
@@ -3519,7 +3514,7 @@
       <c r="AL4" s="201"/>
       <c r="AM4" s="199" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 12</v>
+        <v>Week 18</v>
       </c>
       <c r="AN4" s="200"/>
       <c r="AO4" s="200"/>
@@ -3529,7 +3524,7 @@
       <c r="AS4" s="201"/>
       <c r="AT4" s="199" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 13</v>
+        <v>Week 19</v>
       </c>
       <c r="AU4" s="200"/>
       <c r="AV4" s="200"/>
@@ -3539,7 +3534,7 @@
       <c r="AZ4" s="201"/>
       <c r="BA4" s="199" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 14</v>
+        <v>Week 20</v>
       </c>
       <c r="BB4" s="200"/>
       <c r="BC4" s="200"/>
@@ -3549,7 +3544,7 @@
       <c r="BG4" s="201"/>
       <c r="BH4" s="199" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 15</v>
+        <v>Week 21</v>
       </c>
       <c r="BI4" s="200"/>
       <c r="BJ4" s="200"/>
@@ -3559,7 +3554,7 @@
       <c r="BN4" s="201"/>
       <c r="BO4" s="199" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 16</v>
+        <v>Week 22</v>
       </c>
       <c r="BP4" s="200"/>
       <c r="BQ4" s="200"/>
@@ -3569,7 +3564,7 @@
       <c r="BU4" s="201"/>
       <c r="BV4" s="199" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 17</v>
+        <v>Week 23</v>
       </c>
       <c r="BW4" s="200"/>
       <c r="BX4" s="200"/>
@@ -3579,7 +3574,7 @@
       <c r="CB4" s="201"/>
       <c r="CC4" s="199" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 18</v>
+        <v>Week 24</v>
       </c>
       <c r="CD4" s="200"/>
       <c r="CE4" s="200"/>
@@ -3589,7 +3584,7 @@
       <c r="CI4" s="201"/>
       <c r="CJ4" s="199" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 19</v>
+        <v>Week 25</v>
       </c>
       <c r="CK4" s="200"/>
       <c r="CL4" s="200"/>
@@ -3599,7 +3594,7 @@
       <c r="CP4" s="201"/>
       <c r="CQ4" s="199" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 20</v>
+        <v>Week 26</v>
       </c>
       <c r="CR4" s="200"/>
       <c r="CS4" s="200"/>
@@ -3609,7 +3604,7 @@
       <c r="CW4" s="201"/>
       <c r="CX4" s="199" t="str">
         <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 21</v>
+        <v>Week 27</v>
       </c>
       <c r="CY4" s="200"/>
       <c r="CZ4" s="200"/>
@@ -3619,7 +3614,7 @@
       <c r="DD4" s="201"/>
       <c r="DE4" s="199" t="str">
         <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 22</v>
+        <v>Week 28</v>
       </c>
       <c r="DF4" s="200"/>
       <c r="DG4" s="200"/>
@@ -3629,7 +3624,7 @@
       <c r="DK4" s="201"/>
       <c r="DL4" s="199" t="str">
         <f>"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 23</v>
+        <v>Week 29</v>
       </c>
       <c r="DM4" s="200"/>
       <c r="DN4" s="200"/>
@@ -3639,7 +3634,7 @@
       <c r="DR4" s="201"/>
       <c r="DS4" s="199" t="str">
         <f>"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 24</v>
+        <v>Week 30</v>
       </c>
       <c r="DT4" s="200"/>
       <c r="DU4" s="200"/>
@@ -3649,7 +3644,7 @@
       <c r="DY4" s="201"/>
       <c r="DZ4" s="199" t="str">
         <f>"Week "&amp;(DS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 25</v>
+        <v>Week 31</v>
       </c>
       <c r="EA4" s="200"/>
       <c r="EB4" s="200"/>
@@ -3659,7 +3654,7 @@
       <c r="EF4" s="201"/>
       <c r="EG4" s="199" t="str">
         <f>"Week "&amp;(DZ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 26</v>
+        <v>Week 32</v>
       </c>
       <c r="EH4" s="200"/>
       <c r="EI4" s="200"/>
@@ -3669,7 +3664,7 @@
       <c r="EM4" s="201"/>
       <c r="EN4" s="199" t="str">
         <f>"Week "&amp;(EG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 27</v>
+        <v>Week 33</v>
       </c>
       <c r="EO4" s="200"/>
       <c r="EP4" s="200"/>
@@ -3679,7 +3674,7 @@
       <c r="ET4" s="201"/>
       <c r="EU4" s="199" t="str">
         <f>"Week "&amp;(EN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 28</v>
+        <v>Week 34</v>
       </c>
       <c r="EV4" s="200"/>
       <c r="EW4" s="200"/>
@@ -3689,7 +3684,7 @@
       <c r="FA4" s="201"/>
       <c r="FB4" s="199" t="str">
         <f>"Week "&amp;(EU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 29</v>
+        <v>Week 35</v>
       </c>
       <c r="FC4" s="200"/>
       <c r="FD4" s="200"/>
@@ -3699,7 +3694,7 @@
       <c r="FH4" s="201"/>
       <c r="FI4" s="199" t="str">
         <f>"Week "&amp;(FB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 30</v>
+        <v>Week 36</v>
       </c>
       <c r="FJ4" s="200"/>
       <c r="FK4" s="200"/>
@@ -3709,7 +3704,7 @@
       <c r="FO4" s="201"/>
       <c r="FP4" s="199" t="str">
         <f>"Week "&amp;(FI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 31</v>
+        <v>Week 37</v>
       </c>
       <c r="FQ4" s="200"/>
       <c r="FR4" s="200"/>
@@ -3719,7 +3714,7 @@
       <c r="FV4" s="201"/>
       <c r="FW4" s="199" t="str">
         <f>"Week "&amp;(FP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 32</v>
+        <v>Week 38</v>
       </c>
       <c r="FX4" s="200"/>
       <c r="FY4" s="200"/>
@@ -3729,7 +3724,7 @@
       <c r="GC4" s="201"/>
       <c r="GD4" s="199" t="str">
         <f>"Week "&amp;(FW6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 33</v>
+        <v>Week 39</v>
       </c>
       <c r="GE4" s="200"/>
       <c r="GF4" s="200"/>
@@ -3739,7 +3734,7 @@
       <c r="GJ4" s="201"/>
       <c r="GK4" s="199" t="str">
         <f>"Week "&amp;(GD6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 34</v>
+        <v>Week 40</v>
       </c>
       <c r="GL4" s="200"/>
       <c r="GM4" s="200"/>
@@ -3749,7 +3744,7 @@
       <c r="GQ4" s="201"/>
       <c r="GR4" s="199" t="str">
         <f>"Week "&amp;(GK6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 35</v>
+        <v>Week 41</v>
       </c>
       <c r="GS4" s="200"/>
       <c r="GT4" s="200"/>
@@ -3759,7 +3754,7 @@
       <c r="GX4" s="201"/>
       <c r="GY4" s="199" t="str">
         <f>"Week "&amp;(GR6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 36</v>
+        <v>Week 42</v>
       </c>
       <c r="GZ4" s="200"/>
       <c r="HA4" s="200"/>
@@ -3769,7 +3764,7 @@
       <c r="HE4" s="201"/>
       <c r="HF4" s="199" t="str">
         <f>"Week "&amp;(GY6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 37</v>
+        <v>Week 43</v>
       </c>
       <c r="HG4" s="200"/>
       <c r="HH4" s="200"/>
@@ -3779,7 +3774,7 @@
       <c r="HL4" s="201"/>
       <c r="HM4" s="199" t="str">
         <f>"Week "&amp;(HF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 38</v>
+        <v>Week 44</v>
       </c>
       <c r="HN4" s="200"/>
       <c r="HO4" s="200"/>
@@ -3789,7 +3784,7 @@
       <c r="HS4" s="201"/>
       <c r="HT4" s="199" t="str">
         <f>"Week "&amp;(HM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 39</v>
+        <v>Week 45</v>
       </c>
       <c r="HU4" s="200"/>
       <c r="HV4" s="200"/>
@@ -3799,7 +3794,7 @@
       <c r="HZ4" s="201"/>
       <c r="IA4" s="199" t="str">
         <f>"Week "&amp;(HT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 40</v>
+        <v>Week 46</v>
       </c>
       <c r="IB4" s="200"/>
       <c r="IC4" s="200"/>
@@ -3809,7 +3804,7 @@
       <c r="IG4" s="201"/>
       <c r="IH4" s="199" t="str">
         <f>"Week "&amp;(IA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 41</v>
+        <v>Week 47</v>
       </c>
       <c r="II4" s="200"/>
       <c r="IJ4" s="200"/>
@@ -3819,7 +3814,7 @@
       <c r="IN4" s="201"/>
       <c r="IO4" s="199" t="str">
         <f>"Week "&amp;(IH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 42</v>
+        <v>Week 48</v>
       </c>
       <c r="IP4" s="200"/>
       <c r="IQ4" s="200"/>
@@ -3828,7 +3823,7 @@
       <c r="IT4" s="200"/>
       <c r="IU4" s="201"/>
     </row>
-    <row r="5" spans="1:255" s="24" customFormat="1" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:255" s="24" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
       <c r="B5" s="73" t="s">
         <v>15</v>
@@ -3844,7 +3839,7 @@
       <c r="I5" s="71"/>
       <c r="K5" s="210">
         <f>K6</f>
-        <v>45348</v>
+        <v>45390</v>
       </c>
       <c r="L5" s="197"/>
       <c r="M5" s="197"/>
@@ -3854,7 +3849,7 @@
       <c r="Q5" s="212"/>
       <c r="R5" s="210">
         <f>R6</f>
-        <v>45355</v>
+        <v>45397</v>
       </c>
       <c r="S5" s="197"/>
       <c r="T5" s="197"/>
@@ -3864,7 +3859,7 @@
       <c r="X5" s="211"/>
       <c r="Y5" s="213">
         <f>Y6</f>
-        <v>45362</v>
+        <v>45404</v>
       </c>
       <c r="Z5" s="197"/>
       <c r="AA5" s="197"/>
@@ -3874,7 +3869,7 @@
       <c r="AE5" s="214"/>
       <c r="AF5" s="205">
         <f>AF6</f>
-        <v>45369</v>
+        <v>45411</v>
       </c>
       <c r="AG5" s="197"/>
       <c r="AH5" s="197"/>
@@ -3884,7 +3879,7 @@
       <c r="AL5" s="206"/>
       <c r="AM5" s="215">
         <f>AM6</f>
-        <v>45376</v>
+        <v>45418</v>
       </c>
       <c r="AN5" s="197"/>
       <c r="AO5" s="197"/>
@@ -3894,7 +3889,7 @@
       <c r="AS5" s="216"/>
       <c r="AT5" s="217">
         <f>AT6</f>
-        <v>45383</v>
+        <v>45425</v>
       </c>
       <c r="AU5" s="197"/>
       <c r="AV5" s="197"/>
@@ -3904,7 +3899,7 @@
       <c r="AZ5" s="218"/>
       <c r="BA5" s="196">
         <f>BA6</f>
-        <v>45390</v>
+        <v>45432</v>
       </c>
       <c r="BB5" s="197"/>
       <c r="BC5" s="197"/>
@@ -3914,7 +3909,7 @@
       <c r="BG5" s="198"/>
       <c r="BH5" s="202">
         <f>BH6</f>
-        <v>45397</v>
+        <v>45439</v>
       </c>
       <c r="BI5" s="197"/>
       <c r="BJ5" s="197"/>
@@ -3924,7 +3919,7 @@
       <c r="BN5" s="203"/>
       <c r="BO5" s="196">
         <f>BO6</f>
-        <v>45404</v>
+        <v>45446</v>
       </c>
       <c r="BP5" s="197"/>
       <c r="BQ5" s="197"/>
@@ -3934,7 +3929,7 @@
       <c r="BU5" s="198"/>
       <c r="BV5" s="202">
         <f>BV6</f>
-        <v>45411</v>
+        <v>45453</v>
       </c>
       <c r="BW5" s="197"/>
       <c r="BX5" s="197"/>
@@ -3944,7 +3939,7 @@
       <c r="CB5" s="203"/>
       <c r="CC5" s="202">
         <f>CC6</f>
-        <v>45418</v>
+        <v>45460</v>
       </c>
       <c r="CD5" s="197"/>
       <c r="CE5" s="197"/>
@@ -3954,7 +3949,7 @@
       <c r="CI5" s="203"/>
       <c r="CJ5" s="196">
         <f>CJ6</f>
-        <v>45425</v>
+        <v>45467</v>
       </c>
       <c r="CK5" s="197"/>
       <c r="CL5" s="197"/>
@@ -3964,7 +3959,7 @@
       <c r="CP5" s="198"/>
       <c r="CQ5" s="202">
         <f>CQ6</f>
-        <v>45432</v>
+        <v>45474</v>
       </c>
       <c r="CR5" s="197"/>
       <c r="CS5" s="197"/>
@@ -3974,7 +3969,7 @@
       <c r="CW5" s="203"/>
       <c r="CX5" s="202">
         <f>CX6</f>
-        <v>45439</v>
+        <v>45481</v>
       </c>
       <c r="CY5" s="197"/>
       <c r="CZ5" s="197"/>
@@ -3984,7 +3979,7 @@
       <c r="DD5" s="203"/>
       <c r="DE5" s="196">
         <f>DE6</f>
-        <v>45446</v>
+        <v>45488</v>
       </c>
       <c r="DF5" s="197"/>
       <c r="DG5" s="197"/>
@@ -3994,7 +3989,7 @@
       <c r="DK5" s="198"/>
       <c r="DL5" s="202">
         <f>DL6</f>
-        <v>45453</v>
+        <v>45495</v>
       </c>
       <c r="DM5" s="197"/>
       <c r="DN5" s="197"/>
@@ -4004,7 +3999,7 @@
       <c r="DR5" s="203"/>
       <c r="DS5" s="202">
         <f>DS6</f>
-        <v>45460</v>
+        <v>45502</v>
       </c>
       <c r="DT5" s="197"/>
       <c r="DU5" s="197"/>
@@ -4014,7 +4009,7 @@
       <c r="DY5" s="203"/>
       <c r="DZ5" s="196">
         <f>DZ6</f>
-        <v>45467</v>
+        <v>45509</v>
       </c>
       <c r="EA5" s="197"/>
       <c r="EB5" s="197"/>
@@ -4024,7 +4019,7 @@
       <c r="EF5" s="198"/>
       <c r="EG5" s="202">
         <f>EG6</f>
-        <v>45474</v>
+        <v>45516</v>
       </c>
       <c r="EH5" s="197"/>
       <c r="EI5" s="197"/>
@@ -4034,7 +4029,7 @@
       <c r="EM5" s="203"/>
       <c r="EN5" s="202">
         <f>EN6</f>
-        <v>45481</v>
+        <v>45523</v>
       </c>
       <c r="EO5" s="197"/>
       <c r="EP5" s="197"/>
@@ -4044,7 +4039,7 @@
       <c r="ET5" s="203"/>
       <c r="EU5" s="196">
         <f>EU6</f>
-        <v>45488</v>
+        <v>45530</v>
       </c>
       <c r="EV5" s="197"/>
       <c r="EW5" s="197"/>
@@ -4054,7 +4049,7 @@
       <c r="FA5" s="198"/>
       <c r="FB5" s="202">
         <f>FB6</f>
-        <v>45495</v>
+        <v>45537</v>
       </c>
       <c r="FC5" s="197"/>
       <c r="FD5" s="197"/>
@@ -4064,7 +4059,7 @@
       <c r="FH5" s="203"/>
       <c r="FI5" s="202">
         <f>FI6</f>
-        <v>45502</v>
+        <v>45544</v>
       </c>
       <c r="FJ5" s="197"/>
       <c r="FK5" s="197"/>
@@ -4074,7 +4069,7 @@
       <c r="FO5" s="203"/>
       <c r="FP5" s="196">
         <f>FP6</f>
-        <v>45509</v>
+        <v>45551</v>
       </c>
       <c r="FQ5" s="197"/>
       <c r="FR5" s="197"/>
@@ -4084,7 +4079,7 @@
       <c r="FV5" s="198"/>
       <c r="FW5" s="202">
         <f>FW6</f>
-        <v>45516</v>
+        <v>45558</v>
       </c>
       <c r="FX5" s="197"/>
       <c r="FY5" s="197"/>
@@ -4094,7 +4089,7 @@
       <c r="GC5" s="203"/>
       <c r="GD5" s="202">
         <f>GD6</f>
-        <v>45523</v>
+        <v>45565</v>
       </c>
       <c r="GE5" s="197"/>
       <c r="GF5" s="197"/>
@@ -4104,7 +4099,7 @@
       <c r="GJ5" s="203"/>
       <c r="GK5" s="196">
         <f>GK6</f>
-        <v>45530</v>
+        <v>45572</v>
       </c>
       <c r="GL5" s="197"/>
       <c r="GM5" s="197"/>
@@ -4114,7 +4109,7 @@
       <c r="GQ5" s="198"/>
       <c r="GR5" s="202">
         <f>GR6</f>
-        <v>45537</v>
+        <v>45579</v>
       </c>
       <c r="GS5" s="197"/>
       <c r="GT5" s="197"/>
@@ -4124,7 +4119,7 @@
       <c r="GX5" s="203"/>
       <c r="GY5" s="196">
         <f>GY6</f>
-        <v>45544</v>
+        <v>45586</v>
       </c>
       <c r="GZ5" s="197"/>
       <c r="HA5" s="197"/>
@@ -4134,7 +4129,7 @@
       <c r="HE5" s="198"/>
       <c r="HF5" s="202">
         <f>HF6</f>
-        <v>45551</v>
+        <v>45593</v>
       </c>
       <c r="HG5" s="197"/>
       <c r="HH5" s="197"/>
@@ -4144,7 +4139,7 @@
       <c r="HL5" s="203"/>
       <c r="HM5" s="196">
         <f>HM6</f>
-        <v>45558</v>
+        <v>45600</v>
       </c>
       <c r="HN5" s="197"/>
       <c r="HO5" s="197"/>
@@ -4154,7 +4149,7 @@
       <c r="HS5" s="198"/>
       <c r="HT5" s="202">
         <f>HT6</f>
-        <v>45565</v>
+        <v>45607</v>
       </c>
       <c r="HU5" s="197"/>
       <c r="HV5" s="197"/>
@@ -4164,7 +4159,7 @@
       <c r="HZ5" s="203"/>
       <c r="IA5" s="196">
         <f>IA6</f>
-        <v>45572</v>
+        <v>45614</v>
       </c>
       <c r="IB5" s="197"/>
       <c r="IC5" s="197"/>
@@ -4174,7 +4169,7 @@
       <c r="IG5" s="198"/>
       <c r="IH5" s="202">
         <f>IH6</f>
-        <v>45579</v>
+        <v>45621</v>
       </c>
       <c r="II5" s="197"/>
       <c r="IJ5" s="197"/>
@@ -4184,7 +4179,7 @@
       <c r="IN5" s="203"/>
       <c r="IO5" s="196">
         <f>IO6</f>
-        <v>45586</v>
+        <v>45628</v>
       </c>
       <c r="IP5" s="197"/>
       <c r="IQ5" s="197"/>
@@ -4193,983 +4188,983 @@
       <c r="IT5" s="197"/>
       <c r="IU5" s="198"/>
     </row>
-    <row r="6" spans="1:255" s="22" customFormat="1" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:255" s="22" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="84"/>
       <c r="K6" s="33">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
-        <v>45348</v>
+        <v>45390</v>
       </c>
       <c r="L6" s="23">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>45349</v>
+        <v>45391</v>
       </c>
       <c r="M6" s="23">
         <f t="shared" si="0"/>
-        <v>45350</v>
+        <v>45392</v>
       </c>
       <c r="N6" s="23">
         <f t="shared" si="0"/>
-        <v>45351</v>
+        <v>45393</v>
       </c>
       <c r="O6" s="23">
         <f t="shared" si="0"/>
-        <v>45352</v>
+        <v>45394</v>
       </c>
       <c r="P6" s="23">
         <f t="shared" si="0"/>
-        <v>45353</v>
+        <v>45395</v>
       </c>
       <c r="Q6" s="34">
         <f t="shared" si="0"/>
-        <v>45354</v>
+        <v>45396</v>
       </c>
       <c r="R6" s="33">
         <f t="shared" si="0"/>
-        <v>45355</v>
+        <v>45397</v>
       </c>
       <c r="S6" s="23">
         <f t="shared" si="0"/>
-        <v>45356</v>
+        <v>45398</v>
       </c>
       <c r="T6" s="23">
         <f t="shared" si="0"/>
-        <v>45357</v>
+        <v>45399</v>
       </c>
       <c r="U6" s="23">
         <f>T6+1</f>
-        <v>45358</v>
+        <v>45400</v>
       </c>
       <c r="V6" s="23">
         <f>U6+1</f>
-        <v>45359</v>
+        <v>45401</v>
       </c>
       <c r="W6" s="23">
         <f>V6+1</f>
-        <v>45360</v>
+        <v>45402</v>
       </c>
       <c r="X6" s="35">
         <f t="shared" si="0"/>
-        <v>45361</v>
+        <v>45403</v>
       </c>
       <c r="Y6" s="36">
         <f t="shared" si="0"/>
-        <v>45362</v>
+        <v>45404</v>
       </c>
       <c r="Z6" s="23">
         <f t="shared" si="0"/>
-        <v>45363</v>
+        <v>45405</v>
       </c>
       <c r="AA6" s="23">
         <f t="shared" si="0"/>
-        <v>45364</v>
+        <v>45406</v>
       </c>
       <c r="AB6" s="23">
         <f t="shared" si="0"/>
-        <v>45365</v>
+        <v>45407</v>
       </c>
       <c r="AC6" s="23">
         <f t="shared" si="0"/>
-        <v>45366</v>
+        <v>45408</v>
       </c>
       <c r="AD6" s="23">
         <f t="shared" si="0"/>
-        <v>45367</v>
+        <v>45409</v>
       </c>
       <c r="AE6" s="37">
         <f t="shared" si="0"/>
-        <v>45368</v>
+        <v>45410</v>
       </c>
       <c r="AF6" s="38">
         <f t="shared" si="0"/>
-        <v>45369</v>
+        <v>45411</v>
       </c>
       <c r="AG6" s="23">
         <f t="shared" si="0"/>
-        <v>45370</v>
+        <v>45412</v>
       </c>
       <c r="AH6" s="23">
         <f t="shared" si="0"/>
-        <v>45371</v>
+        <v>45413</v>
       </c>
       <c r="AI6" s="23">
         <f t="shared" si="0"/>
-        <v>45372</v>
+        <v>45414</v>
       </c>
       <c r="AJ6" s="23">
         <f t="shared" si="0"/>
-        <v>45373</v>
+        <v>45415</v>
       </c>
       <c r="AK6" s="23">
         <f t="shared" si="0"/>
-        <v>45374</v>
+        <v>45416</v>
       </c>
       <c r="AL6" s="39">
         <f t="shared" si="0"/>
-        <v>45375</v>
+        <v>45417</v>
       </c>
       <c r="AM6" s="40">
         <f t="shared" si="0"/>
-        <v>45376</v>
+        <v>45418</v>
       </c>
       <c r="AN6" s="23">
         <f t="shared" si="0"/>
-        <v>45377</v>
+        <v>45419</v>
       </c>
       <c r="AO6" s="23">
         <f t="shared" si="0"/>
-        <v>45378</v>
+        <v>45420</v>
       </c>
       <c r="AP6" s="23">
         <f t="shared" si="0"/>
-        <v>45379</v>
+        <v>45421</v>
       </c>
       <c r="AQ6" s="23">
         <f t="shared" si="0"/>
-        <v>45380</v>
+        <v>45422</v>
       </c>
       <c r="AR6" s="23">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>45381</v>
+        <v>45423</v>
       </c>
       <c r="AS6" s="41">
         <f t="shared" si="1"/>
-        <v>45382</v>
+        <v>45424</v>
       </c>
       <c r="AT6" s="42">
         <f t="shared" si="1"/>
-        <v>45383</v>
+        <v>45425</v>
       </c>
       <c r="AU6" s="23">
         <f t="shared" si="1"/>
-        <v>45384</v>
+        <v>45426</v>
       </c>
       <c r="AV6" s="23">
         <f t="shared" si="1"/>
-        <v>45385</v>
+        <v>45427</v>
       </c>
       <c r="AW6" s="23">
         <f t="shared" si="1"/>
-        <v>45386</v>
+        <v>45428</v>
       </c>
       <c r="AX6" s="23">
         <f t="shared" si="1"/>
-        <v>45387</v>
+        <v>45429</v>
       </c>
       <c r="AY6" s="23">
         <f t="shared" si="1"/>
-        <v>45388</v>
+        <v>45430</v>
       </c>
       <c r="AZ6" s="43">
         <f t="shared" si="1"/>
-        <v>45389</v>
+        <v>45431</v>
       </c>
       <c r="BA6" s="44">
         <f t="shared" si="1"/>
-        <v>45390</v>
+        <v>45432</v>
       </c>
       <c r="BB6" s="23">
         <f t="shared" si="1"/>
-        <v>45391</v>
+        <v>45433</v>
       </c>
       <c r="BC6" s="23">
         <f t="shared" si="1"/>
-        <v>45392</v>
+        <v>45434</v>
       </c>
       <c r="BD6" s="23">
         <f t="shared" si="1"/>
-        <v>45393</v>
+        <v>45435</v>
       </c>
       <c r="BE6" s="23">
         <f t="shared" si="1"/>
-        <v>45394</v>
+        <v>45436</v>
       </c>
       <c r="BF6" s="23">
         <f t="shared" si="1"/>
-        <v>45395</v>
+        <v>45437</v>
       </c>
       <c r="BG6" s="45">
         <f t="shared" si="1"/>
-        <v>45396</v>
+        <v>45438</v>
       </c>
       <c r="BH6" s="46">
         <f t="shared" si="1"/>
-        <v>45397</v>
+        <v>45439</v>
       </c>
       <c r="BI6" s="23">
         <f t="shared" si="1"/>
-        <v>45398</v>
+        <v>45440</v>
       </c>
       <c r="BJ6" s="23">
         <f t="shared" si="1"/>
-        <v>45399</v>
+        <v>45441</v>
       </c>
       <c r="BK6" s="23">
         <f t="shared" si="1"/>
-        <v>45400</v>
+        <v>45442</v>
       </c>
       <c r="BL6" s="23">
         <f t="shared" si="1"/>
-        <v>45401</v>
+        <v>45443</v>
       </c>
       <c r="BM6" s="23">
         <f t="shared" si="1"/>
-        <v>45402</v>
+        <v>45444</v>
       </c>
       <c r="BN6" s="47">
         <f t="shared" si="1"/>
-        <v>45403</v>
+        <v>45445</v>
       </c>
       <c r="BO6" s="44">
         <f t="shared" ref="BO6:CT6" si="2">BN6+1</f>
-        <v>45404</v>
+        <v>45446</v>
       </c>
       <c r="BP6" s="23">
         <f t="shared" si="2"/>
-        <v>45405</v>
+        <v>45447</v>
       </c>
       <c r="BQ6" s="23">
         <f t="shared" si="2"/>
-        <v>45406</v>
+        <v>45448</v>
       </c>
       <c r="BR6" s="23">
         <f t="shared" si="2"/>
-        <v>45407</v>
+        <v>45449</v>
       </c>
       <c r="BS6" s="23">
         <f t="shared" si="2"/>
-        <v>45408</v>
+        <v>45450</v>
       </c>
       <c r="BT6" s="23">
         <f t="shared" si="2"/>
-        <v>45409</v>
+        <v>45451</v>
       </c>
       <c r="BU6" s="45">
         <f t="shared" si="2"/>
-        <v>45410</v>
+        <v>45452</v>
       </c>
       <c r="BV6" s="46">
         <f t="shared" si="2"/>
-        <v>45411</v>
+        <v>45453</v>
       </c>
       <c r="BW6" s="23">
         <f t="shared" si="2"/>
-        <v>45412</v>
+        <v>45454</v>
       </c>
       <c r="BX6" s="23">
         <f t="shared" si="2"/>
-        <v>45413</v>
+        <v>45455</v>
       </c>
       <c r="BY6" s="23">
         <f t="shared" si="2"/>
-        <v>45414</v>
+        <v>45456</v>
       </c>
       <c r="BZ6" s="23">
         <f t="shared" si="2"/>
-        <v>45415</v>
+        <v>45457</v>
       </c>
       <c r="CA6" s="23">
         <f t="shared" si="2"/>
-        <v>45416</v>
+        <v>45458</v>
       </c>
       <c r="CB6" s="47">
         <f t="shared" si="2"/>
-        <v>45417</v>
+        <v>45459</v>
       </c>
       <c r="CC6" s="46">
         <f t="shared" si="2"/>
-        <v>45418</v>
+        <v>45460</v>
       </c>
       <c r="CD6" s="23">
         <f t="shared" si="2"/>
-        <v>45419</v>
+        <v>45461</v>
       </c>
       <c r="CE6" s="23">
         <f t="shared" si="2"/>
-        <v>45420</v>
+        <v>45462</v>
       </c>
       <c r="CF6" s="23">
         <f t="shared" si="2"/>
-        <v>45421</v>
+        <v>45463</v>
       </c>
       <c r="CG6" s="23">
         <f t="shared" si="2"/>
-        <v>45422</v>
+        <v>45464</v>
       </c>
       <c r="CH6" s="23">
         <f t="shared" si="2"/>
-        <v>45423</v>
+        <v>45465</v>
       </c>
       <c r="CI6" s="47">
         <f t="shared" si="2"/>
-        <v>45424</v>
+        <v>45466</v>
       </c>
       <c r="CJ6" s="44">
         <f t="shared" si="2"/>
-        <v>45425</v>
+        <v>45467</v>
       </c>
       <c r="CK6" s="23">
         <f t="shared" si="2"/>
-        <v>45426</v>
+        <v>45468</v>
       </c>
       <c r="CL6" s="23">
         <f t="shared" si="2"/>
-        <v>45427</v>
+        <v>45469</v>
       </c>
       <c r="CM6" s="23">
         <f t="shared" si="2"/>
-        <v>45428</v>
+        <v>45470</v>
       </c>
       <c r="CN6" s="23">
         <f t="shared" si="2"/>
-        <v>45429</v>
+        <v>45471</v>
       </c>
       <c r="CO6" s="23">
         <f t="shared" si="2"/>
-        <v>45430</v>
+        <v>45472</v>
       </c>
       <c r="CP6" s="45">
         <f t="shared" si="2"/>
-        <v>45431</v>
+        <v>45473</v>
       </c>
       <c r="CQ6" s="46">
         <f t="shared" si="2"/>
-        <v>45432</v>
+        <v>45474</v>
       </c>
       <c r="CR6" s="23">
         <f t="shared" si="2"/>
-        <v>45433</v>
+        <v>45475</v>
       </c>
       <c r="CS6" s="23">
         <f t="shared" si="2"/>
-        <v>45434</v>
+        <v>45476</v>
       </c>
       <c r="CT6" s="23">
         <f t="shared" si="2"/>
-        <v>45435</v>
+        <v>45477</v>
       </c>
       <c r="CU6" s="23">
         <f t="shared" ref="CU6:DZ6" si="3">CT6+1</f>
-        <v>45436</v>
+        <v>45478</v>
       </c>
       <c r="CV6" s="23">
         <f t="shared" si="3"/>
-        <v>45437</v>
+        <v>45479</v>
       </c>
       <c r="CW6" s="47">
         <f t="shared" si="3"/>
-        <v>45438</v>
+        <v>45480</v>
       </c>
       <c r="CX6" s="46">
         <f t="shared" si="3"/>
-        <v>45439</v>
+        <v>45481</v>
       </c>
       <c r="CY6" s="23">
         <f t="shared" si="3"/>
-        <v>45440</v>
+        <v>45482</v>
       </c>
       <c r="CZ6" s="23">
         <f t="shared" si="3"/>
-        <v>45441</v>
+        <v>45483</v>
       </c>
       <c r="DA6" s="23">
         <f t="shared" si="3"/>
-        <v>45442</v>
+        <v>45484</v>
       </c>
       <c r="DB6" s="23">
         <f t="shared" si="3"/>
-        <v>45443</v>
+        <v>45485</v>
       </c>
       <c r="DC6" s="23">
         <f t="shared" si="3"/>
-        <v>45444</v>
+        <v>45486</v>
       </c>
       <c r="DD6" s="47">
         <f t="shared" si="3"/>
-        <v>45445</v>
+        <v>45487</v>
       </c>
       <c r="DE6" s="44">
         <f t="shared" si="3"/>
-        <v>45446</v>
+        <v>45488</v>
       </c>
       <c r="DF6" s="23">
         <f t="shared" si="3"/>
-        <v>45447</v>
+        <v>45489</v>
       </c>
       <c r="DG6" s="23">
         <f t="shared" si="3"/>
-        <v>45448</v>
+        <v>45490</v>
       </c>
       <c r="DH6" s="23">
         <f t="shared" si="3"/>
-        <v>45449</v>
+        <v>45491</v>
       </c>
       <c r="DI6" s="23">
         <f t="shared" si="3"/>
-        <v>45450</v>
+        <v>45492</v>
       </c>
       <c r="DJ6" s="23">
         <f t="shared" si="3"/>
-        <v>45451</v>
+        <v>45493</v>
       </c>
       <c r="DK6" s="45">
         <f t="shared" si="3"/>
-        <v>45452</v>
+        <v>45494</v>
       </c>
       <c r="DL6" s="46">
         <f t="shared" si="3"/>
-        <v>45453</v>
+        <v>45495</v>
       </c>
       <c r="DM6" s="23">
         <f t="shared" si="3"/>
-        <v>45454</v>
+        <v>45496</v>
       </c>
       <c r="DN6" s="23">
         <f t="shared" si="3"/>
-        <v>45455</v>
+        <v>45497</v>
       </c>
       <c r="DO6" s="23">
         <f t="shared" si="3"/>
-        <v>45456</v>
+        <v>45498</v>
       </c>
       <c r="DP6" s="23">
         <f t="shared" si="3"/>
-        <v>45457</v>
+        <v>45499</v>
       </c>
       <c r="DQ6" s="23">
         <f t="shared" si="3"/>
-        <v>45458</v>
+        <v>45500</v>
       </c>
       <c r="DR6" s="47">
         <f t="shared" si="3"/>
-        <v>45459</v>
+        <v>45501</v>
       </c>
       <c r="DS6" s="46">
         <f t="shared" si="3"/>
-        <v>45460</v>
+        <v>45502</v>
       </c>
       <c r="DT6" s="23">
         <f t="shared" si="3"/>
-        <v>45461</v>
+        <v>45503</v>
       </c>
       <c r="DU6" s="23">
         <f t="shared" si="3"/>
-        <v>45462</v>
+        <v>45504</v>
       </c>
       <c r="DV6" s="23">
         <f t="shared" si="3"/>
-        <v>45463</v>
+        <v>45505</v>
       </c>
       <c r="DW6" s="23">
         <f t="shared" si="3"/>
-        <v>45464</v>
+        <v>45506</v>
       </c>
       <c r="DX6" s="23">
         <f t="shared" si="3"/>
-        <v>45465</v>
+        <v>45507</v>
       </c>
       <c r="DY6" s="47">
         <f t="shared" si="3"/>
-        <v>45466</v>
+        <v>45508</v>
       </c>
       <c r="DZ6" s="44">
         <f t="shared" si="3"/>
-        <v>45467</v>
+        <v>45509</v>
       </c>
       <c r="EA6" s="23">
         <f t="shared" ref="EA6:FF6" si="4">DZ6+1</f>
-        <v>45468</v>
+        <v>45510</v>
       </c>
       <c r="EB6" s="23">
         <f t="shared" si="4"/>
-        <v>45469</v>
+        <v>45511</v>
       </c>
       <c r="EC6" s="23">
         <f t="shared" si="4"/>
-        <v>45470</v>
+        <v>45512</v>
       </c>
       <c r="ED6" s="23">
         <f t="shared" si="4"/>
-        <v>45471</v>
+        <v>45513</v>
       </c>
       <c r="EE6" s="23">
         <f t="shared" si="4"/>
-        <v>45472</v>
+        <v>45514</v>
       </c>
       <c r="EF6" s="45">
         <f t="shared" si="4"/>
-        <v>45473</v>
+        <v>45515</v>
       </c>
       <c r="EG6" s="46">
         <f t="shared" si="4"/>
-        <v>45474</v>
+        <v>45516</v>
       </c>
       <c r="EH6" s="23">
         <f t="shared" si="4"/>
-        <v>45475</v>
+        <v>45517</v>
       </c>
       <c r="EI6" s="23">
         <f t="shared" si="4"/>
-        <v>45476</v>
+        <v>45518</v>
       </c>
       <c r="EJ6" s="23">
         <f t="shared" si="4"/>
-        <v>45477</v>
+        <v>45519</v>
       </c>
       <c r="EK6" s="23">
         <f t="shared" si="4"/>
-        <v>45478</v>
+        <v>45520</v>
       </c>
       <c r="EL6" s="23">
         <f t="shared" si="4"/>
-        <v>45479</v>
+        <v>45521</v>
       </c>
       <c r="EM6" s="47">
         <f t="shared" si="4"/>
-        <v>45480</v>
+        <v>45522</v>
       </c>
       <c r="EN6" s="46">
         <f t="shared" si="4"/>
-        <v>45481</v>
+        <v>45523</v>
       </c>
       <c r="EO6" s="23">
         <f t="shared" si="4"/>
-        <v>45482</v>
+        <v>45524</v>
       </c>
       <c r="EP6" s="23">
         <f t="shared" si="4"/>
-        <v>45483</v>
+        <v>45525</v>
       </c>
       <c r="EQ6" s="23">
         <f t="shared" si="4"/>
-        <v>45484</v>
+        <v>45526</v>
       </c>
       <c r="ER6" s="23">
         <f t="shared" si="4"/>
-        <v>45485</v>
+        <v>45527</v>
       </c>
       <c r="ES6" s="23">
         <f t="shared" si="4"/>
-        <v>45486</v>
+        <v>45528</v>
       </c>
       <c r="ET6" s="47">
         <f t="shared" si="4"/>
-        <v>45487</v>
+        <v>45529</v>
       </c>
       <c r="EU6" s="44">
         <f t="shared" si="4"/>
-        <v>45488</v>
+        <v>45530</v>
       </c>
       <c r="EV6" s="23">
         <f t="shared" si="4"/>
-        <v>45489</v>
+        <v>45531</v>
       </c>
       <c r="EW6" s="23">
         <f t="shared" si="4"/>
-        <v>45490</v>
+        <v>45532</v>
       </c>
       <c r="EX6" s="23">
         <f t="shared" si="4"/>
-        <v>45491</v>
+        <v>45533</v>
       </c>
       <c r="EY6" s="23">
         <f t="shared" si="4"/>
-        <v>45492</v>
+        <v>45534</v>
       </c>
       <c r="EZ6" s="23">
         <f t="shared" si="4"/>
-        <v>45493</v>
+        <v>45535</v>
       </c>
       <c r="FA6" s="45">
         <f t="shared" si="4"/>
-        <v>45494</v>
+        <v>45536</v>
       </c>
       <c r="FB6" s="46">
         <f t="shared" si="4"/>
-        <v>45495</v>
+        <v>45537</v>
       </c>
       <c r="FC6" s="23">
         <f t="shared" si="4"/>
-        <v>45496</v>
+        <v>45538</v>
       </c>
       <c r="FD6" s="23">
         <f t="shared" si="4"/>
-        <v>45497</v>
+        <v>45539</v>
       </c>
       <c r="FE6" s="23">
         <f t="shared" si="4"/>
-        <v>45498</v>
+        <v>45540</v>
       </c>
       <c r="FF6" s="23">
         <f t="shared" si="4"/>
-        <v>45499</v>
+        <v>45541</v>
       </c>
       <c r="FG6" s="23">
         <f t="shared" ref="FG6:GL6" si="5">FF6+1</f>
-        <v>45500</v>
+        <v>45542</v>
       </c>
       <c r="FH6" s="47">
         <f t="shared" si="5"/>
-        <v>45501</v>
+        <v>45543</v>
       </c>
       <c r="FI6" s="46">
         <f t="shared" si="5"/>
-        <v>45502</v>
+        <v>45544</v>
       </c>
       <c r="FJ6" s="23">
         <f t="shared" si="5"/>
-        <v>45503</v>
+        <v>45545</v>
       </c>
       <c r="FK6" s="23">
         <f t="shared" si="5"/>
-        <v>45504</v>
+        <v>45546</v>
       </c>
       <c r="FL6" s="23">
         <f t="shared" si="5"/>
-        <v>45505</v>
+        <v>45547</v>
       </c>
       <c r="FM6" s="23">
         <f t="shared" si="5"/>
-        <v>45506</v>
+        <v>45548</v>
       </c>
       <c r="FN6" s="23">
         <f t="shared" si="5"/>
-        <v>45507</v>
+        <v>45549</v>
       </c>
       <c r="FO6" s="47">
         <f t="shared" si="5"/>
-        <v>45508</v>
+        <v>45550</v>
       </c>
       <c r="FP6" s="44">
         <f t="shared" si="5"/>
-        <v>45509</v>
+        <v>45551</v>
       </c>
       <c r="FQ6" s="23">
         <f t="shared" si="5"/>
-        <v>45510</v>
+        <v>45552</v>
       </c>
       <c r="FR6" s="23">
         <f t="shared" si="5"/>
-        <v>45511</v>
+        <v>45553</v>
       </c>
       <c r="FS6" s="23">
         <f t="shared" si="5"/>
-        <v>45512</v>
+        <v>45554</v>
       </c>
       <c r="FT6" s="23">
         <f t="shared" si="5"/>
-        <v>45513</v>
+        <v>45555</v>
       </c>
       <c r="FU6" s="23">
         <f t="shared" si="5"/>
-        <v>45514</v>
+        <v>45556</v>
       </c>
       <c r="FV6" s="45">
         <f t="shared" si="5"/>
-        <v>45515</v>
+        <v>45557</v>
       </c>
       <c r="FW6" s="46">
         <f t="shared" si="5"/>
-        <v>45516</v>
+        <v>45558</v>
       </c>
       <c r="FX6" s="23">
         <f t="shared" si="5"/>
-        <v>45517</v>
+        <v>45559</v>
       </c>
       <c r="FY6" s="23">
         <f t="shared" si="5"/>
-        <v>45518</v>
+        <v>45560</v>
       </c>
       <c r="FZ6" s="23">
         <f t="shared" si="5"/>
-        <v>45519</v>
+        <v>45561</v>
       </c>
       <c r="GA6" s="23">
         <f t="shared" si="5"/>
-        <v>45520</v>
+        <v>45562</v>
       </c>
       <c r="GB6" s="23">
         <f t="shared" si="5"/>
-        <v>45521</v>
+        <v>45563</v>
       </c>
       <c r="GC6" s="47">
         <f t="shared" si="5"/>
-        <v>45522</v>
+        <v>45564</v>
       </c>
       <c r="GD6" s="46">
         <f t="shared" si="5"/>
-        <v>45523</v>
+        <v>45565</v>
       </c>
       <c r="GE6" s="23">
         <f t="shared" si="5"/>
-        <v>45524</v>
+        <v>45566</v>
       </c>
       <c r="GF6" s="23">
         <f t="shared" si="5"/>
-        <v>45525</v>
+        <v>45567</v>
       </c>
       <c r="GG6" s="23">
         <f t="shared" si="5"/>
-        <v>45526</v>
+        <v>45568</v>
       </c>
       <c r="GH6" s="23">
         <f t="shared" si="5"/>
-        <v>45527</v>
+        <v>45569</v>
       </c>
       <c r="GI6" s="23">
         <f t="shared" si="5"/>
-        <v>45528</v>
+        <v>45570</v>
       </c>
       <c r="GJ6" s="47">
         <f t="shared" si="5"/>
-        <v>45529</v>
+        <v>45571</v>
       </c>
       <c r="GK6" s="44">
         <f t="shared" si="5"/>
-        <v>45530</v>
+        <v>45572</v>
       </c>
       <c r="GL6" s="23">
         <f t="shared" si="5"/>
-        <v>45531</v>
+        <v>45573</v>
       </c>
       <c r="GM6" s="23">
         <f t="shared" ref="GM6:HR6" si="6">GL6+1</f>
-        <v>45532</v>
+        <v>45574</v>
       </c>
       <c r="GN6" s="23">
         <f t="shared" si="6"/>
-        <v>45533</v>
+        <v>45575</v>
       </c>
       <c r="GO6" s="23">
         <f t="shared" si="6"/>
-        <v>45534</v>
+        <v>45576</v>
       </c>
       <c r="GP6" s="23">
         <f t="shared" si="6"/>
-        <v>45535</v>
+        <v>45577</v>
       </c>
       <c r="GQ6" s="45">
         <f t="shared" si="6"/>
-        <v>45536</v>
+        <v>45578</v>
       </c>
       <c r="GR6" s="46">
         <f t="shared" si="6"/>
-        <v>45537</v>
+        <v>45579</v>
       </c>
       <c r="GS6" s="23">
         <f t="shared" si="6"/>
-        <v>45538</v>
+        <v>45580</v>
       </c>
       <c r="GT6" s="23">
         <f t="shared" si="6"/>
-        <v>45539</v>
+        <v>45581</v>
       </c>
       <c r="GU6" s="23">
         <f t="shared" si="6"/>
-        <v>45540</v>
+        <v>45582</v>
       </c>
       <c r="GV6" s="23">
         <f t="shared" si="6"/>
-        <v>45541</v>
+        <v>45583</v>
       </c>
       <c r="GW6" s="23">
         <f t="shared" si="6"/>
-        <v>45542</v>
+        <v>45584</v>
       </c>
       <c r="GX6" s="47">
         <f t="shared" si="6"/>
-        <v>45543</v>
+        <v>45585</v>
       </c>
       <c r="GY6" s="44">
         <f t="shared" si="6"/>
-        <v>45544</v>
+        <v>45586</v>
       </c>
       <c r="GZ6" s="23">
         <f t="shared" si="6"/>
-        <v>45545</v>
+        <v>45587</v>
       </c>
       <c r="HA6" s="23">
         <f t="shared" si="6"/>
-        <v>45546</v>
+        <v>45588</v>
       </c>
       <c r="HB6" s="23">
         <f t="shared" si="6"/>
-        <v>45547</v>
+        <v>45589</v>
       </c>
       <c r="HC6" s="23">
         <f t="shared" si="6"/>
-        <v>45548</v>
+        <v>45590</v>
       </c>
       <c r="HD6" s="23">
         <f t="shared" si="6"/>
-        <v>45549</v>
+        <v>45591</v>
       </c>
       <c r="HE6" s="45">
         <f t="shared" si="6"/>
-        <v>45550</v>
+        <v>45592</v>
       </c>
       <c r="HF6" s="46">
         <f t="shared" si="6"/>
-        <v>45551</v>
+        <v>45593</v>
       </c>
       <c r="HG6" s="23">
         <f t="shared" si="6"/>
-        <v>45552</v>
+        <v>45594</v>
       </c>
       <c r="HH6" s="23">
         <f t="shared" si="6"/>
-        <v>45553</v>
+        <v>45595</v>
       </c>
       <c r="HI6" s="23">
         <f t="shared" si="6"/>
-        <v>45554</v>
+        <v>45596</v>
       </c>
       <c r="HJ6" s="23">
         <f t="shared" si="6"/>
-        <v>45555</v>
+        <v>45597</v>
       </c>
       <c r="HK6" s="23">
         <f t="shared" si="6"/>
-        <v>45556</v>
+        <v>45598</v>
       </c>
       <c r="HL6" s="47">
         <f t="shared" si="6"/>
-        <v>45557</v>
+        <v>45599</v>
       </c>
       <c r="HM6" s="44">
         <f t="shared" si="6"/>
-        <v>45558</v>
+        <v>45600</v>
       </c>
       <c r="HN6" s="23">
         <f t="shared" si="6"/>
-        <v>45559</v>
+        <v>45601</v>
       </c>
       <c r="HO6" s="23">
         <f t="shared" si="6"/>
-        <v>45560</v>
+        <v>45602</v>
       </c>
       <c r="HP6" s="23">
         <f t="shared" si="6"/>
-        <v>45561</v>
+        <v>45603</v>
       </c>
       <c r="HQ6" s="23">
         <f t="shared" si="6"/>
-        <v>45562</v>
+        <v>45604</v>
       </c>
       <c r="HR6" s="23">
         <f t="shared" si="6"/>
-        <v>45563</v>
+        <v>45605</v>
       </c>
       <c r="HS6" s="45">
         <f t="shared" ref="HS6:IT6" si="7">HR6+1</f>
-        <v>45564</v>
+        <v>45606</v>
       </c>
       <c r="HT6" s="46">
         <f t="shared" si="7"/>
-        <v>45565</v>
+        <v>45607</v>
       </c>
       <c r="HU6" s="23">
         <f t="shared" si="7"/>
-        <v>45566</v>
+        <v>45608</v>
       </c>
       <c r="HV6" s="23">
         <f t="shared" si="7"/>
-        <v>45567</v>
+        <v>45609</v>
       </c>
       <c r="HW6" s="23">
         <f t="shared" si="7"/>
-        <v>45568</v>
+        <v>45610</v>
       </c>
       <c r="HX6" s="23">
         <f t="shared" si="7"/>
-        <v>45569</v>
+        <v>45611</v>
       </c>
       <c r="HY6" s="23">
         <f t="shared" si="7"/>
-        <v>45570</v>
+        <v>45612</v>
       </c>
       <c r="HZ6" s="47">
         <f t="shared" si="7"/>
-        <v>45571</v>
+        <v>45613</v>
       </c>
       <c r="IA6" s="44">
         <f t="shared" si="7"/>
-        <v>45572</v>
+        <v>45614</v>
       </c>
       <c r="IB6" s="23">
         <f t="shared" si="7"/>
-        <v>45573</v>
+        <v>45615</v>
       </c>
       <c r="IC6" s="23">
         <f t="shared" si="7"/>
-        <v>45574</v>
+        <v>45616</v>
       </c>
       <c r="ID6" s="23">
         <f t="shared" si="7"/>
-        <v>45575</v>
+        <v>45617</v>
       </c>
       <c r="IE6" s="23">
         <f t="shared" si="7"/>
-        <v>45576</v>
+        <v>45618</v>
       </c>
       <c r="IF6" s="23">
         <f t="shared" si="7"/>
-        <v>45577</v>
+        <v>45619</v>
       </c>
       <c r="IG6" s="45">
         <f t="shared" si="7"/>
-        <v>45578</v>
+        <v>45620</v>
       </c>
       <c r="IH6" s="46">
         <f t="shared" si="7"/>
-        <v>45579</v>
+        <v>45621</v>
       </c>
       <c r="II6" s="23">
         <f t="shared" si="7"/>
-        <v>45580</v>
+        <v>45622</v>
       </c>
       <c r="IJ6" s="23">
         <f t="shared" si="7"/>
-        <v>45581</v>
+        <v>45623</v>
       </c>
       <c r="IK6" s="23">
         <f t="shared" si="7"/>
-        <v>45582</v>
+        <v>45624</v>
       </c>
       <c r="IL6" s="23">
         <f t="shared" si="7"/>
-        <v>45583</v>
+        <v>45625</v>
       </c>
       <c r="IM6" s="23">
         <f t="shared" si="7"/>
-        <v>45584</v>
+        <v>45626</v>
       </c>
       <c r="IN6" s="47">
         <f t="shared" si="7"/>
-        <v>45585</v>
+        <v>45627</v>
       </c>
       <c r="IO6" s="44">
         <f t="shared" si="7"/>
-        <v>45586</v>
+        <v>45628</v>
       </c>
       <c r="IP6" s="23">
         <f t="shared" si="7"/>
-        <v>45587</v>
+        <v>45629</v>
       </c>
       <c r="IQ6" s="23">
         <f t="shared" si="7"/>
-        <v>45588</v>
+        <v>45630</v>
       </c>
       <c r="IR6" s="23">
         <f t="shared" si="7"/>
-        <v>45589</v>
+        <v>45631</v>
       </c>
       <c r="IS6" s="23">
         <f t="shared" si="7"/>
-        <v>45590</v>
+        <v>45632</v>
       </c>
       <c r="IT6" s="23">
         <f t="shared" si="7"/>
-        <v>45591</v>
+        <v>45633</v>
       </c>
       <c r="IU6" s="45"/>
     </row>
@@ -6180,7 +6175,7 @@
       </c>
       <c r="IU7" s="31"/>
     </row>
-    <row r="8" spans="1:255" s="176" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:255" s="176" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="169" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -6442,7 +6437,7 @@
       <c r="IT8" s="172"/>
       <c r="IU8" s="172"/>
     </row>
-    <row r="9" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="143">
         <v>1</v>
       </c>
@@ -6715,7 +6710,7 @@
       <c r="IT9" s="152"/>
       <c r="IU9" s="152"/>
     </row>
-    <row r="10" spans="1:255" s="153" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:255" s="153" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="143" t="str">
         <f t="shared" ref="A10:A19" si="18">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1</v>
@@ -6989,7 +6984,7 @@
       <c r="IT10" s="152"/>
       <c r="IU10" s="152"/>
     </row>
-    <row r="11" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.1</v>
@@ -7263,7 +7258,7 @@
       <c r="IT11" s="152"/>
       <c r="IU11" s="152"/>
     </row>
-    <row r="12" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.2</v>
@@ -7538,7 +7533,7 @@
       <c r="IT12" s="152"/>
       <c r="IU12" s="152"/>
     </row>
-    <row r="13" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.3</v>
@@ -7812,7 +7807,7 @@
       <c r="IT13" s="152"/>
       <c r="IU13" s="152"/>
     </row>
-    <row r="14" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.4</v>
@@ -8089,7 +8084,7 @@
       <c r="IT14" s="152"/>
       <c r="IU14" s="152"/>
     </row>
-    <row r="15" spans="1:255" s="153" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:255" s="153" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.5</v>
@@ -8366,7 +8361,7 @@
       <c r="IT15" s="152"/>
       <c r="IU15" s="152"/>
     </row>
-    <row r="16" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.6</v>
@@ -8642,7 +8637,7 @@
       <c r="IT16" s="152"/>
       <c r="IU16" s="152"/>
     </row>
-    <row r="17" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.7</v>
@@ -8918,7 +8913,7 @@
       <c r="IT17" s="152"/>
       <c r="IU17" s="152"/>
     </row>
-    <row r="18" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.8</v>
@@ -9192,7 +9187,7 @@
       <c r="IT18" s="152"/>
       <c r="IU18" s="152"/>
     </row>
-    <row r="19" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.9</v>
@@ -9468,7 +9463,7 @@
       <c r="IT19" s="152"/>
       <c r="IU19" s="152"/>
     </row>
-    <row r="20" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="143"/>
       <c r="B20" s="144" t="s">
         <v>32</v>
@@ -9742,7 +9737,7 @@
       <c r="IT20" s="152"/>
       <c r="IU20" s="152"/>
     </row>
-    <row r="21" spans="1:255" s="153" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="143"/>
       <c r="B21" s="144" t="s">
         <v>31</v>
@@ -10016,7 +10011,7 @@
       <c r="IT21" s="152"/>
       <c r="IU21" s="152"/>
     </row>
-    <row r="22" spans="1:255" s="93" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:255" s="93" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="159">
         <v>2</v>
       </c>
@@ -10277,7 +10272,7 @@
       <c r="IT22" s="92"/>
       <c r="IU22" s="92"/>
     </row>
-    <row r="23" spans="1:255" s="105" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:255" s="105" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="95">
         <v>2</v>
       </c>
@@ -10292,17 +10287,17 @@
       </c>
       <c r="F23" s="100">
         <f t="shared" ref="F23:F36" si="21">IF(ISBLANK(E23)," - ",IF(G23=0,E23,E23+G23-1))</f>
-        <v>45432</v>
+        <v>45429</v>
       </c>
       <c r="G23" s="101">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H23" s="102">
         <v>0.3</v>
       </c>
       <c r="I23" s="190">
         <f t="shared" ref="I23:I36" si="22">IF(OR(F23=0,E23=0),0,NETWORKDAYS(E23,F23))</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J23" s="103"/>
       <c r="K23" s="104"/>
@@ -10551,7 +10546,7 @@
       <c r="IT23" s="104"/>
       <c r="IU23" s="104"/>
     </row>
-    <row r="24" spans="1:255" s="105" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:255" s="105" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="95">
         <v>2.1</v>
       </c>
@@ -10825,7 +10820,7 @@
       <c r="IT24" s="104"/>
       <c r="IU24" s="104"/>
     </row>
-    <row r="25" spans="1:255" s="105" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:255" s="105" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="95">
         <v>2.2000000000000002</v>
       </c>
@@ -11099,7 +11094,7 @@
       <c r="IT25" s="104"/>
       <c r="IU25" s="104"/>
     </row>
-    <row r="26" spans="1:255" s="105" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:255" s="105" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="95">
         <v>2.2999999999999998</v>
       </c>
@@ -11373,7 +11368,7 @@
       <c r="IT26" s="104"/>
       <c r="IU26" s="104"/>
     </row>
-    <row r="27" spans="1:255" s="105" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:255" s="105" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="95">
         <v>2.4</v>
       </c>
@@ -11394,7 +11389,7 @@
         <v>16</v>
       </c>
       <c r="H27" s="102">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="I27" s="191">
         <f t="shared" si="22"/>
@@ -11647,16 +11642,14 @@
       <c r="IT27" s="104"/>
       <c r="IU27" s="104"/>
     </row>
-    <row r="28" spans="1:255" s="105" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:255" s="105" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="95">
         <v>2.5</v>
       </c>
       <c r="B28" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="97">
-        <v>2</v>
-      </c>
+      <c r="C28" s="97"/>
       <c r="D28" s="98"/>
       <c r="E28" s="99">
         <f>F27+1</f>
@@ -11664,17 +11657,17 @@
       </c>
       <c r="F28" s="100">
         <f t="shared" si="21"/>
-        <v>45401</v>
+        <v>45404</v>
       </c>
       <c r="G28" s="101">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H28" s="102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="191">
         <f t="shared" si="22"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J28" s="103"/>
       <c r="K28" s="104"/>
@@ -11923,7 +11916,7 @@
       <c r="IT28" s="104"/>
       <c r="IU28" s="104"/>
     </row>
-    <row r="29" spans="1:255" s="105" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="95">
         <v>2.6</v>
       </c>
@@ -12199,7 +12192,7 @@
       <c r="IT29" s="104"/>
       <c r="IU29" s="104"/>
     </row>
-    <row r="30" spans="1:255" s="105" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:255" s="105" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="95">
         <v>2.7</v>
       </c>
@@ -12475,7 +12468,7 @@
       <c r="IT30" s="104"/>
       <c r="IU30" s="104"/>
     </row>
-    <row r="31" spans="1:255" s="105" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="95">
         <v>2.8</v>
       </c>
@@ -12490,17 +12483,17 @@
       </c>
       <c r="F31" s="100">
         <f t="shared" si="21"/>
-        <v>45425</v>
+        <v>45424</v>
       </c>
       <c r="G31" s="101">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H31" s="102">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="I31" s="191">
         <f t="shared" si="22"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J31" s="103"/>
       <c r="K31" s="104"/>
@@ -12749,7 +12742,7 @@
       <c r="IT31" s="104"/>
       <c r="IU31" s="104"/>
     </row>
-    <row r="32" spans="1:255" s="105" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:255" s="105" customFormat="1" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="95" t="s">
         <v>65</v>
       </c>
@@ -13023,7 +13016,7 @@
       <c r="IT32" s="104"/>
       <c r="IU32" s="104"/>
     </row>
-    <row r="33" spans="1:255" s="105" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="95" t="s">
         <v>66</v>
       </c>
@@ -13297,7 +13290,7 @@
       <c r="IT33" s="104"/>
       <c r="IU33" s="104"/>
     </row>
-    <row r="34" spans="1:255" s="105" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="95" t="s">
         <v>67</v>
       </c>
@@ -13312,17 +13305,17 @@
       </c>
       <c r="F34" s="100">
         <f t="shared" si="21"/>
-        <v>45425</v>
+        <v>45424</v>
       </c>
       <c r="G34" s="101">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H34" s="102">
         <v>0</v>
       </c>
       <c r="I34" s="191">
         <f t="shared" si="22"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J34" s="103"/>
       <c r="K34" s="104"/>
@@ -13571,8 +13564,7 @@
       <c r="IT34" s="104"/>
       <c r="IU34" s="104"/>
     </row>
-    <row r="35" spans="1:255" s="105" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A35" s="95"/>
+    <row r="35" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B35" s="96" t="s">
         <v>37</v>
       </c>
@@ -13582,11 +13574,11 @@
       <c r="D35" s="98"/>
       <c r="E35" s="99">
         <f>E36-5</f>
-        <v>45427</v>
+        <v>45424</v>
       </c>
       <c r="F35" s="100">
         <f t="shared" si="21"/>
-        <v>45427</v>
+        <v>45424</v>
       </c>
       <c r="G35" s="101">
         <v>1</v>
@@ -13596,7 +13588,7 @@
       </c>
       <c r="I35" s="191">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" s="103"/>
       <c r="K35" s="104"/>
@@ -13845,7 +13837,7 @@
       <c r="IT35" s="104"/>
       <c r="IU35" s="104"/>
     </row>
-    <row r="36" spans="1:255" s="105" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="95"/>
       <c r="B36" s="96" t="s">
         <v>36</v>
@@ -13855,12 +13847,11 @@
       </c>
       <c r="D36" s="98"/>
       <c r="E36" s="99">
-        <f>F23</f>
-        <v>45432</v>
+        <v>45429</v>
       </c>
       <c r="F36" s="100">
         <f t="shared" si="21"/>
-        <v>45432</v>
+        <v>45429</v>
       </c>
       <c r="G36" s="101">
         <v>1</v>
@@ -14119,7 +14110,7 @@
       <c r="IT36" s="104"/>
       <c r="IU36" s="104"/>
     </row>
-    <row r="37" spans="1:255" s="113" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:255" s="113" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="106">
         <v>3</v>
       </c>
@@ -14380,7 +14371,7 @@
       <c r="IT37" s="109"/>
       <c r="IU37" s="109"/>
     </row>
-    <row r="38" spans="1:255" s="121" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="114">
         <v>3</v>
       </c>
@@ -14391,21 +14382,21 @@
       <c r="D38" s="156"/>
       <c r="E38" s="115">
         <f>$F$23+1</f>
-        <v>45433</v>
+        <v>45430</v>
       </c>
       <c r="F38" s="116">
         <f t="shared" ref="F38:F43" si="23">IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
         <v>45502</v>
       </c>
       <c r="G38" s="117">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H38" s="118">
         <v>0</v>
       </c>
       <c r="I38" s="184">
         <f t="shared" ref="I38:I47" si="24">IF(OR(F38=0,E38=0),0,NETWORKDAYS(E38,F38))</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J38" s="119"/>
       <c r="K38" s="120"/>
@@ -14654,7 +14645,7 @@
       <c r="IT38" s="120"/>
       <c r="IU38" s="120"/>
     </row>
-    <row r="39" spans="1:255" s="121" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:255" s="121" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="114">
         <v>3.1</v>
       </c>
@@ -14665,11 +14656,11 @@
       <c r="D39" s="156"/>
       <c r="E39" s="115">
         <f>E40</f>
-        <v>45433</v>
+        <v>45430</v>
       </c>
       <c r="F39" s="116">
         <f>IF(ISBLANK(E39)," - ",IF(G39=0,E39,E39+G39-1))</f>
-        <v>45436</v>
+        <v>45433</v>
       </c>
       <c r="G39" s="117">
         <v>4</v>
@@ -14679,7 +14670,7 @@
       </c>
       <c r="I39" s="185">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J39" s="119"/>
       <c r="K39" s="120"/>
@@ -14928,7 +14919,7 @@
       <c r="IT39" s="120"/>
       <c r="IU39" s="120"/>
     </row>
-    <row r="40" spans="1:255" s="121" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:255" s="121" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="114">
         <v>3.2</v>
       </c>
@@ -14939,11 +14930,11 @@
       <c r="D40" s="156"/>
       <c r="E40" s="115">
         <f>E38</f>
-        <v>45433</v>
+        <v>45430</v>
       </c>
       <c r="F40" s="116">
         <f t="shared" si="23"/>
-        <v>45439</v>
+        <v>45436</v>
       </c>
       <c r="G40" s="117">
         <v>7</v>
@@ -15202,7 +15193,7 @@
       <c r="IT40" s="120"/>
       <c r="IU40" s="120"/>
     </row>
-    <row r="41" spans="1:255" s="121" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:255" s="121" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="114">
         <v>3.3</v>
       </c>
@@ -15213,11 +15204,11 @@
       <c r="D41" s="156"/>
       <c r="E41" s="115">
         <f>MAX(F40,F39)+1</f>
-        <v>45440</v>
+        <v>45437</v>
       </c>
       <c r="F41" s="116">
         <f t="shared" si="23"/>
-        <v>45457</v>
+        <v>45454</v>
       </c>
       <c r="G41" s="117">
         <v>18</v>
@@ -15227,7 +15218,7 @@
       </c>
       <c r="I41" s="185">
         <f t="shared" si="24"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J41" s="119"/>
       <c r="K41" s="120"/>
@@ -15476,7 +15467,7 @@
       <c r="IT41" s="120"/>
       <c r="IU41" s="120"/>
     </row>
-    <row r="42" spans="1:255" s="121" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:255" s="121" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="114">
         <v>3.4</v>
       </c>
@@ -15487,11 +15478,11 @@
       <c r="D42" s="156"/>
       <c r="E42" s="115">
         <f>F41+1</f>
-        <v>45458</v>
+        <v>45455</v>
       </c>
       <c r="F42" s="116">
         <f>IF(ISBLANK(E42)," - ",IF(G42=0,E42,E42+G42-1))</f>
-        <v>45489</v>
+        <v>45486</v>
       </c>
       <c r="G42" s="117">
         <v>32</v>
@@ -15501,7 +15492,7 @@
       </c>
       <c r="I42" s="185">
         <f t="shared" si="24"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J42" s="119"/>
       <c r="K42" s="120"/>
@@ -15750,7 +15741,7 @@
       <c r="IT42" s="120"/>
       <c r="IU42" s="120"/>
     </row>
-    <row r="43" spans="1:255" s="121" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="114" t="s">
         <v>68</v>
       </c>
@@ -15761,11 +15752,11 @@
       <c r="D43" s="156"/>
       <c r="E43" s="115">
         <f>E42</f>
-        <v>45458</v>
+        <v>45455</v>
       </c>
       <c r="F43" s="116">
         <f t="shared" si="23"/>
-        <v>45463</v>
+        <v>45460</v>
       </c>
       <c r="G43" s="117">
         <v>6</v>
@@ -16024,7 +16015,7 @@
       <c r="IT43" s="120"/>
       <c r="IU43" s="120"/>
     </row>
-    <row r="44" spans="1:255" s="121" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:255" s="121" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="114" t="s">
         <v>69</v>
       </c>
@@ -16035,11 +16026,11 @@
       <c r="D44" s="156"/>
       <c r="E44" s="115">
         <f>F43+1</f>
-        <v>45464</v>
+        <v>45461</v>
       </c>
       <c r="F44" s="116">
         <f>IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
-        <v>45468</v>
+        <v>45465</v>
       </c>
       <c r="G44" s="117">
         <v>5</v>
@@ -16049,7 +16040,7 @@
       </c>
       <c r="I44" s="185">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J44" s="119"/>
       <c r="K44" s="120"/>
@@ -16298,7 +16289,7 @@
       <c r="IT44" s="120"/>
       <c r="IU44" s="120"/>
     </row>
-    <row r="45" spans="1:255" s="121" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:255" s="121" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="114" t="s">
         <v>70</v>
       </c>
@@ -16309,11 +16300,11 @@
       <c r="D45" s="156"/>
       <c r="E45" s="115">
         <f>F44+1</f>
-        <v>45469</v>
+        <v>45466</v>
       </c>
       <c r="F45" s="116">
         <f>IF(ISBLANK(E45)," - ",IF(G45=0,E45,E45+G45-1))</f>
-        <v>45489</v>
+        <v>45486</v>
       </c>
       <c r="G45" s="117">
         <v>21</v>
@@ -16572,7 +16563,7 @@
       <c r="IT45" s="120"/>
       <c r="IU45" s="120"/>
     </row>
-    <row r="46" spans="1:255" s="121" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="114"/>
       <c r="B46" s="154" t="s">
         <v>29</v>
@@ -16846,7 +16837,7 @@
       <c r="IT46" s="120"/>
       <c r="IU46" s="120"/>
     </row>
-    <row r="47" spans="1:255" s="121" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="114"/>
       <c r="B47" s="154" t="s">
         <v>30</v>
@@ -17120,7 +17111,7 @@
       <c r="IT47" s="120"/>
       <c r="IU47" s="120"/>
     </row>
-    <row r="48" spans="1:255" s="131" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:255" s="131" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="122">
         <v>4</v>
       </c>
@@ -17381,7 +17372,7 @@
       <c r="IT48" s="125"/>
       <c r="IU48" s="125"/>
     </row>
-    <row r="49" spans="1:255" s="142" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:255" s="142" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
@@ -17656,7 +17647,7 @@
       <c r="IT49" s="141"/>
       <c r="IU49" s="141"/>
     </row>
-    <row r="50" spans="1:255" s="142" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:255" s="142" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.1</v>
@@ -17933,7 +17924,7 @@
       <c r="IT50" s="141"/>
       <c r="IU50" s="141"/>
     </row>
-    <row r="51" spans="1:255" s="142" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:255" s="142" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.2</v>
@@ -18209,7 +18200,7 @@
       <c r="IT51" s="141"/>
       <c r="IU51" s="141"/>
     </row>
-    <row r="52" spans="1:255" s="142" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:255" s="142" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.3</v>
@@ -18486,7 +18477,7 @@
       <c r="IT52" s="141"/>
       <c r="IU52" s="141"/>
     </row>
-    <row r="54" spans="1:255" s="9" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:255" s="9" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="65" t="s">
         <v>1</v>
       </c>
@@ -18745,7 +18736,7 @@
       <c r="IT54" s="3"/>
       <c r="IU54" s="3"/>
     </row>
-    <row r="55" spans="1:255" s="8" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:255" s="8" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A55" s="66" t="s">
         <v>16</v>
       </c>
@@ -19000,7 +18991,7 @@
       <c r="IT55" s="3"/>
       <c r="IU55" s="3"/>
     </row>
-    <row r="56" spans="1:255" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:255" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="54" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -19264,7 +19255,7 @@
       <c r="IT56" s="3"/>
       <c r="IU56" s="3"/>
     </row>
-    <row r="57" spans="1:255" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:255" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -19536,7 +19527,7 @@
       <c r="IT57" s="3"/>
       <c r="IU57" s="3"/>
     </row>
-    <row r="58" spans="1:255" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:255" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -19808,7 +19799,7 @@
       <c r="IT58" s="3"/>
       <c r="IU58" s="3"/>
     </row>
-    <row r="59" spans="1:255" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:255" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
@@ -20078,7 +20069,7 @@
       <c r="IT59" s="3"/>
       <c r="IU59" s="3"/>
     </row>
-    <row r="60" spans="1:255" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:255" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="80" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
@@ -20088,8 +20079,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="73">
@@ -20228,13 +20219,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>28</xdr:col>
-                    <xdr:colOff>99060</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>

</xml_diff>

<commit_message>
more notes, more pictures, more everything
</commit_message>
<xml_diff>
--- a/thesis gantt chart.xlsx
+++ b/thesis gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wings_stuff\srus\TUD\yr5\thesis\thesis_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80792EFB-488D-42B6-9481-2D0607ACAD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97009757-4C39-411C-95C7-AE203D141E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -2630,28 +2630,40 @@
     <xf numFmtId="0" fontId="28" fillId="35" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="59" fillId="23" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="23" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="41" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="41" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="23" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="23" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="63" fillId="24" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -2688,18 +2700,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="41" fillId="23" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2957,13 +2957,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>10886</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>103414</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -3298,69 +3298,69 @@
   <dimension ref="A1:IU63"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+      <pane ySplit="7" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AR36" sqref="AR36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.61328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.15234375" style="1" customWidth="1"/>
     <col min="3" max="3" width="4" style="91" customWidth="1"/>
-    <col min="4" max="4" width="0.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.86328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.86328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="0.59765625" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.3984375" style="1" customWidth="1"/>
-    <col min="67" max="68" width="2.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="2.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="2.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="74" width="1.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="2.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="99" width="2.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="100" max="102" width="1.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="2.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="105" max="106" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="107" max="108" width="1.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="109" max="131" width="2.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="2.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="134" max="137" width="1.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="139" max="162" width="2.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="163" max="165" width="1.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="2.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="168" max="169" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="170" max="192" width="2.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="1.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="2.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="196" max="197" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="198" max="200" width="1.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="202" max="221" width="2.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="2.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="225" max="227" width="1.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="0.84375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.15234375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.61328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.84375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.15234375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.84375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="0.61328125" style="1" customWidth="1"/>
+    <col min="11" max="66" width="2.3828125" style="1" customWidth="1"/>
+    <col min="67" max="68" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="74" width="1.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="99" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="100" max="102" width="1.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="105" max="106" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="107" max="108" width="1.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="109" max="131" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="134" max="137" width="1.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="139" max="162" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="163" max="165" width="1.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="168" max="169" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="170" max="192" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="1.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="196" max="197" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="198" max="200" width="1.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="202" max="221" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="225" max="227" width="1.84375" style="1" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="1.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="2.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="231" max="252" width="2.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="253" max="254" width="2.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="1.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="256" max="16384" width="9.1328125" style="1"/>
+    <col min="229" max="229" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="231" max="252" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="253" max="254" width="2.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="1.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="256" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="12" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:255" s="12" customFormat="1" ht="24.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
         <v>24</v>
       </c>
@@ -3373,23 +3373,23 @@
       <c r="K1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="204"/>
-      <c r="AE1" s="204"/>
-      <c r="AF1" s="204"/>
-      <c r="AG1" s="204"/>
-      <c r="AH1" s="204"/>
-      <c r="AI1" s="204"/>
-      <c r="AJ1" s="204"/>
-      <c r="AK1" s="204"/>
-      <c r="AL1" s="204"/>
-      <c r="AM1" s="204"/>
-      <c r="AN1" s="204"/>
-      <c r="AO1" s="204"/>
-      <c r="AP1" s="204"/>
-      <c r="AQ1" s="204"/>
-      <c r="AR1" s="204"/>
+      <c r="AD1" s="208"/>
+      <c r="AE1" s="208"/>
+      <c r="AF1" s="208"/>
+      <c r="AG1" s="208"/>
+      <c r="AH1" s="208"/>
+      <c r="AI1" s="208"/>
+      <c r="AJ1" s="208"/>
+      <c r="AK1" s="208"/>
+      <c r="AL1" s="208"/>
+      <c r="AM1" s="208"/>
+      <c r="AN1" s="208"/>
+      <c r="AO1" s="208"/>
+      <c r="AP1" s="208"/>
+      <c r="AQ1" s="208"/>
+      <c r="AR1" s="208"/>
     </row>
-    <row r="2" spans="1:255" s="28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:255" s="28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="72" t="s">
         <v>25</v>
       </c>
@@ -3399,7 +3399,7 @@
       <c r="E2" s="25"/>
       <c r="F2" s="27"/>
     </row>
-    <row r="3" spans="1:255" s="61" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:255" s="61" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="57"/>
       <c r="B3" s="58"/>
       <c r="C3" s="83"/>
@@ -3463,735 +3463,735 @@
       <c r="BM3" s="76"/>
       <c r="BN3" s="77"/>
     </row>
-    <row r="4" spans="1:255" s="70" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:255" s="70" customFormat="1" ht="17.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="207">
+      <c r="C4" s="211">
         <v>45295</v>
       </c>
-      <c r="D4" s="208"/>
-      <c r="E4" s="209"/>
+      <c r="D4" s="212"/>
+      <c r="E4" s="213"/>
       <c r="H4" s="73" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="74">
         <v>23</v>
       </c>
-      <c r="K4" s="199"/>
-      <c r="L4" s="200"/>
-      <c r="M4" s="200"/>
-      <c r="N4" s="200"/>
-      <c r="O4" s="200"/>
-      <c r="P4" s="200"/>
-      <c r="Q4" s="201"/>
-      <c r="R4" s="199" t="str">
+      <c r="K4" s="196"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="197"/>
+      <c r="N4" s="197"/>
+      <c r="O4" s="197"/>
+      <c r="P4" s="197"/>
+      <c r="Q4" s="198"/>
+      <c r="R4" s="196" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="S4" s="200"/>
-      <c r="T4" s="200"/>
-      <c r="U4" s="200"/>
-      <c r="V4" s="200"/>
-      <c r="W4" s="200"/>
-      <c r="X4" s="201"/>
-      <c r="Y4" s="199" t="str">
+      <c r="S4" s="197"/>
+      <c r="T4" s="197"/>
+      <c r="U4" s="197"/>
+      <c r="V4" s="197"/>
+      <c r="W4" s="197"/>
+      <c r="X4" s="198"/>
+      <c r="Y4" s="196" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="Z4" s="200"/>
-      <c r="AA4" s="200"/>
-      <c r="AB4" s="200"/>
-      <c r="AC4" s="200"/>
-      <c r="AD4" s="200"/>
-      <c r="AE4" s="201"/>
-      <c r="AF4" s="199" t="str">
+      <c r="Z4" s="197"/>
+      <c r="AA4" s="197"/>
+      <c r="AB4" s="197"/>
+      <c r="AC4" s="197"/>
+      <c r="AD4" s="197"/>
+      <c r="AE4" s="198"/>
+      <c r="AF4" s="196" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AG4" s="200"/>
-      <c r="AH4" s="200"/>
-      <c r="AI4" s="200"/>
-      <c r="AJ4" s="200"/>
-      <c r="AK4" s="200"/>
-      <c r="AL4" s="201"/>
-      <c r="AM4" s="199" t="str">
+      <c r="AG4" s="197"/>
+      <c r="AH4" s="197"/>
+      <c r="AI4" s="197"/>
+      <c r="AJ4" s="197"/>
+      <c r="AK4" s="197"/>
+      <c r="AL4" s="198"/>
+      <c r="AM4" s="196" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="AN4" s="200"/>
-      <c r="AO4" s="200"/>
-      <c r="AP4" s="200"/>
-      <c r="AQ4" s="200"/>
-      <c r="AR4" s="200"/>
-      <c r="AS4" s="201"/>
-      <c r="AT4" s="199" t="str">
+      <c r="AN4" s="197"/>
+      <c r="AO4" s="197"/>
+      <c r="AP4" s="197"/>
+      <c r="AQ4" s="197"/>
+      <c r="AR4" s="197"/>
+      <c r="AS4" s="198"/>
+      <c r="AT4" s="196" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AU4" s="200"/>
-      <c r="AV4" s="200"/>
-      <c r="AW4" s="200"/>
-      <c r="AX4" s="200"/>
-      <c r="AY4" s="200"/>
-      <c r="AZ4" s="201"/>
-      <c r="BA4" s="199" t="str">
+      <c r="AU4" s="197"/>
+      <c r="AV4" s="197"/>
+      <c r="AW4" s="197"/>
+      <c r="AX4" s="197"/>
+      <c r="AY4" s="197"/>
+      <c r="AZ4" s="198"/>
+      <c r="BA4" s="196" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="BB4" s="200"/>
-      <c r="BC4" s="200"/>
-      <c r="BD4" s="200"/>
-      <c r="BE4" s="200"/>
-      <c r="BF4" s="200"/>
-      <c r="BG4" s="201"/>
-      <c r="BH4" s="199" t="str">
+      <c r="BB4" s="197"/>
+      <c r="BC4" s="197"/>
+      <c r="BD4" s="197"/>
+      <c r="BE4" s="197"/>
+      <c r="BF4" s="197"/>
+      <c r="BG4" s="198"/>
+      <c r="BH4" s="196" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="BI4" s="200"/>
-      <c r="BJ4" s="200"/>
-      <c r="BK4" s="200"/>
-      <c r="BL4" s="200"/>
-      <c r="BM4" s="200"/>
-      <c r="BN4" s="201"/>
-      <c r="BO4" s="199" t="str">
+      <c r="BI4" s="197"/>
+      <c r="BJ4" s="197"/>
+      <c r="BK4" s="197"/>
+      <c r="BL4" s="197"/>
+      <c r="BM4" s="197"/>
+      <c r="BN4" s="198"/>
+      <c r="BO4" s="196" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="BP4" s="200"/>
-      <c r="BQ4" s="200"/>
-      <c r="BR4" s="200"/>
-      <c r="BS4" s="200"/>
-      <c r="BT4" s="200"/>
-      <c r="BU4" s="201"/>
-      <c r="BV4" s="199" t="str">
+      <c r="BP4" s="197"/>
+      <c r="BQ4" s="197"/>
+      <c r="BR4" s="197"/>
+      <c r="BS4" s="197"/>
+      <c r="BT4" s="197"/>
+      <c r="BU4" s="198"/>
+      <c r="BV4" s="196" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BW4" s="200"/>
-      <c r="BX4" s="200"/>
-      <c r="BY4" s="200"/>
-      <c r="BZ4" s="200"/>
-      <c r="CA4" s="200"/>
-      <c r="CB4" s="201"/>
-      <c r="CC4" s="199" t="str">
+      <c r="BW4" s="197"/>
+      <c r="BX4" s="197"/>
+      <c r="BY4" s="197"/>
+      <c r="BZ4" s="197"/>
+      <c r="CA4" s="197"/>
+      <c r="CB4" s="198"/>
+      <c r="CC4" s="196" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="CD4" s="200"/>
-      <c r="CE4" s="200"/>
-      <c r="CF4" s="200"/>
-      <c r="CG4" s="200"/>
-      <c r="CH4" s="200"/>
-      <c r="CI4" s="201"/>
-      <c r="CJ4" s="199" t="str">
+      <c r="CD4" s="197"/>
+      <c r="CE4" s="197"/>
+      <c r="CF4" s="197"/>
+      <c r="CG4" s="197"/>
+      <c r="CH4" s="197"/>
+      <c r="CI4" s="198"/>
+      <c r="CJ4" s="196" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 33</v>
       </c>
-      <c r="CK4" s="200"/>
-      <c r="CL4" s="200"/>
-      <c r="CM4" s="200"/>
-      <c r="CN4" s="200"/>
-      <c r="CO4" s="200"/>
-      <c r="CP4" s="201"/>
-      <c r="CQ4" s="199" t="str">
+      <c r="CK4" s="197"/>
+      <c r="CL4" s="197"/>
+      <c r="CM4" s="197"/>
+      <c r="CN4" s="197"/>
+      <c r="CO4" s="197"/>
+      <c r="CP4" s="198"/>
+      <c r="CQ4" s="196" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 34</v>
       </c>
-      <c r="CR4" s="200"/>
-      <c r="CS4" s="200"/>
-      <c r="CT4" s="200"/>
-      <c r="CU4" s="200"/>
-      <c r="CV4" s="200"/>
-      <c r="CW4" s="201"/>
-      <c r="CX4" s="199" t="str">
+      <c r="CR4" s="197"/>
+      <c r="CS4" s="197"/>
+      <c r="CT4" s="197"/>
+      <c r="CU4" s="197"/>
+      <c r="CV4" s="197"/>
+      <c r="CW4" s="198"/>
+      <c r="CX4" s="196" t="str">
         <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 35</v>
       </c>
-      <c r="CY4" s="200"/>
-      <c r="CZ4" s="200"/>
-      <c r="DA4" s="200"/>
-      <c r="DB4" s="200"/>
-      <c r="DC4" s="200"/>
-      <c r="DD4" s="201"/>
-      <c r="DE4" s="199" t="str">
+      <c r="CY4" s="197"/>
+      <c r="CZ4" s="197"/>
+      <c r="DA4" s="197"/>
+      <c r="DB4" s="197"/>
+      <c r="DC4" s="197"/>
+      <c r="DD4" s="198"/>
+      <c r="DE4" s="196" t="str">
         <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 36</v>
       </c>
-      <c r="DF4" s="200"/>
-      <c r="DG4" s="200"/>
-      <c r="DH4" s="200"/>
-      <c r="DI4" s="200"/>
-      <c r="DJ4" s="200"/>
-      <c r="DK4" s="201"/>
-      <c r="DL4" s="199" t="str">
+      <c r="DF4" s="197"/>
+      <c r="DG4" s="197"/>
+      <c r="DH4" s="197"/>
+      <c r="DI4" s="197"/>
+      <c r="DJ4" s="197"/>
+      <c r="DK4" s="198"/>
+      <c r="DL4" s="196" t="str">
         <f>"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 37</v>
       </c>
-      <c r="DM4" s="200"/>
-      <c r="DN4" s="200"/>
-      <c r="DO4" s="200"/>
-      <c r="DP4" s="200"/>
-      <c r="DQ4" s="200"/>
-      <c r="DR4" s="201"/>
-      <c r="DS4" s="199" t="str">
+      <c r="DM4" s="197"/>
+      <c r="DN4" s="197"/>
+      <c r="DO4" s="197"/>
+      <c r="DP4" s="197"/>
+      <c r="DQ4" s="197"/>
+      <c r="DR4" s="198"/>
+      <c r="DS4" s="196" t="str">
         <f>"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 38</v>
       </c>
-      <c r="DT4" s="200"/>
-      <c r="DU4" s="200"/>
-      <c r="DV4" s="200"/>
-      <c r="DW4" s="200"/>
-      <c r="DX4" s="200"/>
-      <c r="DY4" s="201"/>
-      <c r="DZ4" s="199" t="str">
+      <c r="DT4" s="197"/>
+      <c r="DU4" s="197"/>
+      <c r="DV4" s="197"/>
+      <c r="DW4" s="197"/>
+      <c r="DX4" s="197"/>
+      <c r="DY4" s="198"/>
+      <c r="DZ4" s="196" t="str">
         <f>"Week "&amp;(DS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 39</v>
       </c>
-      <c r="EA4" s="200"/>
-      <c r="EB4" s="200"/>
-      <c r="EC4" s="200"/>
-      <c r="ED4" s="200"/>
-      <c r="EE4" s="200"/>
-      <c r="EF4" s="201"/>
-      <c r="EG4" s="199" t="str">
+      <c r="EA4" s="197"/>
+      <c r="EB4" s="197"/>
+      <c r="EC4" s="197"/>
+      <c r="ED4" s="197"/>
+      <c r="EE4" s="197"/>
+      <c r="EF4" s="198"/>
+      <c r="EG4" s="196" t="str">
         <f>"Week "&amp;(DZ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 40</v>
       </c>
-      <c r="EH4" s="200"/>
-      <c r="EI4" s="200"/>
-      <c r="EJ4" s="200"/>
-      <c r="EK4" s="200"/>
-      <c r="EL4" s="200"/>
-      <c r="EM4" s="201"/>
-      <c r="EN4" s="199" t="str">
+      <c r="EH4" s="197"/>
+      <c r="EI4" s="197"/>
+      <c r="EJ4" s="197"/>
+      <c r="EK4" s="197"/>
+      <c r="EL4" s="197"/>
+      <c r="EM4" s="198"/>
+      <c r="EN4" s="196" t="str">
         <f>"Week "&amp;(EG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 41</v>
       </c>
-      <c r="EO4" s="200"/>
-      <c r="EP4" s="200"/>
-      <c r="EQ4" s="200"/>
-      <c r="ER4" s="200"/>
-      <c r="ES4" s="200"/>
-      <c r="ET4" s="201"/>
-      <c r="EU4" s="199" t="str">
+      <c r="EO4" s="197"/>
+      <c r="EP4" s="197"/>
+      <c r="EQ4" s="197"/>
+      <c r="ER4" s="197"/>
+      <c r="ES4" s="197"/>
+      <c r="ET4" s="198"/>
+      <c r="EU4" s="196" t="str">
         <f>"Week "&amp;(EN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 42</v>
       </c>
-      <c r="EV4" s="200"/>
-      <c r="EW4" s="200"/>
-      <c r="EX4" s="200"/>
-      <c r="EY4" s="200"/>
-      <c r="EZ4" s="200"/>
-      <c r="FA4" s="201"/>
-      <c r="FB4" s="199" t="str">
+      <c r="EV4" s="197"/>
+      <c r="EW4" s="197"/>
+      <c r="EX4" s="197"/>
+      <c r="EY4" s="197"/>
+      <c r="EZ4" s="197"/>
+      <c r="FA4" s="198"/>
+      <c r="FB4" s="196" t="str">
         <f>"Week "&amp;(EU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 43</v>
       </c>
-      <c r="FC4" s="200"/>
-      <c r="FD4" s="200"/>
-      <c r="FE4" s="200"/>
-      <c r="FF4" s="200"/>
-      <c r="FG4" s="200"/>
-      <c r="FH4" s="201"/>
-      <c r="FI4" s="199" t="str">
+      <c r="FC4" s="197"/>
+      <c r="FD4" s="197"/>
+      <c r="FE4" s="197"/>
+      <c r="FF4" s="197"/>
+      <c r="FG4" s="197"/>
+      <c r="FH4" s="198"/>
+      <c r="FI4" s="196" t="str">
         <f>"Week "&amp;(FB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 44</v>
       </c>
-      <c r="FJ4" s="200"/>
-      <c r="FK4" s="200"/>
-      <c r="FL4" s="200"/>
-      <c r="FM4" s="200"/>
-      <c r="FN4" s="200"/>
-      <c r="FO4" s="201"/>
-      <c r="FP4" s="199" t="str">
+      <c r="FJ4" s="197"/>
+      <c r="FK4" s="197"/>
+      <c r="FL4" s="197"/>
+      <c r="FM4" s="197"/>
+      <c r="FN4" s="197"/>
+      <c r="FO4" s="198"/>
+      <c r="FP4" s="196" t="str">
         <f>"Week "&amp;(FI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 45</v>
       </c>
-      <c r="FQ4" s="200"/>
-      <c r="FR4" s="200"/>
-      <c r="FS4" s="200"/>
-      <c r="FT4" s="200"/>
-      <c r="FU4" s="200"/>
-      <c r="FV4" s="201"/>
-      <c r="FW4" s="199" t="str">
+      <c r="FQ4" s="197"/>
+      <c r="FR4" s="197"/>
+      <c r="FS4" s="197"/>
+      <c r="FT4" s="197"/>
+      <c r="FU4" s="197"/>
+      <c r="FV4" s="198"/>
+      <c r="FW4" s="196" t="str">
         <f>"Week "&amp;(FP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 46</v>
       </c>
-      <c r="FX4" s="200"/>
-      <c r="FY4" s="200"/>
-      <c r="FZ4" s="200"/>
-      <c r="GA4" s="200"/>
-      <c r="GB4" s="200"/>
-      <c r="GC4" s="201"/>
-      <c r="GD4" s="199" t="str">
+      <c r="FX4" s="197"/>
+      <c r="FY4" s="197"/>
+      <c r="FZ4" s="197"/>
+      <c r="GA4" s="197"/>
+      <c r="GB4" s="197"/>
+      <c r="GC4" s="198"/>
+      <c r="GD4" s="196" t="str">
         <f>"Week "&amp;(FW6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 47</v>
       </c>
-      <c r="GE4" s="200"/>
-      <c r="GF4" s="200"/>
-      <c r="GG4" s="200"/>
-      <c r="GH4" s="200"/>
-      <c r="GI4" s="200"/>
-      <c r="GJ4" s="201"/>
-      <c r="GK4" s="199" t="str">
+      <c r="GE4" s="197"/>
+      <c r="GF4" s="197"/>
+      <c r="GG4" s="197"/>
+      <c r="GH4" s="197"/>
+      <c r="GI4" s="197"/>
+      <c r="GJ4" s="198"/>
+      <c r="GK4" s="196" t="str">
         <f>"Week "&amp;(GD6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 48</v>
       </c>
-      <c r="GL4" s="200"/>
-      <c r="GM4" s="200"/>
-      <c r="GN4" s="200"/>
-      <c r="GO4" s="200"/>
-      <c r="GP4" s="200"/>
-      <c r="GQ4" s="201"/>
-      <c r="GR4" s="199" t="str">
+      <c r="GL4" s="197"/>
+      <c r="GM4" s="197"/>
+      <c r="GN4" s="197"/>
+      <c r="GO4" s="197"/>
+      <c r="GP4" s="197"/>
+      <c r="GQ4" s="198"/>
+      <c r="GR4" s="196" t="str">
         <f>"Week "&amp;(GK6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 49</v>
       </c>
-      <c r="GS4" s="200"/>
-      <c r="GT4" s="200"/>
-      <c r="GU4" s="200"/>
-      <c r="GV4" s="200"/>
-      <c r="GW4" s="200"/>
-      <c r="GX4" s="201"/>
-      <c r="GY4" s="199" t="str">
+      <c r="GS4" s="197"/>
+      <c r="GT4" s="197"/>
+      <c r="GU4" s="197"/>
+      <c r="GV4" s="197"/>
+      <c r="GW4" s="197"/>
+      <c r="GX4" s="198"/>
+      <c r="GY4" s="196" t="str">
         <f>"Week "&amp;(GR6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 50</v>
       </c>
-      <c r="GZ4" s="200"/>
-      <c r="HA4" s="200"/>
-      <c r="HB4" s="200"/>
-      <c r="HC4" s="200"/>
-      <c r="HD4" s="200"/>
-      <c r="HE4" s="201"/>
-      <c r="HF4" s="199" t="str">
+      <c r="GZ4" s="197"/>
+      <c r="HA4" s="197"/>
+      <c r="HB4" s="197"/>
+      <c r="HC4" s="197"/>
+      <c r="HD4" s="197"/>
+      <c r="HE4" s="198"/>
+      <c r="HF4" s="196" t="str">
         <f>"Week "&amp;(GY6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 51</v>
       </c>
-      <c r="HG4" s="200"/>
-      <c r="HH4" s="200"/>
-      <c r="HI4" s="200"/>
-      <c r="HJ4" s="200"/>
-      <c r="HK4" s="200"/>
-      <c r="HL4" s="201"/>
-      <c r="HM4" s="199" t="str">
+      <c r="HG4" s="197"/>
+      <c r="HH4" s="197"/>
+      <c r="HI4" s="197"/>
+      <c r="HJ4" s="197"/>
+      <c r="HK4" s="197"/>
+      <c r="HL4" s="198"/>
+      <c r="HM4" s="196" t="str">
         <f>"Week "&amp;(HF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 52</v>
       </c>
-      <c r="HN4" s="200"/>
-      <c r="HO4" s="200"/>
-      <c r="HP4" s="200"/>
-      <c r="HQ4" s="200"/>
-      <c r="HR4" s="200"/>
-      <c r="HS4" s="201"/>
-      <c r="HT4" s="199" t="str">
+      <c r="HN4" s="197"/>
+      <c r="HO4" s="197"/>
+      <c r="HP4" s="197"/>
+      <c r="HQ4" s="197"/>
+      <c r="HR4" s="197"/>
+      <c r="HS4" s="198"/>
+      <c r="HT4" s="196" t="str">
         <f>"Week "&amp;(HM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 53</v>
       </c>
-      <c r="HU4" s="200"/>
-      <c r="HV4" s="200"/>
-      <c r="HW4" s="200"/>
-      <c r="HX4" s="200"/>
-      <c r="HY4" s="200"/>
-      <c r="HZ4" s="201"/>
-      <c r="IA4" s="199" t="str">
+      <c r="HU4" s="197"/>
+      <c r="HV4" s="197"/>
+      <c r="HW4" s="197"/>
+      <c r="HX4" s="197"/>
+      <c r="HY4" s="197"/>
+      <c r="HZ4" s="198"/>
+      <c r="IA4" s="196" t="str">
         <f>"Week "&amp;(HT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 54</v>
       </c>
-      <c r="IB4" s="200"/>
-      <c r="IC4" s="200"/>
-      <c r="ID4" s="200"/>
-      <c r="IE4" s="200"/>
-      <c r="IF4" s="200"/>
-      <c r="IG4" s="201"/>
-      <c r="IH4" s="199" t="str">
+      <c r="IB4" s="197"/>
+      <c r="IC4" s="197"/>
+      <c r="ID4" s="197"/>
+      <c r="IE4" s="197"/>
+      <c r="IF4" s="197"/>
+      <c r="IG4" s="198"/>
+      <c r="IH4" s="196" t="str">
         <f>"Week "&amp;(IA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 55</v>
       </c>
-      <c r="II4" s="200"/>
-      <c r="IJ4" s="200"/>
-      <c r="IK4" s="200"/>
-      <c r="IL4" s="200"/>
-      <c r="IM4" s="200"/>
-      <c r="IN4" s="201"/>
-      <c r="IO4" s="199" t="str">
+      <c r="II4" s="197"/>
+      <c r="IJ4" s="197"/>
+      <c r="IK4" s="197"/>
+      <c r="IL4" s="197"/>
+      <c r="IM4" s="197"/>
+      <c r="IN4" s="198"/>
+      <c r="IO4" s="196" t="str">
         <f>"Week "&amp;(IH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 56</v>
       </c>
-      <c r="IP4" s="200"/>
-      <c r="IQ4" s="200"/>
-      <c r="IR4" s="200"/>
-      <c r="IS4" s="200"/>
-      <c r="IT4" s="200"/>
-      <c r="IU4" s="201"/>
+      <c r="IP4" s="197"/>
+      <c r="IQ4" s="197"/>
+      <c r="IR4" s="197"/>
+      <c r="IS4" s="197"/>
+      <c r="IT4" s="197"/>
+      <c r="IU4" s="198"/>
     </row>
-    <row r="5" spans="1:255" s="24" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:255" s="24" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="71"/>
       <c r="B5" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="207" t="s">
+      <c r="C5" s="211" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="208"/>
-      <c r="E5" s="209"/>
+      <c r="D5" s="212"/>
+      <c r="E5" s="213"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
       <c r="H5" s="71"/>
       <c r="I5" s="71"/>
-      <c r="K5" s="210">
+      <c r="K5" s="214">
         <f>K6</f>
         <v>45446</v>
       </c>
-      <c r="L5" s="197"/>
-      <c r="M5" s="197"/>
-      <c r="N5" s="197"/>
-      <c r="O5" s="197"/>
-      <c r="P5" s="197"/>
-      <c r="Q5" s="212"/>
-      <c r="R5" s="210">
+      <c r="L5" s="200"/>
+      <c r="M5" s="200"/>
+      <c r="N5" s="200"/>
+      <c r="O5" s="200"/>
+      <c r="P5" s="200"/>
+      <c r="Q5" s="216"/>
+      <c r="R5" s="214">
         <f>R6</f>
         <v>45453</v>
       </c>
-      <c r="S5" s="197"/>
-      <c r="T5" s="197"/>
-      <c r="U5" s="197"/>
-      <c r="V5" s="197"/>
-      <c r="W5" s="197"/>
-      <c r="X5" s="211"/>
-      <c r="Y5" s="213">
+      <c r="S5" s="200"/>
+      <c r="T5" s="200"/>
+      <c r="U5" s="200"/>
+      <c r="V5" s="200"/>
+      <c r="W5" s="200"/>
+      <c r="X5" s="215"/>
+      <c r="Y5" s="217">
         <f>Y6</f>
         <v>45460</v>
       </c>
-      <c r="Z5" s="197"/>
-      <c r="AA5" s="197"/>
-      <c r="AB5" s="197"/>
-      <c r="AC5" s="197"/>
-      <c r="AD5" s="197"/>
-      <c r="AE5" s="214"/>
-      <c r="AF5" s="205">
+      <c r="Z5" s="200"/>
+      <c r="AA5" s="200"/>
+      <c r="AB5" s="200"/>
+      <c r="AC5" s="200"/>
+      <c r="AD5" s="200"/>
+      <c r="AE5" s="218"/>
+      <c r="AF5" s="209">
         <f>AF6</f>
         <v>45467</v>
       </c>
-      <c r="AG5" s="197"/>
-      <c r="AH5" s="197"/>
-      <c r="AI5" s="197"/>
-      <c r="AJ5" s="197"/>
-      <c r="AK5" s="197"/>
-      <c r="AL5" s="206"/>
-      <c r="AM5" s="215">
+      <c r="AG5" s="200"/>
+      <c r="AH5" s="200"/>
+      <c r="AI5" s="200"/>
+      <c r="AJ5" s="200"/>
+      <c r="AK5" s="200"/>
+      <c r="AL5" s="210"/>
+      <c r="AM5" s="202">
         <f>AM6</f>
         <v>45474</v>
       </c>
-      <c r="AN5" s="197"/>
-      <c r="AO5" s="197"/>
-      <c r="AP5" s="197"/>
-      <c r="AQ5" s="197"/>
-      <c r="AR5" s="197"/>
-      <c r="AS5" s="216"/>
-      <c r="AT5" s="217">
+      <c r="AN5" s="200"/>
+      <c r="AO5" s="200"/>
+      <c r="AP5" s="200"/>
+      <c r="AQ5" s="200"/>
+      <c r="AR5" s="200"/>
+      <c r="AS5" s="203"/>
+      <c r="AT5" s="204">
         <f>AT6</f>
         <v>45481</v>
       </c>
-      <c r="AU5" s="197"/>
-      <c r="AV5" s="197"/>
-      <c r="AW5" s="197"/>
-      <c r="AX5" s="197"/>
-      <c r="AY5" s="197"/>
-      <c r="AZ5" s="218"/>
-      <c r="BA5" s="196">
+      <c r="AU5" s="200"/>
+      <c r="AV5" s="200"/>
+      <c r="AW5" s="200"/>
+      <c r="AX5" s="200"/>
+      <c r="AY5" s="200"/>
+      <c r="AZ5" s="205"/>
+      <c r="BA5" s="206">
         <f>BA6</f>
         <v>45488</v>
       </c>
-      <c r="BB5" s="197"/>
-      <c r="BC5" s="197"/>
-      <c r="BD5" s="197"/>
-      <c r="BE5" s="197"/>
-      <c r="BF5" s="197"/>
-      <c r="BG5" s="198"/>
-      <c r="BH5" s="202">
+      <c r="BB5" s="200"/>
+      <c r="BC5" s="200"/>
+      <c r="BD5" s="200"/>
+      <c r="BE5" s="200"/>
+      <c r="BF5" s="200"/>
+      <c r="BG5" s="207"/>
+      <c r="BH5" s="199">
         <f>BH6</f>
         <v>45495</v>
       </c>
-      <c r="BI5" s="197"/>
-      <c r="BJ5" s="197"/>
-      <c r="BK5" s="197"/>
-      <c r="BL5" s="197"/>
-      <c r="BM5" s="197"/>
-      <c r="BN5" s="203"/>
-      <c r="BO5" s="196">
+      <c r="BI5" s="200"/>
+      <c r="BJ5" s="200"/>
+      <c r="BK5" s="200"/>
+      <c r="BL5" s="200"/>
+      <c r="BM5" s="200"/>
+      <c r="BN5" s="201"/>
+      <c r="BO5" s="206">
         <f>BO6</f>
         <v>45502</v>
       </c>
-      <c r="BP5" s="197"/>
-      <c r="BQ5" s="197"/>
-      <c r="BR5" s="197"/>
-      <c r="BS5" s="197"/>
-      <c r="BT5" s="197"/>
-      <c r="BU5" s="198"/>
-      <c r="BV5" s="202">
+      <c r="BP5" s="200"/>
+      <c r="BQ5" s="200"/>
+      <c r="BR5" s="200"/>
+      <c r="BS5" s="200"/>
+      <c r="BT5" s="200"/>
+      <c r="BU5" s="207"/>
+      <c r="BV5" s="199">
         <f>BV6</f>
         <v>45509</v>
       </c>
-      <c r="BW5" s="197"/>
-      <c r="BX5" s="197"/>
-      <c r="BY5" s="197"/>
-      <c r="BZ5" s="197"/>
-      <c r="CA5" s="197"/>
-      <c r="CB5" s="203"/>
-      <c r="CC5" s="202">
+      <c r="BW5" s="200"/>
+      <c r="BX5" s="200"/>
+      <c r="BY5" s="200"/>
+      <c r="BZ5" s="200"/>
+      <c r="CA5" s="200"/>
+      <c r="CB5" s="201"/>
+      <c r="CC5" s="199">
         <f>CC6</f>
         <v>45516</v>
       </c>
-      <c r="CD5" s="197"/>
-      <c r="CE5" s="197"/>
-      <c r="CF5" s="197"/>
-      <c r="CG5" s="197"/>
-      <c r="CH5" s="197"/>
-      <c r="CI5" s="203"/>
-      <c r="CJ5" s="196">
+      <c r="CD5" s="200"/>
+      <c r="CE5" s="200"/>
+      <c r="CF5" s="200"/>
+      <c r="CG5" s="200"/>
+      <c r="CH5" s="200"/>
+      <c r="CI5" s="201"/>
+      <c r="CJ5" s="206">
         <f>CJ6</f>
         <v>45523</v>
       </c>
-      <c r="CK5" s="197"/>
-      <c r="CL5" s="197"/>
-      <c r="CM5" s="197"/>
-      <c r="CN5" s="197"/>
-      <c r="CO5" s="197"/>
-      <c r="CP5" s="198"/>
-      <c r="CQ5" s="202">
+      <c r="CK5" s="200"/>
+      <c r="CL5" s="200"/>
+      <c r="CM5" s="200"/>
+      <c r="CN5" s="200"/>
+      <c r="CO5" s="200"/>
+      <c r="CP5" s="207"/>
+      <c r="CQ5" s="199">
         <f>CQ6</f>
         <v>45530</v>
       </c>
-      <c r="CR5" s="197"/>
-      <c r="CS5" s="197"/>
-      <c r="CT5" s="197"/>
-      <c r="CU5" s="197"/>
-      <c r="CV5" s="197"/>
-      <c r="CW5" s="203"/>
-      <c r="CX5" s="202">
+      <c r="CR5" s="200"/>
+      <c r="CS5" s="200"/>
+      <c r="CT5" s="200"/>
+      <c r="CU5" s="200"/>
+      <c r="CV5" s="200"/>
+      <c r="CW5" s="201"/>
+      <c r="CX5" s="199">
         <f>CX6</f>
         <v>45537</v>
       </c>
-      <c r="CY5" s="197"/>
-      <c r="CZ5" s="197"/>
-      <c r="DA5" s="197"/>
-      <c r="DB5" s="197"/>
-      <c r="DC5" s="197"/>
-      <c r="DD5" s="203"/>
-      <c r="DE5" s="196">
+      <c r="CY5" s="200"/>
+      <c r="CZ5" s="200"/>
+      <c r="DA5" s="200"/>
+      <c r="DB5" s="200"/>
+      <c r="DC5" s="200"/>
+      <c r="DD5" s="201"/>
+      <c r="DE5" s="206">
         <f>DE6</f>
         <v>45544</v>
       </c>
-      <c r="DF5" s="197"/>
-      <c r="DG5" s="197"/>
-      <c r="DH5" s="197"/>
-      <c r="DI5" s="197"/>
-      <c r="DJ5" s="197"/>
-      <c r="DK5" s="198"/>
-      <c r="DL5" s="202">
+      <c r="DF5" s="200"/>
+      <c r="DG5" s="200"/>
+      <c r="DH5" s="200"/>
+      <c r="DI5" s="200"/>
+      <c r="DJ5" s="200"/>
+      <c r="DK5" s="207"/>
+      <c r="DL5" s="199">
         <f>DL6</f>
         <v>45551</v>
       </c>
-      <c r="DM5" s="197"/>
-      <c r="DN5" s="197"/>
-      <c r="DO5" s="197"/>
-      <c r="DP5" s="197"/>
-      <c r="DQ5" s="197"/>
-      <c r="DR5" s="203"/>
-      <c r="DS5" s="202">
+      <c r="DM5" s="200"/>
+      <c r="DN5" s="200"/>
+      <c r="DO5" s="200"/>
+      <c r="DP5" s="200"/>
+      <c r="DQ5" s="200"/>
+      <c r="DR5" s="201"/>
+      <c r="DS5" s="199">
         <f>DS6</f>
         <v>45558</v>
       </c>
-      <c r="DT5" s="197"/>
-      <c r="DU5" s="197"/>
-      <c r="DV5" s="197"/>
-      <c r="DW5" s="197"/>
-      <c r="DX5" s="197"/>
-      <c r="DY5" s="203"/>
-      <c r="DZ5" s="196">
+      <c r="DT5" s="200"/>
+      <c r="DU5" s="200"/>
+      <c r="DV5" s="200"/>
+      <c r="DW5" s="200"/>
+      <c r="DX5" s="200"/>
+      <c r="DY5" s="201"/>
+      <c r="DZ5" s="206">
         <f>DZ6</f>
         <v>45565</v>
       </c>
-      <c r="EA5" s="197"/>
-      <c r="EB5" s="197"/>
-      <c r="EC5" s="197"/>
-      <c r="ED5" s="197"/>
-      <c r="EE5" s="197"/>
-      <c r="EF5" s="198"/>
-      <c r="EG5" s="202">
+      <c r="EA5" s="200"/>
+      <c r="EB5" s="200"/>
+      <c r="EC5" s="200"/>
+      <c r="ED5" s="200"/>
+      <c r="EE5" s="200"/>
+      <c r="EF5" s="207"/>
+      <c r="EG5" s="199">
         <f>EG6</f>
         <v>45572</v>
       </c>
-      <c r="EH5" s="197"/>
-      <c r="EI5" s="197"/>
-      <c r="EJ5" s="197"/>
-      <c r="EK5" s="197"/>
-      <c r="EL5" s="197"/>
-      <c r="EM5" s="203"/>
-      <c r="EN5" s="202">
+      <c r="EH5" s="200"/>
+      <c r="EI5" s="200"/>
+      <c r="EJ5" s="200"/>
+      <c r="EK5" s="200"/>
+      <c r="EL5" s="200"/>
+      <c r="EM5" s="201"/>
+      <c r="EN5" s="199">
         <f>EN6</f>
         <v>45579</v>
       </c>
-      <c r="EO5" s="197"/>
-      <c r="EP5" s="197"/>
-      <c r="EQ5" s="197"/>
-      <c r="ER5" s="197"/>
-      <c r="ES5" s="197"/>
-      <c r="ET5" s="203"/>
-      <c r="EU5" s="196">
+      <c r="EO5" s="200"/>
+      <c r="EP5" s="200"/>
+      <c r="EQ5" s="200"/>
+      <c r="ER5" s="200"/>
+      <c r="ES5" s="200"/>
+      <c r="ET5" s="201"/>
+      <c r="EU5" s="206">
         <f>EU6</f>
         <v>45586</v>
       </c>
-      <c r="EV5" s="197"/>
-      <c r="EW5" s="197"/>
-      <c r="EX5" s="197"/>
-      <c r="EY5" s="197"/>
-      <c r="EZ5" s="197"/>
-      <c r="FA5" s="198"/>
-      <c r="FB5" s="202">
+      <c r="EV5" s="200"/>
+      <c r="EW5" s="200"/>
+      <c r="EX5" s="200"/>
+      <c r="EY5" s="200"/>
+      <c r="EZ5" s="200"/>
+      <c r="FA5" s="207"/>
+      <c r="FB5" s="199">
         <f>FB6</f>
         <v>45593</v>
       </c>
-      <c r="FC5" s="197"/>
-      <c r="FD5" s="197"/>
-      <c r="FE5" s="197"/>
-      <c r="FF5" s="197"/>
-      <c r="FG5" s="197"/>
-      <c r="FH5" s="203"/>
-      <c r="FI5" s="202">
+      <c r="FC5" s="200"/>
+      <c r="FD5" s="200"/>
+      <c r="FE5" s="200"/>
+      <c r="FF5" s="200"/>
+      <c r="FG5" s="200"/>
+      <c r="FH5" s="201"/>
+      <c r="FI5" s="199">
         <f>FI6</f>
         <v>45600</v>
       </c>
-      <c r="FJ5" s="197"/>
-      <c r="FK5" s="197"/>
-      <c r="FL5" s="197"/>
-      <c r="FM5" s="197"/>
-      <c r="FN5" s="197"/>
-      <c r="FO5" s="203"/>
-      <c r="FP5" s="196">
+      <c r="FJ5" s="200"/>
+      <c r="FK5" s="200"/>
+      <c r="FL5" s="200"/>
+      <c r="FM5" s="200"/>
+      <c r="FN5" s="200"/>
+      <c r="FO5" s="201"/>
+      <c r="FP5" s="206">
         <f>FP6</f>
         <v>45607</v>
       </c>
-      <c r="FQ5" s="197"/>
-      <c r="FR5" s="197"/>
-      <c r="FS5" s="197"/>
-      <c r="FT5" s="197"/>
-      <c r="FU5" s="197"/>
-      <c r="FV5" s="198"/>
-      <c r="FW5" s="202">
+      <c r="FQ5" s="200"/>
+      <c r="FR5" s="200"/>
+      <c r="FS5" s="200"/>
+      <c r="FT5" s="200"/>
+      <c r="FU5" s="200"/>
+      <c r="FV5" s="207"/>
+      <c r="FW5" s="199">
         <f>FW6</f>
         <v>45614</v>
       </c>
-      <c r="FX5" s="197"/>
-      <c r="FY5" s="197"/>
-      <c r="FZ5" s="197"/>
-      <c r="GA5" s="197"/>
-      <c r="GB5" s="197"/>
-      <c r="GC5" s="203"/>
-      <c r="GD5" s="202">
+      <c r="FX5" s="200"/>
+      <c r="FY5" s="200"/>
+      <c r="FZ5" s="200"/>
+      <c r="GA5" s="200"/>
+      <c r="GB5" s="200"/>
+      <c r="GC5" s="201"/>
+      <c r="GD5" s="199">
         <f>GD6</f>
         <v>45621</v>
       </c>
-      <c r="GE5" s="197"/>
-      <c r="GF5" s="197"/>
-      <c r="GG5" s="197"/>
-      <c r="GH5" s="197"/>
-      <c r="GI5" s="197"/>
-      <c r="GJ5" s="203"/>
-      <c r="GK5" s="196">
+      <c r="GE5" s="200"/>
+      <c r="GF5" s="200"/>
+      <c r="GG5" s="200"/>
+      <c r="GH5" s="200"/>
+      <c r="GI5" s="200"/>
+      <c r="GJ5" s="201"/>
+      <c r="GK5" s="206">
         <f>GK6</f>
         <v>45628</v>
       </c>
-      <c r="GL5" s="197"/>
-      <c r="GM5" s="197"/>
-      <c r="GN5" s="197"/>
-      <c r="GO5" s="197"/>
-      <c r="GP5" s="197"/>
-      <c r="GQ5" s="198"/>
-      <c r="GR5" s="202">
+      <c r="GL5" s="200"/>
+      <c r="GM5" s="200"/>
+      <c r="GN5" s="200"/>
+      <c r="GO5" s="200"/>
+      <c r="GP5" s="200"/>
+      <c r="GQ5" s="207"/>
+      <c r="GR5" s="199">
         <f>GR6</f>
         <v>45635</v>
       </c>
-      <c r="GS5" s="197"/>
-      <c r="GT5" s="197"/>
-      <c r="GU5" s="197"/>
-      <c r="GV5" s="197"/>
-      <c r="GW5" s="197"/>
-      <c r="GX5" s="203"/>
-      <c r="GY5" s="196">
+      <c r="GS5" s="200"/>
+      <c r="GT5" s="200"/>
+      <c r="GU5" s="200"/>
+      <c r="GV5" s="200"/>
+      <c r="GW5" s="200"/>
+      <c r="GX5" s="201"/>
+      <c r="GY5" s="206">
         <f>GY6</f>
         <v>45642</v>
       </c>
-      <c r="GZ5" s="197"/>
-      <c r="HA5" s="197"/>
-      <c r="HB5" s="197"/>
-      <c r="HC5" s="197"/>
-      <c r="HD5" s="197"/>
-      <c r="HE5" s="198"/>
-      <c r="HF5" s="202">
+      <c r="GZ5" s="200"/>
+      <c r="HA5" s="200"/>
+      <c r="HB5" s="200"/>
+      <c r="HC5" s="200"/>
+      <c r="HD5" s="200"/>
+      <c r="HE5" s="207"/>
+      <c r="HF5" s="199">
         <f>HF6</f>
         <v>45649</v>
       </c>
-      <c r="HG5" s="197"/>
-      <c r="HH5" s="197"/>
-      <c r="HI5" s="197"/>
-      <c r="HJ5" s="197"/>
-      <c r="HK5" s="197"/>
-      <c r="HL5" s="203"/>
-      <c r="HM5" s="196">
+      <c r="HG5" s="200"/>
+      <c r="HH5" s="200"/>
+      <c r="HI5" s="200"/>
+      <c r="HJ5" s="200"/>
+      <c r="HK5" s="200"/>
+      <c r="HL5" s="201"/>
+      <c r="HM5" s="206">
         <f>HM6</f>
         <v>45656</v>
       </c>
-      <c r="HN5" s="197"/>
-      <c r="HO5" s="197"/>
-      <c r="HP5" s="197"/>
-      <c r="HQ5" s="197"/>
-      <c r="HR5" s="197"/>
-      <c r="HS5" s="198"/>
-      <c r="HT5" s="202">
+      <c r="HN5" s="200"/>
+      <c r="HO5" s="200"/>
+      <c r="HP5" s="200"/>
+      <c r="HQ5" s="200"/>
+      <c r="HR5" s="200"/>
+      <c r="HS5" s="207"/>
+      <c r="HT5" s="199">
         <f>HT6</f>
         <v>45663</v>
       </c>
-      <c r="HU5" s="197"/>
-      <c r="HV5" s="197"/>
-      <c r="HW5" s="197"/>
-      <c r="HX5" s="197"/>
-      <c r="HY5" s="197"/>
-      <c r="HZ5" s="203"/>
-      <c r="IA5" s="196">
+      <c r="HU5" s="200"/>
+      <c r="HV5" s="200"/>
+      <c r="HW5" s="200"/>
+      <c r="HX5" s="200"/>
+      <c r="HY5" s="200"/>
+      <c r="HZ5" s="201"/>
+      <c r="IA5" s="206">
         <f>IA6</f>
         <v>45670</v>
       </c>
-      <c r="IB5" s="197"/>
-      <c r="IC5" s="197"/>
-      <c r="ID5" s="197"/>
-      <c r="IE5" s="197"/>
-      <c r="IF5" s="197"/>
-      <c r="IG5" s="198"/>
-      <c r="IH5" s="202">
+      <c r="IB5" s="200"/>
+      <c r="IC5" s="200"/>
+      <c r="ID5" s="200"/>
+      <c r="IE5" s="200"/>
+      <c r="IF5" s="200"/>
+      <c r="IG5" s="207"/>
+      <c r="IH5" s="199">
         <f>IH6</f>
         <v>45677</v>
       </c>
-      <c r="II5" s="197"/>
-      <c r="IJ5" s="197"/>
-      <c r="IK5" s="197"/>
-      <c r="IL5" s="197"/>
-      <c r="IM5" s="197"/>
-      <c r="IN5" s="203"/>
-      <c r="IO5" s="196">
+      <c r="II5" s="200"/>
+      <c r="IJ5" s="200"/>
+      <c r="IK5" s="200"/>
+      <c r="IL5" s="200"/>
+      <c r="IM5" s="200"/>
+      <c r="IN5" s="201"/>
+      <c r="IO5" s="206">
         <f>IO6</f>
         <v>45684</v>
       </c>
-      <c r="IP5" s="197"/>
-      <c r="IQ5" s="197"/>
-      <c r="IR5" s="197"/>
-      <c r="IS5" s="197"/>
-      <c r="IT5" s="197"/>
-      <c r="IU5" s="198"/>
+      <c r="IP5" s="200"/>
+      <c r="IQ5" s="200"/>
+      <c r="IR5" s="200"/>
+      <c r="IS5" s="200"/>
+      <c r="IT5" s="200"/>
+      <c r="IU5" s="207"/>
     </row>
-    <row r="6" spans="1:255" s="22" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:255" s="22" customFormat="1" ht="8.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="84"/>
       <c r="K6" s="33">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="IU6" s="45"/>
     </row>
-    <row r="7" spans="1:255" s="21" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:255" s="21" customFormat="1" ht="21.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
@@ -6178,7 +6178,7 @@
       </c>
       <c r="IU7" s="31"/>
     </row>
-    <row r="8" spans="1:255" s="176" customFormat="1" ht="17.649999999999999" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:255" s="176" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="169" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -6440,7 +6440,7 @@
       <c r="IT8" s="172"/>
       <c r="IU8" s="172"/>
     </row>
-    <row r="9" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A9" s="143">
         <v>1</v>
       </c>
@@ -6713,7 +6713,7 @@
       <c r="IT9" s="152"/>
       <c r="IU9" s="152"/>
     </row>
-    <row r="10" spans="1:255" s="153" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:255" s="153" customFormat="1" ht="23.15" x14ac:dyDescent="0.3">
       <c r="A10" s="143" t="str">
         <f t="shared" ref="A10:A19" si="18">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1</v>
@@ -6987,7 +6987,7 @@
       <c r="IT10" s="152"/>
       <c r="IU10" s="152"/>
     </row>
-    <row r="11" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A11" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.1</v>
@@ -7261,7 +7261,7 @@
       <c r="IT11" s="152"/>
       <c r="IU11" s="152"/>
     </row>
-    <row r="12" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A12" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.2</v>
@@ -7536,7 +7536,7 @@
       <c r="IT12" s="152"/>
       <c r="IU12" s="152"/>
     </row>
-    <row r="13" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A13" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.3</v>
@@ -7810,7 +7810,7 @@
       <c r="IT13" s="152"/>
       <c r="IU13" s="152"/>
     </row>
-    <row r="14" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A14" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.4</v>
@@ -8087,7 +8087,7 @@
       <c r="IT14" s="152"/>
       <c r="IU14" s="152"/>
     </row>
-    <row r="15" spans="1:255" s="153" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:255" s="153" customFormat="1" ht="23.15" x14ac:dyDescent="0.3">
       <c r="A15" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.5</v>
@@ -8364,7 +8364,7 @@
       <c r="IT15" s="152"/>
       <c r="IU15" s="152"/>
     </row>
-    <row r="16" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.6</v>
@@ -8640,7 +8640,7 @@
       <c r="IT16" s="152"/>
       <c r="IU16" s="152"/>
     </row>
-    <row r="17" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.7</v>
@@ -8916,7 +8916,7 @@
       <c r="IT17" s="152"/>
       <c r="IU17" s="152"/>
     </row>
-    <row r="18" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.8</v>
@@ -9190,7 +9190,7 @@
       <c r="IT18" s="152"/>
       <c r="IU18" s="152"/>
     </row>
-    <row r="19" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.9</v>
@@ -9466,7 +9466,7 @@
       <c r="IT19" s="152"/>
       <c r="IU19" s="152"/>
     </row>
-    <row r="20" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="143"/>
       <c r="B20" s="144" t="s">
         <v>31</v>
@@ -9740,7 +9740,7 @@
       <c r="IT20" s="152"/>
       <c r="IU20" s="152"/>
     </row>
-    <row r="21" spans="1:255" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="143"/>
       <c r="B21" s="144" t="s">
         <v>30</v>
@@ -10014,7 +10014,7 @@
       <c r="IT21" s="152"/>
       <c r="IU21" s="152"/>
     </row>
-    <row r="22" spans="1:255" s="93" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:255" s="93" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="159">
         <v>2</v>
       </c>
@@ -10275,7 +10275,7 @@
       <c r="IT22" s="92"/>
       <c r="IU22" s="92"/>
     </row>
-    <row r="23" spans="1:255" s="105" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:255" s="105" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="95">
         <v>2</v>
       </c>
@@ -10549,7 +10549,7 @@
       <c r="IT23" s="104"/>
       <c r="IU23" s="104"/>
     </row>
-    <row r="24" spans="1:255" s="105" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:255" s="105" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="95">
         <v>2.1</v>
       </c>
@@ -10823,7 +10823,7 @@
       <c r="IT24" s="104"/>
       <c r="IU24" s="104"/>
     </row>
-    <row r="25" spans="1:255" s="105" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:255" s="105" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="95">
         <v>2.2000000000000002</v>
       </c>
@@ -11097,7 +11097,7 @@
       <c r="IT25" s="104"/>
       <c r="IU25" s="104"/>
     </row>
-    <row r="26" spans="1:255" s="105" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:255" s="105" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="95">
         <v>2.2999999999999998</v>
       </c>
@@ -11371,7 +11371,7 @@
       <c r="IT26" s="104"/>
       <c r="IU26" s="104"/>
     </row>
-    <row r="27" spans="1:255" s="105" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:255" s="105" customFormat="1" ht="21.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="95">
         <v>2.4</v>
       </c>
@@ -11645,7 +11645,7 @@
       <c r="IT27" s="104"/>
       <c r="IU27" s="104"/>
     </row>
-    <row r="28" spans="1:255" s="105" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A28" s="95">
         <v>2.5</v>
       </c>
@@ -11919,7 +11919,7 @@
       <c r="IT28" s="104"/>
       <c r="IU28" s="104"/>
     </row>
-    <row r="29" spans="1:255" s="105" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="95">
         <v>2.6</v>
       </c>
@@ -12195,7 +12195,7 @@
       <c r="IT29" s="104"/>
       <c r="IU29" s="104"/>
     </row>
-    <row r="30" spans="1:255" s="105" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:255" s="105" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="95">
         <v>2.7</v>
       </c>
@@ -12471,7 +12471,7 @@
       <c r="IT30" s="104"/>
       <c r="IU30" s="104"/>
     </row>
-    <row r="31" spans="1:255" s="105" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="95">
         <v>2.8</v>
       </c>
@@ -12745,7 +12745,7 @@
       <c r="IT31" s="104"/>
       <c r="IU31" s="104"/>
     </row>
-    <row r="32" spans="1:255" s="105" customFormat="1" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:255" s="105" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="95" t="s">
         <v>63</v>
       </c>
@@ -13019,7 +13019,7 @@
       <c r="IT32" s="104"/>
       <c r="IU32" s="104"/>
     </row>
-    <row r="33" spans="1:255" s="105" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A33" s="95" t="s">
         <v>64</v>
       </c>
@@ -13293,7 +13293,7 @@
       <c r="IT33" s="104"/>
       <c r="IU33" s="104"/>
     </row>
-    <row r="34" spans="1:255" s="105" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A34" s="95" t="s">
         <v>65</v>
       </c>
@@ -13567,7 +13567,7 @@
       <c r="IT34" s="104"/>
       <c r="IU34" s="104"/>
     </row>
-    <row r="35" spans="1:255" s="105" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="B35" s="96" t="s">
         <v>36</v>
       </c>
@@ -13840,7 +13840,7 @@
       <c r="IT35" s="104"/>
       <c r="IU35" s="104"/>
     </row>
-    <row r="36" spans="1:255" s="105" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A36" s="95"/>
       <c r="B36" s="96" t="s">
         <v>35</v>
@@ -14113,7 +14113,7 @@
       <c r="IT36" s="104"/>
       <c r="IU36" s="104"/>
     </row>
-    <row r="37" spans="1:255" s="113" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:255" s="113" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A37" s="106">
         <v>3</v>
       </c>
@@ -14374,7 +14374,7 @@
       <c r="IT37" s="109"/>
       <c r="IU37" s="109"/>
     </row>
-    <row r="38" spans="1:255" s="121" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A38" s="114">
         <v>3</v>
       </c>
@@ -14648,7 +14648,7 @@
       <c r="IT38" s="120"/>
       <c r="IU38" s="120"/>
     </row>
-    <row r="39" spans="1:255" s="121" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:255" s="121" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="114">
         <v>3.1</v>
       </c>
@@ -14922,7 +14922,7 @@
       <c r="IT39" s="120"/>
       <c r="IU39" s="120"/>
     </row>
-    <row r="40" spans="1:255" s="121" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:255" s="121" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="114">
         <v>3.2</v>
       </c>
@@ -15196,7 +15196,7 @@
       <c r="IT40" s="120"/>
       <c r="IU40" s="120"/>
     </row>
-    <row r="41" spans="1:255" s="121" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A41" s="114">
         <v>3.3</v>
       </c>
@@ -15470,7 +15470,7 @@
       <c r="IT41" s="120"/>
       <c r="IU41" s="120"/>
     </row>
-    <row r="42" spans="1:255" s="121" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A42" s="114">
         <v>3.3</v>
       </c>
@@ -15491,7 +15491,7 @@
         <v>9</v>
       </c>
       <c r="H42" s="118">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="I42" s="185">
         <f t="shared" ref="I42" si="26">IF(OR(F42=0,E42=0),0,NETWORKDAYS(E42,F42))</f>
@@ -15744,7 +15744,7 @@
       <c r="IT42" s="120"/>
       <c r="IU42" s="120"/>
     </row>
-    <row r="43" spans="1:255" s="121" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:255" s="121" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="114">
         <v>3.4</v>
       </c>
@@ -15765,7 +15765,7 @@
         <v>33</v>
       </c>
       <c r="H43" s="118">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I43" s="185">
         <f t="shared" si="24"/>
@@ -16018,7 +16018,7 @@
       <c r="IT43" s="120"/>
       <c r="IU43" s="120"/>
     </row>
-    <row r="44" spans="1:255" s="121" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A44" s="114" t="s">
         <v>66</v>
       </c>
@@ -16292,7 +16292,7 @@
       <c r="IT44" s="120"/>
       <c r="IU44" s="120"/>
     </row>
-    <row r="45" spans="1:255" s="121" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:255" s="121" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="114" t="s">
         <v>67</v>
       </c>
@@ -16566,7 +16566,7 @@
       <c r="IT45" s="120"/>
       <c r="IU45" s="120"/>
     </row>
-    <row r="46" spans="1:255" s="121" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:255" s="121" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="114" t="s">
         <v>68</v>
       </c>
@@ -16840,7 +16840,7 @@
       <c r="IT46" s="120"/>
       <c r="IU46" s="120"/>
     </row>
-    <row r="47" spans="1:255" s="121" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A47" s="114"/>
       <c r="B47" s="154" t="s">
         <v>28</v>
@@ -17114,7 +17114,7 @@
       <c r="IT47" s="120"/>
       <c r="IU47" s="120"/>
     </row>
-    <row r="48" spans="1:255" s="121" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A48" s="114"/>
       <c r="B48" s="154" t="s">
         <v>29</v>
@@ -17388,7 +17388,7 @@
       <c r="IT48" s="120"/>
       <c r="IU48" s="120"/>
     </row>
-    <row r="49" spans="1:255" s="131" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:255" s="131" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A49" s="122">
         <v>4</v>
       </c>
@@ -17649,7 +17649,7 @@
       <c r="IT49" s="125"/>
       <c r="IU49" s="125"/>
     </row>
-    <row r="50" spans="1:255" s="142" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:255" s="142" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A50" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
@@ -17924,7 +17924,7 @@
       <c r="IT50" s="141"/>
       <c r="IU50" s="141"/>
     </row>
-    <row r="51" spans="1:255" s="142" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:255" s="142" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A51" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.1</v>
@@ -18201,7 +18201,7 @@
       <c r="IT51" s="141"/>
       <c r="IU51" s="141"/>
     </row>
-    <row r="52" spans="1:255" s="142" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:255" s="142" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A52" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.2</v>
@@ -18478,7 +18478,7 @@
       <c r="IT52" s="141"/>
       <c r="IU52" s="141"/>
     </row>
-    <row r="53" spans="1:255" s="142" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:255" s="142" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A53" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.3</v>
@@ -18755,7 +18755,7 @@
       <c r="IT53" s="141"/>
       <c r="IU53" s="141"/>
     </row>
-    <row r="55" spans="1:255" s="9" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:255" s="9" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="65" t="s">
         <v>1</v>
       </c>
@@ -19014,7 +19014,7 @@
       <c r="IT55" s="3"/>
       <c r="IU55" s="3"/>
     </row>
-    <row r="56" spans="1:255" s="8" customFormat="1" ht="17.649999999999999" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:255" s="8" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A56" s="66" t="s">
         <v>16</v>
       </c>
@@ -19269,7 +19269,7 @@
       <c r="IT56" s="3"/>
       <c r="IU56" s="3"/>
     </row>
-    <row r="57" spans="1:255" s="8" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:255" s="8" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A57" s="54" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -19533,7 +19533,7 @@
       <c r="IT57" s="3"/>
       <c r="IU57" s="3"/>
     </row>
-    <row r="58" spans="1:255" s="8" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:255" s="8" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A58" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -19805,7 +19805,7 @@
       <c r="IT58" s="3"/>
       <c r="IU58" s="3"/>
     </row>
-    <row r="59" spans="1:255" s="8" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:255" s="8" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A59" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -20077,7 +20077,7 @@
       <c r="IT59" s="3"/>
       <c r="IU59" s="3"/>
     </row>
-    <row r="60" spans="1:255" s="8" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:255" s="8" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
       <c r="A60" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
@@ -20347,7 +20347,7 @@
       <c r="IT60" s="3"/>
       <c r="IU60" s="3"/>
     </row>
-    <row r="61" spans="1:255" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:255" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="80" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
@@ -20357,54 +20357,25 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="73">
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="AD1:AR1"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AF5:AL5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="FI4:FO4"/>
-    <mergeCell ref="FP4:FV4"/>
-    <mergeCell ref="EG4:EM4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE5:DK5"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="DS5:DY5"/>
-    <mergeCell ref="DZ5:EF5"/>
-    <mergeCell ref="EG5:EM5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DS4:DY4"/>
-    <mergeCell ref="DZ4:EF4"/>
+    <mergeCell ref="IO5:IU5"/>
+    <mergeCell ref="IO4:IU4"/>
+    <mergeCell ref="HT4:HZ4"/>
+    <mergeCell ref="IA4:IG4"/>
+    <mergeCell ref="IH4:IN4"/>
+    <mergeCell ref="HM5:HS5"/>
+    <mergeCell ref="HT5:HZ5"/>
+    <mergeCell ref="IA5:IG5"/>
+    <mergeCell ref="IH5:IN5"/>
+    <mergeCell ref="GY4:HE4"/>
+    <mergeCell ref="HF4:HL4"/>
+    <mergeCell ref="GY5:HE5"/>
+    <mergeCell ref="HF5:HL5"/>
+    <mergeCell ref="HM4:HS4"/>
     <mergeCell ref="FW4:GC4"/>
     <mergeCell ref="GD4:GJ4"/>
     <mergeCell ref="GK4:GQ4"/>
@@ -20421,20 +20392,49 @@
     <mergeCell ref="EN4:ET4"/>
     <mergeCell ref="EU4:FA4"/>
     <mergeCell ref="FB4:FH4"/>
-    <mergeCell ref="HM5:HS5"/>
-    <mergeCell ref="HT5:HZ5"/>
-    <mergeCell ref="IA5:IG5"/>
-    <mergeCell ref="IH5:IN5"/>
-    <mergeCell ref="GY4:HE4"/>
-    <mergeCell ref="HF4:HL4"/>
-    <mergeCell ref="GY5:HE5"/>
-    <mergeCell ref="HF5:HL5"/>
-    <mergeCell ref="HM4:HS4"/>
-    <mergeCell ref="IO5:IU5"/>
-    <mergeCell ref="IO4:IU4"/>
-    <mergeCell ref="HT4:HZ4"/>
-    <mergeCell ref="IA4:IG4"/>
-    <mergeCell ref="IH4:IN4"/>
+    <mergeCell ref="FI4:FO4"/>
+    <mergeCell ref="FP4:FV4"/>
+    <mergeCell ref="EG4:EM4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="DS5:DY5"/>
+    <mergeCell ref="DZ5:EF5"/>
+    <mergeCell ref="EG5:EM5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DS4:DY4"/>
+    <mergeCell ref="DZ4:EF4"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="AD1:AR1"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="AF5:AL5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="BH4:BN4"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="AM5:AS5"/>
+    <mergeCell ref="AT4:AZ4"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="BA4:BG4"/>
+    <mergeCell ref="BA5:BG5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H56:H60 H8:H53">
@@ -20497,13 +20497,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>10886</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>28</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>103414</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>

</xml_diff>

<commit_message>
added meeting notes, pictures
</commit_message>
<xml_diff>
--- a/thesis gantt chart.xlsx
+++ b/thesis gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wings_stuff\srus\TUD\yr5\thesis\thesis_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97009757-4C39-411C-95C7-AE203D141E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B15DEE-3B2A-4DA0-8274-326A49791C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-69" yWindow="-69" windowWidth="26469" windowHeight="15875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -2630,6 +2630,15 @@
     <xf numFmtId="0" fontId="28" fillId="35" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="59" fillId="23" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2642,28 +2651,7 @@
     <xf numFmtId="167" fontId="41" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="41" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="63" fillId="24" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -2700,6 +2688,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="41" fillId="23" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2957,13 +2957,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>10886</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>103414</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -3297,70 +3297,70 @@
   </sheetPr>
   <dimension ref="A1:IU63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR36" sqref="AR36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AT46" sqref="AT46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.61328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.15234375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="4" style="91" customWidth="1"/>
-    <col min="4" max="4" width="0.84375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.15234375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.61328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.84375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.15234375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.84375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="0.61328125" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.3828125" style="1" customWidth="1"/>
-    <col min="67" max="68" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="74" width="1.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="99" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="100" max="102" width="1.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="105" max="106" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="107" max="108" width="1.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="109" max="131" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="134" max="137" width="1.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="139" max="162" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="163" max="165" width="1.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="168" max="169" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="170" max="192" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="1.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="196" max="197" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="198" max="200" width="1.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="202" max="221" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="225" max="227" width="1.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="0.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="0.5703125" style="1" customWidth="1"/>
+    <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
+    <col min="67" max="68" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="74" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="99" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="100" max="102" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="105" max="106" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="107" max="108" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="109" max="131" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="134" max="137" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="139" max="162" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="163" max="165" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="168" max="169" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="170" max="192" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="196" max="197" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="198" max="200" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="202" max="221" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="225" max="227" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="1.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="2.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="231" max="252" width="2.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="253" max="254" width="2.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="1.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="256" max="16384" width="9.15234375" style="1"/>
+    <col min="229" max="229" width="1.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="231" max="252" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="253" max="254" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="256" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="12" customFormat="1" ht="24.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:255" s="12" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="78" t="s">
         <v>24</v>
       </c>
@@ -3373,23 +3373,23 @@
       <c r="K1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="208"/>
-      <c r="AE1" s="208"/>
-      <c r="AF1" s="208"/>
-      <c r="AG1" s="208"/>
-      <c r="AH1" s="208"/>
-      <c r="AI1" s="208"/>
-      <c r="AJ1" s="208"/>
-      <c r="AK1" s="208"/>
-      <c r="AL1" s="208"/>
-      <c r="AM1" s="208"/>
-      <c r="AN1" s="208"/>
-      <c r="AO1" s="208"/>
-      <c r="AP1" s="208"/>
-      <c r="AQ1" s="208"/>
-      <c r="AR1" s="208"/>
+      <c r="AD1" s="204"/>
+      <c r="AE1" s="204"/>
+      <c r="AF1" s="204"/>
+      <c r="AG1" s="204"/>
+      <c r="AH1" s="204"/>
+      <c r="AI1" s="204"/>
+      <c r="AJ1" s="204"/>
+      <c r="AK1" s="204"/>
+      <c r="AL1" s="204"/>
+      <c r="AM1" s="204"/>
+      <c r="AN1" s="204"/>
+      <c r="AO1" s="204"/>
+      <c r="AP1" s="204"/>
+      <c r="AQ1" s="204"/>
+      <c r="AR1" s="204"/>
     </row>
-    <row r="2" spans="1:255" s="28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:255" s="28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="72" t="s">
         <v>25</v>
       </c>
@@ -3399,7 +3399,7 @@
       <c r="E2" s="25"/>
       <c r="F2" s="27"/>
     </row>
-    <row r="3" spans="1:255" s="61" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:255" s="61" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="57"/>
       <c r="B3" s="58"/>
       <c r="C3" s="83"/>
@@ -3463,735 +3463,735 @@
       <c r="BM3" s="76"/>
       <c r="BN3" s="77"/>
     </row>
-    <row r="4" spans="1:255" s="70" customFormat="1" ht="17.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:255" s="70" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="211">
+      <c r="C4" s="207">
         <v>45295</v>
       </c>
-      <c r="D4" s="212"/>
-      <c r="E4" s="213"/>
+      <c r="D4" s="208"/>
+      <c r="E4" s="209"/>
       <c r="H4" s="73" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="74">
         <v>23</v>
       </c>
-      <c r="K4" s="196"/>
-      <c r="L4" s="197"/>
-      <c r="M4" s="197"/>
-      <c r="N4" s="197"/>
-      <c r="O4" s="197"/>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="198"/>
-      <c r="R4" s="196" t="str">
+      <c r="K4" s="199"/>
+      <c r="L4" s="200"/>
+      <c r="M4" s="200"/>
+      <c r="N4" s="200"/>
+      <c r="O4" s="200"/>
+      <c r="P4" s="200"/>
+      <c r="Q4" s="201"/>
+      <c r="R4" s="199" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="S4" s="197"/>
-      <c r="T4" s="197"/>
-      <c r="U4" s="197"/>
-      <c r="V4" s="197"/>
-      <c r="W4" s="197"/>
-      <c r="X4" s="198"/>
-      <c r="Y4" s="196" t="str">
+      <c r="S4" s="200"/>
+      <c r="T4" s="200"/>
+      <c r="U4" s="200"/>
+      <c r="V4" s="200"/>
+      <c r="W4" s="200"/>
+      <c r="X4" s="201"/>
+      <c r="Y4" s="199" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="Z4" s="197"/>
-      <c r="AA4" s="197"/>
-      <c r="AB4" s="197"/>
-      <c r="AC4" s="197"/>
-      <c r="AD4" s="197"/>
-      <c r="AE4" s="198"/>
-      <c r="AF4" s="196" t="str">
+      <c r="Z4" s="200"/>
+      <c r="AA4" s="200"/>
+      <c r="AB4" s="200"/>
+      <c r="AC4" s="200"/>
+      <c r="AD4" s="200"/>
+      <c r="AE4" s="201"/>
+      <c r="AF4" s="199" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AG4" s="197"/>
-      <c r="AH4" s="197"/>
-      <c r="AI4" s="197"/>
-      <c r="AJ4" s="197"/>
-      <c r="AK4" s="197"/>
-      <c r="AL4" s="198"/>
-      <c r="AM4" s="196" t="str">
+      <c r="AG4" s="200"/>
+      <c r="AH4" s="200"/>
+      <c r="AI4" s="200"/>
+      <c r="AJ4" s="200"/>
+      <c r="AK4" s="200"/>
+      <c r="AL4" s="201"/>
+      <c r="AM4" s="199" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="AN4" s="197"/>
-      <c r="AO4" s="197"/>
-      <c r="AP4" s="197"/>
-      <c r="AQ4" s="197"/>
-      <c r="AR4" s="197"/>
-      <c r="AS4" s="198"/>
-      <c r="AT4" s="196" t="str">
+      <c r="AN4" s="200"/>
+      <c r="AO4" s="200"/>
+      <c r="AP4" s="200"/>
+      <c r="AQ4" s="200"/>
+      <c r="AR4" s="200"/>
+      <c r="AS4" s="201"/>
+      <c r="AT4" s="199" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AU4" s="197"/>
-      <c r="AV4" s="197"/>
-      <c r="AW4" s="197"/>
-      <c r="AX4" s="197"/>
-      <c r="AY4" s="197"/>
-      <c r="AZ4" s="198"/>
-      <c r="BA4" s="196" t="str">
+      <c r="AU4" s="200"/>
+      <c r="AV4" s="200"/>
+      <c r="AW4" s="200"/>
+      <c r="AX4" s="200"/>
+      <c r="AY4" s="200"/>
+      <c r="AZ4" s="201"/>
+      <c r="BA4" s="199" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="BB4" s="197"/>
-      <c r="BC4" s="197"/>
-      <c r="BD4" s="197"/>
-      <c r="BE4" s="197"/>
-      <c r="BF4" s="197"/>
-      <c r="BG4" s="198"/>
-      <c r="BH4" s="196" t="str">
+      <c r="BB4" s="200"/>
+      <c r="BC4" s="200"/>
+      <c r="BD4" s="200"/>
+      <c r="BE4" s="200"/>
+      <c r="BF4" s="200"/>
+      <c r="BG4" s="201"/>
+      <c r="BH4" s="199" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="BI4" s="197"/>
-      <c r="BJ4" s="197"/>
-      <c r="BK4" s="197"/>
-      <c r="BL4" s="197"/>
-      <c r="BM4" s="197"/>
-      <c r="BN4" s="198"/>
-      <c r="BO4" s="196" t="str">
+      <c r="BI4" s="200"/>
+      <c r="BJ4" s="200"/>
+      <c r="BK4" s="200"/>
+      <c r="BL4" s="200"/>
+      <c r="BM4" s="200"/>
+      <c r="BN4" s="201"/>
+      <c r="BO4" s="199" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="BP4" s="197"/>
-      <c r="BQ4" s="197"/>
-      <c r="BR4" s="197"/>
-      <c r="BS4" s="197"/>
-      <c r="BT4" s="197"/>
-      <c r="BU4" s="198"/>
-      <c r="BV4" s="196" t="str">
+      <c r="BP4" s="200"/>
+      <c r="BQ4" s="200"/>
+      <c r="BR4" s="200"/>
+      <c r="BS4" s="200"/>
+      <c r="BT4" s="200"/>
+      <c r="BU4" s="201"/>
+      <c r="BV4" s="199" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BW4" s="197"/>
-      <c r="BX4" s="197"/>
-      <c r="BY4" s="197"/>
-      <c r="BZ4" s="197"/>
-      <c r="CA4" s="197"/>
-      <c r="CB4" s="198"/>
-      <c r="CC4" s="196" t="str">
+      <c r="BW4" s="200"/>
+      <c r="BX4" s="200"/>
+      <c r="BY4" s="200"/>
+      <c r="BZ4" s="200"/>
+      <c r="CA4" s="200"/>
+      <c r="CB4" s="201"/>
+      <c r="CC4" s="199" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="CD4" s="197"/>
-      <c r="CE4" s="197"/>
-      <c r="CF4" s="197"/>
-      <c r="CG4" s="197"/>
-      <c r="CH4" s="197"/>
-      <c r="CI4" s="198"/>
-      <c r="CJ4" s="196" t="str">
+      <c r="CD4" s="200"/>
+      <c r="CE4" s="200"/>
+      <c r="CF4" s="200"/>
+      <c r="CG4" s="200"/>
+      <c r="CH4" s="200"/>
+      <c r="CI4" s="201"/>
+      <c r="CJ4" s="199" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 33</v>
       </c>
-      <c r="CK4" s="197"/>
-      <c r="CL4" s="197"/>
-      <c r="CM4" s="197"/>
-      <c r="CN4" s="197"/>
-      <c r="CO4" s="197"/>
-      <c r="CP4" s="198"/>
-      <c r="CQ4" s="196" t="str">
+      <c r="CK4" s="200"/>
+      <c r="CL4" s="200"/>
+      <c r="CM4" s="200"/>
+      <c r="CN4" s="200"/>
+      <c r="CO4" s="200"/>
+      <c r="CP4" s="201"/>
+      <c r="CQ4" s="199" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 34</v>
       </c>
-      <c r="CR4" s="197"/>
-      <c r="CS4" s="197"/>
-      <c r="CT4" s="197"/>
-      <c r="CU4" s="197"/>
-      <c r="CV4" s="197"/>
-      <c r="CW4" s="198"/>
-      <c r="CX4" s="196" t="str">
+      <c r="CR4" s="200"/>
+      <c r="CS4" s="200"/>
+      <c r="CT4" s="200"/>
+      <c r="CU4" s="200"/>
+      <c r="CV4" s="200"/>
+      <c r="CW4" s="201"/>
+      <c r="CX4" s="199" t="str">
         <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 35</v>
       </c>
-      <c r="CY4" s="197"/>
-      <c r="CZ4" s="197"/>
-      <c r="DA4" s="197"/>
-      <c r="DB4" s="197"/>
-      <c r="DC4" s="197"/>
-      <c r="DD4" s="198"/>
-      <c r="DE4" s="196" t="str">
+      <c r="CY4" s="200"/>
+      <c r="CZ4" s="200"/>
+      <c r="DA4" s="200"/>
+      <c r="DB4" s="200"/>
+      <c r="DC4" s="200"/>
+      <c r="DD4" s="201"/>
+      <c r="DE4" s="199" t="str">
         <f>"Week "&amp;(CX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 36</v>
       </c>
-      <c r="DF4" s="197"/>
-      <c r="DG4" s="197"/>
-      <c r="DH4" s="197"/>
-      <c r="DI4" s="197"/>
-      <c r="DJ4" s="197"/>
-      <c r="DK4" s="198"/>
-      <c r="DL4" s="196" t="str">
+      <c r="DF4" s="200"/>
+      <c r="DG4" s="200"/>
+      <c r="DH4" s="200"/>
+      <c r="DI4" s="200"/>
+      <c r="DJ4" s="200"/>
+      <c r="DK4" s="201"/>
+      <c r="DL4" s="199" t="str">
         <f>"Week "&amp;(DE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 37</v>
       </c>
-      <c r="DM4" s="197"/>
-      <c r="DN4" s="197"/>
-      <c r="DO4" s="197"/>
-      <c r="DP4" s="197"/>
-      <c r="DQ4" s="197"/>
-      <c r="DR4" s="198"/>
-      <c r="DS4" s="196" t="str">
+      <c r="DM4" s="200"/>
+      <c r="DN4" s="200"/>
+      <c r="DO4" s="200"/>
+      <c r="DP4" s="200"/>
+      <c r="DQ4" s="200"/>
+      <c r="DR4" s="201"/>
+      <c r="DS4" s="199" t="str">
         <f>"Week "&amp;(DL6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 38</v>
       </c>
-      <c r="DT4" s="197"/>
-      <c r="DU4" s="197"/>
-      <c r="DV4" s="197"/>
-      <c r="DW4" s="197"/>
-      <c r="DX4" s="197"/>
-      <c r="DY4" s="198"/>
-      <c r="DZ4" s="196" t="str">
+      <c r="DT4" s="200"/>
+      <c r="DU4" s="200"/>
+      <c r="DV4" s="200"/>
+      <c r="DW4" s="200"/>
+      <c r="DX4" s="200"/>
+      <c r="DY4" s="201"/>
+      <c r="DZ4" s="199" t="str">
         <f>"Week "&amp;(DS6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 39</v>
       </c>
-      <c r="EA4" s="197"/>
-      <c r="EB4" s="197"/>
-      <c r="EC4" s="197"/>
-      <c r="ED4" s="197"/>
-      <c r="EE4" s="197"/>
-      <c r="EF4" s="198"/>
-      <c r="EG4" s="196" t="str">
+      <c r="EA4" s="200"/>
+      <c r="EB4" s="200"/>
+      <c r="EC4" s="200"/>
+      <c r="ED4" s="200"/>
+      <c r="EE4" s="200"/>
+      <c r="EF4" s="201"/>
+      <c r="EG4" s="199" t="str">
         <f>"Week "&amp;(DZ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 40</v>
       </c>
-      <c r="EH4" s="197"/>
-      <c r="EI4" s="197"/>
-      <c r="EJ4" s="197"/>
-      <c r="EK4" s="197"/>
-      <c r="EL4" s="197"/>
-      <c r="EM4" s="198"/>
-      <c r="EN4" s="196" t="str">
+      <c r="EH4" s="200"/>
+      <c r="EI4" s="200"/>
+      <c r="EJ4" s="200"/>
+      <c r="EK4" s="200"/>
+      <c r="EL4" s="200"/>
+      <c r="EM4" s="201"/>
+      <c r="EN4" s="199" t="str">
         <f>"Week "&amp;(EG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 41</v>
       </c>
-      <c r="EO4" s="197"/>
-      <c r="EP4" s="197"/>
-      <c r="EQ4" s="197"/>
-      <c r="ER4" s="197"/>
-      <c r="ES4" s="197"/>
-      <c r="ET4" s="198"/>
-      <c r="EU4" s="196" t="str">
+      <c r="EO4" s="200"/>
+      <c r="EP4" s="200"/>
+      <c r="EQ4" s="200"/>
+      <c r="ER4" s="200"/>
+      <c r="ES4" s="200"/>
+      <c r="ET4" s="201"/>
+      <c r="EU4" s="199" t="str">
         <f>"Week "&amp;(EN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 42</v>
       </c>
-      <c r="EV4" s="197"/>
-      <c r="EW4" s="197"/>
-      <c r="EX4" s="197"/>
-      <c r="EY4" s="197"/>
-      <c r="EZ4" s="197"/>
-      <c r="FA4" s="198"/>
-      <c r="FB4" s="196" t="str">
+      <c r="EV4" s="200"/>
+      <c r="EW4" s="200"/>
+      <c r="EX4" s="200"/>
+      <c r="EY4" s="200"/>
+      <c r="EZ4" s="200"/>
+      <c r="FA4" s="201"/>
+      <c r="FB4" s="199" t="str">
         <f>"Week "&amp;(EU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 43</v>
       </c>
-      <c r="FC4" s="197"/>
-      <c r="FD4" s="197"/>
-      <c r="FE4" s="197"/>
-      <c r="FF4" s="197"/>
-      <c r="FG4" s="197"/>
-      <c r="FH4" s="198"/>
-      <c r="FI4" s="196" t="str">
+      <c r="FC4" s="200"/>
+      <c r="FD4" s="200"/>
+      <c r="FE4" s="200"/>
+      <c r="FF4" s="200"/>
+      <c r="FG4" s="200"/>
+      <c r="FH4" s="201"/>
+      <c r="FI4" s="199" t="str">
         <f>"Week "&amp;(FB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 44</v>
       </c>
-      <c r="FJ4" s="197"/>
-      <c r="FK4" s="197"/>
-      <c r="FL4" s="197"/>
-      <c r="FM4" s="197"/>
-      <c r="FN4" s="197"/>
-      <c r="FO4" s="198"/>
-      <c r="FP4" s="196" t="str">
+      <c r="FJ4" s="200"/>
+      <c r="FK4" s="200"/>
+      <c r="FL4" s="200"/>
+      <c r="FM4" s="200"/>
+      <c r="FN4" s="200"/>
+      <c r="FO4" s="201"/>
+      <c r="FP4" s="199" t="str">
         <f>"Week "&amp;(FI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 45</v>
       </c>
-      <c r="FQ4" s="197"/>
-      <c r="FR4" s="197"/>
-      <c r="FS4" s="197"/>
-      <c r="FT4" s="197"/>
-      <c r="FU4" s="197"/>
-      <c r="FV4" s="198"/>
-      <c r="FW4" s="196" t="str">
+      <c r="FQ4" s="200"/>
+      <c r="FR4" s="200"/>
+      <c r="FS4" s="200"/>
+      <c r="FT4" s="200"/>
+      <c r="FU4" s="200"/>
+      <c r="FV4" s="201"/>
+      <c r="FW4" s="199" t="str">
         <f>"Week "&amp;(FP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 46</v>
       </c>
-      <c r="FX4" s="197"/>
-      <c r="FY4" s="197"/>
-      <c r="FZ4" s="197"/>
-      <c r="GA4" s="197"/>
-      <c r="GB4" s="197"/>
-      <c r="GC4" s="198"/>
-      <c r="GD4" s="196" t="str">
+      <c r="FX4" s="200"/>
+      <c r="FY4" s="200"/>
+      <c r="FZ4" s="200"/>
+      <c r="GA4" s="200"/>
+      <c r="GB4" s="200"/>
+      <c r="GC4" s="201"/>
+      <c r="GD4" s="199" t="str">
         <f>"Week "&amp;(FW6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 47</v>
       </c>
-      <c r="GE4" s="197"/>
-      <c r="GF4" s="197"/>
-      <c r="GG4" s="197"/>
-      <c r="GH4" s="197"/>
-      <c r="GI4" s="197"/>
-      <c r="GJ4" s="198"/>
-      <c r="GK4" s="196" t="str">
+      <c r="GE4" s="200"/>
+      <c r="GF4" s="200"/>
+      <c r="GG4" s="200"/>
+      <c r="GH4" s="200"/>
+      <c r="GI4" s="200"/>
+      <c r="GJ4" s="201"/>
+      <c r="GK4" s="199" t="str">
         <f>"Week "&amp;(GD6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 48</v>
       </c>
-      <c r="GL4" s="197"/>
-      <c r="GM4" s="197"/>
-      <c r="GN4" s="197"/>
-      <c r="GO4" s="197"/>
-      <c r="GP4" s="197"/>
-      <c r="GQ4" s="198"/>
-      <c r="GR4" s="196" t="str">
+      <c r="GL4" s="200"/>
+      <c r="GM4" s="200"/>
+      <c r="GN4" s="200"/>
+      <c r="GO4" s="200"/>
+      <c r="GP4" s="200"/>
+      <c r="GQ4" s="201"/>
+      <c r="GR4" s="199" t="str">
         <f>"Week "&amp;(GK6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 49</v>
       </c>
-      <c r="GS4" s="197"/>
-      <c r="GT4" s="197"/>
-      <c r="GU4" s="197"/>
-      <c r="GV4" s="197"/>
-      <c r="GW4" s="197"/>
-      <c r="GX4" s="198"/>
-      <c r="GY4" s="196" t="str">
+      <c r="GS4" s="200"/>
+      <c r="GT4" s="200"/>
+      <c r="GU4" s="200"/>
+      <c r="GV4" s="200"/>
+      <c r="GW4" s="200"/>
+      <c r="GX4" s="201"/>
+      <c r="GY4" s="199" t="str">
         <f>"Week "&amp;(GR6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 50</v>
       </c>
-      <c r="GZ4" s="197"/>
-      <c r="HA4" s="197"/>
-      <c r="HB4" s="197"/>
-      <c r="HC4" s="197"/>
-      <c r="HD4" s="197"/>
-      <c r="HE4" s="198"/>
-      <c r="HF4" s="196" t="str">
+      <c r="GZ4" s="200"/>
+      <c r="HA4" s="200"/>
+      <c r="HB4" s="200"/>
+      <c r="HC4" s="200"/>
+      <c r="HD4" s="200"/>
+      <c r="HE4" s="201"/>
+      <c r="HF4" s="199" t="str">
         <f>"Week "&amp;(GY6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 51</v>
       </c>
-      <c r="HG4" s="197"/>
-      <c r="HH4" s="197"/>
-      <c r="HI4" s="197"/>
-      <c r="HJ4" s="197"/>
-      <c r="HK4" s="197"/>
-      <c r="HL4" s="198"/>
-      <c r="HM4" s="196" t="str">
+      <c r="HG4" s="200"/>
+      <c r="HH4" s="200"/>
+      <c r="HI4" s="200"/>
+      <c r="HJ4" s="200"/>
+      <c r="HK4" s="200"/>
+      <c r="HL4" s="201"/>
+      <c r="HM4" s="199" t="str">
         <f>"Week "&amp;(HF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 52</v>
       </c>
-      <c r="HN4" s="197"/>
-      <c r="HO4" s="197"/>
-      <c r="HP4" s="197"/>
-      <c r="HQ4" s="197"/>
-      <c r="HR4" s="197"/>
-      <c r="HS4" s="198"/>
-      <c r="HT4" s="196" t="str">
+      <c r="HN4" s="200"/>
+      <c r="HO4" s="200"/>
+      <c r="HP4" s="200"/>
+      <c r="HQ4" s="200"/>
+      <c r="HR4" s="200"/>
+      <c r="HS4" s="201"/>
+      <c r="HT4" s="199" t="str">
         <f>"Week "&amp;(HM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 53</v>
       </c>
-      <c r="HU4" s="197"/>
-      <c r="HV4" s="197"/>
-      <c r="HW4" s="197"/>
-      <c r="HX4" s="197"/>
-      <c r="HY4" s="197"/>
-      <c r="HZ4" s="198"/>
-      <c r="IA4" s="196" t="str">
+      <c r="HU4" s="200"/>
+      <c r="HV4" s="200"/>
+      <c r="HW4" s="200"/>
+      <c r="HX4" s="200"/>
+      <c r="HY4" s="200"/>
+      <c r="HZ4" s="201"/>
+      <c r="IA4" s="199" t="str">
         <f>"Week "&amp;(HT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 54</v>
       </c>
-      <c r="IB4" s="197"/>
-      <c r="IC4" s="197"/>
-      <c r="ID4" s="197"/>
-      <c r="IE4" s="197"/>
-      <c r="IF4" s="197"/>
-      <c r="IG4" s="198"/>
-      <c r="IH4" s="196" t="str">
+      <c r="IB4" s="200"/>
+      <c r="IC4" s="200"/>
+      <c r="ID4" s="200"/>
+      <c r="IE4" s="200"/>
+      <c r="IF4" s="200"/>
+      <c r="IG4" s="201"/>
+      <c r="IH4" s="199" t="str">
         <f>"Week "&amp;(IA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 55</v>
       </c>
-      <c r="II4" s="197"/>
-      <c r="IJ4" s="197"/>
-      <c r="IK4" s="197"/>
-      <c r="IL4" s="197"/>
-      <c r="IM4" s="197"/>
-      <c r="IN4" s="198"/>
-      <c r="IO4" s="196" t="str">
+      <c r="II4" s="200"/>
+      <c r="IJ4" s="200"/>
+      <c r="IK4" s="200"/>
+      <c r="IL4" s="200"/>
+      <c r="IM4" s="200"/>
+      <c r="IN4" s="201"/>
+      <c r="IO4" s="199" t="str">
         <f>"Week "&amp;(IH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 56</v>
       </c>
-      <c r="IP4" s="197"/>
-      <c r="IQ4" s="197"/>
-      <c r="IR4" s="197"/>
-      <c r="IS4" s="197"/>
-      <c r="IT4" s="197"/>
-      <c r="IU4" s="198"/>
+      <c r="IP4" s="200"/>
+      <c r="IQ4" s="200"/>
+      <c r="IR4" s="200"/>
+      <c r="IS4" s="200"/>
+      <c r="IT4" s="200"/>
+      <c r="IU4" s="201"/>
     </row>
-    <row r="5" spans="1:255" s="24" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:255" s="24" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
       <c r="B5" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="211" t="s">
+      <c r="C5" s="207" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="212"/>
-      <c r="E5" s="213"/>
+      <c r="D5" s="208"/>
+      <c r="E5" s="209"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
       <c r="H5" s="71"/>
       <c r="I5" s="71"/>
-      <c r="K5" s="214">
+      <c r="K5" s="210">
         <f>K6</f>
         <v>45446</v>
       </c>
-      <c r="L5" s="200"/>
-      <c r="M5" s="200"/>
-      <c r="N5" s="200"/>
-      <c r="O5" s="200"/>
-      <c r="P5" s="200"/>
-      <c r="Q5" s="216"/>
-      <c r="R5" s="214">
+      <c r="L5" s="197"/>
+      <c r="M5" s="197"/>
+      <c r="N5" s="197"/>
+      <c r="O5" s="197"/>
+      <c r="P5" s="197"/>
+      <c r="Q5" s="212"/>
+      <c r="R5" s="210">
         <f>R6</f>
         <v>45453</v>
       </c>
-      <c r="S5" s="200"/>
-      <c r="T5" s="200"/>
-      <c r="U5" s="200"/>
-      <c r="V5" s="200"/>
-      <c r="W5" s="200"/>
-      <c r="X5" s="215"/>
-      <c r="Y5" s="217">
+      <c r="S5" s="197"/>
+      <c r="T5" s="197"/>
+      <c r="U5" s="197"/>
+      <c r="V5" s="197"/>
+      <c r="W5" s="197"/>
+      <c r="X5" s="211"/>
+      <c r="Y5" s="213">
         <f>Y6</f>
         <v>45460</v>
       </c>
-      <c r="Z5" s="200"/>
-      <c r="AA5" s="200"/>
-      <c r="AB5" s="200"/>
-      <c r="AC5" s="200"/>
-      <c r="AD5" s="200"/>
-      <c r="AE5" s="218"/>
-      <c r="AF5" s="209">
+      <c r="Z5" s="197"/>
+      <c r="AA5" s="197"/>
+      <c r="AB5" s="197"/>
+      <c r="AC5" s="197"/>
+      <c r="AD5" s="197"/>
+      <c r="AE5" s="214"/>
+      <c r="AF5" s="205">
         <f>AF6</f>
         <v>45467</v>
       </c>
-      <c r="AG5" s="200"/>
-      <c r="AH5" s="200"/>
-      <c r="AI5" s="200"/>
-      <c r="AJ5" s="200"/>
-      <c r="AK5" s="200"/>
-      <c r="AL5" s="210"/>
-      <c r="AM5" s="202">
+      <c r="AG5" s="197"/>
+      <c r="AH5" s="197"/>
+      <c r="AI5" s="197"/>
+      <c r="AJ5" s="197"/>
+      <c r="AK5" s="197"/>
+      <c r="AL5" s="206"/>
+      <c r="AM5" s="215">
         <f>AM6</f>
         <v>45474</v>
       </c>
-      <c r="AN5" s="200"/>
-      <c r="AO5" s="200"/>
-      <c r="AP5" s="200"/>
-      <c r="AQ5" s="200"/>
-      <c r="AR5" s="200"/>
-      <c r="AS5" s="203"/>
-      <c r="AT5" s="204">
+      <c r="AN5" s="197"/>
+      <c r="AO5" s="197"/>
+      <c r="AP5" s="197"/>
+      <c r="AQ5" s="197"/>
+      <c r="AR5" s="197"/>
+      <c r="AS5" s="216"/>
+      <c r="AT5" s="217">
         <f>AT6</f>
         <v>45481</v>
       </c>
-      <c r="AU5" s="200"/>
-      <c r="AV5" s="200"/>
-      <c r="AW5" s="200"/>
-      <c r="AX5" s="200"/>
-      <c r="AY5" s="200"/>
-      <c r="AZ5" s="205"/>
-      <c r="BA5" s="206">
+      <c r="AU5" s="197"/>
+      <c r="AV5" s="197"/>
+      <c r="AW5" s="197"/>
+      <c r="AX5" s="197"/>
+      <c r="AY5" s="197"/>
+      <c r="AZ5" s="218"/>
+      <c r="BA5" s="196">
         <f>BA6</f>
         <v>45488</v>
       </c>
-      <c r="BB5" s="200"/>
-      <c r="BC5" s="200"/>
-      <c r="BD5" s="200"/>
-      <c r="BE5" s="200"/>
-      <c r="BF5" s="200"/>
-      <c r="BG5" s="207"/>
-      <c r="BH5" s="199">
+      <c r="BB5" s="197"/>
+      <c r="BC5" s="197"/>
+      <c r="BD5" s="197"/>
+      <c r="BE5" s="197"/>
+      <c r="BF5" s="197"/>
+      <c r="BG5" s="198"/>
+      <c r="BH5" s="202">
         <f>BH6</f>
         <v>45495</v>
       </c>
-      <c r="BI5" s="200"/>
-      <c r="BJ5" s="200"/>
-      <c r="BK5" s="200"/>
-      <c r="BL5" s="200"/>
-      <c r="BM5" s="200"/>
-      <c r="BN5" s="201"/>
-      <c r="BO5" s="206">
+      <c r="BI5" s="197"/>
+      <c r="BJ5" s="197"/>
+      <c r="BK5" s="197"/>
+      <c r="BL5" s="197"/>
+      <c r="BM5" s="197"/>
+      <c r="BN5" s="203"/>
+      <c r="BO5" s="196">
         <f>BO6</f>
         <v>45502</v>
       </c>
-      <c r="BP5" s="200"/>
-      <c r="BQ5" s="200"/>
-      <c r="BR5" s="200"/>
-      <c r="BS5" s="200"/>
-      <c r="BT5" s="200"/>
-      <c r="BU5" s="207"/>
-      <c r="BV5" s="199">
+      <c r="BP5" s="197"/>
+      <c r="BQ5" s="197"/>
+      <c r="BR5" s="197"/>
+      <c r="BS5" s="197"/>
+      <c r="BT5" s="197"/>
+      <c r="BU5" s="198"/>
+      <c r="BV5" s="202">
         <f>BV6</f>
         <v>45509</v>
       </c>
-      <c r="BW5" s="200"/>
-      <c r="BX5" s="200"/>
-      <c r="BY5" s="200"/>
-      <c r="BZ5" s="200"/>
-      <c r="CA5" s="200"/>
-      <c r="CB5" s="201"/>
-      <c r="CC5" s="199">
+      <c r="BW5" s="197"/>
+      <c r="BX5" s="197"/>
+      <c r="BY5" s="197"/>
+      <c r="BZ5" s="197"/>
+      <c r="CA5" s="197"/>
+      <c r="CB5" s="203"/>
+      <c r="CC5" s="202">
         <f>CC6</f>
         <v>45516</v>
       </c>
-      <c r="CD5" s="200"/>
-      <c r="CE5" s="200"/>
-      <c r="CF5" s="200"/>
-      <c r="CG5" s="200"/>
-      <c r="CH5" s="200"/>
-      <c r="CI5" s="201"/>
-      <c r="CJ5" s="206">
+      <c r="CD5" s="197"/>
+      <c r="CE5" s="197"/>
+      <c r="CF5" s="197"/>
+      <c r="CG5" s="197"/>
+      <c r="CH5" s="197"/>
+      <c r="CI5" s="203"/>
+      <c r="CJ5" s="196">
         <f>CJ6</f>
         <v>45523</v>
       </c>
-      <c r="CK5" s="200"/>
-      <c r="CL5" s="200"/>
-      <c r="CM5" s="200"/>
-      <c r="CN5" s="200"/>
-      <c r="CO5" s="200"/>
-      <c r="CP5" s="207"/>
-      <c r="CQ5" s="199">
+      <c r="CK5" s="197"/>
+      <c r="CL5" s="197"/>
+      <c r="CM5" s="197"/>
+      <c r="CN5" s="197"/>
+      <c r="CO5" s="197"/>
+      <c r="CP5" s="198"/>
+      <c r="CQ5" s="202">
         <f>CQ6</f>
         <v>45530</v>
       </c>
-      <c r="CR5" s="200"/>
-      <c r="CS5" s="200"/>
-      <c r="CT5" s="200"/>
-      <c r="CU5" s="200"/>
-      <c r="CV5" s="200"/>
-      <c r="CW5" s="201"/>
-      <c r="CX5" s="199">
+      <c r="CR5" s="197"/>
+      <c r="CS5" s="197"/>
+      <c r="CT5" s="197"/>
+      <c r="CU5" s="197"/>
+      <c r="CV5" s="197"/>
+      <c r="CW5" s="203"/>
+      <c r="CX5" s="202">
         <f>CX6</f>
         <v>45537</v>
       </c>
-      <c r="CY5" s="200"/>
-      <c r="CZ5" s="200"/>
-      <c r="DA5" s="200"/>
-      <c r="DB5" s="200"/>
-      <c r="DC5" s="200"/>
-      <c r="DD5" s="201"/>
-      <c r="DE5" s="206">
+      <c r="CY5" s="197"/>
+      <c r="CZ5" s="197"/>
+      <c r="DA5" s="197"/>
+      <c r="DB5" s="197"/>
+      <c r="DC5" s="197"/>
+      <c r="DD5" s="203"/>
+      <c r="DE5" s="196">
         <f>DE6</f>
         <v>45544</v>
       </c>
-      <c r="DF5" s="200"/>
-      <c r="DG5" s="200"/>
-      <c r="DH5" s="200"/>
-      <c r="DI5" s="200"/>
-      <c r="DJ5" s="200"/>
-      <c r="DK5" s="207"/>
-      <c r="DL5" s="199">
+      <c r="DF5" s="197"/>
+      <c r="DG5" s="197"/>
+      <c r="DH5" s="197"/>
+      <c r="DI5" s="197"/>
+      <c r="DJ5" s="197"/>
+      <c r="DK5" s="198"/>
+      <c r="DL5" s="202">
         <f>DL6</f>
         <v>45551</v>
       </c>
-      <c r="DM5" s="200"/>
-      <c r="DN5" s="200"/>
-      <c r="DO5" s="200"/>
-      <c r="DP5" s="200"/>
-      <c r="DQ5" s="200"/>
-      <c r="DR5" s="201"/>
-      <c r="DS5" s="199">
+      <c r="DM5" s="197"/>
+      <c r="DN5" s="197"/>
+      <c r="DO5" s="197"/>
+      <c r="DP5" s="197"/>
+      <c r="DQ5" s="197"/>
+      <c r="DR5" s="203"/>
+      <c r="DS5" s="202">
         <f>DS6</f>
         <v>45558</v>
       </c>
-      <c r="DT5" s="200"/>
-      <c r="DU5" s="200"/>
-      <c r="DV5" s="200"/>
-      <c r="DW5" s="200"/>
-      <c r="DX5" s="200"/>
-      <c r="DY5" s="201"/>
-      <c r="DZ5" s="206">
+      <c r="DT5" s="197"/>
+      <c r="DU5" s="197"/>
+      <c r="DV5" s="197"/>
+      <c r="DW5" s="197"/>
+      <c r="DX5" s="197"/>
+      <c r="DY5" s="203"/>
+      <c r="DZ5" s="196">
         <f>DZ6</f>
         <v>45565</v>
       </c>
-      <c r="EA5" s="200"/>
-      <c r="EB5" s="200"/>
-      <c r="EC5" s="200"/>
-      <c r="ED5" s="200"/>
-      <c r="EE5" s="200"/>
-      <c r="EF5" s="207"/>
-      <c r="EG5" s="199">
+      <c r="EA5" s="197"/>
+      <c r="EB5" s="197"/>
+      <c r="EC5" s="197"/>
+      <c r="ED5" s="197"/>
+      <c r="EE5" s="197"/>
+      <c r="EF5" s="198"/>
+      <c r="EG5" s="202">
         <f>EG6</f>
         <v>45572</v>
       </c>
-      <c r="EH5" s="200"/>
-      <c r="EI5" s="200"/>
-      <c r="EJ5" s="200"/>
-      <c r="EK5" s="200"/>
-      <c r="EL5" s="200"/>
-      <c r="EM5" s="201"/>
-      <c r="EN5" s="199">
+      <c r="EH5" s="197"/>
+      <c r="EI5" s="197"/>
+      <c r="EJ5" s="197"/>
+      <c r="EK5" s="197"/>
+      <c r="EL5" s="197"/>
+      <c r="EM5" s="203"/>
+      <c r="EN5" s="202">
         <f>EN6</f>
         <v>45579</v>
       </c>
-      <c r="EO5" s="200"/>
-      <c r="EP5" s="200"/>
-      <c r="EQ5" s="200"/>
-      <c r="ER5" s="200"/>
-      <c r="ES5" s="200"/>
-      <c r="ET5" s="201"/>
-      <c r="EU5" s="206">
+      <c r="EO5" s="197"/>
+      <c r="EP5" s="197"/>
+      <c r="EQ5" s="197"/>
+      <c r="ER5" s="197"/>
+      <c r="ES5" s="197"/>
+      <c r="ET5" s="203"/>
+      <c r="EU5" s="196">
         <f>EU6</f>
         <v>45586</v>
       </c>
-      <c r="EV5" s="200"/>
-      <c r="EW5" s="200"/>
-      <c r="EX5" s="200"/>
-      <c r="EY5" s="200"/>
-      <c r="EZ5" s="200"/>
-      <c r="FA5" s="207"/>
-      <c r="FB5" s="199">
+      <c r="EV5" s="197"/>
+      <c r="EW5" s="197"/>
+      <c r="EX5" s="197"/>
+      <c r="EY5" s="197"/>
+      <c r="EZ5" s="197"/>
+      <c r="FA5" s="198"/>
+      <c r="FB5" s="202">
         <f>FB6</f>
         <v>45593</v>
       </c>
-      <c r="FC5" s="200"/>
-      <c r="FD5" s="200"/>
-      <c r="FE5" s="200"/>
-      <c r="FF5" s="200"/>
-      <c r="FG5" s="200"/>
-      <c r="FH5" s="201"/>
-      <c r="FI5" s="199">
+      <c r="FC5" s="197"/>
+      <c r="FD5" s="197"/>
+      <c r="FE5" s="197"/>
+      <c r="FF5" s="197"/>
+      <c r="FG5" s="197"/>
+      <c r="FH5" s="203"/>
+      <c r="FI5" s="202">
         <f>FI6</f>
         <v>45600</v>
       </c>
-      <c r="FJ5" s="200"/>
-      <c r="FK5" s="200"/>
-      <c r="FL5" s="200"/>
-      <c r="FM5" s="200"/>
-      <c r="FN5" s="200"/>
-      <c r="FO5" s="201"/>
-      <c r="FP5" s="206">
+      <c r="FJ5" s="197"/>
+      <c r="FK5" s="197"/>
+      <c r="FL5" s="197"/>
+      <c r="FM5" s="197"/>
+      <c r="FN5" s="197"/>
+      <c r="FO5" s="203"/>
+      <c r="FP5" s="196">
         <f>FP6</f>
         <v>45607</v>
       </c>
-      <c r="FQ5" s="200"/>
-      <c r="FR5" s="200"/>
-      <c r="FS5" s="200"/>
-      <c r="FT5" s="200"/>
-      <c r="FU5" s="200"/>
-      <c r="FV5" s="207"/>
-      <c r="FW5" s="199">
+      <c r="FQ5" s="197"/>
+      <c r="FR5" s="197"/>
+      <c r="FS5" s="197"/>
+      <c r="FT5" s="197"/>
+      <c r="FU5" s="197"/>
+      <c r="FV5" s="198"/>
+      <c r="FW5" s="202">
         <f>FW6</f>
         <v>45614</v>
       </c>
-      <c r="FX5" s="200"/>
-      <c r="FY5" s="200"/>
-      <c r="FZ5" s="200"/>
-      <c r="GA5" s="200"/>
-      <c r="GB5" s="200"/>
-      <c r="GC5" s="201"/>
-      <c r="GD5" s="199">
+      <c r="FX5" s="197"/>
+      <c r="FY5" s="197"/>
+      <c r="FZ5" s="197"/>
+      <c r="GA5" s="197"/>
+      <c r="GB5" s="197"/>
+      <c r="GC5" s="203"/>
+      <c r="GD5" s="202">
         <f>GD6</f>
         <v>45621</v>
       </c>
-      <c r="GE5" s="200"/>
-      <c r="GF5" s="200"/>
-      <c r="GG5" s="200"/>
-      <c r="GH5" s="200"/>
-      <c r="GI5" s="200"/>
-      <c r="GJ5" s="201"/>
-      <c r="GK5" s="206">
+      <c r="GE5" s="197"/>
+      <c r="GF5" s="197"/>
+      <c r="GG5" s="197"/>
+      <c r="GH5" s="197"/>
+      <c r="GI5" s="197"/>
+      <c r="GJ5" s="203"/>
+      <c r="GK5" s="196">
         <f>GK6</f>
         <v>45628</v>
       </c>
-      <c r="GL5" s="200"/>
-      <c r="GM5" s="200"/>
-      <c r="GN5" s="200"/>
-      <c r="GO5" s="200"/>
-      <c r="GP5" s="200"/>
-      <c r="GQ5" s="207"/>
-      <c r="GR5" s="199">
+      <c r="GL5" s="197"/>
+      <c r="GM5" s="197"/>
+      <c r="GN5" s="197"/>
+      <c r="GO5" s="197"/>
+      <c r="GP5" s="197"/>
+      <c r="GQ5" s="198"/>
+      <c r="GR5" s="202">
         <f>GR6</f>
         <v>45635</v>
       </c>
-      <c r="GS5" s="200"/>
-      <c r="GT5" s="200"/>
-      <c r="GU5" s="200"/>
-      <c r="GV5" s="200"/>
-      <c r="GW5" s="200"/>
-      <c r="GX5" s="201"/>
-      <c r="GY5" s="206">
+      <c r="GS5" s="197"/>
+      <c r="GT5" s="197"/>
+      <c r="GU5" s="197"/>
+      <c r="GV5" s="197"/>
+      <c r="GW5" s="197"/>
+      <c r="GX5" s="203"/>
+      <c r="GY5" s="196">
         <f>GY6</f>
         <v>45642</v>
       </c>
-      <c r="GZ5" s="200"/>
-      <c r="HA5" s="200"/>
-      <c r="HB5" s="200"/>
-      <c r="HC5" s="200"/>
-      <c r="HD5" s="200"/>
-      <c r="HE5" s="207"/>
-      <c r="HF5" s="199">
+      <c r="GZ5" s="197"/>
+      <c r="HA5" s="197"/>
+      <c r="HB5" s="197"/>
+      <c r="HC5" s="197"/>
+      <c r="HD5" s="197"/>
+      <c r="HE5" s="198"/>
+      <c r="HF5" s="202">
         <f>HF6</f>
         <v>45649</v>
       </c>
-      <c r="HG5" s="200"/>
-      <c r="HH5" s="200"/>
-      <c r="HI5" s="200"/>
-      <c r="HJ5" s="200"/>
-      <c r="HK5" s="200"/>
-      <c r="HL5" s="201"/>
-      <c r="HM5" s="206">
+      <c r="HG5" s="197"/>
+      <c r="HH5" s="197"/>
+      <c r="HI5" s="197"/>
+      <c r="HJ5" s="197"/>
+      <c r="HK5" s="197"/>
+      <c r="HL5" s="203"/>
+      <c r="HM5" s="196">
         <f>HM6</f>
         <v>45656</v>
       </c>
-      <c r="HN5" s="200"/>
-      <c r="HO5" s="200"/>
-      <c r="HP5" s="200"/>
-      <c r="HQ5" s="200"/>
-      <c r="HR5" s="200"/>
-      <c r="HS5" s="207"/>
-      <c r="HT5" s="199">
+      <c r="HN5" s="197"/>
+      <c r="HO5" s="197"/>
+      <c r="HP5" s="197"/>
+      <c r="HQ5" s="197"/>
+      <c r="HR5" s="197"/>
+      <c r="HS5" s="198"/>
+      <c r="HT5" s="202">
         <f>HT6</f>
         <v>45663</v>
       </c>
-      <c r="HU5" s="200"/>
-      <c r="HV5" s="200"/>
-      <c r="HW5" s="200"/>
-      <c r="HX5" s="200"/>
-      <c r="HY5" s="200"/>
-      <c r="HZ5" s="201"/>
-      <c r="IA5" s="206">
+      <c r="HU5" s="197"/>
+      <c r="HV5" s="197"/>
+      <c r="HW5" s="197"/>
+      <c r="HX5" s="197"/>
+      <c r="HY5" s="197"/>
+      <c r="HZ5" s="203"/>
+      <c r="IA5" s="196">
         <f>IA6</f>
         <v>45670</v>
       </c>
-      <c r="IB5" s="200"/>
-      <c r="IC5" s="200"/>
-      <c r="ID5" s="200"/>
-      <c r="IE5" s="200"/>
-      <c r="IF5" s="200"/>
-      <c r="IG5" s="207"/>
-      <c r="IH5" s="199">
+      <c r="IB5" s="197"/>
+      <c r="IC5" s="197"/>
+      <c r="ID5" s="197"/>
+      <c r="IE5" s="197"/>
+      <c r="IF5" s="197"/>
+      <c r="IG5" s="198"/>
+      <c r="IH5" s="202">
         <f>IH6</f>
         <v>45677</v>
       </c>
-      <c r="II5" s="200"/>
-      <c r="IJ5" s="200"/>
-      <c r="IK5" s="200"/>
-      <c r="IL5" s="200"/>
-      <c r="IM5" s="200"/>
-      <c r="IN5" s="201"/>
-      <c r="IO5" s="206">
+      <c r="II5" s="197"/>
+      <c r="IJ5" s="197"/>
+      <c r="IK5" s="197"/>
+      <c r="IL5" s="197"/>
+      <c r="IM5" s="197"/>
+      <c r="IN5" s="203"/>
+      <c r="IO5" s="196">
         <f>IO6</f>
         <v>45684</v>
       </c>
-      <c r="IP5" s="200"/>
-      <c r="IQ5" s="200"/>
-      <c r="IR5" s="200"/>
-      <c r="IS5" s="200"/>
-      <c r="IT5" s="200"/>
-      <c r="IU5" s="207"/>
+      <c r="IP5" s="197"/>
+      <c r="IQ5" s="197"/>
+      <c r="IR5" s="197"/>
+      <c r="IS5" s="197"/>
+      <c r="IT5" s="197"/>
+      <c r="IU5" s="198"/>
     </row>
-    <row r="6" spans="1:255" s="22" customFormat="1" ht="8.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:255" s="22" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="84"/>
       <c r="K6" s="33">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="IU6" s="45"/>
     </row>
-    <row r="7" spans="1:255" s="21" customFormat="1" ht="21.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:255" s="21" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
@@ -6178,7 +6178,7 @@
       </c>
       <c r="IU7" s="31"/>
     </row>
-    <row r="8" spans="1:255" s="176" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:255" s="176" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="169" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -6440,7 +6440,7 @@
       <c r="IT8" s="172"/>
       <c r="IU8" s="172"/>
     </row>
-    <row r="9" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="143">
         <v>1</v>
       </c>
@@ -6713,7 +6713,7 @@
       <c r="IT9" s="152"/>
       <c r="IU9" s="152"/>
     </row>
-    <row r="10" spans="1:255" s="153" customFormat="1" ht="23.15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:255" s="153" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="143" t="str">
         <f t="shared" ref="A10:A19" si="18">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1</v>
@@ -6987,7 +6987,7 @@
       <c r="IT10" s="152"/>
       <c r="IU10" s="152"/>
     </row>
-    <row r="11" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.1</v>
@@ -7261,7 +7261,7 @@
       <c r="IT11" s="152"/>
       <c r="IU11" s="152"/>
     </row>
-    <row r="12" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.2</v>
@@ -7283,7 +7283,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="150">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="I12" s="187">
         <f>IF(OR(F12=0,E12=0),0,NETWORKDAYS(E12,F12))</f>
@@ -7536,7 +7536,7 @@
       <c r="IT12" s="152"/>
       <c r="IU12" s="152"/>
     </row>
-    <row r="13" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.3</v>
@@ -7557,7 +7557,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="150">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I13" s="187">
         <f>IF(OR(F13=0,E13=0),0,NETWORKDAYS(E13,F13))</f>
@@ -7810,7 +7810,7 @@
       <c r="IT13" s="152"/>
       <c r="IU13" s="152"/>
     </row>
-    <row r="14" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.4</v>
@@ -8087,7 +8087,7 @@
       <c r="IT14" s="152"/>
       <c r="IU14" s="152"/>
     </row>
-    <row r="15" spans="1:255" s="153" customFormat="1" ht="23.15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:255" s="153" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.5</v>
@@ -8364,7 +8364,7 @@
       <c r="IT15" s="152"/>
       <c r="IU15" s="152"/>
     </row>
-    <row r="16" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:255" s="153" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.6</v>
@@ -8640,7 +8640,7 @@
       <c r="IT16" s="152"/>
       <c r="IU16" s="152"/>
     </row>
-    <row r="17" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.7</v>
@@ -8916,7 +8916,7 @@
       <c r="IT17" s="152"/>
       <c r="IU17" s="152"/>
     </row>
-    <row r="18" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.8</v>
@@ -8937,7 +8937,7 @@
         <v>14</v>
       </c>
       <c r="H18" s="150">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I18" s="187">
         <f t="shared" si="20"/>
@@ -9190,7 +9190,7 @@
       <c r="IT18" s="152"/>
       <c r="IU18" s="152"/>
     </row>
-    <row r="19" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="143" t="str">
         <f t="shared" si="18"/>
         <v>1.1.9</v>
@@ -9466,7 +9466,7 @@
       <c r="IT19" s="152"/>
       <c r="IU19" s="152"/>
     </row>
-    <row r="20" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="143"/>
       <c r="B20" s="144" t="s">
         <v>31</v>
@@ -9740,7 +9740,7 @@
       <c r="IT20" s="152"/>
       <c r="IU20" s="152"/>
     </row>
-    <row r="21" spans="1:255" s="153" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:255" s="153" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="143"/>
       <c r="B21" s="144" t="s">
         <v>30</v>
@@ -10014,7 +10014,7 @@
       <c r="IT21" s="152"/>
       <c r="IU21" s="152"/>
     </row>
-    <row r="22" spans="1:255" s="93" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:255" s="93" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="159">
         <v>2</v>
       </c>
@@ -10275,7 +10275,7 @@
       <c r="IT22" s="92"/>
       <c r="IU22" s="92"/>
     </row>
-    <row r="23" spans="1:255" s="105" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:255" s="105" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="95">
         <v>2</v>
       </c>
@@ -10296,7 +10296,7 @@
         <v>77</v>
       </c>
       <c r="H23" s="102">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="I23" s="190">
         <f t="shared" ref="I23:I36" si="22">IF(OR(F23=0,E23=0),0,NETWORKDAYS(E23,F23))</f>
@@ -10549,7 +10549,7 @@
       <c r="IT23" s="104"/>
       <c r="IU23" s="104"/>
     </row>
-    <row r="24" spans="1:255" s="105" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:255" s="105" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="95">
         <v>2.1</v>
       </c>
@@ -10823,7 +10823,7 @@
       <c r="IT24" s="104"/>
       <c r="IU24" s="104"/>
     </row>
-    <row r="25" spans="1:255" s="105" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:255" s="105" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="95">
         <v>2.2000000000000002</v>
       </c>
@@ -11097,7 +11097,7 @@
       <c r="IT25" s="104"/>
       <c r="IU25" s="104"/>
     </row>
-    <row r="26" spans="1:255" s="105" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:255" s="105" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="95">
         <v>2.2999999999999998</v>
       </c>
@@ -11371,7 +11371,7 @@
       <c r="IT26" s="104"/>
       <c r="IU26" s="104"/>
     </row>
-    <row r="27" spans="1:255" s="105" customFormat="1" ht="21.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:255" s="105" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="95">
         <v>2.4</v>
       </c>
@@ -11645,7 +11645,7 @@
       <c r="IT27" s="104"/>
       <c r="IU27" s="104"/>
     </row>
-    <row r="28" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:255" s="105" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="95">
         <v>2.5</v>
       </c>
@@ -11919,7 +11919,7 @@
       <c r="IT28" s="104"/>
       <c r="IU28" s="104"/>
     </row>
-    <row r="29" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="95">
         <v>2.6</v>
       </c>
@@ -12195,7 +12195,7 @@
       <c r="IT29" s="104"/>
       <c r="IU29" s="104"/>
     </row>
-    <row r="30" spans="1:255" s="105" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:255" s="105" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="95">
         <v>2.7</v>
       </c>
@@ -12471,7 +12471,7 @@
       <c r="IT30" s="104"/>
       <c r="IU30" s="104"/>
     </row>
-    <row r="31" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:255" s="105" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A31" s="95">
         <v>2.8</v>
       </c>
@@ -12492,7 +12492,7 @@
         <v>20</v>
       </c>
       <c r="H31" s="102">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="I31" s="191">
         <f t="shared" si="22"/>
@@ -12745,7 +12745,7 @@
       <c r="IT31" s="104"/>
       <c r="IU31" s="104"/>
     </row>
-    <row r="32" spans="1:255" s="105" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:255" s="105" customFormat="1" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="95" t="s">
         <v>63</v>
       </c>
@@ -12766,7 +12766,7 @@
         <v>7</v>
       </c>
       <c r="H32" s="102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="191">
         <f t="shared" si="22"/>
@@ -13019,7 +13019,7 @@
       <c r="IT32" s="104"/>
       <c r="IU32" s="104"/>
     </row>
-    <row r="33" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="95" t="s">
         <v>64</v>
       </c>
@@ -13040,7 +13040,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="191">
         <f t="shared" si="22"/>
@@ -13293,7 +13293,7 @@
       <c r="IT33" s="104"/>
       <c r="IU33" s="104"/>
     </row>
-    <row r="34" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="95" t="s">
         <v>65</v>
       </c>
@@ -13314,7 +13314,7 @@
         <v>8</v>
       </c>
       <c r="H34" s="102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="191">
         <f t="shared" si="22"/>
@@ -13567,7 +13567,7 @@
       <c r="IT34" s="104"/>
       <c r="IU34" s="104"/>
     </row>
-    <row r="35" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B35" s="96" t="s">
         <v>36</v>
       </c>
@@ -13840,7 +13840,7 @@
       <c r="IT35" s="104"/>
       <c r="IU35" s="104"/>
     </row>
-    <row r="36" spans="1:255" s="105" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:255" s="105" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="95"/>
       <c r="B36" s="96" t="s">
         <v>35</v>
@@ -14113,7 +14113,7 @@
       <c r="IT36" s="104"/>
       <c r="IU36" s="104"/>
     </row>
-    <row r="37" spans="1:255" s="113" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:255" s="113" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="106">
         <v>3</v>
       </c>
@@ -14374,7 +14374,7 @@
       <c r="IT37" s="109"/>
       <c r="IU37" s="109"/>
     </row>
-    <row r="38" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="114">
         <v>3</v>
       </c>
@@ -14395,7 +14395,7 @@
         <v>73</v>
       </c>
       <c r="H38" s="118">
-        <v>0</v>
+        <v>0.78</v>
       </c>
       <c r="I38" s="184">
         <f t="shared" ref="I38:I48" si="24">IF(OR(F38=0,E38=0),0,NETWORKDAYS(E38,F38))</f>
@@ -14648,7 +14648,7 @@
       <c r="IT38" s="120"/>
       <c r="IU38" s="120"/>
     </row>
-    <row r="39" spans="1:255" s="121" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:255" s="121" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="114">
         <v>3.1</v>
       </c>
@@ -14669,7 +14669,7 @@
         <v>7</v>
       </c>
       <c r="H39" s="118">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I39" s="185">
         <f t="shared" si="24"/>
@@ -14922,7 +14922,7 @@
       <c r="IT39" s="120"/>
       <c r="IU39" s="120"/>
     </row>
-    <row r="40" spans="1:255" s="121" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:255" s="121" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="114">
         <v>3.2</v>
       </c>
@@ -15196,7 +15196,7 @@
       <c r="IT40" s="120"/>
       <c r="IU40" s="120"/>
     </row>
-    <row r="41" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="114">
         <v>3.3</v>
       </c>
@@ -15470,7 +15470,7 @@
       <c r="IT41" s="120"/>
       <c r="IU41" s="120"/>
     </row>
-    <row r="42" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="114">
         <v>3.3</v>
       </c>
@@ -15744,7 +15744,7 @@
       <c r="IT42" s="120"/>
       <c r="IU42" s="120"/>
     </row>
-    <row r="43" spans="1:255" s="121" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:255" s="121" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="114">
         <v>3.4</v>
       </c>
@@ -15759,17 +15759,17 @@
       </c>
       <c r="F43" s="116">
         <f>IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
-        <v>45495</v>
+        <v>45498</v>
       </c>
       <c r="G43" s="117">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H43" s="118">
-        <v>0.2</v>
+        <v>0.65</v>
       </c>
       <c r="I43" s="185">
         <f t="shared" si="24"/>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J43" s="119"/>
       <c r="K43" s="120"/>
@@ -16018,7 +16018,7 @@
       <c r="IT43" s="120"/>
       <c r="IU43" s="120"/>
     </row>
-    <row r="44" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="114" t="s">
         <v>66</v>
       </c>
@@ -16039,7 +16039,7 @@
         <v>6</v>
       </c>
       <c r="H44" s="118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="185">
         <f t="shared" si="24"/>
@@ -16292,7 +16292,7 @@
       <c r="IT44" s="120"/>
       <c r="IU44" s="120"/>
     </row>
-    <row r="45" spans="1:255" s="121" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:255" s="121" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="114" t="s">
         <v>67</v>
       </c>
@@ -16313,7 +16313,7 @@
         <v>5</v>
       </c>
       <c r="H45" s="118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="185">
         <f t="shared" si="24"/>
@@ -16566,7 +16566,7 @@
       <c r="IT45" s="120"/>
       <c r="IU45" s="120"/>
     </row>
-    <row r="46" spans="1:255" s="121" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:255" s="121" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="114" t="s">
         <v>68</v>
       </c>
@@ -16581,17 +16581,17 @@
       </c>
       <c r="F46" s="116">
         <f>IF(ISBLANK(E46)," - ",IF(G46=0,E46,E46+G46-1))</f>
-        <v>45495</v>
+        <v>45498</v>
       </c>
       <c r="G46" s="117">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H46" s="118">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I46" s="185">
         <f t="shared" si="24"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J46" s="119"/>
       <c r="K46" s="120"/>
@@ -16840,7 +16840,7 @@
       <c r="IT46" s="120"/>
       <c r="IU46" s="120"/>
     </row>
-    <row r="47" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="114"/>
       <c r="B47" s="154" t="s">
         <v>28</v>
@@ -16850,12 +16850,12 @@
       </c>
       <c r="D47" s="156"/>
       <c r="E47" s="115">
-        <f>E48-5</f>
-        <v>45497</v>
+        <f>E48-2</f>
+        <v>45500</v>
       </c>
       <c r="F47" s="116">
         <f>IF(ISBLANK(E47)," - ",IF(G47=0,E47,E47+G47-1))</f>
-        <v>45497</v>
+        <v>45500</v>
       </c>
       <c r="G47" s="117">
         <v>1</v>
@@ -16865,7 +16865,7 @@
       </c>
       <c r="I47" s="185">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" s="119"/>
       <c r="K47" s="120"/>
@@ -17114,7 +17114,7 @@
       <c r="IT47" s="120"/>
       <c r="IU47" s="120"/>
     </row>
-    <row r="48" spans="1:255" s="121" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:255" s="121" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="114"/>
       <c r="B48" s="154" t="s">
         <v>29</v>
@@ -17388,7 +17388,7 @@
       <c r="IT48" s="120"/>
       <c r="IU48" s="120"/>
     </row>
-    <row r="49" spans="1:255" s="131" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:255" s="131" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="122">
         <v>4</v>
       </c>
@@ -17649,7 +17649,7 @@
       <c r="IT49" s="125"/>
       <c r="IU49" s="125"/>
     </row>
-    <row r="50" spans="1:255" s="142" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:255" s="142" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
@@ -17924,7 +17924,7 @@
       <c r="IT50" s="141"/>
       <c r="IU50" s="141"/>
     </row>
-    <row r="51" spans="1:255" s="142" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:255" s="142" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.1</v>
@@ -18201,7 +18201,7 @@
       <c r="IT51" s="141"/>
       <c r="IU51" s="141"/>
     </row>
-    <row r="52" spans="1:255" s="142" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:255" s="142" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.2</v>
@@ -18478,7 +18478,7 @@
       <c r="IT52" s="141"/>
       <c r="IU52" s="141"/>
     </row>
-    <row r="53" spans="1:255" s="142" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:255" s="142" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="132" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.1.3</v>
@@ -18755,7 +18755,7 @@
       <c r="IT53" s="141"/>
       <c r="IU53" s="141"/>
     </row>
-    <row r="55" spans="1:255" s="9" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:255" s="9" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="65" t="s">
         <v>1</v>
       </c>
@@ -19014,7 +19014,7 @@
       <c r="IT55" s="3"/>
       <c r="IU55" s="3"/>
     </row>
-    <row r="56" spans="1:255" s="8" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:255" s="8" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A56" s="66" t="s">
         <v>16</v>
       </c>
@@ -19269,7 +19269,7 @@
       <c r="IT56" s="3"/>
       <c r="IU56" s="3"/>
     </row>
-    <row r="57" spans="1:255" s="8" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:255" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="54" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -19533,7 +19533,7 @@
       <c r="IT57" s="3"/>
       <c r="IU57" s="3"/>
     </row>
-    <row r="58" spans="1:255" s="8" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:255" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -19805,7 +19805,7 @@
       <c r="IT58" s="3"/>
       <c r="IU58" s="3"/>
     </row>
-    <row r="59" spans="1:255" s="8" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:255" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -20077,7 +20077,7 @@
       <c r="IT59" s="3"/>
       <c r="IU59" s="3"/>
     </row>
-    <row r="60" spans="1:255" s="8" customFormat="1" ht="17.600000000000001" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:255" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
@@ -20347,7 +20347,7 @@
       <c r="IT60" s="3"/>
       <c r="IU60" s="3"/>
     </row>
-    <row r="61" spans="1:255" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:255" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="80" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
@@ -20357,25 +20357,54 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:255" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="73">
-    <mergeCell ref="IO5:IU5"/>
-    <mergeCell ref="IO4:IU4"/>
-    <mergeCell ref="HT4:HZ4"/>
-    <mergeCell ref="IA4:IG4"/>
-    <mergeCell ref="IH4:IN4"/>
-    <mergeCell ref="HM5:HS5"/>
-    <mergeCell ref="HT5:HZ5"/>
-    <mergeCell ref="IA5:IG5"/>
-    <mergeCell ref="IH5:IN5"/>
-    <mergeCell ref="GY4:HE4"/>
-    <mergeCell ref="HF4:HL4"/>
-    <mergeCell ref="GY5:HE5"/>
-    <mergeCell ref="HF5:HL5"/>
-    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="BH4:BN4"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="AM5:AS5"/>
+    <mergeCell ref="AT4:AZ4"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="BA4:BG4"/>
+    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="AD1:AR1"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="AF5:AL5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="FI4:FO4"/>
+    <mergeCell ref="FP4:FV4"/>
+    <mergeCell ref="EG4:EM4"/>
+    <mergeCell ref="CX5:DD5"/>
+    <mergeCell ref="DE5:DK5"/>
+    <mergeCell ref="DL5:DR5"/>
+    <mergeCell ref="DS5:DY5"/>
+    <mergeCell ref="DZ5:EF5"/>
+    <mergeCell ref="EG5:EM5"/>
+    <mergeCell ref="CX4:DD4"/>
+    <mergeCell ref="DE4:DK4"/>
+    <mergeCell ref="DL4:DR4"/>
+    <mergeCell ref="DS4:DY4"/>
+    <mergeCell ref="DZ4:EF4"/>
     <mergeCell ref="FW4:GC4"/>
     <mergeCell ref="GD4:GJ4"/>
     <mergeCell ref="GK4:GQ4"/>
@@ -20392,49 +20421,20 @@
     <mergeCell ref="EN4:ET4"/>
     <mergeCell ref="EU4:FA4"/>
     <mergeCell ref="FB4:FH4"/>
-    <mergeCell ref="FI4:FO4"/>
-    <mergeCell ref="FP4:FV4"/>
-    <mergeCell ref="EG4:EM4"/>
-    <mergeCell ref="CX5:DD5"/>
-    <mergeCell ref="DE5:DK5"/>
-    <mergeCell ref="DL5:DR5"/>
-    <mergeCell ref="DS5:DY5"/>
-    <mergeCell ref="DZ5:EF5"/>
-    <mergeCell ref="EG5:EM5"/>
-    <mergeCell ref="CX4:DD4"/>
-    <mergeCell ref="DE4:DK4"/>
-    <mergeCell ref="DL4:DR4"/>
-    <mergeCell ref="DS4:DY4"/>
-    <mergeCell ref="DZ4:EF4"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ5:CW5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="AD1:AR1"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AF5:AL5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="HM5:HS5"/>
+    <mergeCell ref="HT5:HZ5"/>
+    <mergeCell ref="IA5:IG5"/>
+    <mergeCell ref="IH5:IN5"/>
+    <mergeCell ref="GY4:HE4"/>
+    <mergeCell ref="HF4:HL4"/>
+    <mergeCell ref="GY5:HE5"/>
+    <mergeCell ref="HF5:HL5"/>
+    <mergeCell ref="HM4:HS4"/>
+    <mergeCell ref="IO5:IU5"/>
+    <mergeCell ref="IO4:IU4"/>
+    <mergeCell ref="HT4:HZ4"/>
+    <mergeCell ref="IA4:IG4"/>
+    <mergeCell ref="IH4:IN4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H56:H60 H8:H53">
@@ -20482,7 +20482,7 @@
   <pageSetup paperSize="9" scale="53" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="I9 B56 B55 F22 F37 F49 E55:I56 E59:E60 E57:I57 H50:I50 H38:I38 H22:I22 H37:I37 H49:I49" unlockedFormula="1"/>
+    <ignoredError sqref="I9 B56 B55 F22 F37 F49 E55:I56 E59:E60 E57:I57 H50:I50 I38 H22:I22 H37:I37 H49:I49" unlockedFormula="1"/>
     <ignoredError sqref="E32" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
@@ -20497,13 +20497,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>10886</xdr:colOff>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>28</xdr:col>
-                    <xdr:colOff>103414</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>

</xml_diff>